<commit_message>
Implement food vouchers for treated DS-TB and MDR-TB cases
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="73">
   <si>
     <t>parameter</t>
   </si>
@@ -237,6 +237,12 @@
   </si>
   <si>
     <t>program_perc_secondline_dst</t>
+  </si>
+  <si>
+    <t>program_perc_food_voucher_ds</t>
+  </si>
+  <si>
+    <t>program_perc_food_voucher_mdr</t>
   </si>
 </sst>
 </file>
@@ -353,7 +359,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2384,13 +2390,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BR24"/>
+  <dimension ref="A1:BR26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AZ2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="BJ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BB16" sqref="BB16"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3089,9 +3095,7 @@
       <c r="BF16" s="13"/>
       <c r="BG16" s="13"/>
       <c r="BH16" s="13"/>
-      <c r="BJ16" s="13">
-        <v>80</v>
-      </c>
+      <c r="BJ16" s="13"/>
       <c r="BK16" s="13"/>
       <c r="BM16" s="13">
         <v>80</v>
@@ -3103,7 +3107,7 @@
     </row>
     <row r="17" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>4</v>
@@ -3114,164 +3118,29 @@
       <c r="D17" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="6">
-        <v>1</v>
-      </c>
-      <c r="F17" s="14">
-        <v>1</v>
-      </c>
-      <c r="G17" s="14">
-        <v>1.1289570744394</v>
-      </c>
-      <c r="H17" s="14">
-        <v>1.42215881727406</v>
-      </c>
-      <c r="I17" s="14">
-        <v>1.90118931222233</v>
-      </c>
-      <c r="J17" s="14">
-        <v>2.3081073919986701</v>
-      </c>
-      <c r="K17" s="14">
-        <v>2.4974653103104298</v>
-      </c>
-      <c r="L17" s="14">
-        <v>2.9115458645382701</v>
-      </c>
-      <c r="M17" s="14">
-        <v>3.90623450399154</v>
-      </c>
-      <c r="N17" s="14">
-        <v>4.1703507493909102</v>
-      </c>
-      <c r="O17" s="14">
-        <v>4.55399078719985</v>
-      </c>
-      <c r="P17" s="14">
-        <v>5.0047790229916798</v>
-      </c>
-      <c r="Q17" s="14">
-        <v>5.3718558386314896</v>
-      </c>
-      <c r="R17" s="14">
-        <v>6.3137212289735496</v>
-      </c>
-      <c r="S17" s="14">
-        <v>7.4628507238053698</v>
-      </c>
-      <c r="T17" s="14">
-        <v>8.4391855224587609</v>
-      </c>
-      <c r="U17" s="14">
-        <v>9.3018160392078606</v>
-      </c>
-      <c r="V17" s="14">
-        <v>10.2347283365258</v>
-      </c>
-      <c r="W17" s="14">
-        <v>15.386785740408699</v>
-      </c>
-      <c r="X17" s="14">
-        <v>18.9416113416321</v>
-      </c>
-      <c r="Y17" s="14">
-        <v>19.1590871369295</v>
-      </c>
-      <c r="Z17" s="14">
-        <v>19.938817427385899</v>
-      </c>
-      <c r="AA17" s="14">
-        <v>22.702351313969601</v>
-      </c>
-      <c r="AB17" s="14">
-        <v>25.481798063623799</v>
-      </c>
-      <c r="AC17" s="14">
-        <v>28.584806362378998</v>
-      </c>
-      <c r="AD17" s="14">
-        <v>34.090656984785603</v>
-      </c>
-      <c r="AE17" s="14">
-        <v>37.0398409405256</v>
-      </c>
-      <c r="AF17" s="14">
-        <v>39.527551867219898</v>
-      </c>
-      <c r="AG17" s="14">
-        <v>43.633070539419101</v>
-      </c>
-      <c r="AH17" s="14">
-        <v>46.6140802213001</v>
-      </c>
-      <c r="AI17" s="14">
-        <v>50.0989972337483</v>
-      </c>
-      <c r="AJ17" s="14">
-        <v>52.899661134163203</v>
-      </c>
-      <c r="AK17" s="14">
-        <v>57.784910096818798</v>
-      </c>
-      <c r="AL17" s="14">
-        <v>61.2167842323652</v>
-      </c>
-      <c r="AM17" s="14">
-        <v>63.651452282157699</v>
-      </c>
-      <c r="AN17" s="14">
-        <v>67.053941908713696</v>
-      </c>
-      <c r="AO17" s="14">
-        <v>68.8796680497925</v>
-      </c>
-      <c r="AP17" s="14">
-        <v>70.456431535269701</v>
-      </c>
-      <c r="AQ17" s="14">
-        <v>73.858921161825705</v>
-      </c>
-      <c r="AR17" s="14">
-        <v>78.6721991701245</v>
-      </c>
-      <c r="AS17" s="14">
-        <v>82.987551867219906</v>
-      </c>
-      <c r="AT17" s="14">
-        <v>85.394190871369304</v>
-      </c>
-      <c r="AU17" s="14">
-        <v>92.448132780083</v>
-      </c>
-      <c r="AV17" s="14">
-        <v>96.348547717842294</v>
-      </c>
-      <c r="AW17" s="14">
+      <c r="AW17" s="7">
+        <v>20</v>
+      </c>
+      <c r="BE17" s="13"/>
+      <c r="BF17" s="13"/>
+      <c r="BG17" s="13"/>
+      <c r="BH17" s="13"/>
+      <c r="BJ17" s="13"/>
+      <c r="BK17" s="13"/>
+      <c r="BM17" s="13">
+        <v>80</v>
+      </c>
+      <c r="BN17" s="13"/>
+      <c r="BP17" s="7">
         <v>100</v>
       </c>
-      <c r="AX17" s="14">
-        <v>104.647302904564</v>
-      </c>
-      <c r="AY17" s="14">
-        <v>107.966804979253</v>
-      </c>
-      <c r="AZ17" s="14">
-        <v>111.203319502075</v>
-      </c>
-      <c r="BA17" s="14">
-        <v>115.767634854772</v>
-      </c>
-      <c r="BB17" s="14">
-        <v>117.42738589211601</v>
-      </c>
-      <c r="BP17" s="13"/>
     </row>
     <row r="18" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C18" s="5">
         <v>1</v>
@@ -3279,29 +3148,26 @@
       <c r="D18" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AB18" s="7">
-        <v>0</v>
-      </c>
-      <c r="AK18" s="7">
-        <v>3.1</v>
-      </c>
-      <c r="AP18" s="7">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="AU18" s="7">
-        <v>5.2</v>
-      </c>
-      <c r="AZ18" s="7">
-        <v>5.4</v>
-      </c>
-      <c r="BB18" s="7">
-        <v>5.9</v>
-      </c>
-      <c r="BP18" s="13"/>
+      <c r="AW18" s="7">
+        <v>100</v>
+      </c>
+      <c r="BE18" s="13"/>
+      <c r="BF18" s="13"/>
+      <c r="BG18" s="13"/>
+      <c r="BH18" s="13"/>
+      <c r="BJ18" s="13"/>
+      <c r="BK18" s="13"/>
+      <c r="BM18" s="13">
+        <v>80</v>
+      </c>
+      <c r="BN18" s="13"/>
+      <c r="BP18" s="7">
+        <v>100</v>
+      </c>
     </row>
     <row r="19" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>4</v>
@@ -3312,20 +3178,164 @@
       <c r="D19" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AW19" s="7">
-        <v>0.112</v>
-      </c>
-      <c r="BB19" s="7">
-        <v>0.153</v>
+      <c r="E19" s="6">
+        <v>1</v>
+      </c>
+      <c r="F19" s="14">
+        <v>1</v>
+      </c>
+      <c r="G19" s="14">
+        <v>1.1289570744394</v>
+      </c>
+      <c r="H19" s="14">
+        <v>1.42215881727406</v>
+      </c>
+      <c r="I19" s="14">
+        <v>1.90118931222233</v>
+      </c>
+      <c r="J19" s="14">
+        <v>2.3081073919986701</v>
+      </c>
+      <c r="K19" s="14">
+        <v>2.4974653103104298</v>
+      </c>
+      <c r="L19" s="14">
+        <v>2.9115458645382701</v>
+      </c>
+      <c r="M19" s="14">
+        <v>3.90623450399154</v>
+      </c>
+      <c r="N19" s="14">
+        <v>4.1703507493909102</v>
+      </c>
+      <c r="O19" s="14">
+        <v>4.55399078719985</v>
+      </c>
+      <c r="P19" s="14">
+        <v>5.0047790229916798</v>
+      </c>
+      <c r="Q19" s="14">
+        <v>5.3718558386314896</v>
+      </c>
+      <c r="R19" s="14">
+        <v>6.3137212289735496</v>
+      </c>
+      <c r="S19" s="14">
+        <v>7.4628507238053698</v>
+      </c>
+      <c r="T19" s="14">
+        <v>8.4391855224587609</v>
+      </c>
+      <c r="U19" s="14">
+        <v>9.3018160392078606</v>
+      </c>
+      <c r="V19" s="14">
+        <v>10.2347283365258</v>
+      </c>
+      <c r="W19" s="14">
+        <v>15.386785740408699</v>
+      </c>
+      <c r="X19" s="14">
+        <v>18.9416113416321</v>
+      </c>
+      <c r="Y19" s="14">
+        <v>19.1590871369295</v>
+      </c>
+      <c r="Z19" s="14">
+        <v>19.938817427385899</v>
+      </c>
+      <c r="AA19" s="14">
+        <v>22.702351313969601</v>
+      </c>
+      <c r="AB19" s="14">
+        <v>25.481798063623799</v>
+      </c>
+      <c r="AC19" s="14">
+        <v>28.584806362378998</v>
+      </c>
+      <c r="AD19" s="14">
+        <v>34.090656984785603</v>
+      </c>
+      <c r="AE19" s="14">
+        <v>37.0398409405256</v>
+      </c>
+      <c r="AF19" s="14">
+        <v>39.527551867219898</v>
+      </c>
+      <c r="AG19" s="14">
+        <v>43.633070539419101</v>
+      </c>
+      <c r="AH19" s="14">
+        <v>46.6140802213001</v>
+      </c>
+      <c r="AI19" s="14">
+        <v>50.0989972337483</v>
+      </c>
+      <c r="AJ19" s="14">
+        <v>52.899661134163203</v>
+      </c>
+      <c r="AK19" s="14">
+        <v>57.784910096818798</v>
+      </c>
+      <c r="AL19" s="14">
+        <v>61.2167842323652</v>
+      </c>
+      <c r="AM19" s="14">
+        <v>63.651452282157699</v>
+      </c>
+      <c r="AN19" s="14">
+        <v>67.053941908713696</v>
+      </c>
+      <c r="AO19" s="14">
+        <v>68.8796680497925</v>
+      </c>
+      <c r="AP19" s="14">
+        <v>70.456431535269701</v>
+      </c>
+      <c r="AQ19" s="14">
+        <v>73.858921161825705</v>
+      </c>
+      <c r="AR19" s="14">
+        <v>78.6721991701245</v>
+      </c>
+      <c r="AS19" s="14">
+        <v>82.987551867219906</v>
+      </c>
+      <c r="AT19" s="14">
+        <v>85.394190871369304</v>
+      </c>
+      <c r="AU19" s="14">
+        <v>92.448132780083</v>
+      </c>
+      <c r="AV19" s="14">
+        <v>96.348547717842294</v>
+      </c>
+      <c r="AW19" s="14">
+        <v>100</v>
+      </c>
+      <c r="AX19" s="14">
+        <v>104.647302904564</v>
+      </c>
+      <c r="AY19" s="14">
+        <v>107.966804979253</v>
+      </c>
+      <c r="AZ19" s="14">
+        <v>111.203319502075</v>
+      </c>
+      <c r="BA19" s="14">
+        <v>115.767634854772</v>
+      </c>
+      <c r="BB19" s="14">
+        <v>117.42738589211601</v>
       </c>
       <c r="BP19" s="13"/>
     </row>
     <row r="20" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20" s="5">
         <v>1</v>
@@ -3333,84 +3343,102 @@
       <c r="D20" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="AB20" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK20" s="7">
+        <v>3.1</v>
+      </c>
+      <c r="AP20" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AU20" s="7">
+        <v>5.2</v>
+      </c>
+      <c r="AZ20" s="7">
+        <v>5.4</v>
+      </c>
       <c r="BB20" s="7">
+        <v>5.9</v>
+      </c>
+      <c r="BP20" s="13"/>
+    </row>
+    <row r="21" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AW21" s="7">
+        <v>0.112</v>
+      </c>
+      <c r="BB21" s="7">
+        <v>0.153</v>
+      </c>
+      <c r="BP21" s="13"/>
+    </row>
+    <row r="22" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BB22" s="7">
         <f>4.5/98 * 100</f>
         <v>4.591836734693878</v>
       </c>
-      <c r="BN20" s="13">
+      <c r="BN22" s="13">
         <v>2.2999999999999998</v>
       </c>
-      <c r="BP20" s="13"/>
-      <c r="BQ20" s="7">
-        <f>BB20/2</f>
+      <c r="BP22" s="13"/>
+      <c r="BQ22" s="7">
+        <f>BB22/2</f>
         <v>2.295918367346939</v>
       </c>
     </row>
-    <row r="21" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+    <row r="23" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B23" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C23" s="5">
         <v>1</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="BB21" s="7">
+      <c r="BB23" s="7">
         <f>10/98 * 100</f>
         <v>10.204081632653061</v>
       </c>
-      <c r="BN21" s="13">
+      <c r="BN23" s="13">
         <v>5.0999999999999996</v>
       </c>
-      <c r="BP21" s="13"/>
-      <c r="BR21" s="7">
-        <f>BB21/2</f>
+      <c r="BP23" s="13"/>
+      <c r="BR23" s="7">
+        <f>BB23/2</f>
         <v>5.1020408163265305</v>
       </c>
-    </row>
-    <row r="22" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="5">
-        <v>1</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="BB22" s="7">
-        <v>0.4</v>
-      </c>
-      <c r="BP22" s="13"/>
-    </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="5">
-        <v>1</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="BB23" s="7">
-        <v>0.4</v>
-      </c>
-      <c r="BP23" s="13"/>
     </row>
     <row r="24" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>4</v>
@@ -3421,34 +3449,70 @@
       <c r="D24" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="7">
+      <c r="BB24" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="BP24" s="13"/>
+    </row>
+    <row r="25" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BB25" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="BP25" s="13"/>
+    </row>
+    <row r="26" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" s="7">
         <v>0</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G26" s="7">
         <v>30</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I26" s="7">
         <v>50</v>
       </c>
-      <c r="S24" s="7">
+      <c r="S26" s="7">
         <v>50</v>
       </c>
-      <c r="AM24" s="7">
+      <c r="AM26" s="7">
         <v>50</v>
       </c>
-      <c r="AR24" s="7">
+      <c r="AR26" s="7">
         <v>53</v>
       </c>
-      <c r="AW24" s="7">
+      <c r="AW26" s="7">
         <v>55</v>
       </c>
-      <c r="AZ24" s="7">
+      <c r="AZ26" s="7">
         <v>60</v>
       </c>
-      <c r="BB24" s="7">
+      <c r="BB26" s="7">
         <v>62</v>
       </c>
-      <c r="BP24" s="13"/>
+      <c r="BP26" s="13"/>
     </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="4">
@@ -3461,7 +3525,7 @@
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C28:C1048576 C2:C24">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C28:C1048576 C2:C26">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -3481,7 +3545,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D28:D1048576 D16:D24 D2:D13</xm:sqref>
+          <xm:sqref>D28:D1048576 D2:D13 D16:D26</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
First calibration for Bulgaria
Stratified by age, mdr/ds, prison, rural_poor
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="73">
   <si>
     <t>parameter</t>
   </si>
@@ -110,9 +110,6 @@
     <t>demo_household_size</t>
   </si>
   <si>
-    <t>Philippines average houshold size in 2010 https://psa.gov.ph/content/household-population-philippines-reaches-921-million</t>
-  </si>
-  <si>
     <t>program_prop_child_reporting</t>
   </si>
   <si>
@@ -243,6 +240,9 @@
   </si>
   <si>
     <t>program_perc_food_voucher_mdr</t>
+  </si>
+  <si>
+    <t>epi_rr_diabetes</t>
   </si>
 </sst>
 </file>
@@ -339,7 +339,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -360,6 +360,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1123,7 +1129,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1166,6 +1172,13 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="665">
     <cellStyle name="Comma" xfId="664" builtinId="3"/>
@@ -1856,8 +1869,8 @@
       <sheetName val="dropdown_lists"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
@@ -2156,8 +2169,8 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2184,13 +2197,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="16">
-        <v>21</v>
-      </c>
-      <c r="C2" s="17">
-        <v>12</v>
-      </c>
-      <c r="D2" s="17">
-        <v>50</v>
+        <v>10.35</v>
       </c>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
@@ -2207,17 +2214,17 @@
     </row>
     <row r="4" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="19">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
     </row>
     <row r="5" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="19">
         <v>5</v>
@@ -2233,7 +2240,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="21">
-        <v>25800000</v>
+        <v>12200000</v>
       </c>
       <c r="F6" s="22"/>
       <c r="G6" s="22"/>
@@ -2243,15 +2250,12 @@
         <v>27</v>
       </c>
       <c r="B7" s="23">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>28</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="19">
         <v>1.5</v>
@@ -2259,7 +2263,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="19">
         <f>1/3</f>
@@ -2268,7 +2272,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="25">
         <v>26.22</v>
@@ -2279,7 +2283,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="25">
         <v>0</v>
@@ -2290,7 +2294,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="25">
         <v>265450</v>
@@ -2301,7 +2305,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="25">
         <v>3</v>
@@ -2312,7 +2316,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="25">
         <v>1</v>
@@ -2323,7 +2327,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="25">
         <v>26.24</v>
@@ -2334,7 +2338,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="14">
         <v>0</v>
@@ -2342,7 +2346,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="26">
         <v>11575186.195826644</v>
@@ -2350,7 +2354,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" s="14">
         <v>3</v>
@@ -2358,7 +2362,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" s="14">
         <v>1</v>
@@ -2390,13 +2394,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BR26"/>
+  <dimension ref="A1:BR27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="BJ2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AB5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="AC20" sqref="AC20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2417,7 +2421,8 @@
     <col min="34" max="34" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
     <col min="35" max="38" width="7.44140625" style="7" customWidth="1"/>
     <col min="39" max="39" width="7.5546875" style="7" customWidth="1"/>
-    <col min="40" max="50" width="7" style="7" customWidth="1"/>
+    <col min="40" max="49" width="7" style="7" customWidth="1"/>
+    <col min="50" max="50" width="8.88671875" style="7" customWidth="1"/>
     <col min="51" max="52" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
     <col min="53" max="54" width="7.88671875" style="7" customWidth="1"/>
     <col min="55" max="56" width="14" style="7" customWidth="1"/>
@@ -2612,34 +2617,34 @@
         <v>17</v>
       </c>
       <c r="BI1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="BJ1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="BJ1" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="BK1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="BL1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BM1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="BM1" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="BN1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="BO1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="BO1" s="2" t="s">
+      <c r="BP1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="BP1" s="2" t="s">
+      <c r="BQ1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="BR1" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="BQ1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="BR1" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:70" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -2751,11 +2756,8 @@
         <v>3</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="AW5" s="9">
+      <c r="BB5" s="9">
         <v>0</v>
-      </c>
-      <c r="AY5" s="9">
-        <v>2.8</v>
       </c>
       <c r="BD5" s="27">
         <v>99</v>
@@ -2767,7 +2769,7 @@
     </row>
     <row r="6" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>4</v>
@@ -2795,7 +2797,7 @@
     </row>
     <row r="7" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>4</v>
@@ -2817,7 +2819,7 @@
     </row>
     <row r="8" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>4</v>
@@ -2845,7 +2847,7 @@
     </row>
     <row r="9" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>4</v>
@@ -2873,7 +2875,7 @@
     </row>
     <row r="10" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>4</v>
@@ -2902,7 +2904,7 @@
     </row>
     <row r="11" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>4</v>
@@ -2933,7 +2935,7 @@
     </row>
     <row r="12" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>4</v>
@@ -2962,7 +2964,7 @@
     </row>
     <row r="13" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>4</v>
@@ -2991,13 +2993,13 @@
     </row>
     <row r="14" spans="1:70" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B14" s="29" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="29">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>3</v>
@@ -3010,9 +3012,7 @@
       <c r="J14" s="30"/>
       <c r="K14" s="30"/>
       <c r="L14" s="30"/>
-      <c r="M14" s="30">
-        <v>30</v>
-      </c>
+      <c r="M14" s="30"/>
       <c r="N14" s="30"/>
       <c r="O14" s="30"/>
       <c r="P14" s="30"/>
@@ -3021,21 +3021,46 @@
       <c r="S14" s="30"/>
       <c r="T14" s="30"/>
       <c r="U14" s="30"/>
-      <c r="V14" s="30">
-        <v>50</v>
-      </c>
+      <c r="V14" s="30"/>
       <c r="W14" s="30"/>
       <c r="X14" s="30"/>
       <c r="Y14" s="30"/>
       <c r="Z14" s="30"/>
       <c r="AA14" s="30"/>
+      <c r="AB14" s="31">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="31">
+        <v>5</v>
+      </c>
+      <c r="AW14" s="31">
+        <f>80*(1174/2649)</f>
+        <v>35.454888637221593</v>
+      </c>
+      <c r="AX14" s="31">
+        <f>80*(1077/2407)</f>
+        <v>35.795596177814708</v>
+      </c>
+      <c r="AY14" s="31">
+        <f>80*(1094/2280)</f>
+        <v>38.385964912280699</v>
+      </c>
+      <c r="AZ14" s="31">
+        <f>80*(961/1932)</f>
+        <v>39.792960662525878</v>
+      </c>
+      <c r="BA14" s="31">
+        <f>80*(891/1872)</f>
+        <v>38.076923076923073</v>
+      </c>
       <c r="BB14" s="31">
-        <v>80</v>
+        <f>80*782/1660</f>
+        <v>37.686746987951807</v>
       </c>
     </row>
     <row r="15" spans="1:70" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15" s="29" t="s">
         <v>4</v>
@@ -3063,9 +3088,7 @@
       <c r="S15" s="30"/>
       <c r="T15" s="30"/>
       <c r="U15" s="30"/>
-      <c r="V15" s="30">
-        <v>50</v>
-      </c>
+      <c r="V15" s="30"/>
       <c r="W15" s="30"/>
       <c r="X15" s="30"/>
       <c r="Y15" s="30"/>
@@ -3077,7 +3100,7 @@
     </row>
     <row r="16" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>4</v>
@@ -3107,7 +3130,7 @@
     </row>
     <row r="17" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>4</v>
@@ -3137,7 +3160,7 @@
     </row>
     <row r="18" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>4</v>
@@ -3332,7 +3355,7 @@
     </row>
     <row r="20" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>3</v>
@@ -3346,26 +3369,23 @@
       <c r="AB20" s="7">
         <v>0</v>
       </c>
-      <c r="AK20" s="7">
-        <v>3.1</v>
-      </c>
-      <c r="AP20" s="7">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="AU20" s="7">
-        <v>5.2</v>
+      <c r="AS20" s="7">
+        <v>5.4</v>
+      </c>
+      <c r="AY20" s="7">
+        <v>6</v>
       </c>
       <c r="AZ20" s="7">
-        <v>5.4</v>
+        <v>7.63</v>
       </c>
       <c r="BB20" s="7">
-        <v>5.9</v>
+        <v>8.4</v>
       </c>
       <c r="BP20" s="13"/>
     </row>
     <row r="21" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>4</v>
@@ -3386,7 +3406,7 @@
     </row>
     <row r="22" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>4</v>
@@ -3412,7 +3432,7 @@
     </row>
     <row r="23" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>4</v>
@@ -3423,9 +3443,11 @@
       <c r="D23" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="BB23" s="7">
-        <f>10/98 * 100</f>
-        <v>10.204081632653061</v>
+      <c r="F23" s="7">
+        <v>2</v>
+      </c>
+      <c r="AX23" s="7">
+        <v>4.9000000000000004</v>
       </c>
       <c r="BN23" s="13">
         <v>5.0999999999999996</v>
@@ -3433,12 +3455,12 @@
       <c r="BP23" s="13"/>
       <c r="BR23" s="7">
         <f>BB23/2</f>
-        <v>5.1020408163265305</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>4</v>
@@ -3456,7 +3478,7 @@
     </row>
     <row r="25" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>4</v>
@@ -3474,45 +3496,61 @@
     </row>
     <row r="26" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C26" s="5">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="7">
-        <v>0</v>
-      </c>
-      <c r="G26" s="7">
-        <v>30</v>
-      </c>
-      <c r="I26" s="7">
-        <v>50</v>
-      </c>
-      <c r="S26" s="7">
-        <v>50</v>
-      </c>
-      <c r="AM26" s="7">
-        <v>50</v>
-      </c>
-      <c r="AR26" s="7">
-        <v>53</v>
-      </c>
-      <c r="AW26" s="7">
-        <v>55</v>
-      </c>
-      <c r="AZ26" s="7">
-        <v>60</v>
-      </c>
-      <c r="BB26" s="7">
-        <v>62</v>
+      <c r="AG26" s="7">
+        <v>67</v>
       </c>
       <c r="BP26" s="13"/>
+    </row>
+    <row r="27" spans="1:70" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="33">
+        <v>1</v>
+      </c>
+      <c r="D27" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="34">
+        <v>1</v>
+      </c>
+      <c r="K27" s="35">
+        <v>1</v>
+      </c>
+      <c r="U27" s="35">
+        <v>1</v>
+      </c>
+      <c r="V27" s="35">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="BA27" s="35">
+        <v>3.11</v>
+      </c>
+      <c r="BF27" s="36"/>
+      <c r="BG27" s="36"/>
+      <c r="BH27" s="36"/>
+      <c r="BI27" s="36"/>
+      <c r="BJ27" s="36"/>
+      <c r="BK27" s="36"/>
+      <c r="BL27" s="36"/>
+      <c r="BM27" s="36"/>
+      <c r="BN27" s="36"/>
+      <c r="BO27" s="36"/>
+      <c r="BP27" s="36"/>
     </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="4">
@@ -3525,7 +3563,7 @@
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C28:C1048576 C2:C26">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C1048576">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -3534,7 +3572,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="382" yWindow="552" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="382" yWindow="552" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
@@ -3559,6 +3597,12 @@
           </x14:formula1>
           <xm:sqref>D14:D15</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time-variant?" prompt="If no, the most recent value will be selected.">
+          <x14:formula1>
+            <xm:f>[1]dropdown_lists!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>D27</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Update data spreadsheet for Bulgaria
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="78">
   <si>
     <t>parameter</t>
   </si>
@@ -243,6 +243,21 @@
   </si>
   <si>
     <t>epi_rr_diabetes</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_ontreatment_mdr</t>
+  </si>
+  <si>
+    <t>program_prop_shortcourse_mdr_relativeduration</t>
+  </si>
+  <si>
+    <t>Proportional reduction in duration of MDR-TB treatment with short course treatment (also applies to duration of infectiousness)</t>
+  </si>
+  <si>
+    <t>program_prop_treatment_success_shortcoursemdr</t>
+  </si>
+  <si>
+    <t>Treatment success under shortcourse MDR-TB regimens</t>
   </si>
 </sst>
 </file>
@@ -254,7 +269,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,8 +353,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -366,6 +388,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1129,7 +1157,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1179,6 +1207,15 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="665">
     <cellStyle name="Comma" xfId="664" builtinId="3"/>
@@ -1869,8 +1906,8 @@
       <sheetName val="dropdown_lists"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
@@ -2167,10 +2204,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2344,7 +2381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
@@ -2352,7 +2389,7 @@
         <v>11575186.195826644</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
         <v>37</v>
       </c>
@@ -2360,12 +2397,51 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="14">
         <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="38">
+        <f>20/12</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="39"/>
+    </row>
+    <row r="21" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="41">
+        <f>12/20</f>
+        <v>0.6</v>
+      </c>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="41">
+        <v>0.84</v>
+      </c>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="39" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2397,10 +2473,10 @@
   <dimension ref="A1:BR27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AB5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="BB2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC20" sqref="AC20"/>
+      <selection pane="bottomRight" activeCell="BF10" sqref="BF10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2663,9 +2739,7 @@
       <c r="E2" s="1"/>
       <c r="BC2" s="27"/>
       <c r="BD2" s="27"/>
-      <c r="BL2" s="27">
-        <v>99</v>
-      </c>
+      <c r="BL2" s="27"/>
       <c r="BN2" s="27"/>
     </row>
     <row r="3" spans="1:70" x14ac:dyDescent="0.3">
@@ -2759,13 +2833,9 @@
       <c r="BB5" s="9">
         <v>0</v>
       </c>
-      <c r="BD5" s="27">
-        <v>99</v>
-      </c>
+      <c r="BD5" s="27"/>
       <c r="BF5" s="27"/>
-      <c r="BM5" s="27">
-        <v>99</v>
-      </c>
+      <c r="BM5" s="27"/>
     </row>
     <row r="6" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -2833,17 +2903,13 @@
       <c r="BB8" s="7">
         <v>0</v>
       </c>
-      <c r="BE8" s="13">
-        <v>80</v>
-      </c>
+      <c r="BE8" s="13"/>
       <c r="BF8" s="13"/>
       <c r="BG8" s="13"/>
       <c r="BH8" s="13"/>
       <c r="BI8" s="13"/>
       <c r="BJ8" s="13"/>
-      <c r="BM8" s="13">
-        <v>80</v>
-      </c>
+      <c r="BM8" s="13"/>
     </row>
     <row r="9" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
@@ -2863,15 +2929,11 @@
       </c>
       <c r="BE9" s="13"/>
       <c r="BF9" s="13"/>
-      <c r="BG9" s="13">
-        <v>80</v>
-      </c>
+      <c r="BG9" s="13"/>
       <c r="BH9" s="13"/>
       <c r="BI9" s="13"/>
       <c r="BJ9" s="13"/>
-      <c r="BM9" s="13">
-        <v>80</v>
-      </c>
+      <c r="BM9" s="13"/>
     </row>
     <row r="10" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
@@ -2891,15 +2953,13 @@
       </c>
       <c r="BE10" s="13"/>
       <c r="BF10" s="13"/>
-      <c r="BG10" s="13"/>
+      <c r="BG10" s="13">
+        <v>50</v>
+      </c>
       <c r="BH10" s="13"/>
-      <c r="BK10" s="13">
-        <v>90</v>
-      </c>
+      <c r="BK10" s="13"/>
       <c r="BL10" s="13"/>
-      <c r="BM10" s="13">
-        <v>90</v>
-      </c>
+      <c r="BM10" s="13"/>
       <c r="BO10" s="13"/>
     </row>
     <row r="11" spans="1:70" x14ac:dyDescent="0.3">
@@ -2924,14 +2984,10 @@
       <c r="BE11" s="13"/>
       <c r="BF11" s="13"/>
       <c r="BG11" s="13"/>
-      <c r="BH11" s="13">
-        <v>90</v>
-      </c>
+      <c r="BH11" s="13"/>
       <c r="BK11" s="13"/>
       <c r="BL11" s="13"/>
-      <c r="BM11" s="13">
-        <v>90</v>
-      </c>
+      <c r="BM11" s="13"/>
     </row>
     <row r="12" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -2953,14 +3009,10 @@
       <c r="BF12" s="13"/>
       <c r="BG12" s="13"/>
       <c r="BH12" s="13"/>
-      <c r="BI12" s="13">
-        <v>90</v>
-      </c>
+      <c r="BI12" s="13"/>
       <c r="BK12" s="13"/>
       <c r="BL12" s="13"/>
-      <c r="BM12" s="13">
-        <v>90</v>
-      </c>
+      <c r="BM12" s="13"/>
     </row>
     <row r="13" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
@@ -2982,13 +3034,9 @@
       <c r="BF13" s="13"/>
       <c r="BG13" s="13"/>
       <c r="BH13" s="13"/>
-      <c r="BJ13" s="13">
-        <v>80</v>
-      </c>
+      <c r="BJ13" s="13"/>
       <c r="BK13" s="13"/>
-      <c r="BM13" s="13">
-        <v>80</v>
-      </c>
+      <c r="BM13" s="13"/>
       <c r="BN13" s="13"/>
     </row>
     <row r="14" spans="1:70" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -3115,18 +3163,15 @@
         <v>0</v>
       </c>
       <c r="BE16" s="13"/>
-      <c r="BF16" s="13"/>
+      <c r="BF16" s="13">
+        <v>100</v>
+      </c>
       <c r="BG16" s="13"/>
       <c r="BH16" s="13"/>
       <c r="BJ16" s="13"/>
       <c r="BK16" s="13"/>
-      <c r="BM16" s="13">
-        <v>80</v>
-      </c>
+      <c r="BM16" s="13"/>
       <c r="BN16" s="13"/>
-      <c r="BO16" s="7">
-        <v>80</v>
-      </c>
     </row>
     <row r="17" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
@@ -3143,6 +3188,9 @@
       </c>
       <c r="AW17" s="7">
         <v>20</v>
+      </c>
+      <c r="BD17" s="7">
+        <v>100</v>
       </c>
       <c r="BE17" s="13"/>
       <c r="BF17" s="13"/>
@@ -3150,13 +3198,8 @@
       <c r="BH17" s="13"/>
       <c r="BJ17" s="13"/>
       <c r="BK17" s="13"/>
-      <c r="BM17" s="13">
-        <v>80</v>
-      </c>
+      <c r="BM17" s="13"/>
       <c r="BN17" s="13"/>
-      <c r="BP17" s="7">
-        <v>100</v>
-      </c>
     </row>
     <row r="18" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
@@ -3172,6 +3215,9 @@
         <v>3</v>
       </c>
       <c r="AW18" s="7">
+        <v>100</v>
+      </c>
+      <c r="BD18" s="7">
         <v>100</v>
       </c>
       <c r="BE18" s="13"/>
@@ -3180,13 +3226,8 @@
       <c r="BH18" s="13"/>
       <c r="BJ18" s="13"/>
       <c r="BK18" s="13"/>
-      <c r="BM18" s="13">
-        <v>80</v>
-      </c>
+      <c r="BM18" s="13"/>
       <c r="BN18" s="13"/>
-      <c r="BP18" s="7">
-        <v>100</v>
-      </c>
     </row>
     <row r="19" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
@@ -3583,7 +3624,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D28:D1048576 D2:D13 D16:D26</xm:sqref>
+          <xm:sqref>D16:D26 D2:D13 D28:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
Calibration including diabetes. Still not satisfying
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="612" windowWidth="16272" windowHeight="6300" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="612" windowWidth="16272" windowHeight="6300" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="88">
   <si>
     <t>parameter</t>
   </si>
@@ -258,6 +258,36 @@
   </si>
   <si>
     <t>Treatment success under shortcourse MDR-TB regimens</t>
+  </si>
+  <si>
+    <t>start_mdr_introduce_time</t>
+  </si>
+  <si>
+    <t>Calendar year that MDR-TB first begins to emerge</t>
+  </si>
+  <si>
+    <t>end_mdr_introduce_time</t>
+  </si>
+  <si>
+    <t>Calendar year that MDR-TB amplification reaches full parameter value</t>
+  </si>
+  <si>
+    <t>transmission_modifier</t>
+  </si>
+  <si>
+    <t>plot_start_time</t>
+  </si>
+  <si>
+    <t>riskgroup_multiplier_force_infection_ruralpoor</t>
+  </si>
+  <si>
+    <t>riskgroup_multiplier_force_infection_prison</t>
+  </si>
+  <si>
+    <t>program_prop_food_voucher_improvement</t>
+  </si>
+  <si>
+    <t>riskgroup_perc_hiv</t>
   </si>
 </sst>
 </file>
@@ -269,7 +299,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,8 +390,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -394,6 +439,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1157,7 +1214,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1168,7 +1225,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1196,11 +1252,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1216,6 +1270,23 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="12" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="665">
     <cellStyle name="Comma" xfId="664" builtinId="3"/>
@@ -2204,21 +2275,21 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.5546875" style="20" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" style="23" customWidth="1"/>
-    <col min="3" max="5" width="9.109375" style="20"/>
-    <col min="6" max="6" width="13.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="20"/>
+    <col min="1" max="1" width="51.5546875" style="19" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="22" customWidth="1"/>
+    <col min="3" max="5" width="9.109375" style="19"/>
+    <col min="6" max="6" width="13.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2229,155 +2300,155 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="16">
-        <v>10.35</v>
-      </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-    </row>
-    <row r="3" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="B2" s="15">
+        <v>7.8</v>
+      </c>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+    </row>
+    <row r="3" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="19">
-        <v>0.43</v>
-      </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-    </row>
-    <row r="4" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="B3" s="18">
+        <v>0.4</v>
+      </c>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+    </row>
+    <row r="4" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="18">
         <v>1</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-    </row>
-    <row r="5" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="18">
         <v>5</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="16">
         <v>15</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-    </row>
-    <row r="6" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+    </row>
+    <row r="6" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="20">
         <v>12200000</v>
       </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B7" s="22">
         <v>2.7</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="18">
         <v>1.5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="18">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="24">
         <v>26.22</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="24"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="24">
         <v>0</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="24">
         <v>265450</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13" s="24">
         <v>3</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="24">
         <v>1</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B15" s="24">
         <v>26.24</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="13">
         <v>0</v>
       </c>
     </row>
@@ -2385,15 +2456,15 @@
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="26">
+      <c r="B17" s="25">
         <v>11575186.195826644</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="13">
         <v>3</v>
       </c>
     </row>
@@ -2401,51 +2472,137 @@
       <c r="A19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="38">
+      <c r="B20" s="35">
         <f>20/12</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="39"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="36"/>
     </row>
     <row r="21" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="40" t="s">
+      <c r="A21" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="41">
+      <c r="B21" s="38">
         <f>12/20</f>
         <v>0.6</v>
       </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="39" t="s">
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="36" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="B22" s="41">
+      <c r="B22" s="38">
         <v>0.84</v>
       </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="39" t="s">
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="36" t="s">
         <v>77</v>
       </c>
     </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="40">
+        <v>1940</v>
+      </c>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="42" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="40">
+        <v>1950</v>
+      </c>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="22">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" s="22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="22">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="22">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="34"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="36"/>
+    </row>
+    <row r="30" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="34"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="36"/>
+    </row>
+    <row r="31" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="34"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="36"/>
+    </row>
+    <row r="32" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="34"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="36"/>
+    </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="5">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6 F6:G6">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
@@ -2459,6 +2616,10 @@
       <formula2>1</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age unstratified" prompt="Some values you can replace the ones to the left with if you want a manual calibration for the model without age stratification." sqref="H1"/>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:D24">
+      <formula1>-10000</formula1>
+      <formula2>10000</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2470,18 +2631,18 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BR27"/>
+  <dimension ref="A1:BR29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="BB2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="AK5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BF10" sqref="BF10"/>
+      <selection pane="bottomRight" activeCell="AR29" sqref="AR29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="56" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.77734375" style="4" customWidth="1"/>
     <col min="2" max="2" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11" style="5" customWidth="1"/>
     <col min="5" max="5" width="11" style="6" customWidth="1"/>
@@ -2512,16 +2673,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:70" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="2">
@@ -2724,26 +2885,26 @@
       </c>
     </row>
     <row r="2" spans="1:70" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="11">
         <v>0.1</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="BC2" s="27"/>
-      <c r="BD2" s="27"/>
-      <c r="BL2" s="27"/>
-      <c r="BN2" s="27"/>
+      <c r="BC2" s="26"/>
+      <c r="BD2" s="26"/>
+      <c r="BL2" s="26"/>
+      <c r="BN2" s="26"/>
     </row>
     <row r="3" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="44" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -2778,10 +2939,10 @@
       <c r="AZ3" s="8">
         <v>85</v>
       </c>
-      <c r="BM3" s="13"/>
+      <c r="BM3" s="12"/>
     </row>
     <row r="4" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="44" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -2814,31 +2975,31 @@
       <c r="AZ4" s="9"/>
       <c r="BA4" s="9"/>
       <c r="BB4" s="9"/>
-      <c r="BM4" s="13"/>
+      <c r="BM4" s="12"/>
     </row>
     <row r="5" spans="1:70" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>1</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="1"/>
       <c r="BB5" s="9">
         <v>0</v>
       </c>
-      <c r="BD5" s="27"/>
-      <c r="BF5" s="27"/>
-      <c r="BM5" s="27"/>
+      <c r="BD5" s="26"/>
+      <c r="BF5" s="26"/>
+      <c r="BM5" s="26"/>
     </row>
     <row r="6" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="44" t="s">
         <v>40</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -2859,14 +3020,14 @@
       <c r="BB6" s="7">
         <v>0</v>
       </c>
-      <c r="BE6" s="13"/>
-      <c r="BF6" s="13"/>
-      <c r="BG6" s="13"/>
-      <c r="BH6" s="13"/>
-      <c r="BM6" s="13"/>
+      <c r="BE6" s="12"/>
+      <c r="BF6" s="12"/>
+      <c r="BG6" s="12"/>
+      <c r="BH6" s="12"/>
+      <c r="BM6" s="12"/>
     </row>
     <row r="7" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="44" t="s">
         <v>44</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -2881,14 +3042,14 @@
       <c r="BB7" s="7">
         <v>0</v>
       </c>
-      <c r="BE7" s="13"/>
-      <c r="BF7" s="13"/>
-      <c r="BG7" s="13"/>
-      <c r="BH7" s="13"/>
-      <c r="BM7" s="13"/>
+      <c r="BE7" s="12"/>
+      <c r="BF7" s="12"/>
+      <c r="BG7" s="12"/>
+      <c r="BH7" s="12"/>
+      <c r="BM7" s="12"/>
     </row>
     <row r="8" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="44" t="s">
         <v>59</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -2903,16 +3064,16 @@
       <c r="BB8" s="7">
         <v>0</v>
       </c>
-      <c r="BE8" s="13"/>
-      <c r="BF8" s="13"/>
-      <c r="BG8" s="13"/>
-      <c r="BH8" s="13"/>
-      <c r="BI8" s="13"/>
-      <c r="BJ8" s="13"/>
-      <c r="BM8" s="13"/>
+      <c r="BE8" s="12"/>
+      <c r="BF8" s="12"/>
+      <c r="BG8" s="12"/>
+      <c r="BH8" s="12"/>
+      <c r="BI8" s="12"/>
+      <c r="BJ8" s="12"/>
+      <c r="BM8" s="12"/>
     </row>
     <row r="9" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="44" t="s">
         <v>58</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -2927,16 +3088,16 @@
       <c r="BB9" s="7">
         <v>0</v>
       </c>
-      <c r="BE9" s="13"/>
-      <c r="BF9" s="13"/>
-      <c r="BG9" s="13"/>
-      <c r="BH9" s="13"/>
-      <c r="BI9" s="13"/>
-      <c r="BJ9" s="13"/>
-      <c r="BM9" s="13"/>
+      <c r="BE9" s="12"/>
+      <c r="BF9" s="12"/>
+      <c r="BG9" s="12"/>
+      <c r="BH9" s="12"/>
+      <c r="BI9" s="12"/>
+      <c r="BJ9" s="12"/>
+      <c r="BM9" s="12"/>
     </row>
     <row r="10" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="44" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -2951,19 +3112,19 @@
       <c r="BB10" s="7">
         <v>0</v>
       </c>
-      <c r="BE10" s="13"/>
-      <c r="BF10" s="13"/>
-      <c r="BG10" s="13">
+      <c r="BE10" s="12"/>
+      <c r="BF10" s="12"/>
+      <c r="BG10" s="12">
         <v>50</v>
       </c>
-      <c r="BH10" s="13"/>
-      <c r="BK10" s="13"/>
-      <c r="BL10" s="13"/>
-      <c r="BM10" s="13"/>
-      <c r="BO10" s="13"/>
+      <c r="BH10" s="12"/>
+      <c r="BK10" s="12"/>
+      <c r="BL10" s="12"/>
+      <c r="BM10" s="12"/>
+      <c r="BO10" s="12"/>
     </row>
     <row r="11" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="44" t="s">
         <v>60</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -2978,19 +3139,21 @@
       <c r="AW11" s="7">
         <v>0</v>
       </c>
-      <c r="BB11" s="7">
-        <v>5</v>
-      </c>
-      <c r="BE11" s="13"/>
-      <c r="BF11" s="13"/>
-      <c r="BG11" s="13"/>
-      <c r="BH11" s="13"/>
-      <c r="BK11" s="13"/>
-      <c r="BL11" s="13"/>
-      <c r="BM11" s="13"/>
+      <c r="AX11" s="7">
+        <v>10</v>
+      </c>
+      <c r="BE11" s="12"/>
+      <c r="BF11" s="12"/>
+      <c r="BG11" s="12"/>
+      <c r="BH11" s="12">
+        <v>8.4</v>
+      </c>
+      <c r="BK11" s="12"/>
+      <c r="BL11" s="12"/>
+      <c r="BM11" s="12"/>
     </row>
     <row r="12" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="44" t="s">
         <v>66</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -3002,20 +3165,25 @@
       <c r="D12" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="BB12" s="7">
+      <c r="AW12" s="7">
         <v>0</v>
       </c>
-      <c r="BE12" s="13"/>
-      <c r="BF12" s="13"/>
-      <c r="BG12" s="13"/>
-      <c r="BH12" s="13"/>
-      <c r="BI12" s="13"/>
-      <c r="BK12" s="13"/>
-      <c r="BL12" s="13"/>
-      <c r="BM12" s="13"/>
+      <c r="AX12" s="7">
+        <v>10</v>
+      </c>
+      <c r="BE12" s="12"/>
+      <c r="BF12" s="12"/>
+      <c r="BG12" s="12"/>
+      <c r="BH12" s="12">
+        <v>8.4</v>
+      </c>
+      <c r="BI12" s="12"/>
+      <c r="BK12" s="12"/>
+      <c r="BL12" s="12"/>
+      <c r="BM12" s="12"/>
     </row>
     <row r="13" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="44" t="s">
         <v>54</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -3030,124 +3198,124 @@
       <c r="BB13" s="7">
         <v>0</v>
       </c>
-      <c r="BE13" s="13"/>
-      <c r="BF13" s="13"/>
-      <c r="BG13" s="13"/>
-      <c r="BH13" s="13"/>
-      <c r="BJ13" s="13"/>
-      <c r="BK13" s="13"/>
-      <c r="BM13" s="13"/>
-      <c r="BN13" s="13"/>
-    </row>
-    <row r="14" spans="1:70" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="28" t="s">
+      <c r="BE13" s="12"/>
+      <c r="BF13" s="12"/>
+      <c r="BG13" s="12"/>
+      <c r="BH13" s="12"/>
+      <c r="BJ13" s="12"/>
+      <c r="BK13" s="12"/>
+      <c r="BM13" s="12"/>
+      <c r="BN13" s="12"/>
+    </row>
+    <row r="14" spans="1:70" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C14" s="27">
         <v>0.5</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="30"/>
-      <c r="S14" s="30"/>
-      <c r="T14" s="30"/>
-      <c r="U14" s="30"/>
-      <c r="V14" s="30"/>
-      <c r="W14" s="30"/>
-      <c r="X14" s="30"/>
-      <c r="Y14" s="30"/>
-      <c r="Z14" s="30"/>
-      <c r="AA14" s="30"/>
-      <c r="AB14" s="31">
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="28"/>
+      <c r="T14" s="28"/>
+      <c r="U14" s="28"/>
+      <c r="V14" s="28"/>
+      <c r="W14" s="28"/>
+      <c r="X14" s="28"/>
+      <c r="Y14" s="28"/>
+      <c r="Z14" s="28"/>
+      <c r="AA14" s="28"/>
+      <c r="AB14" s="29">
         <v>0</v>
       </c>
-      <c r="AC14" s="31">
+      <c r="AC14" s="29">
         <v>5</v>
       </c>
-      <c r="AW14" s="31">
+      <c r="AW14" s="29">
         <f>80*(1174/2649)</f>
         <v>35.454888637221593</v>
       </c>
-      <c r="AX14" s="31">
+      <c r="AX14" s="29">
         <f>80*(1077/2407)</f>
         <v>35.795596177814708</v>
       </c>
-      <c r="AY14" s="31">
+      <c r="AY14" s="29">
         <f>80*(1094/2280)</f>
         <v>38.385964912280699</v>
       </c>
-      <c r="AZ14" s="31">
+      <c r="AZ14" s="29">
         <f>80*(961/1932)</f>
         <v>39.792960662525878</v>
       </c>
-      <c r="BA14" s="31">
+      <c r="BA14" s="29">
         <f>80*(891/1872)</f>
         <v>38.076923076923073</v>
       </c>
-      <c r="BB14" s="31">
+      <c r="BB14" s="29">
         <f>80*782/1660</f>
         <v>37.686746987951807</v>
       </c>
     </row>
-    <row r="15" spans="1:70" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="28" t="s">
+    <row r="15" spans="1:70" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C15" s="27">
         <v>1</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="30"/>
-      <c r="S15" s="30"/>
-      <c r="T15" s="30"/>
-      <c r="U15" s="30"/>
-      <c r="V15" s="30"/>
-      <c r="W15" s="30"/>
-      <c r="X15" s="30"/>
-      <c r="Y15" s="30"/>
-      <c r="Z15" s="30"/>
-      <c r="AA15" s="30"/>
-      <c r="BB15" s="31">
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="28"/>
+      <c r="S15" s="28"/>
+      <c r="T15" s="28"/>
+      <c r="U15" s="28"/>
+      <c r="V15" s="28"/>
+      <c r="W15" s="28"/>
+      <c r="X15" s="28"/>
+      <c r="Y15" s="28"/>
+      <c r="Z15" s="28"/>
+      <c r="AA15" s="28"/>
+      <c r="BB15" s="29">
         <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="44" t="s">
         <v>67</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -3162,19 +3330,19 @@
       <c r="BB16" s="7">
         <v>0</v>
       </c>
-      <c r="BE16" s="13"/>
-      <c r="BF16" s="13">
+      <c r="BE16" s="12"/>
+      <c r="BF16" s="12">
         <v>100</v>
       </c>
-      <c r="BG16" s="13"/>
-      <c r="BH16" s="13"/>
-      <c r="BJ16" s="13"/>
-      <c r="BK16" s="13"/>
-      <c r="BM16" s="13"/>
-      <c r="BN16" s="13"/>
+      <c r="BG16" s="12"/>
+      <c r="BH16" s="12"/>
+      <c r="BJ16" s="12"/>
+      <c r="BK16" s="12"/>
+      <c r="BM16" s="12"/>
+      <c r="BN16" s="12"/>
     </row>
     <row r="17" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="44" t="s">
         <v>70</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -3187,22 +3355,22 @@
         <v>3</v>
       </c>
       <c r="AW17" s="7">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="BD17" s="7">
         <v>100</v>
       </c>
-      <c r="BE17" s="13"/>
-      <c r="BF17" s="13"/>
-      <c r="BG17" s="13"/>
-      <c r="BH17" s="13"/>
-      <c r="BJ17" s="13"/>
-      <c r="BK17" s="13"/>
-      <c r="BM17" s="13"/>
-      <c r="BN17" s="13"/>
+      <c r="BE17" s="12"/>
+      <c r="BF17" s="12"/>
+      <c r="BG17" s="12"/>
+      <c r="BH17" s="12"/>
+      <c r="BJ17" s="12"/>
+      <c r="BK17" s="12"/>
+      <c r="BM17" s="12"/>
+      <c r="BN17" s="12"/>
     </row>
     <row r="18" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="44" t="s">
         <v>71</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -3220,17 +3388,17 @@
       <c r="BD18" s="7">
         <v>100</v>
       </c>
-      <c r="BE18" s="13"/>
-      <c r="BF18" s="13"/>
-      <c r="BG18" s="13"/>
-      <c r="BH18" s="13"/>
-      <c r="BJ18" s="13"/>
-      <c r="BK18" s="13"/>
-      <c r="BM18" s="13"/>
-      <c r="BN18" s="13"/>
+      <c r="BE18" s="12"/>
+      <c r="BF18" s="12"/>
+      <c r="BG18" s="12"/>
+      <c r="BH18" s="12"/>
+      <c r="BJ18" s="12"/>
+      <c r="BK18" s="12"/>
+      <c r="BM18" s="12"/>
+      <c r="BN18" s="12"/>
     </row>
     <row r="19" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="44" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -3245,158 +3413,158 @@
       <c r="E19" s="6">
         <v>1</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="13">
         <v>1</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="13">
         <v>1.1289570744394</v>
       </c>
-      <c r="H19" s="14">
+      <c r="H19" s="13">
         <v>1.42215881727406</v>
       </c>
-      <c r="I19" s="14">
+      <c r="I19" s="13">
         <v>1.90118931222233</v>
       </c>
-      <c r="J19" s="14">
+      <c r="J19" s="13">
         <v>2.3081073919986701</v>
       </c>
-      <c r="K19" s="14">
+      <c r="K19" s="13">
         <v>2.4974653103104298</v>
       </c>
-      <c r="L19" s="14">
+      <c r="L19" s="13">
         <v>2.9115458645382701</v>
       </c>
-      <c r="M19" s="14">
+      <c r="M19" s="13">
         <v>3.90623450399154</v>
       </c>
-      <c r="N19" s="14">
+      <c r="N19" s="13">
         <v>4.1703507493909102</v>
       </c>
-      <c r="O19" s="14">
+      <c r="O19" s="13">
         <v>4.55399078719985</v>
       </c>
-      <c r="P19" s="14">
+      <c r="P19" s="13">
         <v>5.0047790229916798</v>
       </c>
-      <c r="Q19" s="14">
+      <c r="Q19" s="13">
         <v>5.3718558386314896</v>
       </c>
-      <c r="R19" s="14">
+      <c r="R19" s="13">
         <v>6.3137212289735496</v>
       </c>
-      <c r="S19" s="14">
+      <c r="S19" s="13">
         <v>7.4628507238053698</v>
       </c>
-      <c r="T19" s="14">
+      <c r="T19" s="13">
         <v>8.4391855224587609</v>
       </c>
-      <c r="U19" s="14">
+      <c r="U19" s="13">
         <v>9.3018160392078606</v>
       </c>
-      <c r="V19" s="14">
+      <c r="V19" s="13">
         <v>10.2347283365258</v>
       </c>
-      <c r="W19" s="14">
+      <c r="W19" s="13">
         <v>15.386785740408699</v>
       </c>
-      <c r="X19" s="14">
+      <c r="X19" s="13">
         <v>18.9416113416321</v>
       </c>
-      <c r="Y19" s="14">
+      <c r="Y19" s="13">
         <v>19.1590871369295</v>
       </c>
-      <c r="Z19" s="14">
+      <c r="Z19" s="13">
         <v>19.938817427385899</v>
       </c>
-      <c r="AA19" s="14">
+      <c r="AA19" s="13">
         <v>22.702351313969601</v>
       </c>
-      <c r="AB19" s="14">
+      <c r="AB19" s="13">
         <v>25.481798063623799</v>
       </c>
-      <c r="AC19" s="14">
+      <c r="AC19" s="13">
         <v>28.584806362378998</v>
       </c>
-      <c r="AD19" s="14">
+      <c r="AD19" s="13">
         <v>34.090656984785603</v>
       </c>
-      <c r="AE19" s="14">
+      <c r="AE19" s="13">
         <v>37.0398409405256</v>
       </c>
-      <c r="AF19" s="14">
+      <c r="AF19" s="13">
         <v>39.527551867219898</v>
       </c>
-      <c r="AG19" s="14">
+      <c r="AG19" s="13">
         <v>43.633070539419101</v>
       </c>
-      <c r="AH19" s="14">
+      <c r="AH19" s="13">
         <v>46.6140802213001</v>
       </c>
-      <c r="AI19" s="14">
+      <c r="AI19" s="13">
         <v>50.0989972337483</v>
       </c>
-      <c r="AJ19" s="14">
+      <c r="AJ19" s="13">
         <v>52.899661134163203</v>
       </c>
-      <c r="AK19" s="14">
+      <c r="AK19" s="13">
         <v>57.784910096818798</v>
       </c>
-      <c r="AL19" s="14">
+      <c r="AL19" s="13">
         <v>61.2167842323652</v>
       </c>
-      <c r="AM19" s="14">
+      <c r="AM19" s="13">
         <v>63.651452282157699</v>
       </c>
-      <c r="AN19" s="14">
+      <c r="AN19" s="13">
         <v>67.053941908713696</v>
       </c>
-      <c r="AO19" s="14">
+      <c r="AO19" s="13">
         <v>68.8796680497925</v>
       </c>
-      <c r="AP19" s="14">
+      <c r="AP19" s="13">
         <v>70.456431535269701</v>
       </c>
-      <c r="AQ19" s="14">
+      <c r="AQ19" s="13">
         <v>73.858921161825705</v>
       </c>
-      <c r="AR19" s="14">
+      <c r="AR19" s="13">
         <v>78.6721991701245</v>
       </c>
-      <c r="AS19" s="14">
+      <c r="AS19" s="13">
         <v>82.987551867219906</v>
       </c>
-      <c r="AT19" s="14">
+      <c r="AT19" s="13">
         <v>85.394190871369304</v>
       </c>
-      <c r="AU19" s="14">
+      <c r="AU19" s="13">
         <v>92.448132780083</v>
       </c>
-      <c r="AV19" s="14">
+      <c r="AV19" s="13">
         <v>96.348547717842294</v>
       </c>
-      <c r="AW19" s="14">
+      <c r="AW19" s="13">
         <v>100</v>
       </c>
-      <c r="AX19" s="14">
+      <c r="AX19" s="13">
         <v>104.647302904564</v>
       </c>
-      <c r="AY19" s="14">
+      <c r="AY19" s="13">
         <v>107.966804979253</v>
       </c>
-      <c r="AZ19" s="14">
+      <c r="AZ19" s="13">
         <v>111.203319502075</v>
       </c>
-      <c r="BA19" s="14">
+      <c r="BA19" s="13">
         <v>115.767634854772</v>
       </c>
-      <c r="BB19" s="14">
+      <c r="BB19" s="13">
         <v>117.42738589211601</v>
       </c>
-      <c r="BP19" s="13"/>
+      <c r="BP19" s="12"/>
     </row>
     <row r="20" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>46</v>
+      <c r="A20" s="44" t="s">
+        <v>87</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>3</v>
@@ -3408,28 +3576,16 @@
         <v>3</v>
       </c>
       <c r="AB20" s="7">
-        <v>0</v>
-      </c>
-      <c r="AS20" s="7">
-        <v>5.4</v>
-      </c>
-      <c r="AY20" s="7">
-        <v>6</v>
-      </c>
-      <c r="AZ20" s="7">
-        <v>7.63</v>
-      </c>
-      <c r="BB20" s="7">
-        <v>8.4</v>
-      </c>
-      <c r="BP20" s="13"/>
+        <v>1</v>
+      </c>
+      <c r="BP20" s="12"/>
     </row>
     <row r="21" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>47</v>
+      <c r="A21" s="44" t="s">
+        <v>46</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C21" s="5">
         <v>1</v>
@@ -3437,17 +3593,26 @@
       <c r="D21" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AW21" s="7">
-        <v>0.112</v>
+      <c r="AB21" s="7">
+        <v>1</v>
+      </c>
+      <c r="AS21" s="7">
+        <v>5.4</v>
+      </c>
+      <c r="AY21" s="7">
+        <v>6</v>
+      </c>
+      <c r="AZ21" s="7">
+        <v>7.63</v>
       </c>
       <c r="BB21" s="7">
-        <v>0.153</v>
-      </c>
-      <c r="BP21" s="13"/>
+        <v>8.4</v>
+      </c>
+      <c r="BP21" s="12"/>
     </row>
     <row r="22" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>48</v>
+      <c r="A22" s="44" t="s">
+        <v>47</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>4</v>
@@ -3458,50 +3623,44 @@
       <c r="D22" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="AM22" s="7">
+        <v>0.1</v>
+      </c>
       <c r="BB22" s="7">
+        <f>100*9028/7265000</f>
+        <v>0.12426703372333103</v>
+      </c>
+      <c r="BP22" s="12"/>
+    </row>
+    <row r="23" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A23" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BB23" s="7">
         <f>4.5/98 * 100</f>
         <v>4.591836734693878</v>
       </c>
-      <c r="BN22" s="13">
+      <c r="BN23" s="12">
         <v>2.2999999999999998</v>
       </c>
-      <c r="BP22" s="13"/>
-      <c r="BQ22" s="7">
-        <f>BB22/2</f>
+      <c r="BP23" s="12"/>
+      <c r="BQ23" s="7">
+        <f>BB23/2</f>
         <v>2.295918367346939</v>
       </c>
     </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+    <row r="24" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A24" s="44" t="s">
         <v>49</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="5">
-        <v>1</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F23" s="7">
-        <v>2</v>
-      </c>
-      <c r="AX23" s="7">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="BN23" s="13">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="BP23" s="13"/>
-      <c r="BR23" s="7">
-        <f>BB23/2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>4</v>
@@ -3512,14 +3671,24 @@
       <c r="D24" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="F24" s="7">
+        <v>2</v>
+      </c>
       <c r="BB24" s="7">
-        <v>0.4</v>
-      </c>
-      <c r="BP24" s="13"/>
+        <v>4.5</v>
+      </c>
+      <c r="BN24" s="12">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="BP24" s="12"/>
+      <c r="BR24" s="7">
+        <f>BB24/2</f>
+        <v>2.25</v>
+      </c>
     </row>
     <row r="25" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>51</v>
+      <c r="A25" s="44" t="s">
+        <v>50</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>4</v>
@@ -3533,65 +3702,107 @@
       <c r="BB25" s="7">
         <v>0.4</v>
       </c>
-      <c r="BP25" s="13"/>
+      <c r="BP25" s="12"/>
     </row>
     <row r="26" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>52</v>
+      <c r="A26" s="44" t="s">
+        <v>51</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C26" s="5">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AG26" s="7">
+      <c r="BB26" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="BP26" s="12"/>
+    </row>
+    <row r="27" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A27" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG27" s="7">
         <v>67</v>
       </c>
-      <c r="BP26" s="13"/>
-    </row>
-    <row r="27" spans="1:70" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="32" t="s">
+      <c r="BH27" s="7">
+        <f>95*(1-0.064)</f>
+        <v>88.919999999999987</v>
+      </c>
+      <c r="BP27" s="12"/>
+    </row>
+    <row r="28" spans="1:70" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="B27" s="33" t="s">
+      <c r="B28" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="33">
+      <c r="C28" s="30">
         <v>1</v>
       </c>
-      <c r="D27" s="33" t="s">
+      <c r="D28" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E28" s="31">
         <v>1</v>
       </c>
-      <c r="K27" s="35">
+      <c r="K28" s="32">
         <v>1</v>
       </c>
-      <c r="U27" s="35">
+      <c r="U28" s="32">
         <v>1</v>
       </c>
-      <c r="V27" s="35">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="BA27" s="35">
+      <c r="V28" s="32">
         <v>3.11</v>
       </c>
-      <c r="BF27" s="36"/>
-      <c r="BG27" s="36"/>
-      <c r="BH27" s="36"/>
-      <c r="BI27" s="36"/>
-      <c r="BJ27" s="36"/>
-      <c r="BK27" s="36"/>
-      <c r="BL27" s="36"/>
-      <c r="BM27" s="36"/>
-      <c r="BN27" s="36"/>
-      <c r="BO27" s="36"/>
-      <c r="BP27" s="36"/>
+      <c r="BA28" s="32">
+        <v>3.11</v>
+      </c>
+      <c r="BF28" s="33"/>
+      <c r="BG28" s="33"/>
+      <c r="BH28" s="33"/>
+      <c r="BI28" s="33"/>
+      <c r="BJ28" s="33"/>
+      <c r="BK28" s="33"/>
+      <c r="BL28" s="33"/>
+      <c r="BM28" s="33"/>
+      <c r="BN28" s="33"/>
+      <c r="BO28" s="33"/>
+      <c r="BP28" s="33"/>
+    </row>
+    <row r="29" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A29" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="5">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ29" s="7">
+        <v>1</v>
+      </c>
+      <c r="AR29" s="7">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="4">
@@ -3613,7 +3824,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="382" yWindow="552" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="382" yWindow="552" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
@@ -3624,7 +3835,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D16:D26 D2:D13 D28:D1048576</xm:sqref>
+          <xm:sqref>D29:D1048576 D2:D13 D16:D27</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -3636,13 +3847,7 @@
           <x14:formula1>
             <xm:f>[1]dropdown_lists!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>D14:D15</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time-variant?" prompt="If no, the most recent value will be selected.">
-          <x14:formula1>
-            <xm:f>[1]dropdown_lists!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>D27</xm:sqref>
+          <xm:sqref>D14:D15 D28</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Implementation of NGOs and open Doors activities for Bulgaria
NGOs should normally be applied to specific populations only, which is
not the case in this code. The relevant update will be coming soon.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="94">
   <si>
     <t>parameter</t>
   </si>
@@ -288,6 +288,24 @@
   </si>
   <si>
     <t>riskgroup_perc_hiv</t>
+  </si>
+  <si>
+    <t>program_prop_detection_from_ngo</t>
+  </si>
+  <si>
+    <t>program_prop_detection_from_opendoors</t>
+  </si>
+  <si>
+    <t>program_prop_ipt_from_opendoors</t>
+  </si>
+  <si>
+    <t>program_prop_ipt_from_ngo</t>
+  </si>
+  <si>
+    <t>program_perc_ngo_activities</t>
+  </si>
+  <si>
+    <t>program_perc_opendoors_activities</t>
   </si>
 </sst>
 </file>
@@ -2277,8 +2295,8 @@
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2574,29 +2592,45 @@
       </c>
     </row>
     <row r="29" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="34"/>
-      <c r="B29" s="35"/>
+      <c r="A29" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="35">
+        <v>6.5000000000000002E-2</v>
+      </c>
       <c r="C29" s="35"/>
       <c r="D29" s="35"/>
       <c r="E29" s="36"/>
     </row>
     <row r="30" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="34"/>
-      <c r="B30" s="35"/>
+      <c r="A30" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="35">
+        <v>0.16</v>
+      </c>
       <c r="C30" s="35"/>
       <c r="D30" s="35"/>
       <c r="E30" s="36"/>
     </row>
     <row r="31" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="34"/>
-      <c r="B31" s="35"/>
+      <c r="A31" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" s="35">
+        <v>0.05</v>
+      </c>
       <c r="C31" s="35"/>
       <c r="D31" s="35"/>
       <c r="E31" s="36"/>
     </row>
     <row r="32" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="34"/>
-      <c r="B32" s="35"/>
+      <c r="A32" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="35">
+        <v>0.156</v>
+      </c>
       <c r="C32" s="35"/>
       <c r="D32" s="35"/>
       <c r="E32" s="36"/>
@@ -2631,13 +2665,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BR29"/>
+  <dimension ref="A1:BR31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AK5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="BE8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AR29" sqref="AR29"/>
+      <selection pane="bottomRight" activeCell="BH20" sqref="BH20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3145,9 +3179,7 @@
       <c r="BE11" s="12"/>
       <c r="BF11" s="12"/>
       <c r="BG11" s="12"/>
-      <c r="BH11" s="12">
-        <v>8.4</v>
-      </c>
+      <c r="BH11" s="12"/>
       <c r="BK11" s="12"/>
       <c r="BL11" s="12"/>
       <c r="BM11" s="12"/>
@@ -3174,9 +3206,7 @@
       <c r="BE12" s="12"/>
       <c r="BF12" s="12"/>
       <c r="BG12" s="12"/>
-      <c r="BH12" s="12">
-        <v>8.4</v>
-      </c>
+      <c r="BH12" s="12"/>
       <c r="BI12" s="12"/>
       <c r="BK12" s="12"/>
       <c r="BL12" s="12"/>
@@ -3399,7 +3429,7 @@
     </row>
     <row r="19" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A19" s="44" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>4</v>
@@ -3411,163 +3441,28 @@
         <v>3</v>
       </c>
       <c r="E19" s="6">
-        <v>1</v>
-      </c>
-      <c r="F19" s="13">
-        <v>1</v>
-      </c>
-      <c r="G19" s="13">
-        <v>1.1289570744394</v>
-      </c>
-      <c r="H19" s="13">
-        <v>1.42215881727406</v>
-      </c>
-      <c r="I19" s="13">
-        <v>1.90118931222233</v>
-      </c>
-      <c r="J19" s="13">
-        <v>2.3081073919986701</v>
-      </c>
-      <c r="K19" s="13">
-        <v>2.4974653103104298</v>
-      </c>
-      <c r="L19" s="13">
-        <v>2.9115458645382701</v>
-      </c>
-      <c r="M19" s="13">
-        <v>3.90623450399154</v>
-      </c>
-      <c r="N19" s="13">
-        <v>4.1703507493909102</v>
-      </c>
-      <c r="O19" s="13">
-        <v>4.55399078719985</v>
-      </c>
-      <c r="P19" s="13">
-        <v>5.0047790229916798</v>
-      </c>
-      <c r="Q19" s="13">
-        <v>5.3718558386314896</v>
-      </c>
-      <c r="R19" s="13">
-        <v>6.3137212289735496</v>
-      </c>
-      <c r="S19" s="13">
-        <v>7.4628507238053698</v>
-      </c>
-      <c r="T19" s="13">
-        <v>8.4391855224587609</v>
-      </c>
-      <c r="U19" s="13">
-        <v>9.3018160392078606</v>
-      </c>
-      <c r="V19" s="13">
-        <v>10.2347283365258</v>
-      </c>
-      <c r="W19" s="13">
-        <v>15.386785740408699</v>
-      </c>
-      <c r="X19" s="13">
-        <v>18.9416113416321</v>
-      </c>
-      <c r="Y19" s="13">
-        <v>19.1590871369295</v>
-      </c>
-      <c r="Z19" s="13">
-        <v>19.938817427385899</v>
-      </c>
-      <c r="AA19" s="13">
-        <v>22.702351313969601</v>
-      </c>
-      <c r="AB19" s="13">
-        <v>25.481798063623799</v>
-      </c>
-      <c r="AC19" s="13">
-        <v>28.584806362378998</v>
-      </c>
-      <c r="AD19" s="13">
-        <v>34.090656984785603</v>
-      </c>
-      <c r="AE19" s="13">
-        <v>37.0398409405256</v>
-      </c>
-      <c r="AF19" s="13">
-        <v>39.527551867219898</v>
-      </c>
-      <c r="AG19" s="13">
-        <v>43.633070539419101</v>
-      </c>
-      <c r="AH19" s="13">
-        <v>46.6140802213001</v>
-      </c>
-      <c r="AI19" s="13">
-        <v>50.0989972337483</v>
-      </c>
-      <c r="AJ19" s="13">
-        <v>52.899661134163203</v>
-      </c>
-      <c r="AK19" s="13">
-        <v>57.784910096818798</v>
-      </c>
-      <c r="AL19" s="13">
-        <v>61.2167842323652</v>
-      </c>
-      <c r="AM19" s="13">
-        <v>63.651452282157699</v>
-      </c>
-      <c r="AN19" s="13">
-        <v>67.053941908713696</v>
-      </c>
-      <c r="AO19" s="13">
-        <v>68.8796680497925</v>
-      </c>
-      <c r="AP19" s="13">
-        <v>70.456431535269701</v>
-      </c>
-      <c r="AQ19" s="13">
-        <v>73.858921161825705</v>
-      </c>
-      <c r="AR19" s="13">
-        <v>78.6721991701245</v>
-      </c>
-      <c r="AS19" s="13">
-        <v>82.987551867219906</v>
-      </c>
-      <c r="AT19" s="13">
-        <v>85.394190871369304</v>
-      </c>
-      <c r="AU19" s="13">
-        <v>92.448132780083</v>
-      </c>
-      <c r="AV19" s="13">
-        <v>96.348547717842294</v>
-      </c>
-      <c r="AW19" s="13">
         <v>100</v>
       </c>
-      <c r="AX19" s="13">
-        <v>104.647302904564</v>
-      </c>
-      <c r="AY19" s="13">
-        <v>107.966804979253</v>
-      </c>
-      <c r="AZ19" s="13">
-        <v>111.203319502075</v>
-      </c>
-      <c r="BA19" s="13">
-        <v>115.767634854772</v>
-      </c>
-      <c r="BB19" s="13">
-        <v>117.42738589211601</v>
-      </c>
-      <c r="BP19" s="12"/>
+      <c r="BB19" s="7">
+        <v>100</v>
+      </c>
+      <c r="BE19" s="12"/>
+      <c r="BF19" s="12"/>
+      <c r="BG19" s="12"/>
+      <c r="BH19" s="12">
+        <v>0</v>
+      </c>
+      <c r="BJ19" s="12"/>
+      <c r="BK19" s="12"/>
+      <c r="BM19" s="12"/>
+      <c r="BN19" s="12"/>
     </row>
     <row r="20" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A20" s="44" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C20" s="5">
         <v>1</v>
@@ -3575,17 +3470,29 @@
       <c r="D20" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AB20" s="7">
-        <v>1</v>
-      </c>
-      <c r="BP20" s="12"/>
+      <c r="E20" s="6">
+        <v>100</v>
+      </c>
+      <c r="BB20" s="7">
+        <v>100</v>
+      </c>
+      <c r="BE20" s="12"/>
+      <c r="BF20" s="12"/>
+      <c r="BG20" s="12"/>
+      <c r="BH20" s="12">
+        <v>0</v>
+      </c>
+      <c r="BJ20" s="12"/>
+      <c r="BK20" s="12"/>
+      <c r="BM20" s="12"/>
+      <c r="BN20" s="12"/>
     </row>
     <row r="21" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A21" s="44" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C21" s="5">
         <v>1</v>
@@ -3593,29 +3500,164 @@
       <c r="D21" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AB21" s="7">
+      <c r="E21" s="6">
         <v>1</v>
       </c>
-      <c r="AS21" s="7">
-        <v>5.4</v>
-      </c>
-      <c r="AY21" s="7">
-        <v>6</v>
-      </c>
-      <c r="AZ21" s="7">
-        <v>7.63</v>
-      </c>
-      <c r="BB21" s="7">
-        <v>8.4</v>
+      <c r="F21" s="13">
+        <v>1</v>
+      </c>
+      <c r="G21" s="13">
+        <v>1.1289570744394</v>
+      </c>
+      <c r="H21" s="13">
+        <v>1.42215881727406</v>
+      </c>
+      <c r="I21" s="13">
+        <v>1.90118931222233</v>
+      </c>
+      <c r="J21" s="13">
+        <v>2.3081073919986701</v>
+      </c>
+      <c r="K21" s="13">
+        <v>2.4974653103104298</v>
+      </c>
+      <c r="L21" s="13">
+        <v>2.9115458645382701</v>
+      </c>
+      <c r="M21" s="13">
+        <v>3.90623450399154</v>
+      </c>
+      <c r="N21" s="13">
+        <v>4.1703507493909102</v>
+      </c>
+      <c r="O21" s="13">
+        <v>4.55399078719985</v>
+      </c>
+      <c r="P21" s="13">
+        <v>5.0047790229916798</v>
+      </c>
+      <c r="Q21" s="13">
+        <v>5.3718558386314896</v>
+      </c>
+      <c r="R21" s="13">
+        <v>6.3137212289735496</v>
+      </c>
+      <c r="S21" s="13">
+        <v>7.4628507238053698</v>
+      </c>
+      <c r="T21" s="13">
+        <v>8.4391855224587609</v>
+      </c>
+      <c r="U21" s="13">
+        <v>9.3018160392078606</v>
+      </c>
+      <c r="V21" s="13">
+        <v>10.2347283365258</v>
+      </c>
+      <c r="W21" s="13">
+        <v>15.386785740408699</v>
+      </c>
+      <c r="X21" s="13">
+        <v>18.9416113416321</v>
+      </c>
+      <c r="Y21" s="13">
+        <v>19.1590871369295</v>
+      </c>
+      <c r="Z21" s="13">
+        <v>19.938817427385899</v>
+      </c>
+      <c r="AA21" s="13">
+        <v>22.702351313969601</v>
+      </c>
+      <c r="AB21" s="13">
+        <v>25.481798063623799</v>
+      </c>
+      <c r="AC21" s="13">
+        <v>28.584806362378998</v>
+      </c>
+      <c r="AD21" s="13">
+        <v>34.090656984785603</v>
+      </c>
+      <c r="AE21" s="13">
+        <v>37.0398409405256</v>
+      </c>
+      <c r="AF21" s="13">
+        <v>39.527551867219898</v>
+      </c>
+      <c r="AG21" s="13">
+        <v>43.633070539419101</v>
+      </c>
+      <c r="AH21" s="13">
+        <v>46.6140802213001</v>
+      </c>
+      <c r="AI21" s="13">
+        <v>50.0989972337483</v>
+      </c>
+      <c r="AJ21" s="13">
+        <v>52.899661134163203</v>
+      </c>
+      <c r="AK21" s="13">
+        <v>57.784910096818798</v>
+      </c>
+      <c r="AL21" s="13">
+        <v>61.2167842323652</v>
+      </c>
+      <c r="AM21" s="13">
+        <v>63.651452282157699</v>
+      </c>
+      <c r="AN21" s="13">
+        <v>67.053941908713696</v>
+      </c>
+      <c r="AO21" s="13">
+        <v>68.8796680497925</v>
+      </c>
+      <c r="AP21" s="13">
+        <v>70.456431535269701</v>
+      </c>
+      <c r="AQ21" s="13">
+        <v>73.858921161825705</v>
+      </c>
+      <c r="AR21" s="13">
+        <v>78.6721991701245</v>
+      </c>
+      <c r="AS21" s="13">
+        <v>82.987551867219906</v>
+      </c>
+      <c r="AT21" s="13">
+        <v>85.394190871369304</v>
+      </c>
+      <c r="AU21" s="13">
+        <v>92.448132780083</v>
+      </c>
+      <c r="AV21" s="13">
+        <v>96.348547717842294</v>
+      </c>
+      <c r="AW21" s="13">
+        <v>100</v>
+      </c>
+      <c r="AX21" s="13">
+        <v>104.647302904564</v>
+      </c>
+      <c r="AY21" s="13">
+        <v>107.966804979253</v>
+      </c>
+      <c r="AZ21" s="13">
+        <v>111.203319502075</v>
+      </c>
+      <c r="BA21" s="13">
+        <v>115.767634854772</v>
+      </c>
+      <c r="BB21" s="13">
+        <v>117.42738589211601</v>
       </c>
       <c r="BP21" s="12"/>
     </row>
     <row r="22" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A22" s="44" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22" s="5">
         <v>1</v>
@@ -3623,90 +3665,92 @@
       <c r="D22" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AM22" s="7">
+      <c r="AB22" s="7">
+        <v>1</v>
+      </c>
+      <c r="BP22" s="12"/>
+    </row>
+    <row r="23" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A23" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB23" s="7">
+        <v>1</v>
+      </c>
+      <c r="AS23" s="7">
+        <v>5.4</v>
+      </c>
+      <c r="AY23" s="7">
+        <v>6</v>
+      </c>
+      <c r="AZ23" s="7">
+        <v>7.63</v>
+      </c>
+      <c r="BB23" s="7">
+        <v>8.4</v>
+      </c>
+      <c r="BP23" s="12"/>
+    </row>
+    <row r="24" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A24" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="5">
+        <v>1</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM24" s="7">
         <v>0.1</v>
       </c>
-      <c r="BB22" s="7">
+      <c r="BB24" s="7">
         <f>100*9028/7265000</f>
         <v>0.12426703372333103</v>
       </c>
-      <c r="BP22" s="12"/>
-    </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A23" s="44" t="s">
+      <c r="BP24" s="12"/>
+    </row>
+    <row r="25" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A25" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C25" s="5">
         <v>1</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D25" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="BB23" s="7">
+      <c r="BB25" s="7">
         <f>4.5/98 * 100</f>
         <v>4.591836734693878</v>
       </c>
-      <c r="BN23" s="12">
+      <c r="BN25" s="12">
         <v>2.2999999999999998</v>
       </c>
-      <c r="BP23" s="12"/>
-      <c r="BQ23" s="7">
-        <f>BB23/2</f>
+      <c r="BP25" s="12"/>
+      <c r="BQ25" s="7">
+        <f>BB25/2</f>
         <v>2.295918367346939</v>
       </c>
-    </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A24" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="5">
-        <v>1</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F24" s="7">
-        <v>2</v>
-      </c>
-      <c r="BB24" s="7">
-        <v>4.5</v>
-      </c>
-      <c r="BN24" s="12">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="BP24" s="12"/>
-      <c r="BR24" s="7">
-        <f>BB24/2</f>
-        <v>2.25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A25" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="5">
-        <v>1</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="BB25" s="7">
-        <v>0.4</v>
-      </c>
-      <c r="BP25" s="12"/>
     </row>
     <row r="26" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A26" s="44" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>4</v>
@@ -3717,90 +3761,132 @@
       <c r="D26" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="F26" s="7">
+        <v>2</v>
+      </c>
       <c r="BB26" s="7">
-        <v>0.4</v>
+        <v>4.5</v>
+      </c>
+      <c r="BN26" s="12">
+        <v>5.0999999999999996</v>
       </c>
       <c r="BP26" s="12"/>
+      <c r="BR26" s="7">
+        <f>BB26/2</f>
+        <v>2.25</v>
+      </c>
     </row>
     <row r="27" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A27" s="44" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C27" s="5">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AG27" s="7">
-        <v>67</v>
-      </c>
-      <c r="BH27" s="7">
-        <f>95*(1-0.064)</f>
-        <v>88.919999999999987</v>
+      <c r="BB27" s="7">
+        <v>0.4</v>
       </c>
       <c r="BP27" s="12"/>
     </row>
-    <row r="28" spans="1:70" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="B28" s="30" t="s">
+    <row r="28" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A28" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="5">
+        <v>1</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="30">
-        <v>1</v>
-      </c>
-      <c r="D28" s="30" t="s">
+      <c r="BB28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="BP28" s="12"/>
+    </row>
+    <row r="29" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A29" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="31">
-        <v>1</v>
-      </c>
-      <c r="K28" s="32">
-        <v>1</v>
-      </c>
-      <c r="U28" s="32">
-        <v>1</v>
-      </c>
-      <c r="V28" s="32">
-        <v>3.11</v>
-      </c>
-      <c r="BA28" s="32">
-        <v>3.11</v>
-      </c>
-      <c r="BF28" s="33"/>
-      <c r="BG28" s="33"/>
-      <c r="BH28" s="33"/>
-      <c r="BI28" s="33"/>
-      <c r="BJ28" s="33"/>
-      <c r="BK28" s="33"/>
-      <c r="BL28" s="33"/>
-      <c r="BM28" s="33"/>
-      <c r="BN28" s="33"/>
-      <c r="BO28" s="33"/>
-      <c r="BP28" s="33"/>
-    </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A29" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="C29" s="5">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AQ29" s="7">
+      <c r="AG29" s="7">
+        <v>67</v>
+      </c>
+      <c r="BP29" s="12"/>
+    </row>
+    <row r="30" spans="1:70" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="30">
         <v>1</v>
       </c>
-      <c r="AR29" s="7">
+      <c r="D30" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="31">
+        <v>1</v>
+      </c>
+      <c r="K30" s="32">
+        <v>1</v>
+      </c>
+      <c r="U30" s="32">
+        <v>1</v>
+      </c>
+      <c r="V30" s="32">
+        <v>3.11</v>
+      </c>
+      <c r="BA30" s="32">
+        <v>3.11</v>
+      </c>
+      <c r="BF30" s="33"/>
+      <c r="BG30" s="33"/>
+      <c r="BH30" s="33"/>
+      <c r="BI30" s="33"/>
+      <c r="BJ30" s="33"/>
+      <c r="BK30" s="33"/>
+      <c r="BL30" s="33"/>
+      <c r="BM30" s="33"/>
+      <c r="BN30" s="33"/>
+      <c r="BO30" s="33"/>
+      <c r="BP30" s="33"/>
+    </row>
+    <row r="31" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A31" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="5">
+        <v>1</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ31" s="7">
+        <v>1</v>
+      </c>
+      <c r="AR31" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3835,7 +3921,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D29:D1048576 D2:D13 D16:D27</xm:sqref>
+          <xm:sqref>D31:D1048576 D2:D13 D16:D29</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -3847,7 +3933,7 @@
           <x14:formula1>
             <xm:f>[1]dropdown_lists!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>D14:D15 D28</xm:sqref>
+          <xm:sqref>D14:D15 D30</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Update code for NGOs activities. Now applies to specific risk groups
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="612" windowWidth="16272" windowHeight="6300" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="612" windowWidth="16272" windowHeight="6300" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -2295,8 +2295,8 @@
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2596,7 +2596,7 @@
         <v>88</v>
       </c>
       <c r="B29" s="35">
-        <v>6.5000000000000002E-2</v>
+        <v>0.13</v>
       </c>
       <c r="C29" s="35"/>
       <c r="D29" s="35"/>
@@ -2607,7 +2607,7 @@
         <v>91</v>
       </c>
       <c r="B30" s="35">
-        <v>0.16</v>
+        <v>0.32</v>
       </c>
       <c r="C30" s="35"/>
       <c r="D30" s="35"/>
@@ -2667,11 +2667,11 @@
   </sheetPr>
   <dimension ref="A1:BR31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="BE8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="BF5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BH20" sqref="BH20"/>
+      <selection pane="bottomRight" activeCell="BI20" sqref="BI20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3452,7 +3452,9 @@
       <c r="BH19" s="12">
         <v>0</v>
       </c>
-      <c r="BJ19" s="12"/>
+      <c r="BJ19" s="12">
+        <v>0</v>
+      </c>
       <c r="BK19" s="12"/>
       <c r="BM19" s="12"/>
       <c r="BN19" s="12"/>
@@ -3479,10 +3481,13 @@
       <c r="BE20" s="12"/>
       <c r="BF20" s="12"/>
       <c r="BG20" s="12"/>
-      <c r="BH20" s="12">
+      <c r="BH20" s="12"/>
+      <c r="BI20" s="7">
         <v>0</v>
       </c>
-      <c r="BJ20" s="12"/>
+      <c r="BJ20" s="12">
+        <v>0</v>
+      </c>
       <c r="BK20" s="12"/>
       <c r="BM20" s="12"/>
       <c r="BN20" s="12"/>

</xml_diff>

<commit_message>
Remove time_variant request from sheets
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rragonnet\Google Drive\GitHub\AuTuMN\autumn\xls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="612" windowWidth="16272" windowHeight="6300" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -19,12 +14,12 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="93">
   <si>
     <t>parameter</t>
   </si>
@@ -60,9 +55,6 @@
   </si>
   <si>
     <t>program_prop_death_reporting</t>
-  </si>
-  <si>
-    <t>time_variant</t>
   </si>
   <si>
     <t>susceptible_fully</t>
@@ -2046,7 +2038,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2081,7 +2073,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2299,15 +2291,15 @@
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.5546875" style="19" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" style="22" customWidth="1"/>
-    <col min="3" max="5" width="9.109375" style="19"/>
-    <col min="6" max="6" width="13.88671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="19"/>
+    <col min="1" max="1" width="51.5703125" style="19" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="22" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="19"/>
+    <col min="6" max="6" width="13.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2340,7 +2332,7 @@
     </row>
     <row r="4" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="18">
         <v>1</v>
@@ -2350,7 +2342,7 @@
     </row>
     <row r="5" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="18">
         <v>5</v>
@@ -2363,7 +2355,7 @@
     </row>
     <row r="6" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="20">
         <v>12200000</v>
@@ -2373,7 +2365,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="22">
         <v>2.7</v>
@@ -2381,7 +2373,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="18">
         <v>1.5</v>
@@ -2389,7 +2381,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="18">
         <f>1/3</f>
@@ -2398,7 +2390,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="24">
         <v>26.22</v>
@@ -2409,7 +2401,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="24">
         <v>0</v>
@@ -2420,7 +2412,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="24">
         <v>265450</v>
@@ -2431,7 +2423,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="24">
         <v>3</v>
@@ -2442,7 +2434,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="24">
         <v>1</v>
@@ -2453,7 +2445,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="24">
         <v>26.24</v>
@@ -2464,7 +2456,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="13">
         <v>0</v>
@@ -2472,7 +2464,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="25">
         <v>11575186.195826644</v>
@@ -2480,7 +2472,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="13">
         <v>3</v>
@@ -2488,7 +2480,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="13">
         <v>1</v>
@@ -2496,7 +2488,7 @@
     </row>
     <row r="20" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B20" s="35">
         <f>20/12</f>
@@ -2508,7 +2500,7 @@
     </row>
     <row r="21" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B21" s="38">
         <f>12/20</f>
@@ -2517,12 +2509,12 @@
       <c r="C21" s="38"/>
       <c r="D21" s="38"/>
       <c r="E21" s="36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B22" s="38">
         <v>0.84</v>
@@ -2530,12 +2522,12 @@
       <c r="C22" s="38"/>
       <c r="D22" s="38"/>
       <c r="E22" s="36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B23" s="40">
         <v>1940</v>
@@ -2543,12 +2535,12 @@
       <c r="C23" s="41"/>
       <c r="D23" s="41"/>
       <c r="E23" s="42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B24" s="40">
         <v>1950</v>
@@ -2556,12 +2548,12 @@
       <c r="C24" s="41"/>
       <c r="D24" s="41"/>
       <c r="E24" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B25" s="22">
         <v>1995</v>
@@ -2569,7 +2561,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="36" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B26" s="22">
         <v>10</v>
@@ -2577,7 +2569,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B27" s="22">
         <v>15</v>
@@ -2585,7 +2577,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B28" s="22">
         <v>0.5</v>
@@ -2593,7 +2585,7 @@
     </row>
     <row r="29" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B29" s="35">
         <v>0.13</v>
@@ -2604,7 +2596,7 @@
     </row>
     <row r="30" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B30" s="35">
         <v>0.32</v>
@@ -2615,7 +2607,7 @@
     </row>
     <row r="31" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B31" s="35">
         <v>0.05</v>
@@ -2626,7 +2618,7 @@
     </row>
     <row r="32" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B32" s="35">
         <v>0.156</v>
@@ -2665,48 +2657,48 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BR31"/>
+  <dimension ref="A1:BQ31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="BF5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BI20" sqref="BI20"/>
+      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.77734375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="57.7109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11" style="5" customWidth="1"/>
-    <col min="5" max="5" width="11" style="6" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="18" width="7.44140625" style="7" customWidth="1"/>
-    <col min="19" max="24" width="7.33203125" style="7" customWidth="1"/>
-    <col min="25" max="26" width="7.44140625" style="7" customWidth="1"/>
-    <col min="27" max="28" width="7.109375" style="7" customWidth="1"/>
-    <col min="29" max="29" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="30" max="33" width="7.44140625" style="7" customWidth="1"/>
-    <col min="34" max="34" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="35" max="38" width="7.44140625" style="7" customWidth="1"/>
-    <col min="39" max="39" width="7.5546875" style="7" customWidth="1"/>
-    <col min="40" max="49" width="7" style="7" customWidth="1"/>
-    <col min="50" max="50" width="8.88671875" style="7" customWidth="1"/>
-    <col min="51" max="52" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="7.88671875" style="7" customWidth="1"/>
-    <col min="55" max="56" width="14" style="7" customWidth="1"/>
-    <col min="57" max="59" width="14.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="60" max="64" width="14.44140625" style="7" customWidth="1"/>
-    <col min="65" max="65" width="14.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="15.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="67" max="68" width="15" style="7" bestFit="1" customWidth="1"/>
-    <col min="69" max="70" width="15.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="71" max="16384" width="9.109375" style="7"/>
+    <col min="3" max="3" width="11" style="5" customWidth="1"/>
+    <col min="4" max="4" width="11" style="6" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="17" width="7.42578125" style="7" customWidth="1"/>
+    <col min="18" max="23" width="7.28515625" style="7" customWidth="1"/>
+    <col min="24" max="25" width="7.42578125" style="7" customWidth="1"/>
+    <col min="26" max="27" width="7.140625" style="7" customWidth="1"/>
+    <col min="28" max="28" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="29" max="32" width="7.42578125" style="7" customWidth="1"/>
+    <col min="33" max="33" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="34" max="37" width="7.42578125" style="7" customWidth="1"/>
+    <col min="38" max="38" width="7.5703125" style="7" customWidth="1"/>
+    <col min="39" max="48" width="7" style="7" customWidth="1"/>
+    <col min="49" max="49" width="8.85546875" style="7" customWidth="1"/>
+    <col min="50" max="51" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="52" max="53" width="7.85546875" style="7" customWidth="1"/>
+    <col min="54" max="55" width="14" style="7" customWidth="1"/>
+    <col min="56" max="58" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="59" max="63" width="14.42578125" style="7" customWidth="1"/>
+    <col min="64" max="64" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="66" max="67" width="15" style="7" bestFit="1" customWidth="1"/>
+    <col min="68" max="69" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="70" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:69" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
         <v>6</v>
       </c>
@@ -2716,164 +2708,164 @@
       <c r="C1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>12</v>
+      <c r="D1" s="2">
+        <v>1920</v>
       </c>
       <c r="E1" s="2">
-        <v>1920</v>
+        <v>1950</v>
       </c>
       <c r="F1" s="2">
-        <v>1950</v>
+        <v>1960</v>
       </c>
       <c r="G1" s="2">
-        <v>1960</v>
+        <v>1965</v>
       </c>
       <c r="H1" s="2">
-        <v>1965</v>
+        <v>1970</v>
       </c>
       <c r="I1" s="2">
-        <v>1970</v>
+        <v>1971</v>
       </c>
       <c r="J1" s="2">
-        <v>1971</v>
+        <v>1972</v>
       </c>
       <c r="K1" s="2">
-        <v>1972</v>
+        <v>1973</v>
       </c>
       <c r="L1" s="2">
-        <v>1973</v>
+        <v>1974</v>
       </c>
       <c r="M1" s="2">
-        <v>1974</v>
+        <v>1975</v>
       </c>
       <c r="N1" s="2">
-        <v>1975</v>
+        <v>1976</v>
       </c>
       <c r="O1" s="2">
-        <v>1976</v>
+        <v>1977</v>
       </c>
       <c r="P1" s="2">
-        <v>1977</v>
+        <v>1978</v>
       </c>
       <c r="Q1" s="2">
-        <v>1978</v>
+        <v>1979</v>
       </c>
       <c r="R1" s="2">
-        <v>1979</v>
+        <v>1980</v>
       </c>
       <c r="S1" s="2">
-        <v>1980</v>
+        <v>1981</v>
       </c>
       <c r="T1" s="2">
-        <v>1981</v>
+        <v>1982</v>
       </c>
       <c r="U1" s="2">
-        <v>1982</v>
+        <v>1983</v>
       </c>
       <c r="V1" s="2">
-        <v>1983</v>
+        <v>1984</v>
       </c>
       <c r="W1" s="2">
-        <v>1984</v>
+        <v>1985</v>
       </c>
       <c r="X1" s="2">
-        <v>1985</v>
+        <v>1986</v>
       </c>
       <c r="Y1" s="2">
-        <v>1986</v>
+        <v>1987</v>
       </c>
       <c r="Z1" s="2">
-        <v>1987</v>
+        <v>1988</v>
       </c>
       <c r="AA1" s="2">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="AB1" s="2">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="AC1" s="2">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="AD1" s="2">
-        <v>1991</v>
+        <v>1992</v>
       </c>
       <c r="AE1" s="2">
-        <v>1992</v>
+        <v>1993</v>
       </c>
       <c r="AF1" s="2">
-        <v>1993</v>
+        <v>1994</v>
       </c>
       <c r="AG1" s="2">
-        <v>1994</v>
+        <v>1995</v>
       </c>
       <c r="AH1" s="2">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="AI1" s="2">
-        <v>1996</v>
+        <v>1997</v>
       </c>
       <c r="AJ1" s="2">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="AK1" s="2">
-        <v>1998</v>
+        <v>1999</v>
       </c>
       <c r="AL1" s="2">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="AM1" s="2">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="AN1" s="2">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="AO1" s="2">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="AP1" s="2">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="AQ1" s="2">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="AR1" s="2">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="AS1" s="2">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="AT1" s="2">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="AU1" s="2">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="AV1" s="2">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="AW1" s="2">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="AX1" s="2">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="AY1" s="2">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="AZ1" s="2">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="BA1" s="2">
-        <v>2014</v>
-      </c>
-      <c r="BB1" s="2">
         <v>2015</v>
       </c>
+      <c r="BB1" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="BC1" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BD1" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="BE1" s="2" t="s">
         <v>14</v>
@@ -2885,13 +2877,13 @@
         <v>16</v>
       </c>
       <c r="BH1" s="2" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="BI1" s="2" t="s">
         <v>42</v>
       </c>
       <c r="BJ1" s="2" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="BK1" s="2" t="s">
         <v>55</v>
@@ -2900,7 +2892,7 @@
         <v>56</v>
       </c>
       <c r="BM1" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="BN1" s="2" t="s">
         <v>61</v>
@@ -2909,18 +2901,15 @@
         <v>62</v>
       </c>
       <c r="BP1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="BQ1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="BQ1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="BR1" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:70" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>3</v>
@@ -2928,18 +2917,15 @@
       <c r="C2" s="11">
         <v>0.1</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="BB2" s="26"/>
       <c r="BC2" s="26"/>
-      <c r="BD2" s="26"/>
-      <c r="BL2" s="26"/>
-      <c r="BN2" s="26"/>
-    </row>
-    <row r="3" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BK2" s="26"/>
+      <c r="BM2" s="26"/>
+    </row>
+    <row r="3" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A3" s="44" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>3</v>
@@ -2947,9 +2933,7 @@
       <c r="C3" s="5">
         <v>0.2</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="AG3" s="8"/>
       <c r="AH3" s="8"/>
       <c r="AI3" s="8"/>
       <c r="AJ3" s="8"/>
@@ -2966,18 +2950,17 @@
       <c r="AU3" s="8"/>
       <c r="AV3" s="8"/>
       <c r="AW3" s="8"/>
-      <c r="AX3" s="8"/>
+      <c r="AX3" s="8">
+        <v>93</v>
+      </c>
       <c r="AY3" s="8">
-        <v>93</v>
-      </c>
-      <c r="AZ3" s="8">
         <v>85</v>
       </c>
-      <c r="BM3" s="12"/>
-    </row>
-    <row r="4" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BL3" s="12"/>
+    </row>
+    <row r="4" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A4" s="44" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>3</v>
@@ -2985,21 +2968,19 @@
       <c r="C4" s="5">
         <v>0.2</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AH4" s="9"/>
+      <c r="AG4" s="9"/>
+      <c r="AH4" s="8"/>
       <c r="AI4" s="8"/>
       <c r="AJ4" s="8"/>
       <c r="AK4" s="8"/>
-      <c r="AL4" s="8"/>
-      <c r="AM4" s="9"/>
+      <c r="AL4" s="9"/>
+      <c r="AM4" s="8"/>
       <c r="AN4" s="8"/>
       <c r="AO4" s="8"/>
       <c r="AP4" s="8"/>
-      <c r="AQ4" s="8"/>
-      <c r="AR4" s="9"/>
-      <c r="AS4" s="8"/>
+      <c r="AQ4" s="9"/>
+      <c r="AR4" s="8"/>
+      <c r="AS4" s="9"/>
       <c r="AT4" s="9"/>
       <c r="AU4" s="9"/>
       <c r="AV4" s="9"/>
@@ -3008,12 +2989,11 @@
       <c r="AY4" s="9"/>
       <c r="AZ4" s="9"/>
       <c r="BA4" s="9"/>
-      <c r="BB4" s="9"/>
-      <c r="BM4" s="12"/>
-    </row>
-    <row r="5" spans="1:70" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BL4" s="12"/>
+    </row>
+    <row r="5" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>4</v>
@@ -3021,20 +3001,17 @@
       <c r="C5" s="11">
         <v>1</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="BB5" s="9">
+      <c r="D5" s="1"/>
+      <c r="BA5" s="9">
         <v>0</v>
       </c>
-      <c r="BD5" s="26"/>
-      <c r="BF5" s="26"/>
-      <c r="BM5" s="26"/>
-    </row>
-    <row r="6" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BC5" s="26"/>
+      <c r="BE5" s="26"/>
+      <c r="BL5" s="26"/>
+    </row>
+    <row r="6" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A6" s="44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>4</v>
@@ -3042,27 +3019,24 @@
       <c r="C6" s="5">
         <v>1</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="7">
+      <c r="F6" s="7">
         <v>0</v>
       </c>
-      <c r="AE6" s="7">
+      <c r="AD6" s="7">
         <v>0</v>
       </c>
-      <c r="BB6" s="7">
+      <c r="BA6" s="7">
         <v>0</v>
       </c>
+      <c r="BD6" s="12"/>
       <c r="BE6" s="12"/>
       <c r="BF6" s="12"/>
       <c r="BG6" s="12"/>
-      <c r="BH6" s="12"/>
-      <c r="BM6" s="12"/>
-    </row>
-    <row r="7" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BL6" s="12"/>
+    </row>
+    <row r="7" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A7" s="44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>4</v>
@@ -3070,21 +3044,18 @@
       <c r="C7" s="5">
         <v>1</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="BB7" s="7">
+      <c r="BA7" s="7">
         <v>0</v>
       </c>
+      <c r="BD7" s="12"/>
       <c r="BE7" s="12"/>
       <c r="BF7" s="12"/>
       <c r="BG7" s="12"/>
-      <c r="BH7" s="12"/>
-      <c r="BM7" s="12"/>
-    </row>
-    <row r="8" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BL7" s="12"/>
+    </row>
+    <row r="8" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A8" s="44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>4</v>
@@ -3092,23 +3063,20 @@
       <c r="C8" s="5">
         <v>1</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="BB8" s="7">
+      <c r="BA8" s="7">
         <v>0</v>
       </c>
+      <c r="BD8" s="12"/>
       <c r="BE8" s="12"/>
       <c r="BF8" s="12"/>
       <c r="BG8" s="12"/>
       <c r="BH8" s="12"/>
       <c r="BI8" s="12"/>
-      <c r="BJ8" s="12"/>
-      <c r="BM8" s="12"/>
-    </row>
-    <row r="9" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BL8" s="12"/>
+    </row>
+    <row r="9" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A9" s="44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>4</v>
@@ -3116,23 +3084,20 @@
       <c r="C9" s="5">
         <v>1</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="BB9" s="7">
+      <c r="BA9" s="7">
         <v>0</v>
       </c>
+      <c r="BD9" s="12"/>
       <c r="BE9" s="12"/>
       <c r="BF9" s="12"/>
       <c r="BG9" s="12"/>
       <c r="BH9" s="12"/>
       <c r="BI9" s="12"/>
-      <c r="BJ9" s="12"/>
-      <c r="BM9" s="12"/>
-    </row>
-    <row r="10" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BL9" s="12"/>
+    </row>
+    <row r="10" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A10" s="44" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>4</v>
@@ -3140,26 +3105,23 @@
       <c r="C10" s="5">
         <v>1</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="BB10" s="7">
+      <c r="BA10" s="7">
         <v>0</v>
       </c>
+      <c r="BD10" s="12"/>
       <c r="BE10" s="12"/>
-      <c r="BF10" s="12"/>
-      <c r="BG10" s="12">
+      <c r="BF10" s="12">
         <v>50</v>
       </c>
-      <c r="BH10" s="12"/>
+      <c r="BG10" s="12"/>
+      <c r="BJ10" s="12"/>
       <c r="BK10" s="12"/>
       <c r="BL10" s="12"/>
-      <c r="BM10" s="12"/>
-      <c r="BO10" s="12"/>
-    </row>
-    <row r="11" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BN10" s="12"/>
+    </row>
+    <row r="11" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A11" s="44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>4</v>
@@ -3167,26 +3129,23 @@
       <c r="C11" s="5">
         <v>1</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>3</v>
+      <c r="AV11" s="7">
+        <v>0</v>
       </c>
       <c r="AW11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AX11" s="7">
         <v>10</v>
       </c>
+      <c r="BD11" s="12"/>
       <c r="BE11" s="12"/>
       <c r="BF11" s="12"/>
       <c r="BG11" s="12"/>
-      <c r="BH11" s="12"/>
+      <c r="BJ11" s="12"/>
       <c r="BK11" s="12"/>
       <c r="BL11" s="12"/>
-      <c r="BM11" s="12"/>
-    </row>
-    <row r="12" spans="1:70" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A12" s="44" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>4</v>
@@ -3194,27 +3153,24 @@
       <c r="C12" s="5">
         <v>1</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>3</v>
+      <c r="AV12" s="7">
+        <v>0</v>
       </c>
       <c r="AW12" s="7">
-        <v>0</v>
-      </c>
-      <c r="AX12" s="7">
         <v>10</v>
       </c>
+      <c r="BD12" s="12"/>
       <c r="BE12" s="12"/>
       <c r="BF12" s="12"/>
       <c r="BG12" s="12"/>
       <c r="BH12" s="12"/>
-      <c r="BI12" s="12"/>
+      <c r="BJ12" s="12"/>
       <c r="BK12" s="12"/>
       <c r="BL12" s="12"/>
-      <c r="BM12" s="12"/>
-    </row>
-    <row r="13" spans="1:70" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A13" s="44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>4</v>
@@ -3222,24 +3178,21 @@
       <c r="C13" s="5">
         <v>1</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="BB13" s="7">
+      <c r="BA13" s="7">
         <v>0</v>
       </c>
+      <c r="BD13" s="12"/>
       <c r="BE13" s="12"/>
       <c r="BF13" s="12"/>
       <c r="BG13" s="12"/>
-      <c r="BH13" s="12"/>
+      <c r="BI13" s="12"/>
       <c r="BJ13" s="12"/>
-      <c r="BK13" s="12"/>
+      <c r="BL13" s="12"/>
       <c r="BM13" s="12"/>
-      <c r="BN13" s="12"/>
-    </row>
-    <row r="14" spans="1:70" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:69" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" s="27" t="s">
         <v>4</v>
@@ -3247,9 +3200,7 @@
       <c r="C14" s="27">
         <v>0.5</v>
       </c>
-      <c r="D14" s="27" t="s">
-        <v>3</v>
-      </c>
+      <c r="D14" s="28"/>
       <c r="E14" s="28"/>
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
@@ -3272,41 +3223,40 @@
       <c r="X14" s="28"/>
       <c r="Y14" s="28"/>
       <c r="Z14" s="28"/>
-      <c r="AA14" s="28"/>
+      <c r="AA14" s="29">
+        <v>0</v>
+      </c>
       <c r="AB14" s="29">
-        <v>0</v>
-      </c>
-      <c r="AC14" s="29">
         <v>5</v>
       </c>
-      <c r="AW14" s="29">
+      <c r="AV14" s="29">
         <f>80*(1174/2649)</f>
         <v>35.454888637221593</v>
       </c>
-      <c r="AX14" s="29">
+      <c r="AW14" s="29">
         <f>80*(1077/2407)</f>
         <v>35.795596177814708</v>
       </c>
-      <c r="AY14" s="29">
+      <c r="AX14" s="29">
         <f>80*(1094/2280)</f>
         <v>38.385964912280699</v>
       </c>
-      <c r="AZ14" s="29">
+      <c r="AY14" s="29">
         <f>80*(961/1932)</f>
         <v>39.792960662525878</v>
       </c>
-      <c r="BA14" s="29">
+      <c r="AZ14" s="29">
         <f>80*(891/1872)</f>
         <v>38.076923076923073</v>
       </c>
-      <c r="BB14" s="29">
+      <c r="BA14" s="29">
         <f>80*782/1660</f>
         <v>37.686746987951807</v>
       </c>
     </row>
-    <row r="15" spans="1:70" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:69" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B15" s="27" t="s">
         <v>4</v>
@@ -3314,9 +3264,7 @@
       <c r="C15" s="27">
         <v>1</v>
       </c>
-      <c r="D15" s="27" t="s">
-        <v>3</v>
-      </c>
+      <c r="D15" s="28"/>
       <c r="E15" s="28"/>
       <c r="F15" s="28"/>
       <c r="G15" s="28"/>
@@ -3339,14 +3287,13 @@
       <c r="X15" s="28"/>
       <c r="Y15" s="28"/>
       <c r="Z15" s="28"/>
-      <c r="AA15" s="28"/>
-      <c r="BB15" s="29">
+      <c r="BA15" s="29">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A16" s="44" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>4</v>
@@ -3354,26 +3301,23 @@
       <c r="C16" s="5">
         <v>1</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="BB16" s="7">
+      <c r="BA16" s="7">
         <v>0</v>
       </c>
-      <c r="BE16" s="12"/>
-      <c r="BF16" s="12">
+      <c r="BD16" s="12"/>
+      <c r="BE16" s="12">
         <v>100</v>
       </c>
+      <c r="BF16" s="12"/>
       <c r="BG16" s="12"/>
-      <c r="BH16" s="12"/>
+      <c r="BI16" s="12"/>
       <c r="BJ16" s="12"/>
-      <c r="BK16" s="12"/>
+      <c r="BL16" s="12"/>
       <c r="BM16" s="12"/>
-      <c r="BN16" s="12"/>
-    </row>
-    <row r="17" spans="1:70" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A17" s="44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>4</v>
@@ -3381,27 +3325,24 @@
       <c r="C17" s="5">
         <v>1</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AW17" s="7">
+      <c r="AV17" s="7">
         <v>50</v>
       </c>
-      <c r="BD17" s="7">
+      <c r="BC17" s="7">
         <v>100</v>
       </c>
+      <c r="BD17" s="12"/>
       <c r="BE17" s="12"/>
       <c r="BF17" s="12"/>
       <c r="BG17" s="12"/>
-      <c r="BH17" s="12"/>
+      <c r="BI17" s="12"/>
       <c r="BJ17" s="12"/>
-      <c r="BK17" s="12"/>
+      <c r="BL17" s="12"/>
       <c r="BM17" s="12"/>
-      <c r="BN17" s="12"/>
-    </row>
-    <row r="18" spans="1:70" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A18" s="44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>4</v>
@@ -3409,27 +3350,24 @@
       <c r="C18" s="5">
         <v>1</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AW18" s="7">
+      <c r="AV18" s="7">
         <v>100</v>
       </c>
-      <c r="BD18" s="7">
+      <c r="BC18" s="7">
         <v>100</v>
       </c>
+      <c r="BD18" s="12"/>
       <c r="BE18" s="12"/>
       <c r="BF18" s="12"/>
       <c r="BG18" s="12"/>
-      <c r="BH18" s="12"/>
+      <c r="BI18" s="12"/>
       <c r="BJ18" s="12"/>
-      <c r="BK18" s="12"/>
+      <c r="BL18" s="12"/>
       <c r="BM18" s="12"/>
-      <c r="BN18" s="12"/>
-    </row>
-    <row r="19" spans="1:70" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A19" s="44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>4</v>
@@ -3437,31 +3375,28 @@
       <c r="C19" s="5">
         <v>1</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="6">
+      <c r="D19" s="6">
         <v>100</v>
       </c>
-      <c r="BB19" s="7">
+      <c r="BA19" s="7">
         <v>100</v>
       </c>
+      <c r="BD19" s="12"/>
       <c r="BE19" s="12"/>
       <c r="BF19" s="12"/>
-      <c r="BG19" s="12"/>
-      <c r="BH19" s="12">
+      <c r="BG19" s="12">
         <v>0</v>
       </c>
-      <c r="BJ19" s="12">
+      <c r="BI19" s="12">
         <v>0</v>
       </c>
-      <c r="BK19" s="12"/>
+      <c r="BJ19" s="12"/>
+      <c r="BL19" s="12"/>
       <c r="BM19" s="12"/>
-      <c r="BN19" s="12"/>
-    </row>
-    <row r="20" spans="1:70" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A20" s="44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>4</v>
@@ -3469,32 +3404,29 @@
       <c r="C20" s="5">
         <v>1</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="6">
+      <c r="D20" s="6">
         <v>100</v>
       </c>
-      <c r="BB20" s="7">
+      <c r="BA20" s="7">
         <v>100</v>
       </c>
+      <c r="BD20" s="12"/>
       <c r="BE20" s="12"/>
       <c r="BF20" s="12"/>
       <c r="BG20" s="12"/>
-      <c r="BH20" s="12"/>
-      <c r="BI20" s="7">
+      <c r="BH20" s="7">
         <v>0</v>
       </c>
-      <c r="BJ20" s="12">
+      <c r="BI20" s="12">
         <v>0</v>
       </c>
-      <c r="BK20" s="12"/>
+      <c r="BJ20" s="12"/>
+      <c r="BL20" s="12"/>
       <c r="BM20" s="12"/>
-      <c r="BN20" s="12"/>
-    </row>
-    <row r="21" spans="1:70" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A21" s="44" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>4</v>
@@ -3502,164 +3434,161 @@
       <c r="C21" s="5">
         <v>1</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="6">
+      <c r="D21" s="6">
         <v>1</v>
       </c>
+      <c r="E21" s="13">
+        <v>1</v>
+      </c>
       <c r="F21" s="13">
-        <v>1</v>
+        <v>1.1289570744394</v>
       </c>
       <c r="G21" s="13">
-        <v>1.1289570744394</v>
+        <v>1.42215881727406</v>
       </c>
       <c r="H21" s="13">
-        <v>1.42215881727406</v>
+        <v>1.90118931222233</v>
       </c>
       <c r="I21" s="13">
-        <v>1.90118931222233</v>
+        <v>2.3081073919986701</v>
       </c>
       <c r="J21" s="13">
-        <v>2.3081073919986701</v>
+        <v>2.4974653103104298</v>
       </c>
       <c r="K21" s="13">
-        <v>2.4974653103104298</v>
+        <v>2.9115458645382701</v>
       </c>
       <c r="L21" s="13">
-        <v>2.9115458645382701</v>
+        <v>3.90623450399154</v>
       </c>
       <c r="M21" s="13">
-        <v>3.90623450399154</v>
+        <v>4.1703507493909102</v>
       </c>
       <c r="N21" s="13">
-        <v>4.1703507493909102</v>
+        <v>4.55399078719985</v>
       </c>
       <c r="O21" s="13">
-        <v>4.55399078719985</v>
+        <v>5.0047790229916798</v>
       </c>
       <c r="P21" s="13">
-        <v>5.0047790229916798</v>
+        <v>5.3718558386314896</v>
       </c>
       <c r="Q21" s="13">
-        <v>5.3718558386314896</v>
+        <v>6.3137212289735496</v>
       </c>
       <c r="R21" s="13">
-        <v>6.3137212289735496</v>
+        <v>7.4628507238053698</v>
       </c>
       <c r="S21" s="13">
-        <v>7.4628507238053698</v>
+        <v>8.4391855224587609</v>
       </c>
       <c r="T21" s="13">
-        <v>8.4391855224587609</v>
+        <v>9.3018160392078606</v>
       </c>
       <c r="U21" s="13">
-        <v>9.3018160392078606</v>
+        <v>10.2347283365258</v>
       </c>
       <c r="V21" s="13">
-        <v>10.2347283365258</v>
+        <v>15.386785740408699</v>
       </c>
       <c r="W21" s="13">
-        <v>15.386785740408699</v>
+        <v>18.9416113416321</v>
       </c>
       <c r="X21" s="13">
-        <v>18.9416113416321</v>
+        <v>19.1590871369295</v>
       </c>
       <c r="Y21" s="13">
-        <v>19.1590871369295</v>
+        <v>19.938817427385899</v>
       </c>
       <c r="Z21" s="13">
-        <v>19.938817427385899</v>
+        <v>22.702351313969601</v>
       </c>
       <c r="AA21" s="13">
-        <v>22.702351313969601</v>
+        <v>25.481798063623799</v>
       </c>
       <c r="AB21" s="13">
-        <v>25.481798063623799</v>
+        <v>28.584806362378998</v>
       </c>
       <c r="AC21" s="13">
-        <v>28.584806362378998</v>
+        <v>34.090656984785603</v>
       </c>
       <c r="AD21" s="13">
-        <v>34.090656984785603</v>
+        <v>37.0398409405256</v>
       </c>
       <c r="AE21" s="13">
-        <v>37.0398409405256</v>
+        <v>39.527551867219898</v>
       </c>
       <c r="AF21" s="13">
-        <v>39.527551867219898</v>
+        <v>43.633070539419101</v>
       </c>
       <c r="AG21" s="13">
-        <v>43.633070539419101</v>
+        <v>46.6140802213001</v>
       </c>
       <c r="AH21" s="13">
-        <v>46.6140802213001</v>
+        <v>50.0989972337483</v>
       </c>
       <c r="AI21" s="13">
-        <v>50.0989972337483</v>
+        <v>52.899661134163203</v>
       </c>
       <c r="AJ21" s="13">
-        <v>52.899661134163203</v>
+        <v>57.784910096818798</v>
       </c>
       <c r="AK21" s="13">
-        <v>57.784910096818798</v>
+        <v>61.2167842323652</v>
       </c>
       <c r="AL21" s="13">
-        <v>61.2167842323652</v>
+        <v>63.651452282157699</v>
       </c>
       <c r="AM21" s="13">
-        <v>63.651452282157699</v>
+        <v>67.053941908713696</v>
       </c>
       <c r="AN21" s="13">
-        <v>67.053941908713696</v>
+        <v>68.8796680497925</v>
       </c>
       <c r="AO21" s="13">
-        <v>68.8796680497925</v>
+        <v>70.456431535269701</v>
       </c>
       <c r="AP21" s="13">
-        <v>70.456431535269701</v>
+        <v>73.858921161825705</v>
       </c>
       <c r="AQ21" s="13">
-        <v>73.858921161825705</v>
+        <v>78.6721991701245</v>
       </c>
       <c r="AR21" s="13">
-        <v>78.6721991701245</v>
+        <v>82.987551867219906</v>
       </c>
       <c r="AS21" s="13">
-        <v>82.987551867219906</v>
+        <v>85.394190871369304</v>
       </c>
       <c r="AT21" s="13">
-        <v>85.394190871369304</v>
+        <v>92.448132780083</v>
       </c>
       <c r="AU21" s="13">
-        <v>92.448132780083</v>
+        <v>96.348547717842294</v>
       </c>
       <c r="AV21" s="13">
-        <v>96.348547717842294</v>
+        <v>100</v>
       </c>
       <c r="AW21" s="13">
-        <v>100</v>
+        <v>104.647302904564</v>
       </c>
       <c r="AX21" s="13">
-        <v>104.647302904564</v>
+        <v>107.966804979253</v>
       </c>
       <c r="AY21" s="13">
-        <v>107.966804979253</v>
+        <v>111.203319502075</v>
       </c>
       <c r="AZ21" s="13">
-        <v>111.203319502075</v>
+        <v>115.767634854772</v>
       </c>
       <c r="BA21" s="13">
-        <v>115.767634854772</v>
-      </c>
-      <c r="BB21" s="13">
         <v>117.42738589211601</v>
       </c>
-      <c r="BP21" s="12"/>
-    </row>
-    <row r="22" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BO21" s="12"/>
+    </row>
+    <row r="22" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A22" s="44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>3</v>
@@ -3667,17 +3596,14 @@
       <c r="C22" s="5">
         <v>1</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB22" s="7">
+      <c r="AA22" s="7">
         <v>1</v>
       </c>
-      <c r="BP22" s="12"/>
-    </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BO22" s="12"/>
+    </row>
+    <row r="23" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A23" s="44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>3</v>
@@ -3685,29 +3611,26 @@
       <c r="C23" s="5">
         <v>1</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB23" s="7">
+      <c r="AA23" s="7">
         <v>1</v>
       </c>
-      <c r="AS23" s="7">
+      <c r="AR23" s="7">
         <v>5.4</v>
       </c>
+      <c r="AX23" s="7">
+        <v>6</v>
+      </c>
       <c r="AY23" s="7">
-        <v>6</v>
-      </c>
-      <c r="AZ23" s="7">
         <v>7.63</v>
       </c>
-      <c r="BB23" s="7">
+      <c r="BA23" s="7">
         <v>8.4</v>
       </c>
-      <c r="BP23" s="12"/>
-    </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BO23" s="12"/>
+    </row>
+    <row r="24" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A24" s="44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>4</v>
@@ -3715,21 +3638,18 @@
       <c r="C24" s="5">
         <v>1</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AM24" s="7">
+      <c r="AL24" s="7">
         <v>0.1</v>
       </c>
-      <c r="BB24" s="7">
+      <c r="BA24" s="7">
         <f>100*9028/7265000</f>
         <v>0.12426703372333103</v>
       </c>
-      <c r="BP24" s="12"/>
-    </row>
-    <row r="25" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BO24" s="12"/>
+    </row>
+    <row r="25" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A25" s="44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>4</v>
@@ -3737,25 +3657,22 @@
       <c r="C25" s="5">
         <v>1</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="BB25" s="7">
+      <c r="BA25" s="7">
         <f>4.5/98 * 100</f>
         <v>4.591836734693878</v>
       </c>
-      <c r="BN25" s="12">
+      <c r="BM25" s="12">
         <v>2.2999999999999998</v>
       </c>
-      <c r="BP25" s="12"/>
-      <c r="BQ25" s="7">
-        <f>BB25/2</f>
+      <c r="BO25" s="12"/>
+      <c r="BP25" s="7">
+        <f>BA25/2</f>
         <v>2.295918367346939</v>
       </c>
     </row>
-    <row r="26" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A26" s="44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>4</v>
@@ -3763,27 +3680,24 @@
       <c r="C26" s="5">
         <v>1</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F26" s="7">
+      <c r="E26" s="7">
         <v>2</v>
       </c>
-      <c r="BB26" s="7">
+      <c r="BA26" s="7">
         <v>4.5</v>
       </c>
-      <c r="BN26" s="12">
+      <c r="BM26" s="12">
         <v>5.0999999999999996</v>
       </c>
-      <c r="BP26" s="12"/>
-      <c r="BR26" s="7">
-        <f>BB26/2</f>
+      <c r="BO26" s="12"/>
+      <c r="BQ26" s="7">
+        <f>BA26/2</f>
         <v>2.25</v>
       </c>
     </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A27" s="44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>4</v>
@@ -3791,17 +3705,14 @@
       <c r="C27" s="5">
         <v>1</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="BB27" s="7">
+      <c r="BA27" s="7">
         <v>0.4</v>
       </c>
-      <c r="BP27" s="12"/>
-    </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BO27" s="12"/>
+    </row>
+    <row r="28" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A28" s="44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>4</v>
@@ -3809,17 +3720,14 @@
       <c r="C28" s="5">
         <v>1</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="BB28" s="7">
+      <c r="BA28" s="7">
         <v>0.4</v>
       </c>
-      <c r="BP28" s="12"/>
-    </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="BO28" s="12"/>
+    </row>
+    <row r="29" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A29" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>3</v>
@@ -3827,17 +3735,14 @@
       <c r="C29" s="5">
         <v>0.3</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AG29" s="7">
+      <c r="AF29" s="7">
         <v>67</v>
       </c>
-      <c r="BP29" s="12"/>
-    </row>
-    <row r="30" spans="1:70" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BO29" s="12"/>
+    </row>
+    <row r="30" spans="1:69" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B30" s="30" t="s">
         <v>3</v>
@@ -3845,24 +3750,22 @@
       <c r="C30" s="30">
         <v>1</v>
       </c>
-      <c r="D30" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="E30" s="31">
+      <c r="D30" s="31">
         <v>1</v>
       </c>
-      <c r="K30" s="32">
+      <c r="J30" s="32">
         <v>1</v>
       </c>
+      <c r="T30" s="32">
+        <v>1</v>
+      </c>
       <c r="U30" s="32">
-        <v>1</v>
-      </c>
-      <c r="V30" s="32">
         <v>3.11</v>
       </c>
-      <c r="BA30" s="32">
+      <c r="AZ30" s="32">
         <v>3.11</v>
       </c>
+      <c r="BE30" s="33"/>
       <c r="BF30" s="33"/>
       <c r="BG30" s="33"/>
       <c r="BH30" s="33"/>
@@ -3873,11 +3776,10 @@
       <c r="BM30" s="33"/>
       <c r="BN30" s="33"/>
       <c r="BO30" s="33"/>
-      <c r="BP30" s="33"/>
-    </row>
-    <row r="31" spans="1:70" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A31" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>4</v>
@@ -3885,24 +3787,21 @@
       <c r="C31" s="5">
         <v>1</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>3</v>
+      <c r="AP31" s="7">
+        <v>1</v>
       </c>
       <c r="AQ31" s="7">
         <v>1</v>
       </c>
-      <c r="AR31" s="7">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="4">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF5 BC5:BD5">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BE5 BB5:BC5">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:D1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BE2 F2:BB5 BC3:BE4 E14:AA15">
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1"/>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BD2 E2:BA5 BB3:BD4 D14:Z15">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -3915,30 +3814,18 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="382" yWindow="552" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="382" yWindow="552" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time-variant?" prompt="If no, the most recent value will be selected.">
-          <x14:formula1>
-            <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>D31:D1048576 D2:D13 D16:D29</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>[1]dropdown_lists!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B14:B15</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time-variant?" prompt="If no, the most recent value will be selected.">
-          <x14:formula1>
-            <xm:f>[1]dropdown_lists!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>D14:D15 D30</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3957,7 +3844,7 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -3967,10 +3854,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
         <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -3981,7 +3868,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3989,7 +3876,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Delete unnecessary data from spreadsheets
Delete unnecessary smoothness values from spreadsheets.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -1987,8 +1987,8 @@
       <sheetName val="dropdown_lists"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
@@ -2660,10 +2660,10 @@
   <dimension ref="A1:BQ31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomRight" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2998,9 +2998,7 @@
       <c r="B5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="11">
-        <v>1</v>
-      </c>
+      <c r="C5" s="11"/>
       <c r="D5" s="1"/>
       <c r="BA5" s="9">
         <v>0</v>
@@ -3015,9 +3013,6 @@
       </c>
       <c r="B6" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="C6" s="5">
-        <v>1</v>
       </c>
       <c r="F6" s="7">
         <v>0</v>
@@ -3041,9 +3036,6 @@
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="5">
-        <v>1</v>
-      </c>
       <c r="BA7" s="7">
         <v>0</v>
       </c>
@@ -3059,9 +3051,6 @@
       </c>
       <c r="B8" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="C8" s="5">
-        <v>1</v>
       </c>
       <c r="BA8" s="7">
         <v>0</v>
@@ -3081,9 +3070,6 @@
       <c r="B9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="5">
-        <v>1</v>
-      </c>
       <c r="BA9" s="7">
         <v>0</v>
       </c>
@@ -3102,9 +3088,6 @@
       <c r="B10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="5">
-        <v>1</v>
-      </c>
       <c r="BA10" s="7">
         <v>0</v>
       </c>
@@ -3125,9 +3108,6 @@
       </c>
       <c r="B11" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="C11" s="5">
-        <v>1</v>
       </c>
       <c r="AV11" s="7">
         <v>0</v>
@@ -3149,9 +3129,6 @@
       </c>
       <c r="B12" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="C12" s="5">
-        <v>1</v>
       </c>
       <c r="AV12" s="7">
         <v>0</v>
@@ -3174,9 +3151,6 @@
       </c>
       <c r="B13" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="C13" s="5">
-        <v>1</v>
       </c>
       <c r="BA13" s="7">
         <v>0</v>
@@ -3261,9 +3235,7 @@
       <c r="B15" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="27">
-        <v>1</v>
-      </c>
+      <c r="C15" s="27"/>
       <c r="D15" s="28"/>
       <c r="E15" s="28"/>
       <c r="F15" s="28"/>
@@ -3298,9 +3270,6 @@
       <c r="B16" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="5">
-        <v>1</v>
-      </c>
       <c r="BA16" s="7">
         <v>0</v>
       </c>
@@ -3321,9 +3290,6 @@
       </c>
       <c r="B17" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="C17" s="5">
-        <v>1</v>
       </c>
       <c r="AV17" s="7">
         <v>50</v>
@@ -3347,9 +3313,6 @@
       <c r="B18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="5">
-        <v>1</v>
-      </c>
       <c r="AV18" s="7">
         <v>100</v>
       </c>
@@ -3372,9 +3335,6 @@
       <c r="B19" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="5">
-        <v>1</v>
-      </c>
       <c r="D19" s="6">
         <v>100</v>
       </c>
@@ -3400,9 +3360,6 @@
       </c>
       <c r="B20" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="C20" s="5">
-        <v>1</v>
       </c>
       <c r="D20" s="6">
         <v>100</v>
@@ -3431,9 +3388,6 @@
       <c r="B21" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="5">
-        <v>1</v>
-      </c>
       <c r="D21" s="6">
         <v>1</v>
       </c>
@@ -3593,9 +3547,6 @@
       <c r="B22" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="5">
-        <v>1</v>
-      </c>
       <c r="AA22" s="7">
         <v>1</v>
       </c>
@@ -3608,9 +3559,6 @@
       <c r="B23" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="5">
-        <v>1</v>
-      </c>
       <c r="AA23" s="7">
         <v>1</v>
       </c>
@@ -3635,9 +3583,6 @@
       <c r="B24" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="5">
-        <v>1</v>
-      </c>
       <c r="AL24" s="7">
         <v>0.1</v>
       </c>
@@ -3653,9 +3598,6 @@
       </c>
       <c r="B25" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="C25" s="5">
-        <v>1</v>
       </c>
       <c r="BA25" s="7">
         <f>4.5/98 * 100</f>
@@ -3677,9 +3619,6 @@
       <c r="B26" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="5">
-        <v>1</v>
-      </c>
       <c r="E26" s="7">
         <v>2</v>
       </c>
@@ -3702,9 +3641,6 @@
       <c r="B27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="5">
-        <v>1</v>
-      </c>
       <c r="BA27" s="7">
         <v>0.4</v>
       </c>
@@ -3717,9 +3653,6 @@
       <c r="B28" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="5">
-        <v>1</v>
-      </c>
       <c r="BA28" s="7">
         <v>0.4</v>
       </c>
@@ -3747,9 +3680,7 @@
       <c r="B30" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="30">
-        <v>1</v>
-      </c>
+      <c r="C30" s="30"/>
       <c r="D30" s="31">
         <v>1</v>
       </c>
@@ -3783,9 +3714,6 @@
       </c>
       <c r="B31" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="C31" s="5">
-        <v>1</v>
       </c>
       <c r="AP31" s="7">
         <v>1</v>

</xml_diff>

<commit_message>
Change approach to making functions constant
Rather than the previous approach of not loading data and just having
one value or de-selecting the time-variant box, now functions that can
be constant can be added to a constant function generation method in
data processing for selection through the GUI.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="91">
   <si>
     <t>parameter</t>
   </si>
@@ -166,12 +166,6 @@
   </si>
   <si>
     <t>riskgroup_perc_ruralpoor</t>
-  </si>
-  <si>
-    <t>epi_prop_smearneg</t>
-  </si>
-  <si>
-    <t>epi_prop_smearpos</t>
   </si>
   <si>
     <t>program_perc_detect</t>
@@ -2381,7 +2375,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B9" s="18">
         <f>1/3</f>
@@ -2488,7 +2482,7 @@
     </row>
     <row r="20" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="34" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B20" s="35">
         <f>20/12</f>
@@ -2500,7 +2494,7 @@
     </row>
     <row r="21" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B21" s="38">
         <f>12/20</f>
@@ -2509,12 +2503,12 @@
       <c r="C21" s="38"/>
       <c r="D21" s="38"/>
       <c r="E21" s="36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="37" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B22" s="38">
         <v>0.84</v>
@@ -2522,12 +2516,12 @@
       <c r="C22" s="38"/>
       <c r="D22" s="38"/>
       <c r="E22" s="36" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="39" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B23" s="40">
         <v>1940</v>
@@ -2535,12 +2529,12 @@
       <c r="C23" s="41"/>
       <c r="D23" s="41"/>
       <c r="E23" s="42" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="39" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B24" s="40">
         <v>1950</v>
@@ -2548,12 +2542,12 @@
       <c r="C24" s="41"/>
       <c r="D24" s="41"/>
       <c r="E24" s="42" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B25" s="22">
         <v>1995</v>
@@ -2561,7 +2555,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="36" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B26" s="22">
         <v>10</v>
@@ -2569,7 +2563,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="36" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B27" s="22">
         <v>15</v>
@@ -2577,7 +2571,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="37" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B28" s="22">
         <v>0.5</v>
@@ -2585,7 +2579,7 @@
     </row>
     <row r="29" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="34" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B29" s="35">
         <v>0.13</v>
@@ -2596,7 +2590,7 @@
     </row>
     <row r="30" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B30" s="35">
         <v>0.32</v>
@@ -2607,7 +2601,7 @@
     </row>
     <row r="31" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="34" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B31" s="35">
         <v>0.05</v>
@@ -2618,7 +2612,7 @@
     </row>
     <row r="32" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="34" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B32" s="35">
         <v>0.156</v>
@@ -2657,13 +2651,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BQ31"/>
+  <dimension ref="A1:BQ29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C31" sqref="C31"/>
+      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2883,28 +2877,28 @@
         <v>42</v>
       </c>
       <c r="BJ1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="BK1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="BL1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BK1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="BL1" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="BM1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BN1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="BO1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="BP1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="BQ1" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="BO1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="BP1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="BQ1" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3047,7 +3041,7 @@
     </row>
     <row r="8" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A8" s="44" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>4</v>
@@ -3065,7 +3059,7 @@
     </row>
     <row r="9" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A9" s="44" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>4</v>
@@ -3104,7 +3098,7 @@
     </row>
     <row r="11" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A11" s="44" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>4</v>
@@ -3125,7 +3119,7 @@
     </row>
     <row r="12" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A12" s="44" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>4</v>
@@ -3147,7 +3141,7 @@
     </row>
     <row r="13" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A13" s="44" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>4</v>
@@ -3166,7 +3160,7 @@
     </row>
     <row r="14" spans="1:69" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="45" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B14" s="27" t="s">
         <v>4</v>
@@ -3230,7 +3224,7 @@
     </row>
     <row r="15" spans="1:69" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="45" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B15" s="27" t="s">
         <v>4</v>
@@ -3265,7 +3259,7 @@
     </row>
     <row r="16" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A16" s="44" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>4</v>
@@ -3286,7 +3280,7 @@
     </row>
     <row r="17" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A17" s="44" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>4</v>
@@ -3308,7 +3302,7 @@
     </row>
     <row r="18" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A18" s="44" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>4</v>
@@ -3330,7 +3324,7 @@
     </row>
     <row r="19" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A19" s="44" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>4</v>
@@ -3356,7 +3350,7 @@
     </row>
     <row r="20" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A20" s="44" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>4</v>
@@ -3542,7 +3536,7 @@
     </row>
     <row r="22" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A22" s="44" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>3</v>
@@ -3639,86 +3633,62 @@
         <v>49</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="AF27" s="7">
+        <v>67</v>
+      </c>
+      <c r="BO27" s="12"/>
+    </row>
+    <row r="28" spans="1:69" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="30"/>
+      <c r="D28" s="31">
+        <v>1</v>
+      </c>
+      <c r="J28" s="32">
+        <v>1</v>
+      </c>
+      <c r="T28" s="32">
+        <v>1</v>
+      </c>
+      <c r="U28" s="32">
+        <v>3.11</v>
+      </c>
+      <c r="AZ28" s="32">
+        <v>3.11</v>
+      </c>
+      <c r="BE28" s="33"/>
+      <c r="BF28" s="33"/>
+      <c r="BG28" s="33"/>
+      <c r="BH28" s="33"/>
+      <c r="BI28" s="33"/>
+      <c r="BJ28" s="33"/>
+      <c r="BK28" s="33"/>
+      <c r="BL28" s="33"/>
+      <c r="BM28" s="33"/>
+      <c r="BN28" s="33"/>
+      <c r="BO28" s="33"/>
+    </row>
+    <row r="29" spans="1:69" x14ac:dyDescent="0.3">
+      <c r="A29" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="BA27" s="7">
-        <v>0.4</v>
-      </c>
-      <c r="BO27" s="12"/>
-    </row>
-    <row r="28" spans="1:69" x14ac:dyDescent="0.3">
-      <c r="A28" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="BA28" s="7">
-        <v>0.4</v>
-      </c>
-      <c r="BO28" s="12"/>
-    </row>
-    <row r="29" spans="1:69" x14ac:dyDescent="0.3">
-      <c r="A29" s="44" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="AF29" s="7">
-        <v>67</v>
-      </c>
-      <c r="BO29" s="12"/>
-    </row>
-    <row r="30" spans="1:69" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="46" t="s">
-        <v>71</v>
-      </c>
-      <c r="B30" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="30"/>
-      <c r="D30" s="31">
+      <c r="AP29" s="7">
         <v>1</v>
       </c>
-      <c r="J30" s="32">
-        <v>1</v>
-      </c>
-      <c r="T30" s="32">
-        <v>1</v>
-      </c>
-      <c r="U30" s="32">
-        <v>3.11</v>
-      </c>
-      <c r="AZ30" s="32">
-        <v>3.11</v>
-      </c>
-      <c r="BE30" s="33"/>
-      <c r="BF30" s="33"/>
-      <c r="BG30" s="33"/>
-      <c r="BH30" s="33"/>
-      <c r="BI30" s="33"/>
-      <c r="BJ30" s="33"/>
-      <c r="BK30" s="33"/>
-      <c r="BL30" s="33"/>
-      <c r="BM30" s="33"/>
-      <c r="BN30" s="33"/>
-      <c r="BO30" s="33"/>
-    </row>
-    <row r="31" spans="1:69" x14ac:dyDescent="0.3">
-      <c r="A31" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="AP31" s="7">
-        <v>1</v>
-      </c>
-      <c r="AQ31" s="7">
+      <c r="AQ29" s="7">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Major change to intervention structures complete
Will explain in more detail through Slack - quite major structural
changes.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="82">
   <si>
     <t>parameter</t>
   </si>
@@ -87,12 +87,6 @@
     <t>econ_cpi</t>
   </si>
   <si>
-    <t>program_perc_vaccination</t>
-  </si>
-  <si>
-    <t>program_perc_xpert</t>
-  </si>
-  <si>
     <t>program_perc_treatment_success</t>
   </si>
   <si>
@@ -105,9 +99,6 @@
     <t>program_prop_child_reporting</t>
   </si>
   <si>
-    <t>program_perc_shortcourse_mdr</t>
-  </si>
-  <si>
     <t>econ_unitcost_ipt</t>
   </si>
   <si>
@@ -138,9 +129,6 @@
     <t>econ_unitcost_xpert</t>
   </si>
   <si>
-    <t>program_perc_xpertacf_prison</t>
-  </si>
-  <si>
     <t>age_breakpoints</t>
   </si>
   <si>
@@ -150,9 +138,6 @@
     <t>scenario_8</t>
   </si>
   <si>
-    <t>program_perc_xpertacf_ruralpoor</t>
-  </si>
-  <si>
     <t>program_number_tests_per_tb_presentation</t>
   </si>
   <si>
@@ -174,39 +159,9 @@
     <t>program_prop_acf_detections_per_round</t>
   </si>
   <si>
-    <t>program_perc_awareness_raising</t>
-  </si>
-  <si>
     <t>scenario_9</t>
   </si>
   <si>
-    <t>program_perc_cxrxpertacf_ruralpoor</t>
-  </si>
-  <si>
-    <t>program_perc_cxrxpertacf_prison</t>
-  </si>
-  <si>
-    <t>program_perc_ipt_age0to5</t>
-  </si>
-  <si>
-    <t>program_perc_ipt_age5to15</t>
-  </si>
-  <si>
-    <t>program_perc_improve_dst</t>
-  </si>
-  <si>
-    <t>program_perc_firstline_dst</t>
-  </si>
-  <si>
-    <t>program_perc_secondline_dst</t>
-  </si>
-  <si>
-    <t>program_perc_food_voucher_ds</t>
-  </si>
-  <si>
-    <t>program_perc_food_voucher_mdr</t>
-  </si>
-  <si>
     <t>epi_rr_diabetes</t>
   </si>
   <si>
@@ -264,10 +219,52 @@
     <t>program_prop_ipt_from_ngo</t>
   </si>
   <si>
-    <t>program_perc_ngo_activities</t>
-  </si>
-  <si>
-    <t>program_perc_opendoors_activities</t>
+    <t>int_perc_vaccination</t>
+  </si>
+  <si>
+    <t>int_perc_xpert</t>
+  </si>
+  <si>
+    <t>int_perc_xpertacf_prison</t>
+  </si>
+  <si>
+    <t>int_perc_xpertacf_ruralpoor</t>
+  </si>
+  <si>
+    <t>int_perc_cxrxpertacf_prison</t>
+  </si>
+  <si>
+    <t>int_perc_cxrxpertacf_ruralpoor</t>
+  </si>
+  <si>
+    <t>int_perc_shortcourse_mdr</t>
+  </si>
+  <si>
+    <t>int_perc_ipt_age0to5</t>
+  </si>
+  <si>
+    <t>int_perc_ipt_age5to15</t>
+  </si>
+  <si>
+    <t>int_perc_awareness_raising</t>
+  </si>
+  <si>
+    <t>int_perc_firstline_dst</t>
+  </si>
+  <si>
+    <t>int_perc_improve_dst</t>
+  </si>
+  <si>
+    <t>int_perc_food_voucher_ds</t>
+  </si>
+  <si>
+    <t>int_perc_food_voucher_mdr</t>
+  </si>
+  <si>
+    <t>int_perc_ngo_activities</t>
+  </si>
+  <si>
+    <t>int_perc_opendoors_activities</t>
   </si>
 </sst>
 </file>
@@ -2277,7 +2274,7 @@
     </row>
     <row r="4" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="18">
         <v>1</v>
@@ -2287,7 +2284,7 @@
     </row>
     <row r="5" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B5" s="18">
         <v>5</v>
@@ -2310,7 +2307,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7" s="22">
         <v>2.7</v>
@@ -2318,7 +2315,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B8" s="18">
         <v>1.5</v>
@@ -2326,7 +2323,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B9" s="18">
         <f>1/3</f>
@@ -2335,7 +2332,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="24" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B10" s="24">
         <v>26.22</v>
@@ -2346,7 +2343,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B11" s="24">
         <v>0</v>
@@ -2357,7 +2354,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B12" s="24">
         <v>265450</v>
@@ -2368,7 +2365,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B13" s="24">
         <v>3</v>
@@ -2379,7 +2376,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B14" s="24">
         <v>1</v>
@@ -2390,7 +2387,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B15" s="24">
         <v>26.24</v>
@@ -2401,7 +2398,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B16" s="13">
         <v>0</v>
@@ -2409,7 +2406,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B17" s="25">
         <v>11575186.195826644</v>
@@ -2417,7 +2414,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="24" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B18" s="13">
         <v>3</v>
@@ -2425,7 +2422,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B19" s="13">
         <v>1</v>
@@ -2433,7 +2430,7 @@
     </row>
     <row r="20" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B20" s="28">
         <f>20/12</f>
@@ -2445,7 +2442,7 @@
     </row>
     <row r="21" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="30" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B21" s="31">
         <f>12/20</f>
@@ -2454,12 +2451,12 @@
       <c r="C21" s="31"/>
       <c r="D21" s="31"/>
       <c r="E21" s="29" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="30" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B22" s="31">
         <v>0.84</v>
@@ -2467,12 +2464,12 @@
       <c r="C22" s="31"/>
       <c r="D22" s="31"/>
       <c r="E22" s="29" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="32" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B23" s="33">
         <v>1940</v>
@@ -2480,12 +2477,12 @@
       <c r="C23" s="34"/>
       <c r="D23" s="34"/>
       <c r="E23" s="35" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="32" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B24" s="33">
         <v>1950</v>
@@ -2493,12 +2490,12 @@
       <c r="C24" s="34"/>
       <c r="D24" s="34"/>
       <c r="E24" s="35" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="35" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B25" s="22">
         <v>1995</v>
@@ -2506,7 +2503,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="29" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="B26" s="22">
         <v>10</v>
@@ -2514,7 +2511,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="29" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B27" s="22">
         <v>15</v>
@@ -2522,7 +2519,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="30" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B28" s="22">
         <v>0.5</v>
@@ -2530,7 +2527,7 @@
     </row>
     <row r="29" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="27" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B29" s="28">
         <v>0.13</v>
@@ -2541,7 +2538,7 @@
     </row>
     <row r="30" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="27" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="B30" s="28">
         <v>0.32</v>
@@ -2550,9 +2547,9 @@
       <c r="D30" s="28"/>
       <c r="E30" s="29"/>
     </row>
-    <row r="31" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="B31" s="28">
         <v>0.05</v>
@@ -2561,9 +2558,9 @@
       <c r="D31" s="28"/>
       <c r="E31" s="29"/>
     </row>
-    <row r="32" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="B32" s="28">
         <v>0.156</v>
@@ -2602,13 +2599,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AC28"/>
+  <dimension ref="A1:AC27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W16" sqref="W16"/>
+      <selection pane="bottomRight" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2715,18 +2712,18 @@
         <v>16</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>3</v>
@@ -2740,7 +2737,7 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="37" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>3</v>
@@ -2761,7 +2758,7 @@
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>3</v>
@@ -2780,7 +2777,7 @@
     </row>
     <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>4</v>
@@ -2795,7 +2792,7 @@
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>4</v>
@@ -2809,7 +2806,7 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>4</v>
@@ -2823,7 +2820,7 @@
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>4</v>
@@ -2839,7 +2836,7 @@
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>4</v>
@@ -2855,7 +2852,7 @@
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>4</v>
@@ -2871,7 +2868,7 @@
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>4</v>
@@ -2888,7 +2885,7 @@
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="37" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>4</v>
@@ -2906,7 +2903,7 @@
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="37" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>4</v>
@@ -2922,7 +2919,7 @@
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>4</v>
@@ -2968,33 +2965,36 @@
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="37" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
       <c r="T15" s="7">
+        <v>0</v>
+      </c>
+      <c r="V15" s="12">
         <v>100</v>
       </c>
+      <c r="W15" s="12"/>
+      <c r="X15" s="12"/>
+      <c r="Z15" s="12"/>
+      <c r="AA15" s="12"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="T16" s="7">
-        <v>0</v>
-      </c>
-      <c r="V16" s="12">
+      <c r="O16" s="7">
+        <v>50</v>
+      </c>
+      <c r="U16" s="7">
         <v>100</v>
       </c>
+      <c r="V16" s="12"/>
       <c r="W16" s="12"/>
       <c r="X16" s="12"/>
       <c r="Z16" s="12"/>
@@ -3002,13 +3002,13 @@
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>4</v>
       </c>
       <c r="O17" s="7">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="U17" s="7">
         <v>100</v>
@@ -3021,21 +3021,25 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="37" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="O18" s="7">
+      <c r="D18" s="6">
         <v>100</v>
       </c>
-      <c r="U18" s="7">
+      <c r="T18" s="7">
         <v>100</v>
       </c>
       <c r="V18" s="12"/>
       <c r="W18" s="12"/>
-      <c r="X18" s="12"/>
-      <c r="Z18" s="12"/>
+      <c r="X18" s="12">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="12">
+        <v>0</v>
+      </c>
       <c r="AA18" s="12"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
@@ -3053,7 +3057,8 @@
       </c>
       <c r="V19" s="12"/>
       <c r="W19" s="12"/>
-      <c r="X19" s="12">
+      <c r="X19" s="12"/>
+      <c r="Y19" s="7">
         <v>0</v>
       </c>
       <c r="Z19" s="12">
@@ -3063,90 +3068,77 @@
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="37" t="s">
-        <v>82</v>
+        <v>21</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="6">
+        <v>1</v>
+      </c>
+      <c r="E20" s="13">
+        <v>1</v>
+      </c>
+      <c r="F20" s="13">
+        <v>2.4974653103104298</v>
+      </c>
+      <c r="G20" s="13">
+        <v>9.3018160392078606</v>
+      </c>
+      <c r="H20" s="13">
+        <v>10.2347283365258</v>
+      </c>
+      <c r="I20" s="13">
+        <v>25.481798063623799</v>
+      </c>
+      <c r="J20" s="13">
+        <v>28.584806362378998</v>
+      </c>
+      <c r="K20" s="13">
+        <v>37.0398409405256</v>
+      </c>
+      <c r="L20" s="13">
+        <v>43.633070539419101</v>
+      </c>
+      <c r="M20" s="13">
+        <v>63.651452282157699</v>
+      </c>
+      <c r="N20" s="13">
+        <v>82.987551867219906</v>
+      </c>
+      <c r="O20" s="13">
         <v>100</v>
       </c>
-      <c r="T20" s="7">
-        <v>100</v>
-      </c>
-      <c r="V20" s="12"/>
-      <c r="W20" s="12"/>
-      <c r="X20" s="12"/>
-      <c r="Y20" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="12">
-        <v>0</v>
-      </c>
-      <c r="AA20" s="12"/>
+      <c r="P20" s="13">
+        <v>104.647302904564</v>
+      </c>
+      <c r="Q20" s="13">
+        <v>107.966804979253</v>
+      </c>
+      <c r="R20" s="13">
+        <v>111.203319502075</v>
+      </c>
+      <c r="S20" s="13">
+        <v>115.767634854772</v>
+      </c>
+      <c r="T20" s="13">
+        <v>117.42738589211601</v>
+      </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="37" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="6">
+        <v>3</v>
+      </c>
+      <c r="I21" s="7">
         <v>1</v>
-      </c>
-      <c r="E21" s="13">
-        <v>1</v>
-      </c>
-      <c r="F21" s="13">
-        <v>2.4974653103104298</v>
-      </c>
-      <c r="G21" s="13">
-        <v>9.3018160392078606</v>
-      </c>
-      <c r="H21" s="13">
-        <v>10.2347283365258</v>
-      </c>
-      <c r="I21" s="13">
-        <v>25.481798063623799</v>
-      </c>
-      <c r="J21" s="13">
-        <v>28.584806362378998</v>
-      </c>
-      <c r="K21" s="13">
-        <v>37.0398409405256</v>
-      </c>
-      <c r="L21" s="13">
-        <v>43.633070539419101</v>
-      </c>
-      <c r="M21" s="13">
-        <v>63.651452282157699</v>
-      </c>
-      <c r="N21" s="13">
-        <v>82.987551867219906</v>
-      </c>
-      <c r="O21" s="13">
-        <v>100</v>
-      </c>
-      <c r="P21" s="13">
-        <v>104.647302904564</v>
-      </c>
-      <c r="Q21" s="13">
-        <v>107.966804979253</v>
-      </c>
-      <c r="R21" s="13">
-        <v>111.203319502075</v>
-      </c>
-      <c r="S21" s="13">
-        <v>115.767634854772</v>
-      </c>
-      <c r="T21" s="13">
-        <v>117.42738589211601</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="37" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>3</v>
@@ -3154,136 +3146,125 @@
       <c r="I22" s="7">
         <v>1</v>
       </c>
+      <c r="N22" s="7">
+        <v>5.4</v>
+      </c>
+      <c r="Q22" s="7">
+        <v>6</v>
+      </c>
+      <c r="R22" s="7">
+        <v>7.63</v>
+      </c>
+      <c r="T22" s="7">
+        <v>8.4</v>
+      </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="37" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I23" s="7">
-        <v>1</v>
-      </c>
-      <c r="N23" s="7">
-        <v>5.4</v>
-      </c>
-      <c r="Q23" s="7">
-        <v>6</v>
-      </c>
-      <c r="R23" s="7">
-        <v>7.63</v>
+        <v>4</v>
+      </c>
+      <c r="M23" s="7">
+        <v>0.1</v>
       </c>
       <c r="T23" s="7">
-        <v>8.4</v>
+        <f>100*9028/7265000</f>
+        <v>0.12426703372333103</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="37" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M24" s="7">
-        <v>0.1</v>
-      </c>
       <c r="T24" s="7">
-        <f>100*9028/7265000</f>
-        <v>0.12426703372333103</v>
+        <f>4.5/98 * 100</f>
+        <v>4.591836734693878</v>
+      </c>
+      <c r="AA24" s="12">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AB24" s="7">
+        <f>T24/2</f>
+        <v>2.295918367346939</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="37" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="E25" s="7">
+        <v>2</v>
+      </c>
       <c r="T25" s="7">
-        <f>4.5/98 * 100</f>
-        <v>4.591836734693878</v>
+        <v>4.5</v>
       </c>
       <c r="AA25" s="12">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="AB25" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="AC25" s="7">
         <f>T25/2</f>
-        <v>2.295918367346939</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="7">
-        <v>2</v>
-      </c>
-      <c r="T26" s="7">
-        <v>4.5</v>
-      </c>
-      <c r="AA26" s="12">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="AC26" s="7">
-        <f>T26/2</f>
-        <v>2.25</v>
+        <v>3</v>
+      </c>
+      <c r="C26" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="L26" s="7">
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="L27" s="7">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A28" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D28" s="6">
+      <c r="D27" s="6">
         <v>1</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F27" s="7">
         <v>1</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G27" s="7">
         <v>1</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H27" s="7">
         <v>3.11</v>
       </c>
-      <c r="S28" s="7">
+      <c r="S27" s="7">
         <v>3.11</v>
       </c>
-      <c r="V28" s="12"/>
-      <c r="W28" s="12"/>
-      <c r="X28" s="12"/>
-      <c r="Y28" s="12"/>
-      <c r="Z28" s="12"/>
-      <c r="AA28" s="12"/>
+      <c r="V27" s="12"/>
+      <c r="W27" s="12"/>
+      <c r="X27" s="12"/>
+      <c r="Y27" s="12"/>
+      <c r="Z27" s="12"/>
+      <c r="AA27" s="12"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" xWindow="382" yWindow="552" count="4">
+  <dataValidations xWindow="382" yWindow="552" count="4">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V5 U5">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:H15 E2:T5 U3:U4">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:H14 E2:T5 U3:U4">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -3296,7 +3277,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" xWindow="382" yWindow="552" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="382" yWindow="552" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
@@ -3307,7 +3288,7 @@
           <x14:formula1>
             <xm:f>[1]dropdown_lists!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>B14:B15</xm:sqref>
+          <xm:sqref>B14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Remove uses of the obselete get_constant_or_variable_param method
Also see Slack post for more detail.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -383,7 +383,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -399,24 +399,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB9DAED"/>
         <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1179,7 +1161,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1217,28 +1199,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="12" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="665">
     <cellStyle name="Comma" xfId="664" builtinId="3"/>
@@ -2229,8 +2208,8 @@
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2428,73 +2407,73 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="27" t="s">
+    <row r="20" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="28">
+      <c r="B20" s="31">
         <f>20/12</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="29"/>
-    </row>
-    <row r="21" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="30" t="s">
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="32"/>
+    </row>
+    <row r="21" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="31">
+      <c r="B21" s="34">
         <f>12/20</f>
         <v>0.6</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="29" t="s">
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="32" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="30" t="s">
+    <row r="22" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="31">
+      <c r="B22" s="34">
         <v>0.84</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="29" t="s">
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="32" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="33">
+      <c r="B23" s="36">
         <v>1940</v>
       </c>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="35" t="s">
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="37" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="33">
+      <c r="B24" s="36">
         <v>1950</v>
       </c>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="35" t="s">
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="37" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="37" t="s">
         <v>57</v>
       </c>
       <c r="B25" s="22">
@@ -2502,7 +2481,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="32" t="s">
         <v>58</v>
       </c>
       <c r="B26" s="22">
@@ -2510,7 +2489,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="32" t="s">
         <v>59</v>
       </c>
       <c r="B27" s="22">
@@ -2518,56 +2497,56 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="30" t="s">
+      <c r="A28" s="33" t="s">
         <v>60</v>
       </c>
       <c r="B28" s="22">
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="27" t="s">
+    <row r="29" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="28">
+      <c r="B29" s="31">
         <v>0.13</v>
       </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="29"/>
-    </row>
-    <row r="30" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="27" t="s">
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="32"/>
+    </row>
+    <row r="30" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="28">
+      <c r="B30" s="31">
         <v>0.32</v>
       </c>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="29"/>
-    </row>
-    <row r="31" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="27" t="s">
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="32"/>
+    </row>
+    <row r="31" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="B31" s="28">
+      <c r="B31" s="31">
         <v>0.05</v>
       </c>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="29"/>
-    </row>
-    <row r="32" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="27" t="s">
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="32"/>
+    </row>
+    <row r="32" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="28">
+      <c r="B32" s="31">
         <v>0.156</v>
       </c>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="29"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="32"/>
     </row>
   </sheetData>
   <dataValidations count="5">
@@ -2601,7 +2580,7 @@
   </sheetPr>
   <dimension ref="A1:AC27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2633,7 +2612,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="27" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="10" t="s">
@@ -2722,7 +2701,7 @@
       </c>
     </row>
     <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="28" t="s">
         <v>66</v>
       </c>
       <c r="B2" s="11" t="s">
@@ -2736,7 +2715,7 @@
       <c r="AA2" s="26"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="28" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -2757,7 +2736,7 @@
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="28" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -2776,7 +2755,7 @@
       <c r="T4" s="9"/>
     </row>
     <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="28" t="s">
         <v>67</v>
       </c>
       <c r="B5" s="11" t="s">
@@ -2791,7 +2770,7 @@
       <c r="V5" s="26"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="28" t="s">
         <v>68</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -2805,7 +2784,7 @@
       <c r="X6" s="12"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="28" t="s">
         <v>69</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -2819,7 +2798,7 @@
       <c r="X7" s="12"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="28" t="s">
         <v>70</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -2835,7 +2814,7 @@
       <c r="Z8" s="12"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="28" t="s">
         <v>71</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -2851,7 +2830,7 @@
       <c r="Z9" s="12"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="28" t="s">
         <v>72</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -2867,7 +2846,7 @@
       <c r="X10" s="12"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="28" t="s">
         <v>73</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -2884,7 +2863,7 @@
       <c r="X11" s="12"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="28" t="s">
         <v>74</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -2902,7 +2881,7 @@
       <c r="Y12" s="12"/>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="28" t="s">
         <v>75</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -2918,7 +2897,7 @@
       <c r="AA13" s="12"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="28" t="s">
         <v>76</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -2927,11 +2906,11 @@
       <c r="C14" s="5">
         <v>0.5</v>
       </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
       <c r="I14" s="7">
         <v>0</v>
       </c>
@@ -2964,7 +2943,7 @@
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="28" t="s">
         <v>77</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -2982,7 +2961,7 @@
       <c r="AA15" s="12"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="28" t="s">
         <v>78</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -3001,7 +2980,7 @@
       <c r="AA16" s="12"/>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="28" t="s">
         <v>79</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -3020,7 +2999,7 @@
       <c r="AA17" s="12"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="28" t="s">
         <v>80</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -3043,7 +3022,7 @@
       <c r="AA18" s="12"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="28" t="s">
         <v>81</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -3067,7 +3046,7 @@
       <c r="AA19" s="12"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="28" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -3126,7 +3105,7 @@
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="28" t="s">
         <v>61</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -3137,7 +3116,7 @@
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="28" t="s">
         <v>40</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -3160,7 +3139,7 @@
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A23" s="37" t="s">
+      <c r="A23" s="28" t="s">
         <v>41</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -3175,7 +3154,7 @@
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="28" t="s">
         <v>42</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -3194,7 +3173,7 @@
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A25" s="37" t="s">
+      <c r="A25" s="28" t="s">
         <v>43</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -3215,7 +3194,7 @@
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A26" s="37" t="s">
+      <c r="A26" s="28" t="s">
         <v>44</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -3229,7 +3208,7 @@
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="28" t="s">
         <v>47</v>
       </c>
       <c r="B27" s="5" t="s">

</xml_diff>

<commit_message>
Update impact of NGO and Open Doors programs
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdoan\Github\AuTuMN\autumn\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807"/>
   </bookViews>
@@ -14,7 +19,7 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1959,7 +1964,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1994,7 +1999,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2208,8 +2213,8 @@
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2509,7 +2514,7 @@
         <v>62</v>
       </c>
       <c r="B29" s="31">
-        <v>0.13</v>
+        <v>0.25</v>
       </c>
       <c r="C29" s="31"/>
       <c r="D29" s="31"/>
@@ -2520,7 +2525,7 @@
         <v>65</v>
       </c>
       <c r="B30" s="31">
-        <v>0.32</v>
+        <v>0.38</v>
       </c>
       <c r="C30" s="31"/>
       <c r="D30" s="31"/>
@@ -2542,7 +2547,7 @@
         <v>64</v>
       </c>
       <c r="B32" s="31">
-        <v>0.156</v>
+        <v>0.04</v>
       </c>
       <c r="C32" s="31"/>
       <c r="D32" s="31"/>

</xml_diff>

<commit_message>
Revised Bulgaria data inputs
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="83">
   <si>
     <t>parameter</t>
   </si>
@@ -104,36 +104,6 @@
     <t>program_prop_child_reporting</t>
   </si>
   <si>
-    <t>econ_unitcost_ipt</t>
-  </si>
-  <si>
-    <t>econ_inflectioncost_ipt</t>
-  </si>
-  <si>
-    <t>econ_startupcost_ipt</t>
-  </si>
-  <si>
-    <t>econ_startupduration_ipt</t>
-  </si>
-  <si>
-    <t>econ_saturation_ipt</t>
-  </si>
-  <si>
-    <t>econ_inflectioncost_xpert</t>
-  </si>
-  <si>
-    <t>econ_startupcost_xpert</t>
-  </si>
-  <si>
-    <t>econ_startupduration_xpert</t>
-  </si>
-  <si>
-    <t>econ_saturation_xpert</t>
-  </si>
-  <si>
-    <t>econ_unitcost_xpert</t>
-  </si>
-  <si>
     <t>age_breakpoints</t>
   </si>
   <si>
@@ -161,9 +131,6 @@
     <t>program_perc_detect</t>
   </si>
   <si>
-    <t>program_prop_acf_detections_per_round</t>
-  </si>
-  <si>
     <t>scenario_9</t>
   </si>
   <si>
@@ -270,6 +237,42 @@
   </si>
   <si>
     <t>int_perc_opendoors_activities</t>
+  </si>
+  <si>
+    <t>econ_unitcost_food_voucher_ds</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_food_voucher_ds</t>
+  </si>
+  <si>
+    <t>econ_startupcost_food_voucher_ds</t>
+  </si>
+  <si>
+    <t>econ_startupduration_food_voucher_ds</t>
+  </si>
+  <si>
+    <t>econ_saturation_food_voucher_ds</t>
+  </si>
+  <si>
+    <t>econ_unitcost_food_voucher_mdr</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_food_voucher_mdr</t>
+  </si>
+  <si>
+    <t>econ_startupcost_food_voucher_mdr</t>
+  </si>
+  <si>
+    <t>econ_startupduration_food_voucher_mdr</t>
+  </si>
+  <si>
+    <t>econ_saturation_food_voucher_mdr</t>
+  </si>
+  <si>
+    <t>int_prop_food_voucher_improvement</t>
+  </si>
+  <si>
+    <t>Proportional reduction in adverse outcomes from the food voucher intervention</t>
   </si>
 </sst>
 </file>
@@ -388,7 +391,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -404,6 +407,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB9DAED"/>
         <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1166,7 +1187,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1196,11 +1217,7 @@
     <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="664" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="664" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1223,6 +1240,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="665">
     <cellStyle name="Comma" xfId="664" builtinId="3"/>
@@ -2213,8 +2234,8 @@
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2241,7 +2262,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="15">
-        <v>7.8</v>
+        <v>6.8</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
@@ -2268,7 +2289,7 @@
     </row>
     <row r="5" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B5" s="18">
         <v>5</v>
@@ -2293,265 +2314,252 @@
       <c r="A7" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="22">
-        <v>2.7</v>
+      <c r="B7" s="37">
+        <v>2.4</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B8" s="18">
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="18">
-        <f>1/3</f>
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="24">
-        <v>26.22</v>
-      </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="24"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="24">
-        <v>0</v>
-      </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="24">
-        <v>265450</v>
-      </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="24">
-        <v>3</v>
-      </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="24">
-        <v>1</v>
-      </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="24">
-        <v>26.24</v>
-      </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="25">
-        <v>11575186.195826644</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="31">
+    <row r="9" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="29">
         <f>20/12</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="32"/>
-    </row>
-    <row r="21" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="33" t="s">
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="30"/>
+    </row>
+    <row r="10" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="36">
+        <v>0.4</v>
+      </c>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="32">
+        <v>0.86</v>
+      </c>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="34">
+        <v>1940</v>
+      </c>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="34">
+        <v>1950</v>
+      </c>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="22">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="37">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="37">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="34">
-        <f>12/20</f>
-        <v>0.6</v>
-      </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="32" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="33" t="s">
+      <c r="B17" s="22">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="34">
-        <v>0.84</v>
-      </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="32" t="s">
+      <c r="B18" s="29">
+        <v>0.25</v>
+      </c>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="30"/>
+    </row>
+    <row r="19" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="29">
+        <v>0.38</v>
+      </c>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="30"/>
+    </row>
+    <row r="20" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="35" t="s">
+      <c r="B20" s="29">
+        <v>0.05</v>
+      </c>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="30"/>
+    </row>
+    <row r="21" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="36">
-        <v>1940</v>
-      </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="37" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="36">
-        <v>1950</v>
-      </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="37" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="37" t="s">
-        <v>57</v>
+      <c r="B21" s="29">
+        <v>0.04</v>
+      </c>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="30"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="22">
+        <f>8.19*4*10*0.85</f>
+        <v>278.45999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="38" t="s">
+        <v>73</v>
       </c>
       <c r="B25" s="22">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="32" t="s">
-        <v>58</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="38" t="s">
+        <v>74</v>
       </c>
       <c r="B26" s="22">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="32" t="s">
-        <v>59</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="38" t="s">
+        <v>75</v>
       </c>
       <c r="B27" s="22">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="33" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="23" t="s">
+        <v>76</v>
       </c>
       <c r="B28" s="22">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" s="31">
-        <v>0.25</v>
-      </c>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="32"/>
-    </row>
-    <row r="30" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="B30" s="31">
-        <v>0.38</v>
-      </c>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="32"/>
-    </row>
-    <row r="31" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" s="31">
-        <v>0.05</v>
-      </c>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="32"/>
-    </row>
-    <row r="32" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="B32" s="31">
-        <v>0.04</v>
-      </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="32"/>
+        <f>20*4*10*0.65</f>
+        <v>520</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="22">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="5">
@@ -2568,7 +2576,7 @@
       <formula2>1</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age unstratified" prompt="Some values you can replace the ones to the left with if you want a manual calibration for the model without age stratification." sqref="H1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:D24">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12:D13">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
@@ -2589,7 +2597,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2617,7 +2625,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="25" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="10" t="s">
@@ -2696,18 +2704,18 @@
         <v>16</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
-        <v>66</v>
+      <c r="A2" s="26" t="s">
+        <v>55</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>3</v>
@@ -2716,11 +2724,11 @@
         <v>0.1</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="U2" s="26"/>
-      <c r="AA2" s="26"/>
+      <c r="U2" s="24"/>
+      <c r="AA2" s="24"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="26" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -2741,7 +2749,7 @@
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="26" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -2760,8 +2768,8 @@
       <c r="T4" s="9"/>
     </row>
     <row r="5" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
-        <v>67</v>
+      <c r="A5" s="26" t="s">
+        <v>56</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>4</v>
@@ -2771,12 +2779,12 @@
       <c r="T5" s="9">
         <v>0</v>
       </c>
-      <c r="U5" s="26"/>
-      <c r="V5" s="26"/>
+      <c r="U5" s="24"/>
+      <c r="V5" s="24"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
-        <v>68</v>
+      <c r="A6" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>4</v>
@@ -2789,8 +2797,8 @@
       <c r="X6" s="12"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
-        <v>69</v>
+      <c r="A7" s="26" t="s">
+        <v>58</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>4</v>
@@ -2803,8 +2811,8 @@
       <c r="X7" s="12"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
-        <v>70</v>
+      <c r="A8" s="26" t="s">
+        <v>59</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>4</v>
@@ -2819,8 +2827,8 @@
       <c r="Z8" s="12"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
-        <v>71</v>
+      <c r="A9" s="26" t="s">
+        <v>60</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>4</v>
@@ -2835,8 +2843,8 @@
       <c r="Z9" s="12"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
-        <v>72</v>
+      <c r="A10" s="26" t="s">
+        <v>61</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>4</v>
@@ -2851,8 +2859,8 @@
       <c r="X10" s="12"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
-        <v>73</v>
+      <c r="A11" s="26" t="s">
+        <v>62</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>4</v>
@@ -2868,8 +2876,8 @@
       <c r="X11" s="12"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
-        <v>74</v>
+      <c r="A12" s="26" t="s">
+        <v>63</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>4</v>
@@ -2886,8 +2894,8 @@
       <c r="Y12" s="12"/>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
-        <v>75</v>
+      <c r="A13" s="26" t="s">
+        <v>64</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>4</v>
@@ -2902,8 +2910,8 @@
       <c r="AA13" s="12"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
-        <v>76</v>
+      <c r="A14" s="26" t="s">
+        <v>65</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>4</v>
@@ -2911,11 +2919,11 @@
       <c r="C14" s="5">
         <v>0.5</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
       <c r="I14" s="7">
         <v>0</v>
       </c>
@@ -2948,8 +2956,8 @@
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
-        <v>77</v>
+      <c r="A15" s="26" t="s">
+        <v>66</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>4</v>
@@ -2966,16 +2974,16 @@
       <c r="AA15" s="12"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
-        <v>78</v>
+      <c r="A16" s="26" t="s">
+        <v>67</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="O16" s="7">
-        <v>50</v>
-      </c>
-      <c r="U16" s="7">
+        <v>3</v>
+      </c>
+      <c r="O16" s="39">
+        <v>15</v>
+      </c>
+      <c r="U16" s="39">
         <v>100</v>
       </c>
       <c r="V16" s="12"/>
@@ -2985,16 +2993,16 @@
       <c r="AA16" s="12"/>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
-        <v>79</v>
+      <c r="A17" s="26" t="s">
+        <v>68</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="O17" s="7">
+        <v>3</v>
+      </c>
+      <c r="O17" s="39">
         <v>100</v>
       </c>
-      <c r="U17" s="7">
+      <c r="U17" s="39">
         <v>100</v>
       </c>
       <c r="V17" s="12"/>
@@ -3004,8 +3012,8 @@
       <c r="AA17" s="12"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
-        <v>80</v>
+      <c r="A18" s="26" t="s">
+        <v>69</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>4</v>
@@ -3027,8 +3035,8 @@
       <c r="AA18" s="12"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
-        <v>81</v>
+      <c r="A19" s="26" t="s">
+        <v>70</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>4</v>
@@ -3051,7 +3059,7 @@
       <c r="AA19" s="12"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="26" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -3110,8 +3118,8 @@
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
-        <v>61</v>
+      <c r="A21" s="26" t="s">
+        <v>50</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>3</v>
@@ -3121,8 +3129,8 @@
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
-        <v>40</v>
+      <c r="A22" s="26" t="s">
+        <v>30</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>3</v>
@@ -3144,8 +3152,8 @@
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
-        <v>41</v>
+      <c r="A23" s="26" t="s">
+        <v>31</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>4</v>
@@ -3159,8 +3167,8 @@
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
-        <v>42</v>
+      <c r="A24" s="26" t="s">
+        <v>32</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>4</v>
@@ -3178,8 +3186,8 @@
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
-        <v>43</v>
+      <c r="A25" s="26" t="s">
+        <v>33</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>4</v>
@@ -3199,8 +3207,8 @@
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
-        <v>44</v>
+      <c r="A26" s="26" t="s">
+        <v>34</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>3</v>
@@ -3213,8 +3221,8 @@
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
-        <v>47</v>
+      <c r="A27" s="26" t="s">
+        <v>36</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
More revisions of econ and scenatios inputs
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -430,7 +430,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -463,6 +463,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1226,7 +1232,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1291,7 +1297,8 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="664" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="7"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="664" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="664" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="665">
     <cellStyle name="Comma" xfId="664" builtinId="3"/>
@@ -1982,8 +1989,8 @@
       <sheetName val="dropdown_lists"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
@@ -2282,8 +2289,8 @@
   </sheetPr>
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2667,7 +2674,7 @@
         <v>91</v>
       </c>
       <c r="B38" s="43">
-        <v>5742.8999999999987</v>
+        <v>5737</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2682,13 +2689,17 @@
       <c r="A40" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="B40" s="44"/>
+      <c r="B40" s="44">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="B41" s="23"/>
+      <c r="B41" s="45">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="23" t="s">

</xml_diff>

<commit_message>
Whoops, did I sync my spreadsheet changes...
Correction to last commit
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdoan\Github\AuTuMN\autumn\xls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807" activeTab="1"/>
   </bookViews>
@@ -19,7 +14,7 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -224,9 +219,6 @@
     <t>int_perc_firstline_dst</t>
   </si>
   <si>
-    <t>int_perc_improve_dst</t>
-  </si>
-  <si>
     <t>int_perc_food_voucher_ds</t>
   </si>
   <si>
@@ -327,6 +319,9 @@
   </si>
   <si>
     <t>early_time</t>
+  </si>
+  <si>
+    <t>int_perc_bulgaria_improve_dst</t>
   </si>
 </sst>
 </file>
@@ -2028,8 +2023,8 @@
       <sheetName val="dropdown_lists"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
@@ -2079,7 +2074,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2114,7 +2109,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2363,7 +2358,7 @@
     </row>
     <row r="3" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" s="46">
         <v>2</v>
@@ -2373,7 +2368,7 @@
     </row>
     <row r="4" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" s="51">
         <v>1920</v>
@@ -2383,7 +2378,7 @@
     </row>
     <row r="5" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" s="51">
         <v>1920</v>
@@ -2393,7 +2388,7 @@
     </row>
     <row r="6" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B6" s="49">
         <v>0.4</v>
@@ -2403,7 +2398,7 @@
     </row>
     <row r="7" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B7" s="49">
         <v>0.4</v>
@@ -2612,7 +2607,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B27" s="31">
         <v>0.5</v>
@@ -2620,24 +2615,24 @@
       <c r="C27" s="31"/>
       <c r="D27" s="31"/>
       <c r="E27" s="29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B28" s="41">
         <f>8.19*4*10*0.51*0.85</f>
         <v>142.0146</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B29" s="41">
         <v>0</v>
@@ -2645,7 +2640,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B30" s="41">
         <v>0</v>
@@ -2653,7 +2648,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B31" s="41">
         <v>0</v>
@@ -2661,7 +2656,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B32" s="41">
         <v>1</v>
@@ -2669,19 +2664,19 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B33" s="21">
         <f>20*4*10*0.51*0.65</f>
         <v>265.2</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B34" s="21">
         <v>0</v>
@@ -2689,7 +2684,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B35" s="21">
         <v>0</v>
@@ -2697,7 +2692,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B36" s="21">
         <v>0</v>
@@ -2705,7 +2700,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B37" s="21">
         <v>1</v>
@@ -2713,19 +2708,19 @@
     </row>
     <row r="38" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B38" s="37">
         <f>1.02+67.12</f>
         <v>68.14</v>
       </c>
       <c r="E38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="37" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B39" s="37">
         <v>0</v>
@@ -2733,18 +2728,18 @@
     </row>
     <row r="40" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="37" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B40" s="37">
         <v>8028</v>
       </c>
       <c r="E40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B41" s="37">
         <v>1</v>
@@ -2752,7 +2747,7 @@
     </row>
     <row r="42" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B42" s="37">
         <v>1</v>
@@ -2760,7 +2755,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B43" s="42">
         <v>5737</v>
@@ -2768,7 +2763,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B44" s="22">
         <v>0</v>
@@ -2776,7 +2771,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B45" s="43">
         <v>0</v>
@@ -2784,7 +2779,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B46" s="44">
         <v>0</v>
@@ -2792,7 +2787,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B47" s="22">
         <v>0.9</v>
@@ -2831,10 +2826,10 @@
   <dimension ref="A1:AG37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z15" sqref="Z15"/>
+      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3223,7 +3218,7 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>3</v>
@@ -3241,7 +3236,7 @@
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>3</v>
@@ -3263,7 +3258,7 @@
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>3</v>
@@ -3285,7 +3280,7 @@
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>3</v>
@@ -3308,7 +3303,7 @@
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Whoops - another correction to previous commit
Hadn't included economic parameters for Bulgaria improve DST.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="106">
   <si>
     <t>parameter</t>
   </si>
@@ -322,6 +322,21 @@
   </si>
   <si>
     <t>int_perc_bulgaria_improve_dst</t>
+  </si>
+  <si>
+    <t>econ_unitcost_bulgaria_improve_dst</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_bulgaria_improve_dst</t>
+  </si>
+  <si>
+    <t>econ_startupcost_bulgaria_improve_dst</t>
+  </si>
+  <si>
+    <t>econ_startupduration_bulgaria_improve_dst</t>
+  </si>
+  <si>
+    <t>econ_saturation_bulgaria_improve_dst</t>
   </si>
 </sst>
 </file>
@@ -2023,8 +2038,8 @@
       <sheetName val="dropdown_lists"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
@@ -2321,10 +2336,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2753,43 +2768,90 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="22" t="s">
+    <row r="43" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" s="37">
+        <f>1.02+67.12</f>
+        <v>68.14</v>
+      </c>
+      <c r="E43" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="B44" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" s="37">
+        <v>8028</v>
+      </c>
+      <c r="E45" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="B46" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="B47" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="B43" s="42">
+      <c r="B48" s="42">
         <v>5737</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="22" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="B44" s="22">
+      <c r="B49" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="22" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="B45" s="43">
+      <c r="B50" s="43">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="22" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="B46" s="44">
+      <c r="B51" s="44">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="22" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="B47" s="22">
+      <c r="B52" s="22">
         <v>0.9</v>
       </c>
     </row>
@@ -2825,7 +2887,7 @@
   </sheetPr>
   <dimension ref="A1:AG37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
Add code for ambulatory care costs
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="112">
   <si>
     <t>parameter</t>
   </si>
@@ -337,6 +337,24 @@
   </si>
   <si>
     <t>econ_saturation_bulgaria_improve_dst</t>
+  </si>
+  <si>
+    <t>int_perc_ambulatorycare_smearneg</t>
+  </si>
+  <si>
+    <t>econ_unitcost_ambulatorycare_smearneg</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_ambulatorycare_smearneg</t>
+  </si>
+  <si>
+    <t>econ_startupcost_ambulatorycare_smearneg</t>
+  </si>
+  <si>
+    <t>econ_startupduration_ambulatorycare_smearneg</t>
+  </si>
+  <si>
+    <t>econ_saturation_ambulatorycare_smearneg</t>
   </si>
 </sst>
 </file>
@@ -2336,10 +2354,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2855,8 +2873,48 @@
         <v>0.9</v>
       </c>
     </row>
+    <row r="53" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="B53" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="B54" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="B55" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" s="37">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations disablePrompts="1" count="5">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11 F11:G11 B3">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
@@ -2885,13 +2943,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AG37"/>
+  <dimension ref="A1:AG38"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3389,327 +3447,317 @@
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>21</v>
+        <v>106</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="6">
-        <v>1</v>
-      </c>
-      <c r="E20" s="13">
-        <v>1</v>
-      </c>
-      <c r="F20" s="13">
-        <v>2.4974653103104298</v>
-      </c>
-      <c r="G20" s="13">
-        <v>9.3018160392078606</v>
-      </c>
-      <c r="H20" s="13">
-        <v>10.2347283365258</v>
-      </c>
-      <c r="I20" s="13">
-        <v>25.481798063623799</v>
-      </c>
-      <c r="J20" s="13">
-        <v>28.584806362378998</v>
-      </c>
-      <c r="K20" s="13">
-        <v>37.0398409405256</v>
-      </c>
-      <c r="L20" s="13">
-        <v>43.633070539419101</v>
-      </c>
-      <c r="M20" s="13">
-        <v>63.651452282157699</v>
-      </c>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13">
-        <v>82.987551867219906</v>
-      </c>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="13"/>
-      <c r="S20" s="13">
-        <v>100</v>
-      </c>
-      <c r="T20" s="13">
-        <v>104.647302904564</v>
-      </c>
-      <c r="U20" s="13">
-        <v>107.966804979253</v>
-      </c>
-      <c r="V20" s="13">
-        <v>111.203319502075</v>
-      </c>
-      <c r="W20" s="13">
-        <v>115.767634854772</v>
-      </c>
-      <c r="X20" s="13">
-        <v>117.42738589211601</v>
-      </c>
+      <c r="X20" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="12"/>
+      <c r="AA20" s="12"/>
+      <c r="AB20" s="12"/>
+      <c r="AD20" s="12"/>
+      <c r="AE20" s="12"/>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I21" s="7">
+      <c r="D21" s="6">
         <v>1</v>
+      </c>
+      <c r="E21" s="13">
+        <v>1</v>
+      </c>
+      <c r="F21" s="13">
+        <v>2.4974653103104298</v>
+      </c>
+      <c r="G21" s="13">
+        <v>9.3018160392078606</v>
+      </c>
+      <c r="H21" s="13">
+        <v>10.2347283365258</v>
+      </c>
+      <c r="I21" s="13">
+        <v>25.481798063623799</v>
+      </c>
+      <c r="J21" s="13">
+        <v>28.584806362378998</v>
+      </c>
+      <c r="K21" s="13">
+        <v>37.0398409405256</v>
+      </c>
+      <c r="L21" s="13">
+        <v>43.633070539419101</v>
+      </c>
+      <c r="M21" s="13">
+        <v>63.651452282157699</v>
+      </c>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13">
+        <v>82.987551867219906</v>
+      </c>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="13">
+        <v>100</v>
+      </c>
+      <c r="T21" s="13">
+        <v>104.647302904564</v>
+      </c>
+      <c r="U21" s="13">
+        <v>107.966804979253</v>
+      </c>
+      <c r="V21" s="13">
+        <v>111.203319502075</v>
+      </c>
+      <c r="W21" s="13">
+        <v>115.767634854772</v>
+      </c>
+      <c r="X21" s="13">
+        <v>117.42738589211601</v>
       </c>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I22" s="7">
         <v>1</v>
       </c>
-      <c r="O22" s="7">
-        <v>5.4</v>
-      </c>
-      <c r="U22" s="7">
-        <v>6</v>
-      </c>
-      <c r="V22" s="7">
-        <v>7.63</v>
-      </c>
-      <c r="X22" s="7">
-        <v>8.4</v>
-      </c>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M23" s="7">
+      <c r="I23" s="7">
         <v>1</v>
       </c>
+      <c r="O23" s="7">
+        <v>5.4</v>
+      </c>
+      <c r="U23" s="7">
+        <v>6</v>
+      </c>
+      <c r="V23" s="7">
+        <v>7.63</v>
+      </c>
       <c r="X23" s="7">
-        <v>1</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M24" s="7">
+        <v>1</v>
+      </c>
+      <c r="X24" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A25" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="X24" s="7">
+      <c r="X25" s="7">
         <f>4.5/98 * 100</f>
         <v>4.591836734693878</v>
       </c>
-      <c r="AE24" s="12">
+      <c r="AE25" s="12">
         <v>2.2999999999999998</v>
       </c>
-      <c r="AF24" s="7">
-        <f>X24/2</f>
+      <c r="AF25" s="7">
+        <f>X25/2</f>
         <v>2.295918367346939</v>
-      </c>
-    </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="7">
-        <v>2</v>
-      </c>
-      <c r="M25" s="7">
-        <v>6</v>
-      </c>
-      <c r="X25" s="7">
-        <v>10</v>
-      </c>
-      <c r="AE25" s="12">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="AG25" s="7">
-        <f>X25/2</f>
-        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="6"/>
-      <c r="Q26" s="6"/>
-      <c r="R26" s="6"/>
-      <c r="S26" s="6"/>
-      <c r="T26" s="6"/>
-      <c r="U26" s="6"/>
-      <c r="V26" s="6"/>
-      <c r="W26" s="6"/>
-      <c r="X26" s="6"/>
+      <c r="E26" s="7">
+        <v>2</v>
+      </c>
+      <c r="M26" s="7">
+        <v>6</v>
+      </c>
+      <c r="X26" s="7">
+        <v>10</v>
+      </c>
+      <c r="AE26" s="12">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="AG26" s="7">
+        <f>X26/2</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="6">
+      <c r="C27" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
+      <c r="U27" s="6"/>
+      <c r="V27" s="6"/>
+      <c r="W27" s="6"/>
+      <c r="X27" s="6"/>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A28" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="6">
         <v>1</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F28" s="7">
         <v>1</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G28" s="7">
         <v>1</v>
       </c>
-      <c r="H27" s="7">
+      <c r="H28" s="7">
         <v>3.11</v>
       </c>
-      <c r="W27" s="7">
+      <c r="W28" s="7">
         <v>3.11</v>
       </c>
-      <c r="Z27" s="12"/>
-      <c r="AA27" s="12"/>
-      <c r="AB27" s="12"/>
-      <c r="AC27" s="12"/>
-      <c r="AD27" s="12"/>
-      <c r="AE27" s="12"/>
-    </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="D30" s="6">
+      <c r="Z28" s="12"/>
+      <c r="AA28" s="12"/>
+      <c r="AB28" s="12"/>
+      <c r="AC28" s="12"/>
+      <c r="AD28" s="12"/>
+      <c r="AE28" s="12"/>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="D31" s="6">
         <v>69</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E31" s="6">
         <v>69</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F31" s="6">
         <v>69</v>
       </c>
-      <c r="G30" s="6">
+      <c r="G31" s="6">
         <v>69</v>
       </c>
-      <c r="H30" s="6">
+      <c r="H31" s="6">
         <v>69</v>
       </c>
-      <c r="I30" s="6">
+      <c r="I31" s="6">
         <v>69</v>
       </c>
-      <c r="J30" s="6">
+      <c r="J31" s="6">
         <v>69</v>
       </c>
-      <c r="K30" s="6">
+      <c r="K31" s="6">
         <v>69</v>
       </c>
-      <c r="L30" s="6">
+      <c r="L31" s="6">
         <v>69</v>
       </c>
-      <c r="M30" s="6">
+      <c r="M31" s="6">
         <v>69</v>
       </c>
-      <c r="N30" s="6">
+      <c r="N31" s="6">
         <v>90</v>
       </c>
-      <c r="O30" s="6">
+      <c r="O31" s="6">
         <v>90</v>
       </c>
-      <c r="P30" s="6">
+      <c r="P31" s="6">
         <v>90</v>
       </c>
-      <c r="Q30" s="6">
+      <c r="Q31" s="6">
         <v>90</v>
       </c>
-      <c r="R30" s="6"/>
-      <c r="S30" s="6">
+      <c r="R31" s="6"/>
+      <c r="S31" s="6">
         <v>85</v>
       </c>
-      <c r="T30" s="6">
+      <c r="T31" s="6">
         <v>85</v>
       </c>
-      <c r="U30" s="6">
+      <c r="U31" s="6">
         <v>80</v>
       </c>
-      <c r="V30" s="6">
+      <c r="V31" s="6">
         <v>80</v>
       </c>
-      <c r="W30" s="6">
+      <c r="W31" s="6">
         <v>80</v>
       </c>
-      <c r="X30" s="6">
+      <c r="X31" s="6">
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="X32" s="7">
+    <row r="33" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="X33" s="7">
         <f>100*9028/7265000</f>
         <v>0.12426703372333103</v>
       </c>
     </row>
-    <row r="33" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="X33" s="7">
+    <row r="34" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="X34" s="7">
         <v>4.5</v>
-      </c>
-    </row>
-    <row r="35" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="D35" s="6">
-        <v>5</v>
-      </c>
-      <c r="K35" s="7">
-        <v>5</v>
-      </c>
-      <c r="M35" s="9">
-        <v>3</v>
-      </c>
-      <c r="N35" s="9"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
-      <c r="S35" s="9">
-        <v>3</v>
-      </c>
-      <c r="T35" s="9"/>
-      <c r="U35" s="9"/>
-      <c r="V35" s="9"/>
-      <c r="W35" s="9"/>
-      <c r="X35" s="9">
-        <v>0.5</v>
       </c>
     </row>
     <row r="36" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D36" s="6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K36" s="7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="M36" s="9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="N36" s="9"/>
       <c r="O36" s="8"/>
@@ -3717,28 +3765,31 @@
       <c r="Q36" s="8"/>
       <c r="R36" s="8"/>
       <c r="S36" s="9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="T36" s="9"/>
       <c r="U36" s="9"/>
       <c r="V36" s="9"/>
       <c r="W36" s="9"/>
       <c r="X36" s="9">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="37" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D37" s="6">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="K37" s="7">
+        <v>10</v>
       </c>
       <c r="M37" s="9">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N37" s="9"/>
       <c r="O37" s="8"/>
       <c r="P37" s="8"/>
-      <c r="Q37" s="16"/>
-      <c r="R37" s="16"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="8"/>
       <c r="S37" s="9">
         <v>6</v>
       </c>
@@ -3746,7 +3797,30 @@
       <c r="U37" s="9"/>
       <c r="V37" s="9"/>
       <c r="W37" s="9"/>
-      <c r="X37" s="9"/>
+      <c r="X37" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D38" s="6">
+        <v>14</v>
+      </c>
+      <c r="M38" s="9">
+        <v>8</v>
+      </c>
+      <c r="N38" s="9"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="16"/>
+      <c r="R38" s="16"/>
+      <c r="S38" s="9">
+        <v>6</v>
+      </c>
+      <c r="T38" s="9"/>
+      <c r="U38" s="9"/>
+      <c r="V38" s="9"/>
+      <c r="W38" s="9"/>
+      <c r="X38" s="9"/>
     </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="4">
@@ -3755,7 +3829,7 @@
       <formula2>100000000000000000000</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:H14 Y3:Y4 E35:X37 E2:X3 E5:X5">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:H14 Y3:Y4 E36:X38 E2:X3 E5:X5">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Simplify open doors strings
Were across two spreadsheets - rationalise back to defaults sheete.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="110">
   <si>
     <t>parameter</t>
   </si>
@@ -175,12 +175,6 @@
   </si>
   <si>
     <t>program_prop_detection_from_ngo</t>
-  </si>
-  <si>
-    <t>program_prop_detection_from_opendoors</t>
-  </si>
-  <si>
-    <t>program_prop_ipt_from_opendoors</t>
   </si>
   <si>
     <t>program_prop_ipt_from_ngo</t>
@@ -2354,10 +2348,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2391,7 +2385,7 @@
     </row>
     <row r="3" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="45" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B3" s="46">
         <v>2</v>
@@ -2401,7 +2395,7 @@
     </row>
     <row r="4" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B4" s="51">
         <v>1920</v>
@@ -2411,7 +2405,7 @@
     </row>
     <row r="5" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="50" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B5" s="51">
         <v>1920</v>
@@ -2421,7 +2415,7 @@
     </row>
     <row r="6" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B6" s="49">
         <v>0.4</v>
@@ -2431,7 +2425,7 @@
     </row>
     <row r="7" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B7" s="49">
         <v>0.4</v>
@@ -2607,7 +2601,7 @@
     </row>
     <row r="24" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B24" s="28">
         <v>0.38</v>
@@ -2616,39 +2610,37 @@
       <c r="D24" s="28"/>
       <c r="E24" s="29"/>
     </row>
-    <row r="25" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="28">
-        <v>0.05</v>
-      </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="29"/>
-    </row>
-    <row r="26" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="28">
-        <v>0.04</v>
-      </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="29"/>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="41">
+        <f>8.19*4*10*0.51*0.85</f>
+        <v>142.0146</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="B27" s="31">
-        <v>0.5</v>
-      </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="29" t="s">
-        <v>81</v>
+      <c r="A27" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="41">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2656,11 +2648,7 @@
         <v>70</v>
       </c>
       <c r="B28" s="41">
-        <f>8.19*4*10*0.51*0.85</f>
-        <v>142.0146</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>87</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2676,23 +2664,27 @@
         <v>72</v>
       </c>
       <c r="B30" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="21">
+        <f>20*4*10*0.51*0.65</f>
+        <v>265.2</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="21">
         <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="B31" s="41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="B32" s="41">
-        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2700,11 +2692,7 @@
         <v>75</v>
       </c>
       <c r="B33" s="21">
-        <f>20*4*10*0.51*0.65</f>
-        <v>265.2</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>87</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2720,23 +2708,27 @@
         <v>77</v>
       </c>
       <c r="B35" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="37">
+        <f>1.02+67.12</f>
+        <v>68.14</v>
+      </c>
+      <c r="E36" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" s="37">
         <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="B36" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="B37" s="21">
-        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2744,11 +2736,10 @@
         <v>82</v>
       </c>
       <c r="B38" s="37">
-        <f>1.02+67.12</f>
-        <v>68.14</v>
+        <v>8028</v>
       </c>
       <c r="E38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2756,7 +2747,7 @@
         <v>83</v>
       </c>
       <c r="B39" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2764,26 +2755,27 @@
         <v>84</v>
       </c>
       <c r="B40" s="37">
-        <v>8028</v>
-      </c>
-      <c r="E40" t="s">
-        <v>89</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="37" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B41" s="37">
-        <v>1</v>
+        <f>1.02+67.12</f>
+        <v>68.14</v>
+      </c>
+      <c r="E41" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="37" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="B42" s="37">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2791,11 +2783,10 @@
         <v>101</v>
       </c>
       <c r="B43" s="37">
-        <f>1.02+67.12</f>
-        <v>68.14</v>
+        <v>8028</v>
       </c>
       <c r="E43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2803,7 +2794,7 @@
         <v>102</v>
       </c>
       <c r="B44" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2811,41 +2802,38 @@
         <v>103</v>
       </c>
       <c r="B45" s="37">
-        <v>8028</v>
-      </c>
-      <c r="E45" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" s="42">
+        <v>5737</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="22" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="37" t="s">
-        <v>104</v>
-      </c>
-      <c r="B46" s="37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="37" t="s">
-        <v>105</v>
-      </c>
-      <c r="B47" s="37">
-        <v>1</v>
+      <c r="B47" s="22">
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="B48" s="42">
-        <v>5737</v>
+      <c r="B48" s="43">
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="B49" s="22">
+      <c r="B49" s="44">
         <v>0</v>
       </c>
     </row>
@@ -2853,24 +2841,24 @@
       <c r="A50" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="B50" s="43">
+      <c r="B50" s="22">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="B51" s="37">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="B51" s="44">
+    <row r="52" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="B52" s="37">
         <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="B52" s="22">
-        <v>0.9</v>
       </c>
     </row>
     <row r="53" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2897,24 +2885,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="37" t="s">
-        <v>110</v>
-      </c>
-      <c r="B56" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="B57" s="37">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="5">
+  <dataValidations count="5">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11 F11:G11 B3">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
@@ -2945,11 +2917,11 @@
   </sheetPr>
   <dimension ref="A1:AG38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V21" sqref="V21"/>
+      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3079,7 +3051,7 @@
     </row>
     <row r="2" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>3</v>
@@ -3150,7 +3122,7 @@
     </row>
     <row r="5" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>4</v>
@@ -3165,7 +3137,7 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>4</v>
@@ -3179,7 +3151,7 @@
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>4</v>
@@ -3193,7 +3165,7 @@
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>4</v>
@@ -3209,7 +3181,7 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>4</v>
@@ -3225,7 +3197,7 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>4</v>
@@ -3241,7 +3213,7 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>4</v>
@@ -3258,7 +3230,7 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>4</v>
@@ -3276,7 +3248,7 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>4</v>
@@ -3292,7 +3264,7 @@
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>4</v>
@@ -3338,7 +3310,7 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>3</v>
@@ -3356,7 +3328,7 @@
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>3</v>
@@ -3378,7 +3350,7 @@
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="40" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>3</v>
@@ -3400,7 +3372,7 @@
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>3</v>
@@ -3423,7 +3395,7 @@
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>4</v>
@@ -3447,7 +3419,7 @@
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Remove some unnecessary parameters from sheets
Remove unnecessary smear-positive/negative proportions from Bulgaria spreadsheet.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="108">
   <si>
     <t>parameter</t>
   </si>
@@ -301,12 +301,6 @@
   </si>
   <si>
     <t>active</t>
-  </si>
-  <si>
-    <t>epi_prop_smearpos</t>
-  </si>
-  <si>
-    <t>epi_prop_smearneg</t>
   </si>
   <si>
     <t>start_time</t>
@@ -467,7 +461,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -506,12 +500,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1281,7 +1269,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1352,14 +1340,8 @@
     <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="664" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="13" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="13" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="665">
     <cellStyle name="Comma" xfId="664" builtinId="3"/>
@@ -2348,10 +2330,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A6:XFD7"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2394,250 +2376,246 @@
       <c r="G3" s="15"/>
     </row>
     <row r="4" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="B4" s="51">
+      <c r="A4" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="49">
         <v>1920</v>
       </c>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
     <row r="5" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="50" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" s="51">
+      <c r="A5" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="49">
         <v>1920</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" s="49">
-        <v>0.4</v>
-      </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-    </row>
-    <row r="7" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="B7" s="49">
-        <v>0.4</v>
-      </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
+    <row r="6" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="18">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+    </row>
+    <row r="7" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="18">
+        <v>1</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B8" s="18">
-        <v>0.26500000000000001</v>
+        <v>5</v>
+      </c>
+      <c r="C8" s="16">
+        <v>15</v>
       </c>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="18">
-        <v>1</v>
-      </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-    </row>
-    <row r="10" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="18">
-        <v>5</v>
-      </c>
-      <c r="C10" s="16">
-        <v>15</v>
-      </c>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-    </row>
-    <row r="11" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
+      <c r="A9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="47">
+      <c r="B9" s="47">
         <v>10000000</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="36">
+      <c r="B10" s="36">
         <v>2.4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B11" s="18">
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27" t="s">
+    <row r="12" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="28">
+      <c r="B12" s="28">
         <f>20/12</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="29"/>
-    </row>
-    <row r="15" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="30" t="s">
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="29"/>
+    </row>
+    <row r="13" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="35">
+      <c r="B13" s="35">
         <v>0.4</v>
       </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="29" t="s">
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="29" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="30" t="s">
+    <row r="14" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="31">
+      <c r="B14" s="31">
         <v>0.86</v>
       </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="29" t="s">
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="29" t="s">
         <v>41</v>
       </c>
     </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="33">
+        <v>1940</v>
+      </c>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="33">
+        <v>1950</v>
+      </c>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="34" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="33">
-        <v>1940</v>
-      </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="34" t="s">
-        <v>43</v>
+      <c r="A17" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="21">
+        <v>2010</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="33">
-        <v>1950</v>
-      </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="34" t="s">
-        <v>45</v>
+      <c r="A18" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="36">
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="21">
-        <v>2010</v>
+      <c r="A19" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="36">
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="36">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="36">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="30" t="s">
+      <c r="A20" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="21">
+      <c r="B20" s="21">
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="27" t="s">
+    <row r="21" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="28">
+      <c r="B21" s="28">
         <v>0.25</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="29"/>
-    </row>
-    <row r="24" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="27" t="s">
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
+    </row>
+    <row r="22" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="28">
+      <c r="B22" s="28">
         <v>0.38</v>
       </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="29"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="29"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="41">
+        <f>8.19*4*10*0.51*0.85</f>
+        <v>142.0146</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="B25" s="31">
-        <v>0.5</v>
-      </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="29" t="s">
-        <v>79</v>
+      <c r="A25" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="41">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B26" s="41">
-        <f>8.19*4*10*0.51*0.85</f>
-        <v>142.0146</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B27" s="41">
         <v>0</v>
@@ -2645,43 +2623,43 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="37" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B28" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="21">
+        <f>20*4*10*0.51*0.65</f>
+        <v>265.2</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="21">
         <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" s="41">
-        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B31" s="21">
-        <f>20*4*10*0.51*0.65</f>
-        <v>265.2</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B32" s="21">
         <v>0</v>
@@ -2689,73 +2667,77 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B33" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="37">
+        <f>1.02+67.12</f>
+        <v>68.14</v>
+      </c>
+      <c r="E34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="37">
         <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="B34" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="B35" s="21">
-        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="37" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B36" s="37">
+        <v>8028</v>
+      </c>
+      <c r="E36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" s="37">
         <f>1.02+67.12</f>
         <v>68.14</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E39" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="B37" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="B38" s="37">
-        <v>8028</v>
-      </c>
-      <c r="E38" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="B39" s="37">
-        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="37" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="B40" s="37">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2763,11 +2745,10 @@
         <v>99</v>
       </c>
       <c r="B41" s="37">
-        <f>1.02+67.12</f>
-        <v>68.14</v>
+        <v>8028</v>
       </c>
       <c r="E41" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2775,7 +2756,7 @@
         <v>100</v>
       </c>
       <c r="B42" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2783,66 +2764,63 @@
         <v>101</v>
       </c>
       <c r="B43" s="37">
-        <v>8028</v>
-      </c>
-      <c r="E43" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="37" t="s">
-        <v>102</v>
-      </c>
-      <c r="B44" s="37">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="37" t="s">
-        <v>103</v>
-      </c>
-      <c r="B45" s="37">
-        <v>1</v>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" s="42">
+        <v>5737</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" s="22">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="B46" s="42">
-        <v>5737</v>
+        <v>90</v>
+      </c>
+      <c r="B46" s="43">
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="B47" s="22">
+        <v>91</v>
+      </c>
+      <c r="B47" s="44">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="B48" s="43">
+        <v>92</v>
+      </c>
+      <c r="B48" s="22">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="37">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="B49" s="44">
+    <row r="50" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="B50" s="37">
         <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="B50" s="22">
-        <v>0.9</v>
       </c>
     </row>
     <row r="51" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2869,38 +2847,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="37" t="s">
-        <v>108</v>
-      </c>
-      <c r="B54" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="37" t="s">
-        <v>109</v>
-      </c>
-      <c r="B55" s="37">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11 F11:G11 B3">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9 F9:G9 B3">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 F2:G7">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 F2:G5">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F8:G10 B8:B9">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:G8 B6:B7">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age unstratified" prompt="Some values you can replace the ones to the left with if you want a manual calibration for the model without age stratification." sqref="H1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17:D18 B4:B5">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15:D16 B4:B5">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
@@ -3310,7 +3272,7 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>3</v>
@@ -3419,7 +3381,7 @@
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Tidy parameters for vouchers and NGOs
Have tidied the parameters for food vouchers and for NGO activities according to the way I am implementing parameters.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="103">
   <si>
     <t>parameter</t>
   </si>
@@ -168,18 +168,9 @@
     <t>riskgroup_multiplier_force_infection_prison</t>
   </si>
   <si>
-    <t>program_prop_food_voucher_improvement</t>
-  </si>
-  <si>
     <t>riskgroup_perc_hiv</t>
   </si>
   <si>
-    <t>program_prop_detection_from_ngo</t>
-  </si>
-  <si>
-    <t>program_prop_ipt_from_ngo</t>
-  </si>
-  <si>
     <t>int_perc_vaccination</t>
   </si>
   <si>
@@ -253,12 +244,6 @@
   </si>
   <si>
     <t>econ_saturation_food_voucher_mdr</t>
-  </si>
-  <si>
-    <t>int_prop_food_voucher_improvement</t>
-  </si>
-  <si>
-    <t>Proportional reduction in adverse outcomes from the food voucher intervention</t>
   </si>
   <si>
     <t>econ_unitcost_improve_dst</t>
@@ -2330,10 +2315,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2367,7 +2352,7 @@
     </row>
     <row r="3" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="45" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B3" s="46">
         <v>2</v>
@@ -2377,7 +2362,7 @@
     </row>
     <row r="4" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B4" s="49">
         <v>1920</v>
@@ -2387,7 +2372,7 @@
     </row>
     <row r="5" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B5" s="49">
         <v>1920</v>
@@ -2534,7 +2519,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
         <v>48</v>
       </c>
@@ -2542,179 +2527,175 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="21">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="28">
-        <v>0.25</v>
-      </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="29"/>
-    </row>
-    <row r="22" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="28">
-        <v>0.38</v>
-      </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="29"/>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="41">
+        <f>8.19*4*10*0.51*0.85</f>
+        <v>142.0146</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="41">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="B23" s="31">
-        <v>0.5</v>
-      </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="29" t="s">
-        <v>79</v>
+      <c r="A23" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="41">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="37" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B24" s="41">
-        <f>8.19*4*10*0.51*0.85</f>
-        <v>142.0146</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>85</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="B25" s="41">
+      <c r="A25" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="21">
+        <f>20*4*10*0.51*0.65</f>
+        <v>265.2</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="37" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26" s="41">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B27" s="41">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="21">
         <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="B28" s="41">
-        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B29" s="21">
-        <f>20*4*10*0.51*0.65</f>
-        <v>265.2</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="B30" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="37">
+        <f>1.02+67.12</f>
+        <v>68.14</v>
+      </c>
+      <c r="E30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="37">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B31" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="B32" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="22" t="s">
+    <row r="32" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="21">
+      <c r="B32" s="37">
+        <v>8028</v>
+      </c>
+      <c r="E32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="37">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B34" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" s="37">
         <f>1.02+67.12</f>
         <v>68.14</v>
       </c>
-      <c r="E34" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="37" t="s">
+      <c r="E35" t="s">
         <v>81</v>
-      </c>
-      <c r="B35" s="37">
-        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="37" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="B36" s="37">
-        <v>8028</v>
-      </c>
-      <c r="E36" t="s">
-        <v>87</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="37" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="B37" s="37">
-        <v>1</v>
+        <v>8028</v>
+      </c>
+      <c r="E37" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="37" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="B38" s="37">
         <v>1</v>
@@ -2722,128 +2703,89 @@
     </row>
     <row r="39" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B39" s="37">
-        <f>1.02+67.12</f>
-        <v>68.14</v>
-      </c>
-      <c r="E39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" s="42">
+        <v>5737</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="22" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="37" t="s">
-        <v>98</v>
-      </c>
-      <c r="B40" s="37">
+      <c r="B43" s="44">
         <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="B41" s="37">
-        <v>8028</v>
-      </c>
-      <c r="E41" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="37" t="s">
-        <v>100</v>
-      </c>
-      <c r="B42" s="37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="B43" s="37">
-        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="B44" s="42">
-        <v>5737</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="B45" s="22">
+        <v>87</v>
+      </c>
+      <c r="B44" s="22">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="B45" s="37">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="B46" s="43">
+    <row r="46" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="B46" s="37">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="B47" s="44">
+    <row r="47" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="B47" s="37">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="B48" s="22">
-        <v>0.9</v>
+    <row r="48" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="37">
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B49" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="37" t="s">
-        <v>104</v>
-      </c>
-      <c r="B50" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="37" t="s">
-        <v>105</v>
-      </c>
-      <c r="B51" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="37" t="s">
-        <v>106</v>
-      </c>
-      <c r="B52" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="B53" s="37">
         <v>0</v>
       </c>
     </row>
@@ -3013,7 +2955,7 @@
     </row>
     <row r="2" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>3</v>
@@ -3084,7 +3026,7 @@
     </row>
     <row r="5" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>4</v>
@@ -3099,7 +3041,7 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>4</v>
@@ -3113,7 +3055,7 @@
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>4</v>
@@ -3127,7 +3069,7 @@
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>4</v>
@@ -3143,7 +3085,7 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>4</v>
@@ -3159,7 +3101,7 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>4</v>
@@ -3175,7 +3117,7 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>4</v>
@@ -3192,7 +3134,7 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>4</v>
@@ -3210,7 +3152,7 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>4</v>
@@ -3226,7 +3168,7 @@
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>4</v>
@@ -3272,7 +3214,7 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>3</v>
@@ -3290,7 +3232,7 @@
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>3</v>
@@ -3312,7 +3254,7 @@
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="40" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>3</v>
@@ -3334,7 +3276,7 @@
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>3</v>
@@ -3357,7 +3299,7 @@
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>4</v>
@@ -3381,7 +3323,7 @@
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>4</v>
@@ -3460,7 +3402,7 @@
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Update spreadsheets for NGO and opendoors activities
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rragonnet\Google Drive\GitHub\AuTuMN\autumn\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="612" windowWidth="16272" windowHeight="6300" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -2068,7 +2073,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2103,7 +2108,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2317,22 +2322,22 @@
   </sheetPr>
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.5703125" style="19" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="21" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="19"/>
-    <col min="6" max="6" width="13.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="19"/>
+    <col min="1" max="1" width="51.5546875" style="19" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="21" customWidth="1"/>
+    <col min="3" max="5" width="9.109375" style="19"/>
+    <col min="6" max="6" width="13.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2340,7 +2345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
@@ -2350,7 +2355,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="45" t="s">
         <v>88</v>
       </c>
@@ -2360,7 +2365,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="s">
         <v>89</v>
       </c>
@@ -2370,7 +2375,7 @@
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="48" t="s">
         <v>90</v>
       </c>
@@ -2380,7 +2385,7 @@
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>11</v>
       </c>
@@ -2390,7 +2395,7 @@
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
     </row>
-    <row r="7" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>25</v>
       </c>
@@ -2400,7 +2405,7 @@
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
     </row>
-    <row r="8" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>26</v>
       </c>
@@ -2413,7 +2418,7 @@
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
     </row>
-    <row r="9" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
         <v>12</v>
       </c>
@@ -2423,7 +2428,7 @@
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>24</v>
       </c>
@@ -2431,7 +2436,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>29</v>
       </c>
@@ -2439,7 +2444,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
         <v>37</v>
       </c>
@@ -2451,7 +2456,7 @@
       <c r="D12" s="28"/>
       <c r="E12" s="29"/>
     </row>
-    <row r="13" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A13" s="30" t="s">
         <v>38</v>
       </c>
@@ -2464,7 +2469,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" s="30" t="s">
         <v>40</v>
       </c>
@@ -2477,7 +2482,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
         <v>42</v>
       </c>
@@ -2490,7 +2495,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" s="32" t="s">
         <v>44</v>
       </c>
@@ -2503,7 +2508,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A17" s="34" t="s">
         <v>46</v>
       </c>
@@ -2511,7 +2516,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
         <v>47</v>
       </c>
@@ -2519,7 +2524,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="29" t="s">
         <v>48</v>
       </c>
@@ -2527,7 +2532,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="37" t="s">
         <v>65</v>
       </c>
@@ -2539,7 +2544,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
         <v>66</v>
       </c>
@@ -2547,7 +2552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="37" t="s">
         <v>67</v>
       </c>
@@ -2555,7 +2560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="37" t="s">
         <v>68</v>
       </c>
@@ -2563,7 +2568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="37" t="s">
         <v>69</v>
       </c>
@@ -2571,7 +2576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
         <v>70</v>
       </c>
@@ -2583,7 +2588,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
         <v>71</v>
       </c>
@@ -2591,7 +2596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
         <v>72</v>
       </c>
@@ -2599,7 +2604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
         <v>73</v>
       </c>
@@ -2607,7 +2612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="22" t="s">
         <v>74</v>
       </c>
@@ -2615,7 +2620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="37" t="s">
         <v>75</v>
       </c>
@@ -2627,7 +2632,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="37" t="s">
         <v>76</v>
       </c>
@@ -2635,7 +2640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="37" t="s">
         <v>77</v>
       </c>
@@ -2646,7 +2651,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="37" t="s">
         <v>78</v>
       </c>
@@ -2654,7 +2659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="37" t="s">
         <v>79</v>
       </c>
@@ -2662,7 +2667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="37" t="s">
         <v>92</v>
       </c>
@@ -2674,7 +2679,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="37" t="s">
         <v>93</v>
       </c>
@@ -2682,7 +2687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="37" t="s">
         <v>94</v>
       </c>
@@ -2693,7 +2698,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="37" t="s">
         <v>95</v>
       </c>
@@ -2701,7 +2706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="37" t="s">
         <v>96</v>
       </c>
@@ -2709,7 +2714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="22" t="s">
         <v>83</v>
       </c>
@@ -2717,7 +2722,7 @@
         <v>5737</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="22" t="s">
         <v>84</v>
       </c>
@@ -2725,7 +2730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="22" t="s">
         <v>85</v>
       </c>
@@ -2733,7 +2738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="22" t="s">
         <v>86</v>
       </c>
@@ -2741,7 +2746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="22" t="s">
         <v>87</v>
       </c>
@@ -2749,7 +2754,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="45" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="37" t="s">
         <v>98</v>
       </c>
@@ -2757,7 +2762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="37" t="s">
         <v>99</v>
       </c>
@@ -2765,7 +2770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="37" t="s">
         <v>100</v>
       </c>
@@ -2773,7 +2778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="37" t="s">
         <v>101</v>
       </c>
@@ -2781,7 +2786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="37" t="s">
         <v>102</v>
       </c>
@@ -2821,38 +2826,38 @@
   </sheetPr>
   <dimension ref="A1:AG38"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
+      <selection pane="bottomRight" activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="57.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="57.6640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="5" customWidth="1"/>
     <col min="4" max="4" width="11" style="6" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" style="7" customWidth="1"/>
-    <col min="7" max="8" width="7.28515625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="7.140625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="7.42578125" style="7" customWidth="1"/>
-    <col min="13" max="14" width="7.5703125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" style="7" customWidth="1"/>
+    <col min="7" max="8" width="7.33203125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="7.109375" style="7" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="7.44140625" style="7" customWidth="1"/>
+    <col min="13" max="14" width="7.5546875" style="7" customWidth="1"/>
     <col min="15" max="19" width="7" style="7" customWidth="1"/>
-    <col min="20" max="20" width="8.85546875" style="7" customWidth="1"/>
-    <col min="21" max="22" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="7.85546875" style="7" customWidth="1"/>
+    <col min="20" max="20" width="8.88671875" style="7" customWidth="1"/>
+    <col min="21" max="22" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="7.88671875" style="7" customWidth="1"/>
     <col min="25" max="25" width="14" style="7" customWidth="1"/>
-    <col min="26" max="27" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="28" max="30" width="14.42578125" style="7" customWidth="1"/>
-    <col min="31" max="33" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="9.140625" style="7"/>
+    <col min="26" max="27" width="14.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="28" max="30" width="14.44140625" style="7" customWidth="1"/>
+    <col min="31" max="33" width="15.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="34" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>6</v>
       </c>
@@ -2953,7 +2958,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>50</v>
       </c>
@@ -2967,7 +2972,7 @@
       <c r="Y2" s="23"/>
       <c r="AE2" s="23"/>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>22</v>
       </c>
@@ -2992,7 +2997,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
         <v>23</v>
       </c>
@@ -3024,7 +3029,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="5" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
         <v>51</v>
       </c>
@@ -3039,7 +3044,7 @@
       <c r="Y5" s="23"/>
       <c r="Z5" s="23"/>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>52</v>
       </c>
@@ -3053,7 +3058,7 @@
       <c r="AA6" s="12"/>
       <c r="AB6" s="12"/>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
         <v>53</v>
       </c>
@@ -3067,7 +3072,7 @@
       <c r="AA7" s="12"/>
       <c r="AB7" s="12"/>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
         <v>54</v>
       </c>
@@ -3083,7 +3088,7 @@
       <c r="AC8" s="12"/>
       <c r="AD8" s="12"/>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" s="25" t="s">
         <v>55</v>
       </c>
@@ -3099,7 +3104,7 @@
       <c r="AC9" s="12"/>
       <c r="AD9" s="12"/>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
         <v>56</v>
       </c>
@@ -3115,7 +3120,7 @@
       </c>
       <c r="AB10" s="12"/>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
         <v>57</v>
       </c>
@@ -3132,7 +3137,7 @@
       <c r="AA11" s="12"/>
       <c r="AB11" s="12"/>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
         <v>58</v>
       </c>
@@ -3150,7 +3155,7 @@
       <c r="AB12" s="12"/>
       <c r="AC12" s="12"/>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
         <v>59</v>
       </c>
@@ -3166,7 +3171,7 @@
       <c r="AD13" s="12"/>
       <c r="AE13" s="12"/>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
         <v>60</v>
       </c>
@@ -3212,7 +3217,7 @@
         <v>37.686746987951807</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" s="40" t="s">
         <v>91</v>
       </c>
@@ -3230,7 +3235,7 @@
       <c r="AD15" s="12"/>
       <c r="AE15" s="12"/>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" s="40" t="s">
         <v>61</v>
       </c>
@@ -3252,7 +3257,7 @@
       <c r="AD16" s="12"/>
       <c r="AE16" s="12"/>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17" s="40" t="s">
         <v>62</v>
       </c>
@@ -3274,7 +3279,7 @@
       <c r="AD17" s="12"/>
       <c r="AE17" s="12"/>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
         <v>63</v>
       </c>
@@ -3282,10 +3287,10 @@
         <v>3</v>
       </c>
       <c r="D18" s="6">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="X18" s="7">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="Z18" s="12"/>
       <c r="AA18" s="12"/>
@@ -3297,7 +3302,7 @@
       </c>
       <c r="AE18" s="12"/>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19" s="25" t="s">
         <v>64</v>
       </c>
@@ -3305,10 +3310,10 @@
         <v>4</v>
       </c>
       <c r="D19" s="6">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="X19" s="7">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="Z19" s="12"/>
       <c r="AA19" s="12"/>
@@ -3321,7 +3326,7 @@
       </c>
       <c r="AE19" s="12"/>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20" s="25" t="s">
         <v>97</v>
       </c>
@@ -3337,7 +3342,7 @@
       <c r="AD20" s="12"/>
       <c r="AE20" s="12"/>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21" s="25" t="s">
         <v>21</v>
       </c>
@@ -3400,7 +3405,7 @@
         <v>117.42738589211601</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22" s="25" t="s">
         <v>49</v>
       </c>
@@ -3411,7 +3416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23" s="25" t="s">
         <v>30</v>
       </c>
@@ -3434,7 +3439,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24" s="25" t="s">
         <v>31</v>
       </c>
@@ -3448,7 +3453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25" s="25" t="s">
         <v>32</v>
       </c>
@@ -3467,7 +3472,7 @@
         <v>2.295918367346939</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A26" s="25" t="s">
         <v>33</v>
       </c>
@@ -3491,7 +3496,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27" s="25" t="s">
         <v>34</v>
       </c>
@@ -3522,7 +3527,7 @@
       <c r="W27" s="6"/>
       <c r="X27" s="6"/>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A28" s="25" t="s">
         <v>36</v>
       </c>
@@ -3551,7 +3556,7 @@
       <c r="AD28" s="12"/>
       <c r="AE28" s="12"/>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
       <c r="D31" s="6">
         <v>69</v>
       </c>
@@ -3614,18 +3619,18 @@
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:24" x14ac:dyDescent="0.3">
       <c r="X33" s="7">
         <f>100*9028/7265000</f>
         <v>0.12426703372333103</v>
       </c>
     </row>
-    <row r="34" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:24" x14ac:dyDescent="0.3">
       <c r="X34" s="7">
         <v>4.5</v>
       </c>
     </row>
-    <row r="36" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D36" s="6">
         <v>5</v>
       </c>
@@ -3651,7 +3656,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D37" s="6">
         <v>10</v>
       </c>
@@ -3677,7 +3682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D38" s="6">
         <v>14</v>
       </c>
@@ -3748,7 +3753,7 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">

</xml_diff>

<commit_message>
Update Bulgaria data input spreadsheet
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rragonnet\Google Drive\GitHub\AuTuMN\autumn\xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdoan\Github\AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="612" windowWidth="16272" windowHeight="6300" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="109">
   <si>
     <t>parameter</t>
   </si>
@@ -333,6 +333,24 @@
   </si>
   <si>
     <t>econ_saturation_ambulatorycare_smearneg</t>
+  </si>
+  <si>
+    <t>econ_unitcost_ambulatorycare_extrapul</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_ambulatorycare_extrapul</t>
+  </si>
+  <si>
+    <t>econ_startupcost_ambulatorycare_extrapul</t>
+  </si>
+  <si>
+    <t>econ_startupduration_ambulatorycare_extrapul</t>
+  </si>
+  <si>
+    <t>econ_saturation_ambulatorycare_extrapul</t>
+  </si>
+  <si>
+    <t>int_perc_ambulatorycare_extrapul</t>
   </si>
 </sst>
 </file>
@@ -2320,24 +2338,24 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.5546875" style="19" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" style="21" customWidth="1"/>
-    <col min="3" max="5" width="9.109375" style="19"/>
-    <col min="6" max="6" width="13.88671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="19"/>
+    <col min="1" max="1" width="47.28515625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="21" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="19"/>
+    <col min="6" max="6" width="13.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2345,7 +2363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
@@ -2355,7 +2373,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="45" t="s">
         <v>88</v>
       </c>
@@ -2365,7 +2383,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
         <v>89</v>
       </c>
@@ -2375,7 +2393,7 @@
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
         <v>90</v>
       </c>
@@ -2385,17 +2403,17 @@
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="18">
-        <v>0.26500000000000001</v>
+        <v>0.36</v>
       </c>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
     </row>
-    <row r="7" spans="1:7" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>25</v>
       </c>
@@ -2405,7 +2423,7 @@
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
     </row>
-    <row r="8" spans="1:7" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>26</v>
       </c>
@@ -2418,7 +2436,7 @@
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
     </row>
-    <row r="9" spans="1:7" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>12</v>
       </c>
@@ -2428,7 +2446,7 @@
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
     </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>24</v>
       </c>
@@ -2436,7 +2454,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>29</v>
       </c>
@@ -2444,7 +2462,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
         <v>37</v>
       </c>
@@ -2456,7 +2474,7 @@
       <c r="D12" s="28"/>
       <c r="E12" s="29"/>
     </row>
-    <row r="13" spans="1:7" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>38</v>
       </c>
@@ -2469,12 +2487,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
         <v>40</v>
       </c>
       <c r="B14" s="31">
-        <v>0.86</v>
+        <v>0.89</v>
       </c>
       <c r="C14" s="31"/>
       <c r="D14" s="31"/>
@@ -2482,7 +2500,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
         <v>42</v>
       </c>
@@ -2495,7 +2513,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
         <v>44</v>
       </c>
@@ -2508,7 +2526,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="34" t="s">
         <v>46</v>
       </c>
@@ -2516,7 +2534,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
         <v>47</v>
       </c>
@@ -2524,7 +2542,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
         <v>48</v>
       </c>
@@ -2532,19 +2550,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="37" t="s">
         <v>65</v>
       </c>
       <c r="B20" s="41">
-        <f>8.19*4*10*0.51*0.85</f>
-        <v>142.0146</v>
+        <v>92</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="37" t="s">
         <v>66</v>
       </c>
@@ -2552,7 +2569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="37" t="s">
         <v>67</v>
       </c>
@@ -2560,7 +2577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="37" t="s">
         <v>68</v>
       </c>
@@ -2568,7 +2585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="37" t="s">
         <v>69</v>
       </c>
@@ -2576,19 +2593,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>70</v>
       </c>
       <c r="B25" s="21">
-        <f>20*4*10*0.51*0.65</f>
-        <v>265.2</v>
+        <v>857</v>
       </c>
       <c r="E25" s="19" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>71</v>
       </c>
@@ -2596,7 +2612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
         <v>72</v>
       </c>
@@ -2604,7 +2620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
         <v>73</v>
       </c>
@@ -2612,7 +2628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
         <v>74</v>
       </c>
@@ -2620,7 +2636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="37" t="s">
         <v>75</v>
       </c>
@@ -2632,7 +2648,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="37" t="s">
         <v>76</v>
       </c>
@@ -2640,7 +2656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="37" t="s">
         <v>77</v>
       </c>
@@ -2651,7 +2667,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="37" t="s">
         <v>78</v>
       </c>
@@ -2659,7 +2675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="37" t="s">
         <v>79</v>
       </c>
@@ -2667,7 +2683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="37" t="s">
         <v>92</v>
       </c>
@@ -2679,7 +2695,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="37" t="s">
         <v>93</v>
       </c>
@@ -2687,7 +2703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="37" t="s">
         <v>94</v>
       </c>
@@ -2698,7 +2714,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="37" t="s">
         <v>95</v>
       </c>
@@ -2706,7 +2722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="37" t="s">
         <v>96</v>
       </c>
@@ -2714,15 +2730,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
         <v>83</v>
       </c>
       <c r="B40" s="42">
-        <v>5737</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6094</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
         <v>84</v>
       </c>
@@ -2730,7 +2746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
         <v>85</v>
       </c>
@@ -2738,7 +2754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
         <v>86</v>
       </c>
@@ -2746,7 +2762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
         <v>87</v>
       </c>
@@ -2754,15 +2770,15 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="45" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="37" t="s">
         <v>98</v>
       </c>
       <c r="B45" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="37" t="s">
         <v>99</v>
       </c>
@@ -2770,7 +2786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="37" t="s">
         <v>100</v>
       </c>
@@ -2778,7 +2794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="37" t="s">
         <v>101</v>
       </c>
@@ -2786,12 +2802,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="37" t="s">
         <v>102</v>
       </c>
       <c r="B49" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" s="22">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="B51" s="22">
         <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="B52" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B53" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B54" s="22">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2824,40 +2880,40 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AG38"/>
+  <dimension ref="A1:AG39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U18" sqref="U18"/>
+      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.6640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="57.7109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="5" customWidth="1"/>
     <col min="4" max="4" width="11" style="6" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" style="7" customWidth="1"/>
-    <col min="7" max="8" width="7.33203125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="7.109375" style="7" customWidth="1"/>
-    <col min="10" max="10" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="7.44140625" style="7" customWidth="1"/>
-    <col min="13" max="14" width="7.5546875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="7" customWidth="1"/>
+    <col min="7" max="8" width="7.28515625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="7.42578125" style="7" customWidth="1"/>
+    <col min="13" max="14" width="7.5703125" style="7" customWidth="1"/>
     <col min="15" max="19" width="7" style="7" customWidth="1"/>
-    <col min="20" max="20" width="8.88671875" style="7" customWidth="1"/>
-    <col min="21" max="22" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="7.88671875" style="7" customWidth="1"/>
+    <col min="20" max="20" width="8.85546875" style="7" customWidth="1"/>
+    <col min="21" max="22" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="7.85546875" style="7" customWidth="1"/>
     <col min="25" max="25" width="14" style="7" customWidth="1"/>
-    <col min="26" max="27" width="14.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="28" max="30" width="14.44140625" style="7" customWidth="1"/>
-    <col min="31" max="33" width="15.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="9.109375" style="7"/>
+    <col min="26" max="27" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="28" max="30" width="14.42578125" style="7" customWidth="1"/>
+    <col min="31" max="33" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="34" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>6</v>
       </c>
@@ -2958,7 +3014,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>50</v>
       </c>
@@ -2972,7 +3028,7 @@
       <c r="Y2" s="23"/>
       <c r="AE2" s="23"/>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>22</v>
       </c>
@@ -2997,7 +3053,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>23</v>
       </c>
@@ -3007,29 +3063,8 @@
       <c r="C4" s="5">
         <v>0.2</v>
       </c>
-      <c r="R4" s="7">
-        <v>12</v>
-      </c>
-      <c r="S4" s="7">
-        <v>12</v>
-      </c>
-      <c r="T4" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="U4" s="7">
-        <v>9.5</v>
-      </c>
-      <c r="V4" s="7">
-        <v>9</v>
-      </c>
-      <c r="W4" s="7">
-        <v>8.5</v>
-      </c>
-      <c r="X4" s="7">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>51</v>
       </c>
@@ -3044,7 +3079,7 @@
       <c r="Y5" s="23"/>
       <c r="Z5" s="23"/>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>52</v>
       </c>
@@ -3058,7 +3093,7 @@
       <c r="AA6" s="12"/>
       <c r="AB6" s="12"/>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>53</v>
       </c>
@@ -3072,7 +3107,7 @@
       <c r="AA7" s="12"/>
       <c r="AB7" s="12"/>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>54</v>
       </c>
@@ -3088,7 +3123,7 @@
       <c r="AC8" s="12"/>
       <c r="AD8" s="12"/>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>55</v>
       </c>
@@ -3104,12 +3139,15 @@
       <c r="AC9" s="12"/>
       <c r="AD9" s="12"/>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>56</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>4</v>
+      </c>
+      <c r="M10" s="7">
+        <v>0</v>
       </c>
       <c r="X10" s="7">
         <v>0</v>
@@ -3120,42 +3158,36 @@
       </c>
       <c r="AB10" s="12"/>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>57</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="S11" s="7">
-        <v>0</v>
-      </c>
-      <c r="T11" s="7">
-        <v>10</v>
+      <c r="X11" s="7">
+        <v>70</v>
       </c>
       <c r="Z11" s="12"/>
       <c r="AA11" s="12"/>
       <c r="AB11" s="12"/>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>58</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="S12" s="7">
-        <v>0</v>
-      </c>
-      <c r="T12" s="7">
-        <v>10</v>
+      <c r="X12" s="7">
+        <v>70</v>
       </c>
       <c r="Z12" s="12"/>
       <c r="AA12" s="12"/>
       <c r="AB12" s="12"/>
       <c r="AC12" s="12"/>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>59</v>
       </c>
@@ -3171,7 +3203,7 @@
       <c r="AD13" s="12"/>
       <c r="AE13" s="12"/>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>60</v>
       </c>
@@ -3217,7 +3249,7 @@
         <v>37.686746987951807</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
         <v>91</v>
       </c>
@@ -3228,14 +3260,14 @@
         <v>80</v>
       </c>
       <c r="Z15" s="39">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AA15" s="12"/>
       <c r="AB15" s="12"/>
       <c r="AD15" s="12"/>
       <c r="AE15" s="12"/>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="s">
         <v>61</v>
       </c>
@@ -3243,13 +3275,13 @@
         <v>3</v>
       </c>
       <c r="S16" s="38">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="X16" s="38">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="Y16" s="38">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Z16" s="12"/>
       <c r="AA16" s="12"/>
@@ -3257,7 +3289,7 @@
       <c r="AD16" s="12"/>
       <c r="AE16" s="12"/>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="40" t="s">
         <v>62</v>
       </c>
@@ -3265,13 +3297,13 @@
         <v>3</v>
       </c>
       <c r="S17" s="38">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="X17" s="38">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Y17" s="38">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Z17" s="12"/>
       <c r="AA17" s="12"/>
@@ -3279,7 +3311,7 @@
       <c r="AD17" s="12"/>
       <c r="AE17" s="12"/>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>63</v>
       </c>
@@ -3294,15 +3326,13 @@
       </c>
       <c r="Z18" s="12"/>
       <c r="AA18" s="12"/>
-      <c r="AB18" s="12">
+      <c r="AB18" s="39">
         <v>0</v>
       </c>
-      <c r="AD18" s="12">
-        <v>0</v>
-      </c>
+      <c r="AD18" s="12"/>
       <c r="AE18" s="12"/>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>64</v>
       </c>
@@ -3317,16 +3347,16 @@
       </c>
       <c r="Z19" s="12"/>
       <c r="AA19" s="12"/>
-      <c r="AB19" s="12"/>
-      <c r="AC19" s="7">
+      <c r="AB19" s="39">
         <v>0</v>
       </c>
-      <c r="AD19" s="12">
+      <c r="AC19" s="39">
         <v>0</v>
       </c>
+      <c r="AD19" s="12"/>
       <c r="AE19" s="12"/>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>97</v>
       </c>
@@ -3339,369 +3369,300 @@
       <c r="Z20" s="12"/>
       <c r="AA20" s="12"/>
       <c r="AB20" s="12"/>
-      <c r="AD20" s="12"/>
+      <c r="AD20" s="39">
+        <v>99</v>
+      </c>
       <c r="AE20" s="12"/>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z21" s="12"/>
+      <c r="AA21" s="12"/>
+      <c r="AB21" s="12"/>
+      <c r="AD21" s="39">
+        <v>99</v>
+      </c>
+      <c r="AE21" s="12"/>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
         <v>21</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="6">
-        <v>1</v>
-      </c>
-      <c r="E21" s="13">
-        <v>1</v>
-      </c>
-      <c r="F21" s="13">
-        <v>2.4974653103104298</v>
-      </c>
-      <c r="G21" s="13">
-        <v>9.3018160392078606</v>
-      </c>
-      <c r="H21" s="13">
-        <v>10.2347283365258</v>
-      </c>
-      <c r="I21" s="13">
-        <v>25.481798063623799</v>
-      </c>
-      <c r="J21" s="13">
-        <v>28.584806362378998</v>
-      </c>
-      <c r="K21" s="13">
-        <v>37.0398409405256</v>
-      </c>
-      <c r="L21" s="13">
-        <v>43.633070539419101</v>
-      </c>
-      <c r="M21" s="13">
-        <v>63.651452282157699</v>
-      </c>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13">
-        <v>82.987551867219906</v>
-      </c>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13">
-        <v>100</v>
-      </c>
-      <c r="T21" s="13">
-        <v>104.647302904564</v>
-      </c>
-      <c r="U21" s="13">
-        <v>107.966804979253</v>
-      </c>
-      <c r="V21" s="13">
-        <v>111.203319502075</v>
-      </c>
-      <c r="W21" s="13">
-        <v>115.767634854772</v>
-      </c>
-      <c r="X21" s="13">
-        <v>117.42738589211601</v>
-      </c>
-    </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A22" s="25" t="s">
-        <v>49</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I22" s="7">
+      <c r="D22" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="E22" s="13">
+        <v>1</v>
+      </c>
+      <c r="F22" s="13">
+        <v>2.4974653103104298</v>
+      </c>
+      <c r="G22" s="13">
+        <v>9.3018160392078606</v>
+      </c>
+      <c r="H22" s="13">
+        <v>10.2347283365258</v>
+      </c>
+      <c r="I22" s="13">
+        <v>25.481798063623799</v>
+      </c>
+      <c r="J22" s="13">
+        <v>28.584806362378998</v>
+      </c>
+      <c r="K22" s="13">
+        <v>37.0398409405256</v>
+      </c>
+      <c r="L22" s="13">
+        <v>43.633070539419101</v>
+      </c>
+      <c r="M22" s="13">
+        <v>63.651452282157699</v>
+      </c>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13">
+        <v>82.987551867219906</v>
+      </c>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13">
+        <v>100</v>
+      </c>
+      <c r="T22" s="13">
+        <v>104.647302904564</v>
+      </c>
+      <c r="U22" s="13">
+        <v>107.966804979253</v>
+      </c>
+      <c r="V22" s="13">
+        <v>111.203319502075</v>
+      </c>
+      <c r="W22" s="13">
+        <v>115.767634854772</v>
+      </c>
+      <c r="X22" s="13">
+        <v>117.42738589211601</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I23" s="7">
         <v>1</v>
       </c>
-      <c r="O23" s="7">
-        <v>5.4</v>
-      </c>
-      <c r="U23" s="7">
-        <v>6</v>
-      </c>
-      <c r="V23" s="7">
-        <v>7.63</v>
-      </c>
-      <c r="X23" s="7">
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M24" s="7">
+      <c r="I24" s="7">
         <v>1</v>
       </c>
+      <c r="O24" s="7">
+        <v>5.4</v>
+      </c>
+      <c r="U24" s="7">
+        <v>6</v>
+      </c>
+      <c r="V24" s="7">
+        <v>7.63</v>
+      </c>
       <c r="X24" s="7">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A25" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M25" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A25" s="25" t="s">
+      <c r="X25" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A26" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B26" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="X25" s="7">
+      <c r="X26" s="7">
         <f>4.5/98 * 100</f>
         <v>4.591836734693878</v>
       </c>
-      <c r="AE25" s="12">
+      <c r="AE26" s="12">
         <v>2.2999999999999998</v>
       </c>
-      <c r="AF25" s="7">
-        <f>X25/2</f>
+      <c r="AF26" s="7">
+        <f>X26/2</f>
         <v>2.295918367346939</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A26" s="25" t="s">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A27" s="25" t="s">
         <v>33</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" s="7">
-        <v>2</v>
-      </c>
-      <c r="M26" s="7">
-        <v>6</v>
-      </c>
-      <c r="X26" s="7">
-        <v>10</v>
-      </c>
-      <c r="AE26" s="12">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="AG26" s="7">
-        <f>X26/2</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A27" s="25" t="s">
-        <v>34</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="6"/>
-      <c r="R27" s="6"/>
-      <c r="S27" s="6"/>
-      <c r="T27" s="6"/>
-      <c r="U27" s="6"/>
-      <c r="V27" s="6"/>
-      <c r="W27" s="6"/>
-      <c r="X27" s="6"/>
-    </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="E27" s="7">
+        <v>2</v>
+      </c>
+      <c r="M27" s="7">
+        <v>6</v>
+      </c>
+      <c r="X27" s="7">
+        <v>10</v>
+      </c>
+      <c r="AE27" s="12">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="AG27" s="7">
+        <f>X27/2</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="6">
+      <c r="C28" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
+      <c r="U28" s="6"/>
+      <c r="V28" s="6"/>
+      <c r="W28" s="6"/>
+      <c r="X28" s="6"/>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A29" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="6">
         <v>1</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F29" s="7">
         <v>1</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G29" s="7">
         <v>1</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H29" s="7">
         <v>3.11</v>
       </c>
-      <c r="W28" s="7">
+      <c r="W29" s="7">
         <v>3.11</v>
       </c>
-      <c r="Z28" s="12"/>
-      <c r="AA28" s="12"/>
-      <c r="AB28" s="12"/>
-      <c r="AC28" s="12"/>
-      <c r="AD28" s="12"/>
-      <c r="AE28" s="12"/>
-    </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="D31" s="6">
-        <v>69</v>
-      </c>
-      <c r="E31" s="6">
-        <v>69</v>
-      </c>
-      <c r="F31" s="6">
-        <v>69</v>
-      </c>
-      <c r="G31" s="6">
-        <v>69</v>
-      </c>
-      <c r="H31" s="6">
-        <v>69</v>
-      </c>
-      <c r="I31" s="6">
-        <v>69</v>
-      </c>
-      <c r="J31" s="6">
-        <v>69</v>
-      </c>
-      <c r="K31" s="6">
-        <v>69</v>
-      </c>
-      <c r="L31" s="6">
-        <v>69</v>
-      </c>
-      <c r="M31" s="6">
-        <v>69</v>
-      </c>
-      <c r="N31" s="6">
-        <v>90</v>
-      </c>
-      <c r="O31" s="6">
-        <v>90</v>
-      </c>
-      <c r="P31" s="6">
-        <v>90</v>
-      </c>
-      <c r="Q31" s="6">
-        <v>90</v>
-      </c>
-      <c r="R31" s="6"/>
-      <c r="S31" s="6">
-        <v>85</v>
-      </c>
-      <c r="T31" s="6">
-        <v>85</v>
-      </c>
-      <c r="U31" s="6">
-        <v>80</v>
-      </c>
-      <c r="V31" s="6">
-        <v>80</v>
-      </c>
-      <c r="W31" s="6">
-        <v>80</v>
-      </c>
-      <c r="X31" s="6">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="4:24" x14ac:dyDescent="0.3">
-      <c r="X33" s="7">
-        <f>100*9028/7265000</f>
-        <v>0.12426703372333103</v>
-      </c>
-    </row>
-    <row r="34" spans="4:24" x14ac:dyDescent="0.3">
-      <c r="X34" s="7">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="36" spans="4:24" x14ac:dyDescent="0.3">
-      <c r="D36" s="6">
-        <v>5</v>
-      </c>
-      <c r="K36" s="7">
-        <v>5</v>
-      </c>
-      <c r="M36" s="9">
-        <v>3</v>
-      </c>
-      <c r="N36" s="9"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="9">
-        <v>3</v>
-      </c>
-      <c r="T36" s="9"/>
-      <c r="U36" s="9"/>
-      <c r="V36" s="9"/>
-      <c r="W36" s="9"/>
-      <c r="X36" s="9">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="37" spans="4:24" x14ac:dyDescent="0.3">
-      <c r="D37" s="6">
-        <v>10</v>
-      </c>
-      <c r="K37" s="7">
-        <v>10</v>
-      </c>
-      <c r="M37" s="9">
-        <v>6</v>
-      </c>
+      <c r="Z29" s="12"/>
+      <c r="AA29" s="12"/>
+      <c r="AB29" s="12"/>
+      <c r="AC29" s="12"/>
+      <c r="AD29" s="12"/>
+      <c r="AE29" s="12"/>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="6"/>
+      <c r="R32" s="6"/>
+      <c r="S32" s="6"/>
+      <c r="T32" s="6"/>
+      <c r="U32" s="6"/>
+      <c r="V32" s="6"/>
+      <c r="W32" s="6"/>
+      <c r="X32" s="6"/>
+    </row>
+    <row r="37" spans="13:24" x14ac:dyDescent="0.25">
+      <c r="M37" s="9"/>
       <c r="N37" s="9"/>
       <c r="O37" s="8"/>
       <c r="P37" s="8"/>
       <c r="Q37" s="8"/>
       <c r="R37" s="8"/>
-      <c r="S37" s="9">
-        <v>6</v>
-      </c>
+      <c r="S37" s="9"/>
       <c r="T37" s="9"/>
       <c r="U37" s="9"/>
       <c r="V37" s="9"/>
       <c r="W37" s="9"/>
-      <c r="X37" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="4:24" x14ac:dyDescent="0.3">
-      <c r="D38" s="6">
-        <v>14</v>
-      </c>
-      <c r="M38" s="9">
-        <v>8</v>
-      </c>
+      <c r="X37" s="9"/>
+    </row>
+    <row r="38" spans="13:24" x14ac:dyDescent="0.25">
+      <c r="M38" s="9"/>
       <c r="N38" s="9"/>
       <c r="O38" s="8"/>
       <c r="P38" s="8"/>
-      <c r="Q38" s="16"/>
-      <c r="R38" s="16"/>
-      <c r="S38" s="9">
-        <v>6</v>
-      </c>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8"/>
+      <c r="S38" s="9"/>
       <c r="T38" s="9"/>
       <c r="U38" s="9"/>
       <c r="V38" s="9"/>
       <c r="W38" s="9"/>
       <c r="X38" s="9"/>
+    </row>
+    <row r="39" spans="13:24" x14ac:dyDescent="0.25">
+      <c r="M39" s="9"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="16"/>
+      <c r="R39" s="16"/>
+      <c r="S39" s="9"/>
+      <c r="T39" s="9"/>
+      <c r="U39" s="9"/>
+      <c r="V39" s="9"/>
+      <c r="W39" s="9"/>
+      <c r="X39" s="9"/>
     </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="4">
@@ -3710,7 +3671,7 @@
       <formula2>100000000000000000000</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:H14 Y3:Y4 E36:X38 E2:X3 E5:X5">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:H14 Y3:Y4 E37:X39 E2:X3 E5:X5">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -3753,9 +3714,9 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3769,7 +3730,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3780,7 +3741,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Simplify Bulgaria spreadsheet and crude  calibration
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdoan\Github\AuTuMN\autumn\xls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -19,12 +14,12 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="100">
   <si>
     <t>parameter</t>
   </si>
@@ -92,12 +87,6 @@
     <t>econ_cpi</t>
   </si>
   <si>
-    <t>program_perc_treatment_success</t>
-  </si>
-  <si>
-    <t>program_perc_treatment_death</t>
-  </si>
-  <si>
     <t>demo_household_size</t>
   </si>
   <si>
@@ -176,24 +165,6 @@
     <t>riskgroup_perc_hiv</t>
   </si>
   <si>
-    <t>int_perc_vaccination</t>
-  </si>
-  <si>
-    <t>int_perc_xpert</t>
-  </si>
-  <si>
-    <t>int_perc_xpertacf_prison</t>
-  </si>
-  <si>
-    <t>int_perc_xpertacf_ruralpoor</t>
-  </si>
-  <si>
-    <t>int_perc_cxrxpertacf_prison</t>
-  </si>
-  <si>
-    <t>int_perc_cxrxpertacf_ruralpoor</t>
-  </si>
-  <si>
     <t>int_perc_shortcourse_mdr</t>
   </si>
   <si>
@@ -201,9 +172,6 @@
   </si>
   <si>
     <t>int_perc_ipt_age5to15</t>
-  </si>
-  <si>
-    <t>int_perc_awareness_raising</t>
   </si>
   <si>
     <t>int_perc_firstline_dst</t>
@@ -362,7 +330,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -447,20 +415,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1" tint="0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="3" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFC00000"/>
@@ -469,7 +423,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -485,36 +439,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB9DAED"/>
         <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1277,9 +1201,8 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1289,7 +1212,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1306,50 +1228,19 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="12" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="664" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="7"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="664" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="664" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="13" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="664" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="664" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="665">
     <cellStyle name="Comma" xfId="664" builtinId="3"/>
@@ -2091,7 +1982,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2126,7 +2017,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2340,513 +2231,513 @@
   </sheetPr>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:B54"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.28515625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="21" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="19"/>
-    <col min="6" max="6" width="13.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="19"/>
+    <col min="1" max="1" width="47.28515625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="19" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="17"/>
+    <col min="6" max="6" width="13.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="15">
-        <v>6.8</v>
-      </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-    </row>
-    <row r="3" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="46">
+      <c r="B2" s="13">
+        <v>15</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="18">
         <v>2</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-    </row>
-    <row r="4" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" s="49">
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+    </row>
+    <row r="4" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="18">
         <v>1920</v>
       </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-    </row>
-    <row r="5" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="48" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" s="49">
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="18">
         <v>1920</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-    </row>
-    <row r="6" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+    </row>
+    <row r="6" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="16">
         <v>0.36</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-    </row>
-    <row r="7" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="18">
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="16">
         <v>1</v>
       </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-    </row>
-    <row r="8" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="18">
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="16">
         <v>5</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="14">
         <v>15</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-    </row>
-    <row r="9" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+    </row>
+    <row r="9" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="47">
+      <c r="B9" s="23">
         <v>10000000</v>
       </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="36">
+      <c r="A10" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="19">
         <v>2.4</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="18">
+      <c r="A11" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="16">
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="28">
+    <row r="12" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="13">
         <f>20/12</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="29"/>
-    </row>
-    <row r="13" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="17"/>
+    </row>
+    <row r="13" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="16">
+        <v>0.4</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="35">
-        <v>0.4</v>
-      </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="29" t="s">
+      <c r="B14" s="16">
+        <v>0.89</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="17" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="30" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="31">
-        <v>0.89</v>
-      </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="29" t="s">
+      <c r="B15" s="24">
+        <v>1940</v>
+      </c>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="17" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="33">
-        <v>1940</v>
-      </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="34" t="s">
+      <c r="B16" s="24">
+        <v>1950</v>
+      </c>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="17" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="33">
-        <v>1950</v>
-      </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="34" t="s">
+      <c r="B17" s="19">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
+      <c r="B18" s="19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="21">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="36">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="36">
+      <c r="B19" s="19">
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="19">
+        <v>92</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="19">
+        <v>857</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="41">
-        <v>92</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="37" t="s">
+      <c r="B29" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" s="41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" s="41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="B24" s="41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" s="21">
-        <v>857</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="B26" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="B27" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="B28" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="B29" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="B30" s="37">
+      <c r="B30" s="17">
         <f>1.02+67.12</f>
         <v>68.14</v>
       </c>
-      <c r="E30" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="B31" s="37">
+      <c r="E30" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="B32" s="37">
+    <row r="32" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="17">
         <v>8028</v>
       </c>
-      <c r="E32" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="B33" s="37">
+      <c r="E32" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="B34" s="37">
+    <row r="34" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="B35" s="37">
+    <row r="35" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" s="17">
         <f>1.02+67.12</f>
         <v>68.14</v>
       </c>
-      <c r="E35" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="37" t="s">
+      <c r="E35" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="17">
+        <v>8028</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B39" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="25">
+        <v>6094</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B44" s="17">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" s="17">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B36" s="37">
+      <c r="B49" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50" s="17">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B51" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="37" t="s">
-        <v>94</v>
-      </c>
-      <c r="B37" s="37">
-        <v>8028</v>
-      </c>
-      <c r="E37" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="37" t="s">
-        <v>95</v>
-      </c>
-      <c r="B38" s="37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="37" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B39" s="37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="B40" s="42">
-        <v>6094</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="B41" s="22">
+      <c r="B52" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" s="43">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="B43" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="B44" s="22">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="37" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="B45" s="37">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="B46" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="37" t="s">
-        <v>100</v>
-      </c>
-      <c r="B47" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="B48" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="37" t="s">
-        <v>102</v>
-      </c>
-      <c r="B49" s="37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="B50" s="22">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="B51" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="B52" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="B53" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="B54" s="22">
+      <c r="B54" s="17">
         <v>1</v>
       </c>
     </row>
@@ -2872,6 +2763,9 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B12" unlockedFormula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -2880,798 +2774,606 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AG39"/>
+  <dimension ref="A1:AA30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="5" customWidth="1"/>
-    <col min="4" max="4" width="11" style="6" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" style="7" customWidth="1"/>
-    <col min="7" max="8" width="7.28515625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="7.140625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="7.42578125" style="7" customWidth="1"/>
-    <col min="13" max="14" width="7.5703125" style="7" customWidth="1"/>
-    <col min="15" max="19" width="7" style="7" customWidth="1"/>
-    <col min="20" max="20" width="8.85546875" style="7" customWidth="1"/>
-    <col min="21" max="22" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="7.85546875" style="7" customWidth="1"/>
-    <col min="25" max="25" width="14" style="7" customWidth="1"/>
-    <col min="26" max="27" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="28" max="30" width="14.42578125" style="7" customWidth="1"/>
-    <col min="31" max="33" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="57.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11" style="5" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="6" customWidth="1"/>
+    <col min="7" max="8" width="7.28515625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" style="6" customWidth="1"/>
+    <col min="12" max="13" width="7" style="6" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="6" customWidth="1"/>
+    <col min="15" max="16" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="7.85546875" style="6" customWidth="1"/>
+    <col min="19" max="19" width="14" style="6" customWidth="1"/>
+    <col min="20" max="21" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="14.42578125" style="6" customWidth="1"/>
+    <col min="25" max="27" width="15.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1" s="1">
         <v>1920</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="1">
         <v>1950</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="1">
         <v>1972</v>
       </c>
-      <c r="G1" s="2">
+      <c r="G1" s="1">
         <v>1982</v>
       </c>
-      <c r="H1" s="2">
+      <c r="H1" s="1">
         <v>1983</v>
       </c>
-      <c r="I1" s="2">
+      <c r="I1" s="1">
         <v>1989</v>
       </c>
-      <c r="J1" s="2">
+      <c r="J1" s="1">
         <v>1990</v>
       </c>
-      <c r="K1" s="2">
-        <v>1992</v>
-      </c>
-      <c r="L1" s="2">
-        <v>1994</v>
-      </c>
-      <c r="M1" s="2">
+      <c r="K1" s="1">
         <v>2000</v>
       </c>
-      <c r="N1" s="2">
-        <v>2005</v>
-      </c>
-      <c r="O1" s="2">
+      <c r="L1" s="1">
         <v>2006</v>
       </c>
-      <c r="P1" s="2">
-        <v>2007</v>
-      </c>
-      <c r="Q1" s="2">
-        <v>2008</v>
-      </c>
-      <c r="R1" s="2">
-        <v>2009</v>
-      </c>
-      <c r="S1" s="2">
+      <c r="M1" s="1">
         <v>2010</v>
       </c>
-      <c r="T1" s="2">
+      <c r="N1" s="1">
         <v>2011</v>
       </c>
-      <c r="U1" s="2">
+      <c r="O1" s="1">
         <v>2012</v>
       </c>
-      <c r="V1" s="2">
+      <c r="P1" s="1">
         <v>2013</v>
       </c>
-      <c r="W1" s="2">
+      <c r="Q1" s="1">
         <v>2014</v>
       </c>
-      <c r="X1" s="2">
+      <c r="R1" s="1">
         <v>2015</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="S1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="T1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="U1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="V1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="W1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="X1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AE1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="Y1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0</v>
+      </c>
+      <c r="R2" s="6">
+        <v>0</v>
+      </c>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10">
         <v>50</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="11">
-        <v>0.1</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="Y2" s="23"/>
-      <c r="AE2" s="23"/>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8">
-        <v>93</v>
-      </c>
-      <c r="V3" s="8">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="V2" s="10"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="R3" s="6">
+        <v>70</v>
+      </c>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="R4" s="6">
+        <v>70</v>
+      </c>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="1"/>
-      <c r="X5" s="9">
+      <c r="C5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="6">
         <v>0</v>
       </c>
-      <c r="Y5" s="23"/>
-      <c r="Z5" s="23"/>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="X6" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="12"/>
-      <c r="AA6" s="12"/>
-      <c r="AB6" s="12"/>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="X7" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="12"/>
-      <c r="AA7" s="12"/>
-      <c r="AB7" s="12"/>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="X8" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="12"/>
-      <c r="AA8" s="12"/>
-      <c r="AB8" s="12"/>
-      <c r="AC8" s="12"/>
-      <c r="AD8" s="12"/>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="X9" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="12"/>
-      <c r="AA9" s="12"/>
-      <c r="AB9" s="12"/>
-      <c r="AC9" s="12"/>
-      <c r="AD9" s="12"/>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="M10" s="7">
-        <v>0</v>
-      </c>
-      <c r="X10" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="12"/>
-      <c r="AA10" s="39">
-        <v>50</v>
-      </c>
-      <c r="AB10" s="12"/>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="X11" s="7">
-        <v>70</v>
-      </c>
-      <c r="Z11" s="12"/>
-      <c r="AA11" s="12"/>
-      <c r="AB11" s="12"/>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="X12" s="7">
-        <v>70</v>
-      </c>
-      <c r="Z12" s="12"/>
-      <c r="AA12" s="12"/>
-      <c r="AB12" s="12"/>
-      <c r="AC12" s="12"/>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="X13" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="12"/>
-      <c r="AA13" s="12"/>
-      <c r="AB13" s="12"/>
-      <c r="AD13" s="12"/>
-      <c r="AE13" s="12"/>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="7">
-        <v>0</v>
-      </c>
-      <c r="J14" s="7">
+      <c r="J5" s="6">
         <v>5</v>
       </c>
-      <c r="S14" s="7">
+      <c r="M5" s="6">
         <f>80*(1174/2649)</f>
         <v>35.454888637221593</v>
       </c>
-      <c r="T14" s="7">
+      <c r="N5" s="6">
         <f>80*(1077/2407)</f>
         <v>35.795596177814708</v>
       </c>
-      <c r="U14" s="7">
+      <c r="O5" s="6">
         <f>80*(1094/2280)</f>
         <v>38.385964912280699</v>
       </c>
-      <c r="V14" s="7">
+      <c r="P5" s="6">
         <f>80*(961/1932)</f>
         <v>39.792960662525878</v>
       </c>
-      <c r="W14" s="7">
+      <c r="Q5" s="6">
         <f>80*(891/1872)</f>
         <v>38.076923076923073</v>
       </c>
-      <c r="X14" s="7">
+      <c r="R5" s="6">
         <f>80*782/1660</f>
         <v>37.686746987951807</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A15" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" s="5" t="s">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="X15" s="38">
+      <c r="R6" s="6">
         <v>80</v>
       </c>
-      <c r="Z15" s="39">
+      <c r="T6" s="10">
         <v>99</v>
       </c>
-      <c r="AA15" s="12"/>
-      <c r="AB15" s="12"/>
-      <c r="AD15" s="12"/>
-      <c r="AE15" s="12"/>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A16" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="5" t="s">
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="S16" s="38">
+      <c r="M7" s="6">
         <v>50</v>
       </c>
-      <c r="X16" s="38">
+      <c r="R7" s="6">
         <v>50</v>
       </c>
-      <c r="Y16" s="38">
+      <c r="S7" s="6">
         <v>99</v>
       </c>
-      <c r="Z16" s="12"/>
-      <c r="AA16" s="12"/>
-      <c r="AB16" s="12"/>
-      <c r="AD16" s="12"/>
-      <c r="AE16" s="12"/>
-    </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A17" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="5" t="s">
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="S17" s="38">
+      <c r="M8" s="6">
         <v>99</v>
       </c>
-      <c r="X17" s="38">
+      <c r="R8" s="6">
         <v>99</v>
       </c>
-      <c r="Y17" s="38">
+      <c r="S8" s="6">
         <v>99</v>
       </c>
-      <c r="Z17" s="12"/>
-      <c r="AA17" s="12"/>
-      <c r="AB17" s="12"/>
-      <c r="AD17" s="12"/>
-      <c r="AE17" s="12"/>
-    </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="5" t="s">
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D9" s="5">
         <v>50</v>
       </c>
-      <c r="X18" s="7">
+      <c r="R9" s="6">
         <v>50</v>
       </c>
-      <c r="Z18" s="12"/>
-      <c r="AA18" s="12"/>
-      <c r="AB18" s="39">
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10">
         <v>0</v>
       </c>
-      <c r="AD18" s="12"/>
-      <c r="AE18" s="12"/>
-    </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="5" t="s">
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D10" s="5">
         <v>50</v>
       </c>
-      <c r="X19" s="7">
+      <c r="R10" s="6">
         <v>50</v>
       </c>
-      <c r="Z19" s="12"/>
-      <c r="AA19" s="12"/>
-      <c r="AB19" s="39">
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10">
         <v>0</v>
       </c>
-      <c r="AC19" s="39">
+      <c r="W10" s="10">
         <v>0</v>
       </c>
-      <c r="AD19" s="12"/>
-      <c r="AE19" s="12"/>
-    </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="B20" s="5" t="s">
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="X20" s="7">
+      <c r="R11" s="6">
         <v>0</v>
       </c>
-      <c r="Z20" s="12"/>
-      <c r="AA20" s="12"/>
-      <c r="AB20" s="12"/>
-      <c r="AD20" s="39">
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="X11" s="10">
         <v>99</v>
       </c>
-      <c r="AE20" s="12"/>
-    </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z21" s="12"/>
-      <c r="AA21" s="12"/>
-      <c r="AB21" s="12"/>
-      <c r="AD21" s="39">
+      <c r="Y11" s="10"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="AE21" s="12"/>
-    </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
+      <c r="B12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="R12" s="6">
+        <v>0</v>
+      </c>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="X12" s="10">
+        <v>99</v>
+      </c>
+      <c r="Y12" s="10"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D13" s="5">
         <v>1</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E13" s="11">
         <v>1</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F13" s="11">
         <v>2.4974653103104298</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G13" s="11">
         <v>9.3018160392078606</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H13" s="11">
         <v>10.2347283365258</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I13" s="11">
         <v>25.481798063623799</v>
       </c>
-      <c r="J22" s="13">
+      <c r="J13" s="11">
         <v>28.584806362378998</v>
       </c>
-      <c r="K22" s="13">
-        <v>37.0398409405256</v>
-      </c>
-      <c r="L22" s="13">
-        <v>43.633070539419101</v>
-      </c>
-      <c r="M22" s="13">
+      <c r="K13" s="11">
         <v>63.651452282157699</v>
       </c>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13">
+      <c r="L13" s="11">
         <v>82.987551867219906</v>
       </c>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="13">
+      <c r="M13" s="11">
         <v>100</v>
       </c>
-      <c r="T22" s="13">
+      <c r="N13" s="11">
         <v>104.647302904564</v>
       </c>
-      <c r="U22" s="13">
+      <c r="O13" s="11">
         <v>107.966804979253</v>
       </c>
-      <c r="V22" s="13">
+      <c r="P13" s="11">
         <v>111.203319502075</v>
       </c>
-      <c r="W22" s="13">
+      <c r="Q13" s="11">
         <v>115.767634854772</v>
       </c>
-      <c r="X22" s="13">
+      <c r="R13" s="11">
         <v>117.42738589211601</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="5" t="s">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I14" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" s="6">
+        <v>1</v>
+      </c>
+      <c r="L15" s="6">
+        <v>5.4</v>
+      </c>
+      <c r="O15" s="6">
+        <v>6</v>
+      </c>
+      <c r="P15" s="6">
+        <v>7.63</v>
+      </c>
+      <c r="R15" s="6">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16" s="6">
+        <v>1</v>
+      </c>
+      <c r="R16" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I24" s="7">
-        <v>1</v>
-      </c>
-      <c r="O24" s="7">
-        <v>5.4</v>
-      </c>
-      <c r="U24" s="7">
-        <v>6</v>
-      </c>
-      <c r="V24" s="7">
-        <v>7.63</v>
-      </c>
-      <c r="X24" s="7">
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="M25" s="7">
-        <v>1</v>
-      </c>
-      <c r="X25" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="X26" s="7">
+      <c r="R17" s="6">
         <f>4.5/98 * 100</f>
         <v>4.591836734693878</v>
       </c>
-      <c r="AE26" s="12">
+      <c r="Y17" s="10">
         <v>2.2999999999999998</v>
       </c>
-      <c r="AF26" s="7">
-        <f>X26/2</f>
+      <c r="Z17" s="6">
+        <f>R17/2</f>
         <v>2.295918367346939</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="5" t="s">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E18" s="6">
         <v>2</v>
       </c>
-      <c r="M27" s="7">
+      <c r="K18" s="6">
         <v>6</v>
       </c>
-      <c r="X27" s="7">
+      <c r="R18" s="6">
         <v>10</v>
       </c>
-      <c r="AE27" s="12">
+      <c r="Y18" s="10">
         <v>5.0999999999999996</v>
       </c>
-      <c r="AG27" s="7">
-        <f>X27/2</f>
+      <c r="AA18" s="6">
+        <f>R18/2</f>
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A20" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="6"/>
-      <c r="R28" s="6"/>
-      <c r="S28" s="6"/>
-      <c r="T28" s="6"/>
-      <c r="U28" s="6"/>
-      <c r="V28" s="6"/>
-      <c r="W28" s="6"/>
-      <c r="X28" s="6"/>
-    </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D29" s="6">
+      <c r="D20" s="5">
         <v>1</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F20" s="6">
         <v>1</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G20" s="6">
         <v>1</v>
       </c>
-      <c r="H29" s="7">
+      <c r="H20" s="6">
         <v>3.11</v>
       </c>
-      <c r="W29" s="7">
+      <c r="Q20" s="6">
         <v>3.11</v>
       </c>
-      <c r="Z29" s="12"/>
-      <c r="AA29" s="12"/>
-      <c r="AB29" s="12"/>
-      <c r="AC29" s="12"/>
-      <c r="AD29" s="12"/>
-      <c r="AE29" s="12"/>
-    </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="6"/>
-      <c r="R32" s="6"/>
-      <c r="S32" s="6"/>
-      <c r="T32" s="6"/>
-      <c r="U32" s="6"/>
-      <c r="V32" s="6"/>
-      <c r="W32" s="6"/>
-      <c r="X32" s="6"/>
-    </row>
-    <row r="37" spans="13:24" x14ac:dyDescent="0.25">
-      <c r="M37" s="9"/>
-      <c r="N37" s="9"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="8"/>
-      <c r="R37" s="8"/>
-      <c r="S37" s="9"/>
-      <c r="T37" s="9"/>
-      <c r="U37" s="9"/>
-      <c r="V37" s="9"/>
-      <c r="W37" s="9"/>
-      <c r="X37" s="9"/>
-    </row>
-    <row r="38" spans="13:24" x14ac:dyDescent="0.25">
-      <c r="M38" s="9"/>
-      <c r="N38" s="9"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
-      <c r="Q38" s="8"/>
-      <c r="R38" s="8"/>
-      <c r="S38" s="9"/>
-      <c r="T38" s="9"/>
-      <c r="U38" s="9"/>
-      <c r="V38" s="9"/>
-      <c r="W38" s="9"/>
-      <c r="X38" s="9"/>
-    </row>
-    <row r="39" spans="13:24" x14ac:dyDescent="0.25">
-      <c r="M39" s="9"/>
-      <c r="N39" s="9"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="16"/>
-      <c r="R39" s="16"/>
-      <c r="S39" s="9"/>
-      <c r="T39" s="9"/>
-      <c r="U39" s="9"/>
-      <c r="V39" s="9"/>
-      <c r="W39" s="9"/>
-      <c r="X39" s="9"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="10"/>
+      <c r="Y20" s="10"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="K28" s="8"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="K29" s="8"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="8"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="K30" s="8"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
     </row>
   </sheetData>
-  <dataValidations xWindow="382" yWindow="552" count="4">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y5:Z5">
-      <formula1>0</formula1>
-      <formula2>100000000000000000000</formula2>
-    </dataValidation>
+  <dataValidations xWindow="382" yWindow="552" count="3">
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:H14 Y3:Y4 E37:X39 E2:X3 E5:X5">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:H5 E28:R30">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -3684,18 +3386,12 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="382" yWindow="552" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B5</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="382" yWindow="552" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>[1]dropdown_lists!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>B14</xm:sqref>
+          <xm:sqref>B5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Very rough calibration for Bulgaria
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="99">
   <si>
     <t>parameter</t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>demo_household_size</t>
-  </si>
-  <si>
-    <t>program_prop_child_reporting</t>
   </si>
   <si>
     <t>age_breakpoints</t>
@@ -2229,7 +2226,7 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -2259,14 +2256,14 @@
         <v>2</v>
       </c>
       <c r="B2" s="13">
-        <v>15</v>
+        <v>15.9</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="18">
         <v>2</v>
@@ -2276,7 +2273,7 @@
     </row>
     <row r="4" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" s="18">
         <v>1920</v>
@@ -2286,7 +2283,7 @@
     </row>
     <row r="5" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="18">
         <v>1920</v>
@@ -2309,112 +2306,110 @@
         <v>23</v>
       </c>
       <c r="B7" s="16">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="C7" s="14">
+        <v>15</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
     </row>
     <row r="8" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="16">
-        <v>5</v>
-      </c>
-      <c r="C8" s="14">
-        <v>15</v>
-      </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-    </row>
-    <row r="9" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="23">
+        <v>10000000</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="23">
-        <v>10000000</v>
-      </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+        <v>22</v>
+      </c>
+      <c r="B9" s="19">
+        <v>2.4</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="19">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="16">
+      <c r="A10" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="16">
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="13">
+    <row r="11" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="13">
         <f>20/12</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="17"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="17"/>
+    </row>
+    <row r="12" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="16">
+        <v>0.4</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="17" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="13" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B13" s="16">
-        <v>0.4</v>
+        <v>0.89</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="16">
-        <v>0.89</v>
-      </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="24">
+        <v>1950</v>
+      </c>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
       <c r="E14" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B15" s="24">
-        <v>1940</v>
+        <v>1960</v>
       </c>
       <c r="C15" s="24"/>
       <c r="D15" s="24"/>
       <c r="E15" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="24">
-        <v>1950</v>
-      </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="17" t="s">
+      <c r="A16" s="17" t="s">
         <v>43</v>
+      </c>
+      <c r="B16" s="19">
+        <v>1990</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2422,7 +2417,7 @@
         <v>44</v>
       </c>
       <c r="B17" s="19">
-        <v>2010</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2430,15 +2425,18 @@
         <v>45</v>
       </c>
       <c r="B18" s="19">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B19" s="19">
-        <v>13</v>
+        <v>92</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2446,10 +2444,7 @@
         <v>56</v>
       </c>
       <c r="B20" s="19">
-        <v>92</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>71</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2473,7 +2468,7 @@
         <v>59</v>
       </c>
       <c r="B23" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2481,7 +2476,10 @@
         <v>60</v>
       </c>
       <c r="B24" s="19">
-        <v>1</v>
+        <v>857</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2489,10 +2487,7 @@
         <v>61</v>
       </c>
       <c r="B25" s="19">
-        <v>857</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>71</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2516,15 +2511,19 @@
         <v>64</v>
       </c>
       <c r="B28" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="19">
-        <v>1</v>
+      <c r="B29" s="17">
+        <f>1.02+67.12</f>
+        <v>68.14</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2532,11 +2531,7 @@
         <v>66</v>
       </c>
       <c r="B30" s="17">
-        <f>1.02+67.12</f>
-        <v>68.14</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2544,7 +2539,10 @@
         <v>67</v>
       </c>
       <c r="B31" s="17">
-        <v>0</v>
+        <v>8028</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2552,10 +2550,7 @@
         <v>68</v>
       </c>
       <c r="B32" s="17">
-        <v>8028</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>73</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2568,10 +2563,14 @@
     </row>
     <row r="34" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="B34" s="17">
-        <v>1</v>
+        <f>1.02+67.12</f>
+        <v>68.14</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2579,11 +2578,7 @@
         <v>83</v>
       </c>
       <c r="B35" s="17">
-        <f>1.02+67.12</f>
-        <v>68.14</v>
-      </c>
-      <c r="E35" s="14" t="s">
-        <v>72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2591,7 +2586,10 @@
         <v>84</v>
       </c>
       <c r="B36" s="17">
-        <v>0</v>
+        <v>8028</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2599,10 +2597,7 @@
         <v>85</v>
       </c>
       <c r="B37" s="17">
-        <v>8028</v>
-      </c>
-      <c r="E37" s="14" t="s">
-        <v>73</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2613,27 +2608,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B39" s="17">
-        <v>1</v>
+        <v>73</v>
+      </c>
+      <c r="B39" s="25">
+        <v>6094</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="25">
-        <v>6094</v>
+      <c r="B40" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B41" s="17">
+      <c r="B41" s="26">
         <v>0</v>
       </c>
     </row>
@@ -2641,7 +2636,7 @@
       <c r="A42" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B42" s="26">
+      <c r="B42" s="17">
         <v>0</v>
       </c>
     </row>
@@ -2650,15 +2645,15 @@
         <v>77</v>
       </c>
       <c r="B43" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B44" s="17">
-        <v>0.9</v>
+        <v>751</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2666,7 +2661,7 @@
         <v>89</v>
       </c>
       <c r="B45" s="17">
-        <v>751</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2690,15 +2685,15 @@
         <v>92</v>
       </c>
       <c r="B48" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
         <v>93</v>
       </c>
       <c r="B49" s="17">
-        <v>1</v>
+        <v>862</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2706,7 +2701,7 @@
         <v>94</v>
       </c>
       <c r="B50" s="17">
-        <v>862</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2730,20 +2725,12 @@
         <v>97</v>
       </c>
       <c r="B53" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="B54" s="17">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9 F9:G9 B3">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8 F8:G8 B3">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
@@ -2751,12 +2738,12 @@
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:G8 B6:B7">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6 F6:G7">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age unstratified" prompt="Some values you can replace the ones to the left with if you want a manual calibration for the model without age stratification." sqref="H1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15:D16 B4:B5">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14:D15 B4:B5">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
@@ -2764,7 +2751,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B12" unlockedFormula="1"/>
+    <ignoredError sqref="B11" unlockedFormula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2880,18 +2867,18 @@
         <v>16</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="AA1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>4</v>
@@ -2910,7 +2897,7 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>4</v>
@@ -2924,7 +2911,7 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>4</v>
@@ -2939,7 +2926,7 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>
@@ -2985,7 +2972,7 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>3</v>
@@ -3003,7 +2990,7 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>3</v>
@@ -3025,7 +3012,7 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>3</v>
@@ -3047,7 +3034,7 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>3</v>
@@ -3068,7 +3055,7 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>4</v>
@@ -3092,7 +3079,7 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>4</v>
@@ -3110,7 +3097,7 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>4</v>
@@ -3181,7 +3168,7 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>4</v>
@@ -3192,7 +3179,7 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>3</v>
@@ -3215,7 +3202,7 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>3</v>
@@ -3229,7 +3216,7 @@
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>4</v>
@@ -3248,7 +3235,7 @@
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>3</v>
@@ -3272,7 +3259,7 @@
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>3</v>
@@ -3297,7 +3284,7 @@
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Extend automatic calibration to MDR-TB
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="100">
   <si>
     <t>parameter</t>
   </si>
@@ -316,6 +316,9 @@
   </si>
   <si>
     <t>int_perc_ambulatorycare_extrapul</t>
+  </si>
+  <si>
+    <t>tb_perc_mdr_prevalence</t>
   </si>
 </sst>
 </file>
@@ -2226,10 +2229,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2292,164 +2295,166 @@
       <c r="G5" s="13"/>
     </row>
     <row r="6" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="16">
-        <v>0.36</v>
-      </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
+      <c r="A6" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="18">
+        <v>1.2</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
     </row>
     <row r="7" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B7" s="16">
-        <v>5</v>
-      </c>
-      <c r="C7" s="14">
-        <v>15</v>
+        <v>0.36</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
     </row>
     <row r="8" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="16">
+        <v>5</v>
+      </c>
+      <c r="C8" s="14">
+        <v>15</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+    </row>
+    <row r="9" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="23">
+      <c r="B9" s="23">
         <v>10000000</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B10" s="19">
         <v>2.4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B11" s="16">
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+    <row r="12" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B12" s="13">
         <f>20/12</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="17"/>
-    </row>
-    <row r="12" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="16">
-        <v>0.4</v>
-      </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="17" t="s">
-        <v>36</v>
-      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="17"/>
     </row>
     <row r="13" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" s="16">
-        <v>0.89</v>
+        <v>0.4</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="16">
+        <v>0.89</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="17" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="24">
-        <v>1950</v>
-      </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="17" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B15" s="24">
-        <v>1960</v>
+        <v>1950</v>
       </c>
       <c r="C15" s="24"/>
       <c r="D15" s="24"/>
       <c r="E15" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="24">
+        <v>1960</v>
+      </c>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="17" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="19">
-        <v>1990</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="19">
-        <v>6</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" s="19">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B19" s="19">
-        <v>92</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>70</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B20" s="19">
-        <v>0</v>
+        <v>92</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="19">
         <v>0</v>
@@ -2457,7 +2462,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B22" s="19">
         <v>0</v>
@@ -2465,34 +2470,34 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" s="19">
-        <v>857</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>70</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" s="19">
-        <v>0</v>
+        <v>857</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B26" s="19">
         <v>0</v>
@@ -2500,7 +2505,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B27" s="19">
         <v>0</v>
@@ -2508,54 +2513,54 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="19">
+      <c r="B29" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
+    <row r="30" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="17">
+      <c r="B30" s="17">
         <f>1.02+67.12</f>
         <v>68.14</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="E30" s="14" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="17">
-        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B31" s="17">
-        <v>8028</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B32" s="17">
-        <v>1</v>
+        <v>8028</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B33" s="17">
         <v>1</v>
@@ -2563,110 +2568,110 @@
     </row>
     <row r="34" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B34" s="17">
+      <c r="B35" s="17">
         <f>1.02+67.12</f>
         <v>68.14</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E35" s="14" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="B35" s="17">
-        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B36" s="17">
-        <v>8028</v>
-      </c>
-      <c r="E36" s="14" t="s">
-        <v>72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B37" s="17">
-        <v>1</v>
+        <v>8028</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B38" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B39" s="25">
-        <v>6094</v>
+        <v>86</v>
+      </c>
+      <c r="B39" s="17">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="B40" s="17">
-        <v>0</v>
+        <v>73</v>
+      </c>
+      <c r="B40" s="25">
+        <v>6094</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="B41" s="26">
+        <v>74</v>
+      </c>
+      <c r="B41" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="B42" s="17">
+        <v>75</v>
+      </c>
+      <c r="B42" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="B43" s="17">
+      <c r="B44" s="17">
         <v>0.9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="B44" s="17">
-        <v>751</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B45" s="17">
-        <v>0</v>
+        <v>751</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B46" s="17">
         <v>0</v>
@@ -2674,7 +2679,7 @@
     </row>
     <row r="47" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B47" s="17">
         <v>0</v>
@@ -2682,31 +2687,31 @@
     </row>
     <row r="48" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="B48" s="17">
+      <c r="B49" s="17">
         <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="B49" s="17">
-        <v>862</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B50" s="17">
-        <v>0</v>
+        <v>862</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B51" s="17">
         <v>0</v>
@@ -2714,7 +2719,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B52" s="17">
         <v>0</v>
@@ -2722,28 +2727,36 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B53" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="B53" s="17">
+      <c r="B54" s="17">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8 F8:G8 B3">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9 F9:G9 B3">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 F2:G5">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 F2:G6">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6 F6:G7">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7 F7:G8">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age unstratified" prompt="Some values you can replace the ones to the left with if you want a manual calibration for the model without age stratification." sqref="H1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14:D15 B4:B5">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15:D16 B4:B6">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
@@ -2751,7 +2764,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B11" unlockedFormula="1"/>
+    <ignoredError sqref="B12" unlockedFormula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Bulgaria mixing matrix and parameter adjustments
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -14,12 +14,12 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="99">
   <si>
     <t>parameter</t>
   </si>
@@ -313,6 +313,9 @@
   </si>
   <si>
     <t>mdr_introduce_time</t>
+  </si>
+  <si>
+    <t>prop_mix_ruralpoor_from_ruralpoor</t>
   </si>
 </sst>
 </file>
@@ -2223,10 +2226,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2253,7 +2256,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="13">
-        <v>15.9</v>
+        <v>11</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -2424,26 +2427,26 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="B19" s="19">
-        <v>92</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>67</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="19">
-        <v>0</v>
+        <v>92</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" s="19">
         <v>0</v>
@@ -2451,7 +2454,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" s="19">
         <v>0</v>
@@ -2459,34 +2462,34 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24" s="19">
-        <v>857</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>67</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25" s="19">
-        <v>0</v>
+        <v>857</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B26" s="19">
         <v>0</v>
@@ -2494,7 +2497,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="19">
         <v>0</v>
@@ -2502,54 +2505,54 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="19">
+      <c r="B29" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
+    <row r="30" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="17">
+      <c r="B30" s="17">
         <f>1.02+67.12</f>
         <v>68.14</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="E30" s="14" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B30" s="17">
-        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B31" s="17">
-        <v>8028</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B32" s="17">
-        <v>1</v>
+        <v>8028</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B33" s="17">
         <v>1</v>
@@ -2557,110 +2560,110 @@
     </row>
     <row r="34" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="17">
+      <c r="B35" s="17">
         <f>1.02+67.12</f>
         <v>68.14</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E35" s="14" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B35" s="17">
-        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B36" s="17">
-        <v>8028</v>
-      </c>
-      <c r="E36" s="14" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B37" s="17">
-        <v>1</v>
+        <v>8028</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B38" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B39" s="25">
-        <v>6094</v>
+        <v>83</v>
+      </c>
+      <c r="B39" s="17">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B40" s="17">
-        <v>0</v>
+        <v>70</v>
+      </c>
+      <c r="B40" s="25">
+        <v>6094</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="B41" s="26">
+        <v>71</v>
+      </c>
+      <c r="B41" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B42" s="17">
+        <v>72</v>
+      </c>
+      <c r="B42" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="17">
+      <c r="B44" s="17">
         <v>0.9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="B44" s="17">
-        <v>751</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B45" s="17">
-        <v>0</v>
+        <v>751</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B46" s="17">
         <v>0</v>
@@ -2668,7 +2671,7 @@
     </row>
     <row r="47" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B47" s="17">
         <v>0</v>
@@ -2676,31 +2679,31 @@
     </row>
     <row r="48" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="B48" s="17">
+      <c r="B49" s="17">
         <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B49" s="17">
-        <v>862</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B50" s="17">
-        <v>0</v>
+        <v>862</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B51" s="17">
         <v>0</v>
@@ -2708,7 +2711,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B52" s="17">
         <v>0</v>
@@ -2716,9 +2719,17 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B53" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B53" s="17">
+      <c r="B54" s="17">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove epi_rr_diabetes from Bulgaria sheet (old terminology)
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="99">
   <si>
     <t>parameter</t>
   </si>
@@ -120,9 +120,6 @@
     <t>scenario_9</t>
   </si>
   <si>
-    <t>epi_rr_diabetes</t>
-  </si>
-  <si>
     <t>tb_timeperiod_ontreatment_mdr</t>
   </si>
   <si>
@@ -316,6 +313,9 @@
   </si>
   <si>
     <t>prop_mix_ruralpoor_from_ruralpoor</t>
+  </si>
+  <si>
+    <t>prop_mix_diabetes_from_diabetes</t>
   </si>
 </sst>
 </file>
@@ -2226,10 +2226,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2263,7 +2263,7 @@
     </row>
     <row r="3" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="18">
         <v>2</v>
@@ -2273,7 +2273,7 @@
     </row>
     <row r="4" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="18">
         <v>1920</v>
@@ -2283,7 +2283,7 @@
     </row>
     <row r="5" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="18">
         <v>1920</v>
@@ -2293,7 +2293,7 @@
     </row>
     <row r="6" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" s="18">
         <v>1.2</v>
@@ -2352,7 +2352,7 @@
     </row>
     <row r="12" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="13">
         <f>20/12</f>
@@ -2364,7 +2364,7 @@
     </row>
     <row r="13" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="16">
         <v>0.4</v>
@@ -2372,12 +2372,12 @@
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="16">
         <v>0.89</v>
@@ -2385,12 +2385,12 @@
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B15" s="24">
         <v>1950</v>
@@ -2398,12 +2398,12 @@
       <c r="C15" s="24"/>
       <c r="D15" s="24"/>
       <c r="E15" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="19">
         <v>1990</v>
@@ -2411,7 +2411,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="19">
         <v>6</v>
@@ -2419,7 +2419,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="19">
         <v>13</v>
@@ -2427,7 +2427,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B19" s="19">
         <v>0.6</v>
@@ -2435,26 +2435,26 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="B20" s="19">
-        <v>92</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>67</v>
+        <v>5.3999999999999999E-2</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B21" s="19">
-        <v>0</v>
+        <v>92</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B22" s="19">
         <v>0</v>
@@ -2462,7 +2462,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B23" s="19">
         <v>0</v>
@@ -2470,34 +2470,34 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B24" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B25" s="19">
-        <v>857</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>67</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B26" s="19">
-        <v>0</v>
+        <v>857</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B27" s="19">
         <v>0</v>
@@ -2505,7 +2505,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B28" s="19">
         <v>0</v>
@@ -2513,54 +2513,54 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30" s="17">
+      <c r="B31" s="17">
         <f>1.02+67.12</f>
         <v>68.14</v>
       </c>
-      <c r="E30" s="14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" s="17">
-        <v>0</v>
+      <c r="E31" s="14" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B32" s="17">
-        <v>8028</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B33" s="17">
-        <v>1</v>
+        <v>8028</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B34" s="17">
         <v>1</v>
@@ -2568,110 +2568,110 @@
     </row>
     <row r="35" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B35" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="17">
         <f>1.02+67.12</f>
         <v>68.14</v>
       </c>
-      <c r="E35" s="14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B36" s="17">
-        <v>0</v>
+      <c r="E36" s="14" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B37" s="17">
-        <v>8028</v>
-      </c>
-      <c r="E37" s="14" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B38" s="17">
-        <v>1</v>
+        <v>8028</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B39" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B40" s="25">
-        <v>6094</v>
+        <v>82</v>
+      </c>
+      <c r="B40" s="17">
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B41" s="17">
-        <v>0</v>
+        <v>69</v>
+      </c>
+      <c r="B41" s="25">
+        <v>6094</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="B42" s="26">
+        <v>70</v>
+      </c>
+      <c r="B42" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B43" s="17">
+        <v>71</v>
+      </c>
+      <c r="B43" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B44" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B45" s="17">
         <v>0.9</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="B45" s="17">
-        <v>751</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B46" s="17">
-        <v>0</v>
+        <v>751</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B47" s="17">
         <v>0</v>
@@ -2679,7 +2679,7 @@
     </row>
     <row r="48" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B48" s="17">
         <v>0</v>
@@ -2687,31 +2687,31 @@
     </row>
     <row r="49" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B49" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="17">
         <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B50" s="17">
-        <v>862</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B51" s="17">
-        <v>0</v>
+        <v>862</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B52" s="17">
         <v>0</v>
@@ -2719,7 +2719,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B53" s="17">
         <v>0</v>
@@ -2727,9 +2727,17 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B54" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B55" s="17">
         <v>1</v>
       </c>
     </row>
@@ -2766,13 +2774,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AA30"/>
+  <dimension ref="A1:AA29"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2883,7 +2891,7 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>4</v>
@@ -2902,7 +2910,7 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>4</v>
@@ -2916,7 +2924,7 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>4</v>
@@ -2931,7 +2939,7 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>
@@ -2977,7 +2985,7 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>3</v>
@@ -2995,7 +3003,7 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>3</v>
@@ -3017,7 +3025,7 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>3</v>
@@ -3039,7 +3047,7 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>3</v>
@@ -3060,7 +3068,7 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>4</v>
@@ -3084,7 +3092,7 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>4</v>
@@ -3102,7 +3110,7 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>4</v>
@@ -3173,7 +3181,7 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>4</v>
@@ -3188,9 +3196,6 @@
       </c>
       <c r="B15" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="I15" s="6">
-        <v>1</v>
       </c>
       <c r="L15" s="6">
         <v>5.4</v>
@@ -3287,50 +3292,31 @@
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20" s="5">
-        <v>1</v>
-      </c>
-      <c r="F20" s="6">
-        <v>1</v>
-      </c>
-      <c r="G20" s="6">
-        <v>1</v>
-      </c>
-      <c r="H20" s="6">
-        <v>3.11</v>
-      </c>
-      <c r="Q20" s="6">
-        <v>3.11</v>
-      </c>
-      <c r="T20" s="10"/>
-      <c r="U20" s="10"/>
-      <c r="V20" s="10"/>
-      <c r="W20" s="10"/>
-      <c r="X20" s="10"/>
-      <c r="Y20" s="10"/>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="K27" s="8"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8"/>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="K28" s="8"/>
@@ -3352,20 +3338,10 @@
       <c r="Q29" s="8"/>
       <c r="R29" s="8"/>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="K30" s="8"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-    </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="3">
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:H5 E28:R30">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:H5 E27:R29">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Clean up Bulgaria spreadsheet
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rragonnet\Google Drive\GitHub\AuTuMN\autumn\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="612" windowWidth="16272" windowHeight="6300" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -14,12 +19,12 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="94">
   <si>
     <t>parameter</t>
   </si>
@@ -252,24 +257,6 @@
     <t>early_time</t>
   </si>
   <si>
-    <t>int_perc_bulgaria_improve_dst</t>
-  </si>
-  <si>
-    <t>econ_unitcost_bulgaria_improve_dst</t>
-  </si>
-  <si>
-    <t>econ_inflectioncost_bulgaria_improve_dst</t>
-  </si>
-  <si>
-    <t>econ_startupcost_bulgaria_improve_dst</t>
-  </si>
-  <si>
-    <t>econ_startupduration_bulgaria_improve_dst</t>
-  </si>
-  <si>
-    <t>econ_saturation_bulgaria_improve_dst</t>
-  </si>
-  <si>
     <t>int_perc_ambulatorycare_smearneg</t>
   </si>
   <si>
@@ -316,6 +303,9 @@
   </si>
   <si>
     <t>prop_mix_diabetes_from_diabetes</t>
+  </si>
+  <si>
+    <t>int_perc_improve_dst</t>
   </si>
 </sst>
 </file>
@@ -1979,7 +1969,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2014,7 +2004,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2226,24 +2216,24 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.28515625" style="17" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="19" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="17"/>
-    <col min="6" max="6" width="13.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="17"/>
+    <col min="1" max="1" width="47.33203125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="19" customWidth="1"/>
+    <col min="3" max="5" width="9.109375" style="17"/>
+    <col min="6" max="6" width="13.88671875" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2251,7 +2241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
@@ -2261,7 +2251,7 @@
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
     </row>
-    <row r="3" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>74</v>
       </c>
@@ -2271,7 +2261,7 @@
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
     </row>
-    <row r="4" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>75</v>
       </c>
@@ -2281,7 +2271,7 @@
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
     </row>
-    <row r="5" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>76</v>
       </c>
@@ -2291,9 +2281,9 @@
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
     </row>
-    <row r="6" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B6" s="18">
         <v>1.2</v>
@@ -2301,7 +2291,7 @@
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
     </row>
-    <row r="7" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>11</v>
       </c>
@@ -2311,7 +2301,7 @@
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
     </row>
-    <row r="8" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>23</v>
       </c>
@@ -2324,7 +2314,7 @@
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
     </row>
-    <row r="9" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>12</v>
       </c>
@@ -2334,7 +2324,7 @@
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>22</v>
       </c>
@@ -2342,7 +2332,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>26</v>
       </c>
@@ -2350,7 +2340,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>33</v>
       </c>
@@ -2362,7 +2352,7 @@
       <c r="D12" s="13"/>
       <c r="E12" s="17"/>
     </row>
-    <row r="13" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>34</v>
       </c>
@@ -2375,7 +2365,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>36</v>
       </c>
@@ -2388,9 +2378,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B15" s="24">
         <v>1950</v>
@@ -2401,7 +2391,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>39</v>
       </c>
@@ -2409,7 +2399,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>40</v>
       </c>
@@ -2417,7 +2407,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>41</v>
       </c>
@@ -2425,23 +2415,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B19" s="19">
         <v>0.6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B20" s="19">
         <v>5.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>51</v>
       </c>
@@ -2452,7 +2442,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>52</v>
       </c>
@@ -2460,7 +2450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>53</v>
       </c>
@@ -2468,7 +2458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
         <v>54</v>
       </c>
@@ -2476,7 +2466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
         <v>55</v>
       </c>
@@ -2484,7 +2474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
         <v>56</v>
       </c>
@@ -2495,7 +2485,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="17" t="s">
         <v>57</v>
       </c>
@@ -2503,7 +2493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
         <v>58</v>
       </c>
@@ -2511,7 +2501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
         <v>59</v>
       </c>
@@ -2519,7 +2509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
         <v>60</v>
       </c>
@@ -2527,7 +2517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
         <v>61</v>
       </c>
@@ -2539,7 +2529,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="17" t="s">
         <v>62</v>
       </c>
@@ -2547,7 +2537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
         <v>63</v>
       </c>
@@ -2558,7 +2548,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="17" t="s">
         <v>64</v>
       </c>
@@ -2566,7 +2556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
         <v>65</v>
       </c>
@@ -2574,170 +2564,123 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="B36" s="17">
-        <f>1.02+67.12</f>
-        <v>68.14</v>
-      </c>
-      <c r="E36" s="14" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="B36" s="25">
+        <v>6094</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B37" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B38" s="17">
-        <v>8028</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="B38" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B39" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B40" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B41" s="25">
-        <v>6094</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="B41" s="17">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B42" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B43" s="26">
+        <v>80</v>
+      </c>
+      <c r="B43" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B44" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="17" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B45" s="17">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" s="17">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="17" t="s">
         <v>84</v>
-      </c>
-      <c r="B46" s="17">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="17" t="s">
-        <v>85</v>
       </c>
       <c r="B47" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B48" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B49" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B50" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="B51" s="17">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B52" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="B53" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="B54" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="B55" s="17">
         <v>1</v>
       </c>
     </row>
@@ -2776,37 +2719,37 @@
   </sheetPr>
   <dimension ref="A1:AA29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="57.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="57.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="11" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="4" customWidth="1"/>
     <col min="4" max="4" width="11" style="5" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" style="6" customWidth="1"/>
-    <col min="7" max="8" width="7.28515625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="7.140625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" style="6" customWidth="1"/>
+    <col min="7" max="8" width="7.33203125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="7.109375" style="6" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5546875" style="6" customWidth="1"/>
     <col min="12" max="13" width="7" style="6" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="6" customWidth="1"/>
-    <col min="15" max="16" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="7.85546875" style="6" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" style="6" customWidth="1"/>
+    <col min="15" max="16" width="7.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="7.88671875" style="6" customWidth="1"/>
     <col min="19" max="19" width="14" style="6" customWidth="1"/>
-    <col min="20" max="21" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="14.42578125" style="6" customWidth="1"/>
-    <col min="25" max="27" width="15.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="9.140625" style="6"/>
+    <col min="20" max="21" width="14.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="14.44140625" style="6" customWidth="1"/>
+    <col min="25" max="27" width="15.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>6</v>
       </c>
@@ -2889,7 +2832,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>43</v>
       </c>
@@ -2908,7 +2851,7 @@
       </c>
       <c r="V2" s="10"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>44</v>
       </c>
@@ -2922,7 +2865,7 @@
       <c r="U3" s="10"/>
       <c r="V3" s="10"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>45</v>
       </c>
@@ -2937,7 +2880,7 @@
       <c r="V4" s="10"/>
       <c r="W4" s="10"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
         <v>46</v>
       </c>
@@ -2983,9 +2926,9 @@
         <v>37.686746987951807</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>3</v>
@@ -2994,14 +2937,14 @@
         <v>80</v>
       </c>
       <c r="T6" s="10">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="U6" s="10"/>
       <c r="V6" s="10"/>
       <c r="X6" s="10"/>
       <c r="Y6" s="10"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>47</v>
       </c>
@@ -3015,7 +2958,7 @@
         <v>50</v>
       </c>
       <c r="S7" s="6">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="T7" s="10"/>
       <c r="U7" s="10"/>
@@ -3023,7 +2966,7 @@
       <c r="X7" s="10"/>
       <c r="Y7" s="10"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
         <v>48</v>
       </c>
@@ -3031,13 +2974,13 @@
         <v>3</v>
       </c>
       <c r="M8" s="6">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="R8" s="6">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="S8" s="6">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="T8" s="10"/>
       <c r="U8" s="10"/>
@@ -3045,7 +2988,7 @@
       <c r="X8" s="10"/>
       <c r="Y8" s="10"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
         <v>49</v>
       </c>
@@ -3066,7 +3009,7 @@
       <c r="X9" s="10"/>
       <c r="Y9" s="10"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
         <v>50</v>
       </c>
@@ -3081,18 +3024,16 @@
       </c>
       <c r="T10" s="10"/>
       <c r="U10" s="10"/>
-      <c r="V10" s="10">
-        <v>0</v>
-      </c>
+      <c r="V10" s="10"/>
       <c r="W10" s="10">
         <v>0</v>
       </c>
       <c r="X10" s="10"/>
       <c r="Y10" s="10"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>4</v>
@@ -3108,9 +3049,9 @@
       </c>
       <c r="Y11" s="10"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>4</v>
@@ -3126,7 +3067,7 @@
       </c>
       <c r="Y12" s="10"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
         <v>21</v>
       </c>
@@ -3179,7 +3120,7 @@
         <v>117.42738589211601</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>42</v>
       </c>
@@ -3190,7 +3131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
         <v>27</v>
       </c>
@@ -3210,7 +3151,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
         <v>28</v>
       </c>
@@ -3224,7 +3165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
         <v>29</v>
       </c>
@@ -3243,7 +3184,7 @@
         <v>2.295918367346939</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
         <v>30</v>
       </c>
@@ -3267,7 +3208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="21" t="s">
         <v>31</v>
       </c>
@@ -3292,7 +3233,7 @@
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
@@ -3308,7 +3249,7 @@
       <c r="Q22" s="5"/>
       <c r="R22" s="5"/>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="K27" s="8"/>
       <c r="L27" s="7"/>
       <c r="M27" s="8"/>
@@ -3318,7 +3259,7 @@
       <c r="Q27" s="8"/>
       <c r="R27" s="8"/>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="K28" s="8"/>
       <c r="L28" s="7"/>
       <c r="M28" s="8"/>
@@ -3328,7 +3269,7 @@
       <c r="Q28" s="8"/>
       <c r="R28" s="8"/>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="K29" s="8"/>
       <c r="L29" s="7"/>
       <c r="M29" s="8"/>
@@ -3378,9 +3319,9 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3394,7 +3335,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3405,7 +3346,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Edit spreadsheets to include "improve_dst_culturepos" intervention
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="612" windowWidth="16272" windowHeight="6300" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="612" windowWidth="16272" windowHeight="6300" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -209,21 +209,6 @@
     <t>econ_saturation_food_voucher_mdr</t>
   </si>
   <si>
-    <t>econ_unitcost_improve_dst</t>
-  </si>
-  <si>
-    <t>econ_inflectioncost_improve_dst</t>
-  </si>
-  <si>
-    <t>econ_startupcost_improve_dst</t>
-  </si>
-  <si>
-    <t>econ_startupduration_improve_dst</t>
-  </si>
-  <si>
-    <t>econ_saturation_improve_dst</t>
-  </si>
-  <si>
     <t>Months of treatment x 4 weeks x 10 BNG per week x EUR exchange rate x treatment success rate</t>
   </si>
   <si>
@@ -305,7 +290,22 @@
     <t>prop_mix_diabetes_from_diabetes</t>
   </si>
   <si>
-    <t>int_perc_improve_dst</t>
+    <t>int_perc_improve_dst_culturepos</t>
+  </si>
+  <si>
+    <t>econ_unitcost_improve_dst_culturepos</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_improve_dst_culturepos</t>
+  </si>
+  <si>
+    <t>econ_startupcost_improve_dst_culturepos</t>
+  </si>
+  <si>
+    <t>econ_startupduration_improve_dst_culturepos</t>
+  </si>
+  <si>
+    <t>econ_saturation_improve_dst_culturepos</t>
   </si>
 </sst>
 </file>
@@ -2218,7 +2218,7 @@
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
@@ -2253,7 +2253,7 @@
     </row>
     <row r="3" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B3" s="18">
         <v>2</v>
@@ -2263,7 +2263,7 @@
     </row>
     <row r="4" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B4" s="18">
         <v>1920</v>
@@ -2273,7 +2273,7 @@
     </row>
     <row r="5" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B5" s="18">
         <v>1920</v>
@@ -2283,7 +2283,7 @@
     </row>
     <row r="6" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B6" s="18">
         <v>1.2</v>
@@ -2380,7 +2380,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B15" s="24">
         <v>1950</v>
@@ -2417,7 +2417,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B19" s="19">
         <v>0.6</v>
@@ -2425,7 +2425,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B20" s="19">
         <v>5.3999999999999999E-2</v>
@@ -2439,7 +2439,7 @@
         <v>92</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -2482,7 +2482,7 @@
         <v>857</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -2519,19 +2519,19 @@
     </row>
     <row r="31" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="B31" s="17">
         <f>1.02+67.12</f>
         <v>68.14</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="17" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="B32" s="17">
         <v>0</v>
@@ -2539,18 +2539,18 @@
     </row>
     <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="B33" s="17">
         <v>8028</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="17" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="B34" s="17">
         <v>1</v>
@@ -2558,7 +2558,7 @@
     </row>
     <row r="35" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="B35" s="17">
         <v>1</v>
@@ -2566,7 +2566,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B36" s="25">
         <v>6094</v>
@@ -2574,7 +2574,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B37" s="17">
         <v>0</v>
@@ -2582,7 +2582,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="17" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B38" s="26">
         <v>0</v>
@@ -2590,7 +2590,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B39" s="17">
         <v>0</v>
@@ -2598,7 +2598,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B40" s="17">
         <v>0.9</v>
@@ -2606,7 +2606,7 @@
     </row>
     <row r="41" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B41" s="17">
         <v>751</v>
@@ -2614,7 +2614,7 @@
     </row>
     <row r="42" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B42" s="17">
         <v>0</v>
@@ -2622,7 +2622,7 @@
     </row>
     <row r="43" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B43" s="17">
         <v>0</v>
@@ -2630,7 +2630,7 @@
     </row>
     <row r="44" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B44" s="17">
         <v>0</v>
@@ -2638,7 +2638,7 @@
     </row>
     <row r="45" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="17" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B45" s="17">
         <v>1</v>
@@ -2646,7 +2646,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="17" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B46" s="17">
         <v>862</v>
@@ -2654,7 +2654,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="17" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B47" s="17">
         <v>0</v>
@@ -2662,7 +2662,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="17" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B48" s="17">
         <v>0</v>
@@ -2670,7 +2670,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="17" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B49" s="17">
         <v>0</v>
@@ -2678,7 +2678,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="17" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B50" s="17">
         <v>1</v>
@@ -2719,11 +2719,11 @@
   </sheetPr>
   <dimension ref="A1:AA29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2928,7 +2928,7 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>3</v>
@@ -3033,7 +3033,7 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>4</v>
@@ -3051,7 +3051,7 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Revise short-course MDR-TB treatment code
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rragonnet\Google Drive\GitHub\AuTuMN\autumn\xls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="612" windowWidth="16272" windowHeight="6300" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -19,12 +14,12 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="93">
   <si>
     <t>parameter</t>
   </si>
@@ -113,9 +108,6 @@
     <t>riskgroup_perc_prison</t>
   </si>
   <si>
-    <t>riskgroup_perc_urbanpoor</t>
-  </si>
-  <si>
     <t>riskgroup_perc_ruralpoor</t>
   </si>
   <si>
@@ -152,9 +144,6 @@
     <t>riskgroup_multiplier_force_infection_prison</t>
   </si>
   <si>
-    <t>riskgroup_perc_hiv</t>
-  </si>
-  <si>
     <t>int_perc_shortcourse_mdr</t>
   </si>
   <si>
@@ -287,9 +276,6 @@
     <t>prop_mix_ruralpoor_from_ruralpoor</t>
   </si>
   <si>
-    <t>prop_mix_diabetes_from_diabetes</t>
-  </si>
-  <si>
     <t>int_perc_improve_dst</t>
   </si>
   <si>
@@ -306,6 +292,12 @@
   </si>
   <si>
     <t>econ_unitcost_improve_dst</t>
+  </si>
+  <si>
+    <t>prop_mix_ruralpoor_from_diabetes</t>
+  </si>
+  <si>
+    <t>prop_mix_prison_from_diabetes</t>
   </si>
 </sst>
 </file>
@@ -1224,10 +1216,10 @@
     <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="664" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="664" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="664" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="7"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="664" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="665">
     <cellStyle name="Comma" xfId="664" builtinId="3"/>
@@ -1969,7 +1961,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2004,7 +1996,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2216,24 +2208,24 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.33203125" style="17" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" style="19" customWidth="1"/>
-    <col min="3" max="5" width="9.109375" style="17"/>
-    <col min="6" max="6" width="13.88671875" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="17"/>
+    <col min="1" max="1" width="47.28515625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="18" style="19" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="17"/>
+    <col min="6" max="6" width="13.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2241,19 +2233,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="13">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
     </row>
-    <row r="3" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" s="18">
         <v>2</v>
@@ -2261,9 +2253,9 @@
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
     </row>
-    <row r="4" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B4" s="18">
         <v>1920</v>
@@ -2271,9 +2263,9 @@
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
     </row>
-    <row r="5" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B5" s="18">
         <v>1920</v>
@@ -2281,9 +2273,9 @@
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
     </row>
-    <row r="6" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B6" s="18">
         <v>1.2</v>
@@ -2291,7 +2283,7 @@
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
     </row>
-    <row r="7" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>11</v>
       </c>
@@ -2301,7 +2293,7 @@
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
     </row>
-    <row r="8" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>23</v>
       </c>
@@ -2314,7 +2306,7 @@
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
     </row>
-    <row r="9" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>12</v>
       </c>
@@ -2324,7 +2316,7 @@
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>22</v>
       </c>
@@ -2332,7 +2324,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>26</v>
       </c>
@@ -2340,9 +2332,9 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="13">
         <f>20/12</f>
@@ -2352,9 +2344,9 @@
       <c r="D12" s="13"/>
       <c r="E12" s="17"/>
     </row>
-    <row r="13" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="16">
         <v>0.4</v>
@@ -2362,12 +2354,12 @@
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
-        <v>36</v>
       </c>
       <c r="B14" s="16">
         <v>0.89</v>
@@ -2375,12 +2367,12 @@
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B15" s="24">
         <v>1950</v>
@@ -2388,299 +2380,307 @@
       <c r="C15" s="24"/>
       <c r="D15" s="24"/>
       <c r="E15" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
-        <v>39</v>
       </c>
       <c r="B16" s="19">
         <v>1990</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="19">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="19">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B19" s="19">
         <v>0.6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B20" s="19">
-        <v>5.3999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="B21" s="19">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="19">
         <v>92</v>
       </c>
-      <c r="E21" s="17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E22" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B23" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B24" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="19">
+        <v>857</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="17" t="s">
         <v>55</v>
-      </c>
-      <c r="B25" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="19">
-        <v>857</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="17" t="s">
-        <v>58</v>
       </c>
       <c r="B28" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B29" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B30" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="B31" s="17">
+    <row r="32" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="17">
         <f>1.02+67.12</f>
         <v>68.14</v>
       </c>
-      <c r="E31" s="14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="B32" s="17">
+      <c r="E32" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="B33" s="17">
+    <row r="34" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" s="17">
         <v>8028</v>
       </c>
-      <c r="E33" s="14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B34" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E34" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B35" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" s="26">
+        <v>6094</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="25">
-        <v>6094</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="17" t="s">
+      <c r="B39" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="B37" s="17">
+      <c r="B40" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="17" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B39" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40" s="17">
+      <c r="B41" s="17">
         <v>0.9</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B41" s="17">
+    <row r="42" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="17">
         <v>751</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="B42" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B43" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B44" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="17">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="17" t="s">
         <v>77</v>
-      </c>
-      <c r="B45" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="B46" s="17">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B47" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="17" t="s">
-        <v>80</v>
       </c>
       <c r="B48" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B49" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B50" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" s="17">
         <v>1</v>
       </c>
     </row>
@@ -2717,39 +2717,38 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AA29"/>
+  <dimension ref="A1:Z27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P6" sqref="P6"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="57.7109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="11" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="4" customWidth="1"/>
     <col min="4" max="4" width="11" style="5" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" style="6" customWidth="1"/>
-    <col min="7" max="8" width="7.33203125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="7.109375" style="6" customWidth="1"/>
-    <col min="10" max="10" width="7.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5546875" style="6" customWidth="1"/>
-    <col min="12" max="13" width="7" style="6" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="6" customWidth="1"/>
-    <col min="15" max="16" width="7.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="7.88671875" style="6" customWidth="1"/>
-    <col min="19" max="19" width="14" style="6" customWidth="1"/>
-    <col min="20" max="21" width="14.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="14.44140625" style="6" customWidth="1"/>
-    <col min="25" max="27" width="15.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="9.109375" style="6"/>
+    <col min="5" max="5" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" style="6" customWidth="1"/>
+    <col min="10" max="12" width="7" style="6" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="6" customWidth="1"/>
+    <col min="14" max="15" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="7.85546875" style="6" customWidth="1"/>
+    <col min="18" max="18" width="14" style="6" customWidth="1"/>
+    <col min="19" max="20" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="14.42578125" style="6" customWidth="1"/>
+    <col min="24" max="26" width="15.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>6</v>
       </c>
@@ -2766,123 +2765,123 @@
         <v>1950</v>
       </c>
       <c r="F1" s="1">
-        <v>1972</v>
+        <v>1989</v>
       </c>
       <c r="G1" s="1">
-        <v>1982</v>
+        <v>1990</v>
       </c>
       <c r="H1" s="1">
-        <v>1983</v>
+        <v>1994</v>
       </c>
       <c r="I1" s="1">
-        <v>1989</v>
+        <v>2000</v>
       </c>
       <c r="J1" s="1">
-        <v>1990</v>
+        <v>2006</v>
       </c>
       <c r="K1" s="1">
-        <v>2000</v>
+        <v>2008</v>
       </c>
       <c r="L1" s="1">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="M1" s="1">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="N1" s="1">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="O1" s="1">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="P1" s="1">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="Q1" s="1">
-        <v>2014</v>
-      </c>
-      <c r="R1" s="1">
         <v>2015</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="S1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="6">
+      <c r="Q2" s="6">
         <v>0</v>
       </c>
-      <c r="R2" s="6">
-        <v>0</v>
-      </c>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10">
+      <c r="S2" s="10"/>
+      <c r="T2" s="10">
         <v>50</v>
       </c>
-      <c r="V2" s="10"/>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="U2" s="10"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="R3" s="6">
+      <c r="L3" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="6">
         <v>70</v>
       </c>
+      <c r="S3" s="10"/>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="6">
+      <c r="L4" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="6">
         <v>70</v>
       </c>
+      <c r="S4" s="10"/>
       <c r="T4" s="10"/>
       <c r="U4" s="10"/>
       <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>
@@ -2892,105 +2891,102 @@
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="6">
+      <c r="F5" s="6">
         <v>0</v>
       </c>
-      <c r="J5" s="6">
+      <c r="G5" s="6">
         <v>5</v>
       </c>
-      <c r="M5" s="6">
+      <c r="L5" s="6">
         <f>80*(1174/2649)</f>
         <v>35.454888637221593</v>
       </c>
-      <c r="N5" s="6">
+      <c r="M5" s="6">
         <f>80*(1077/2407)</f>
         <v>35.795596177814708</v>
       </c>
-      <c r="O5" s="6">
+      <c r="N5" s="6">
         <f>80*(1094/2280)</f>
         <v>38.385964912280699</v>
       </c>
-      <c r="P5" s="6">
+      <c r="O5" s="6">
         <f>80*(961/1932)</f>
         <v>39.792960662525878</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="P5" s="6">
         <f>80*(891/1872)</f>
         <v>38.076923076923073</v>
       </c>
-      <c r="R5" s="6">
+      <c r="Q5" s="6">
         <f>80*782/1660</f>
         <v>37.686746987951807</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="R6" s="6">
+      <c r="Q6" s="6">
         <v>0</v>
       </c>
-      <c r="T6" s="10">
+      <c r="S6" s="10">
         <v>100</v>
       </c>
+      <c r="T6" s="10"/>
       <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
       <c r="X6" s="10"/>
-      <c r="Y6" s="10"/>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="M7" s="6">
+      <c r="L7" s="6">
         <v>50</v>
       </c>
+      <c r="Q7" s="6">
+        <v>50</v>
+      </c>
       <c r="R7" s="6">
-        <v>50</v>
-      </c>
-      <c r="S7" s="6">
         <v>100</v>
       </c>
+      <c r="S7" s="10"/>
       <c r="T7" s="10"/>
       <c r="U7" s="10"/>
-      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
       <c r="X7" s="10"/>
-      <c r="Y7" s="10"/>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="M8" s="6">
+      <c r="L8" s="6">
+        <v>100</v>
+      </c>
+      <c r="Q8" s="6">
         <v>100</v>
       </c>
       <c r="R8" s="6">
         <v>100</v>
       </c>
-      <c r="S8" s="6">
-        <v>100</v>
-      </c>
+      <c r="S8" s="10"/>
       <c r="T8" s="10"/>
       <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
       <c r="X8" s="10"/>
-      <c r="Y8" s="10"/>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>3</v>
@@ -2998,20 +2994,20 @@
       <c r="D9" s="5">
         <v>50</v>
       </c>
-      <c r="R9" s="6">
+      <c r="Q9" s="6">
         <v>50</v>
       </c>
+      <c r="S9" s="10"/>
       <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10">
+      <c r="U9" s="10">
         <v>0</v>
       </c>
+      <c r="W9" s="10"/>
       <c r="X9" s="10"/>
-      <c r="Y9" s="10"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>4</v>
@@ -3019,55 +3015,55 @@
       <c r="D10" s="5">
         <v>50</v>
       </c>
-      <c r="R10" s="6">
+      <c r="Q10" s="6">
         <v>50</v>
       </c>
+      <c r="S10" s="10"/>
       <c r="T10" s="10"/>
       <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
-      <c r="W10" s="10">
+      <c r="V10" s="10">
         <v>0</v>
       </c>
+      <c r="W10" s="10"/>
       <c r="X10" s="10"/>
-      <c r="Y10" s="10"/>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="R11" s="6">
+      <c r="Q11" s="6">
         <v>0</v>
       </c>
+      <c r="S11" s="10"/>
       <c r="T11" s="10"/>
       <c r="U11" s="10"/>
-      <c r="V11" s="10"/>
-      <c r="X11" s="10">
+      <c r="W11" s="10">
         <v>99</v>
       </c>
-      <c r="Y11" s="10"/>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="X11" s="10"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="R12" s="6">
+      <c r="Q12" s="6">
         <v>0</v>
       </c>
+      <c r="S12" s="10"/>
       <c r="T12" s="10"/>
       <c r="U12" s="10"/>
-      <c r="V12" s="10"/>
-      <c r="X12" s="10">
+      <c r="W12" s="10">
         <v>99</v>
       </c>
-      <c r="Y12" s="10"/>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="X12" s="10"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>21</v>
       </c>
@@ -3081,208 +3077,171 @@
         <v>1</v>
       </c>
       <c r="F13" s="11">
-        <v>2.4974653103104298</v>
+        <v>25.481798063623799</v>
       </c>
       <c r="G13" s="11">
-        <v>9.3018160392078606</v>
-      </c>
-      <c r="H13" s="11">
-        <v>10.2347283365258</v>
-      </c>
+        <v>28.584806362378998</v>
+      </c>
+      <c r="H13" s="11"/>
       <c r="I13" s="11">
-        <v>25.481798063623799</v>
+        <v>63.651452282157699</v>
       </c>
       <c r="J13" s="11">
-        <v>28.584806362378998</v>
-      </c>
-      <c r="K13" s="11">
-        <v>63.651452282157699</v>
-      </c>
+        <v>82.987551867219906</v>
+      </c>
+      <c r="K13" s="11"/>
       <c r="L13" s="11">
-        <v>82.987551867219906</v>
+        <v>100</v>
       </c>
       <c r="M13" s="11">
-        <v>100</v>
+        <v>104.647302904564</v>
       </c>
       <c r="N13" s="11">
-        <v>104.647302904564</v>
+        <v>107.966804979253</v>
       </c>
       <c r="O13" s="11">
-        <v>107.966804979253</v>
+        <v>111.203319502075</v>
       </c>
       <c r="P13" s="11">
-        <v>111.203319502075</v>
+        <v>115.767634854772</v>
       </c>
       <c r="Q13" s="11">
-        <v>115.767634854772</v>
-      </c>
-      <c r="R13" s="11">
         <v>117.42738589211601</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I14" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="J14" s="6">
+        <v>5.4</v>
+      </c>
+      <c r="K14" s="6">
+        <v>5.6</v>
+      </c>
+      <c r="N14" s="6">
+        <v>6</v>
+      </c>
+      <c r="O14" s="6">
+        <v>7.63</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L15" s="6">
-        <v>5.4</v>
-      </c>
-      <c r="O15" s="6">
-        <v>6</v>
-      </c>
-      <c r="P15" s="6">
-        <v>7.63</v>
-      </c>
-      <c r="R15" s="6">
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="I15" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K16" s="6">
-        <v>1</v>
-      </c>
-      <c r="R16" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="I16" s="6">
+        <v>6</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>10</v>
+      </c>
+      <c r="X16" s="10">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="Z16" s="6">
+        <f>Q16/2</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="R17" s="6">
-        <f>4.5/98 * 100</f>
-        <v>4.591836734693878</v>
-      </c>
-      <c r="Y17" s="10">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="Z17" s="6">
-        <f>R17/2</f>
-        <v>2.295918367346939</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A18" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="6">
-        <v>2</v>
-      </c>
-      <c r="K18" s="6">
-        <v>6</v>
-      </c>
-      <c r="R18" s="6">
-        <v>10</v>
-      </c>
-      <c r="Y18" s="10">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="AA18" s="6">
-        <f>R18/2</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A19" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="K27" s="8"/>
-      <c r="L27" s="7"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5">
+        <v>63</v>
+      </c>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I25" s="8"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I26" s="8"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I27" s="8"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="8"/>
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
       <c r="O27" s="8"/>
       <c r="P27" s="8"/>
       <c r="Q27" s="8"/>
-      <c r="R27" s="8"/>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="K28" s="8"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="K29" s="8"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
     </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="3">
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:H5 E27:R29">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:E5 E25:Q27">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -3319,7 +3278,7 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">

</xml_diff>

<commit_message>
Tidying to make treatment support by strain completely replace food vouchers
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="92">
   <si>
     <t>parameter</t>
   </si>
@@ -156,48 +156,12 @@
     <t>int_perc_firstline_dst</t>
   </si>
   <si>
-    <t>int_perc_food_voucher_ds</t>
-  </si>
-  <si>
-    <t>int_perc_food_voucher_mdr</t>
-  </si>
-  <si>
     <t>int_perc_ngo_activities</t>
   </si>
   <si>
     <t>int_perc_opendoors_activities</t>
   </si>
   <si>
-    <t>econ_unitcost_food_voucher_ds</t>
-  </si>
-  <si>
-    <t>econ_inflectioncost_food_voucher_ds</t>
-  </si>
-  <si>
-    <t>econ_startupcost_food_voucher_ds</t>
-  </si>
-  <si>
-    <t>econ_startupduration_food_voucher_ds</t>
-  </si>
-  <si>
-    <t>econ_saturation_food_voucher_ds</t>
-  </si>
-  <si>
-    <t>econ_unitcost_food_voucher_mdr</t>
-  </si>
-  <si>
-    <t>econ_inflectioncost_food_voucher_mdr</t>
-  </si>
-  <si>
-    <t>econ_startupcost_food_voucher_mdr</t>
-  </si>
-  <si>
-    <t>econ_startupduration_food_voucher_mdr</t>
-  </si>
-  <si>
-    <t>econ_saturation_food_voucher_mdr</t>
-  </si>
-  <si>
     <t>Months of treatment x 4 weeks x 10 BNG per week x EUR exchange rate x treatment success rate</t>
   </si>
   <si>
@@ -210,9 +174,6 @@
     <t>econ_unitcost_shortcourse_mdr</t>
   </si>
   <si>
-    <t>econ_inflectioncost_shortcourse_mdr</t>
-  </si>
-  <si>
     <t>econ_startupcost_shortcourse_mdr</t>
   </si>
   <si>
@@ -298,6 +259,42 @@
   </si>
   <si>
     <t>prop_mix_prison_from_diabetes</t>
+  </si>
+  <si>
+    <t>int_perc_treatment_support_relative_mdr</t>
+  </si>
+  <si>
+    <t>int_perc_treatment_support_relative_ds</t>
+  </si>
+  <si>
+    <t>econ_unitcost_treatment_support_relative_ds</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_treatment_support_relative_ds</t>
+  </si>
+  <si>
+    <t>econ_startupcost_treatment_support_relative_ds</t>
+  </si>
+  <si>
+    <t>econ_startupduration_treatment_support_relative_ds</t>
+  </si>
+  <si>
+    <t>econ_saturation_treatment_support_relative_ds</t>
+  </si>
+  <si>
+    <t>econ_unitcost_treatment_support_relative_mdr</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_treatment_support_relative_mdr</t>
+  </si>
+  <si>
+    <t>econ_startupcost_treatment_support_relative_mdr</t>
+  </si>
+  <si>
+    <t>econ_startupduration_treatment_support_relative_mdr</t>
+  </si>
+  <si>
+    <t>econ_saturation_treatment_support_relative_mdr</t>
   </si>
 </sst>
 </file>
@@ -2208,10 +2205,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2245,7 +2242,7 @@
     </row>
     <row r="3" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B3" s="18">
         <v>2</v>
@@ -2255,7 +2252,7 @@
     </row>
     <row r="4" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B4" s="18">
         <v>1920</v>
@@ -2265,7 +2262,7 @@
     </row>
     <row r="5" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B5" s="18">
         <v>1920</v>
@@ -2275,7 +2272,7 @@
     </row>
     <row r="6" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B6" s="18">
         <v>1.2</v>
@@ -2372,7 +2369,7 @@
     </row>
     <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B15" s="24">
         <v>1950</v>
@@ -2409,7 +2406,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B19" s="19">
         <v>0.6</v>
@@ -2417,7 +2414,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B20" s="19">
         <v>0.03</v>
@@ -2425,7 +2422,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="B21" s="19">
         <v>0.03</v>
@@ -2433,18 +2430,18 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="B22" s="19">
         <v>92</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="B23" s="19">
         <v>0</v>
@@ -2452,7 +2449,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="B24" s="19">
         <v>0</v>
@@ -2460,7 +2457,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="B25" s="19">
         <v>0</v>
@@ -2468,7 +2465,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="B26" s="19">
         <v>1</v>
@@ -2476,18 +2473,18 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="B27" s="19">
         <v>857</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="B28" s="19">
         <v>0</v>
@@ -2495,7 +2492,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="B29" s="19">
         <v>0</v>
@@ -2503,7 +2500,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="B30" s="19">
         <v>0</v>
@@ -2511,7 +2508,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="B31" s="19">
         <v>1</v>
@@ -2519,19 +2516,19 @@
     </row>
     <row r="32" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B32" s="17">
         <f>1.02+67.12</f>
         <v>68.14</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B33" s="17">
         <v>0</v>
@@ -2539,18 +2536,18 @@
     </row>
     <row r="34" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B34" s="17">
         <v>8028</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B35" s="17">
         <v>1</v>
@@ -2558,7 +2555,7 @@
     </row>
     <row r="36" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="B36" s="17">
         <v>1</v>
@@ -2566,7 +2563,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B37" s="26">
         <v>6094</v>
@@ -2574,47 +2571,47 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B38" s="17">
+        <v>51</v>
+      </c>
+      <c r="B38" s="25">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="B39" s="25">
+        <v>52</v>
+      </c>
+      <c r="B39" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B40" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B41" s="17">
-        <v>0.9</v>
+        <v>751</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B42" s="17">
-        <v>751</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B43" s="17">
         <v>0</v>
@@ -2622,7 +2619,7 @@
     </row>
     <row r="44" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B44" s="17">
         <v>0</v>
@@ -2630,31 +2627,31 @@
     </row>
     <row r="45" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B45" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B46" s="17">
-        <v>1</v>
+        <v>862</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B47" s="17">
-        <v>862</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B48" s="17">
         <v>0</v>
@@ -2662,7 +2659,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B49" s="17">
         <v>0</v>
@@ -2670,17 +2667,9 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B50" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B51" s="17">
         <v>1</v>
       </c>
     </row>
@@ -2723,7 +2712,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2851,11 +2840,11 @@
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="J3" s="6">
+        <v>0</v>
+      </c>
       <c r="L3" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="6">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="S3" s="10"/>
       <c r="T3" s="10"/>
@@ -2868,11 +2857,11 @@
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="J4" s="6">
+        <v>0</v>
+      </c>
       <c r="L4" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="6">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
@@ -2881,104 +2870,102 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4">
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6">
+        <v>100</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>100</v>
+      </c>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="6">
+        <v>50</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>50</v>
+      </c>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4">
         <v>0.5</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="6">
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="6">
         <v>0</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G7" s="6">
         <v>5</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L7" s="6">
         <f>80*(1174/2649)</f>
         <v>35.454888637221593</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M7" s="6">
         <f>80*(1077/2407)</f>
         <v>35.795596177814708</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N7" s="6">
         <f>80*(1094/2280)</f>
         <v>38.385964912280699</v>
       </c>
-      <c r="O5" s="6">
+      <c r="O7" s="6">
         <f>80*(961/1932)</f>
         <v>39.792960662525878</v>
       </c>
-      <c r="P5" s="6">
+      <c r="P7" s="6">
         <f>80*(891/1872)</f>
         <v>38.076923076923073</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="Q7" s="6">
         <f>80*782/1660</f>
         <v>37.686746987951807</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q6" s="6">
-        <v>0</v>
-      </c>
-      <c r="S6" s="10">
-        <v>100</v>
-      </c>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="W6" s="10"/>
-      <c r="X6" s="10"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="L7" s="6">
-        <v>50</v>
-      </c>
-      <c r="Q7" s="6">
-        <v>50</v>
-      </c>
-      <c r="R7" s="6">
-        <v>100</v>
-      </c>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
-      <c r="W7" s="10"/>
-      <c r="X7" s="10"/>
-    </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L8" s="6">
+      <c r="Q8" s="6">
+        <v>0</v>
+      </c>
+      <c r="S8" s="10">
         <v>100</v>
       </c>
-      <c r="Q8" s="6">
-        <v>100</v>
-      </c>
-      <c r="R8" s="6">
-        <v>100</v>
-      </c>
-      <c r="S8" s="10"/>
       <c r="T8" s="10"/>
       <c r="U8" s="10"/>
       <c r="W8" s="10"/>
@@ -2986,7 +2973,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>3</v>
@@ -3007,7 +2994,7 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>4</v>
@@ -3029,7 +3016,7 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>4</v>
@@ -3047,7 +3034,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>4</v>
@@ -3241,7 +3228,7 @@
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="3">
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:E5 E25:Q27">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:E7 E25:Q27">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -3259,7 +3246,7 @@
           <x14:formula1>
             <xm:f>[1]dropdown_lists!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>B5</xm:sqref>
+          <xm:sqref>B7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Revise input data for IPT
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -2207,8 +2207,8 @@
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2708,11 +2708,11 @@
   </sheetPr>
   <dimension ref="A1:Z27"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2881,9 +2881,6 @@
       <c r="L5" s="6">
         <v>100</v>
       </c>
-      <c r="Q5" s="6">
-        <v>100</v>
-      </c>
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
       <c r="U5" s="10"/>
@@ -2900,9 +2897,6 @@
         <v>0</v>
       </c>
       <c r="L6" s="6">
-        <v>50</v>
-      </c>
-      <c r="Q6" s="6">
         <v>50</v>
       </c>
       <c r="S6" s="10"/>

</xml_diff>

<commit_message>
New code for DST as proposed in Slack
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="88">
   <si>
     <t>parameter</t>
   </si>
@@ -93,12 +93,6 @@
     <t>age_breakpoints</t>
   </si>
   <si>
-    <t>scenario_7</t>
-  </si>
-  <si>
-    <t>scenario_8</t>
-  </si>
-  <si>
     <t>program_number_tests_per_tb_presentation</t>
   </si>
   <si>
@@ -114,9 +108,6 @@
     <t>program_perc_detect</t>
   </si>
   <si>
-    <t>scenario_9</t>
-  </si>
-  <si>
     <t>tb_timeperiod_ontreatment_mdr</t>
   </si>
   <si>
@@ -235,9 +226,6 @@
   </si>
   <si>
     <t>prop_mix_ruralpoor_from_ruralpoor</t>
-  </si>
-  <si>
-    <t>int_perc_improve_dst</t>
   </si>
   <si>
     <t>econ_saturation_improve_dst</t>
@@ -2207,8 +2195,8 @@
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2235,14 +2223,14 @@
         <v>2</v>
       </c>
       <c r="B2" s="13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B3" s="18">
         <v>2</v>
@@ -2252,7 +2240,7 @@
     </row>
     <row r="4" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B4" s="18">
         <v>1920</v>
@@ -2262,7 +2250,7 @@
     </row>
     <row r="5" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B5" s="18">
         <v>1920</v>
@@ -2272,7 +2260,7 @@
     </row>
     <row r="6" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B6" s="18">
         <v>1.2</v>
@@ -2323,7 +2311,7 @@
     </row>
     <row r="11" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="16">
         <v>1.5</v>
@@ -2331,7 +2319,7 @@
     </row>
     <row r="12" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B12" s="13">
         <f>20/12</f>
@@ -2343,7 +2331,7 @@
     </row>
     <row r="13" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B13" s="16">
         <v>0.4</v>
@@ -2351,12 +2339,12 @@
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B14" s="16">
         <v>0.89</v>
@@ -2364,12 +2352,12 @@
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B15" s="24">
         <v>1950</v>
@@ -2377,12 +2365,12 @@
       <c r="C15" s="24"/>
       <c r="D15" s="24"/>
       <c r="E15" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B16" s="19">
         <v>1990</v>
@@ -2390,7 +2378,7 @@
     </row>
     <row r="17" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B17" s="19">
         <v>6</v>
@@ -2398,7 +2386,7 @@
     </row>
     <row r="18" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B18" s="19">
         <v>13</v>
@@ -2406,7 +2394,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B19" s="19">
         <v>0.6</v>
@@ -2414,7 +2402,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B20" s="19">
         <v>0.03</v>
@@ -2422,7 +2410,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B21" s="19">
         <v>0.03</v>
@@ -2430,18 +2418,18 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B22" s="19">
         <v>92</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B23" s="19">
         <v>0</v>
@@ -2449,7 +2437,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B24" s="19">
         <v>0</v>
@@ -2457,7 +2445,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B25" s="19">
         <v>0</v>
@@ -2465,7 +2453,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B26" s="19">
         <v>1</v>
@@ -2473,18 +2461,18 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B27" s="19">
         <v>857</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B28" s="19">
         <v>0</v>
@@ -2492,7 +2480,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B29" s="19">
         <v>0</v>
@@ -2500,7 +2488,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B30" s="19">
         <v>0</v>
@@ -2508,7 +2496,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B31" s="19">
         <v>1</v>
@@ -2516,19 +2504,19 @@
     </row>
     <row r="32" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B32" s="17">
         <f>1.02+67.12</f>
         <v>68.14</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B33" s="17">
         <v>0</v>
@@ -2536,18 +2524,18 @@
     </row>
     <row r="34" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B34" s="17">
         <v>8028</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B35" s="17">
         <v>1</v>
@@ -2555,7 +2543,7 @@
     </row>
     <row r="36" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B36" s="17">
         <v>1</v>
@@ -2563,7 +2551,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B37" s="26">
         <v>6094</v>
@@ -2571,7 +2559,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B38" s="25">
         <v>0</v>
@@ -2579,7 +2567,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B39" s="17">
         <v>0</v>
@@ -2587,7 +2575,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B40" s="17">
         <v>0.9</v>
@@ -2595,7 +2583,7 @@
     </row>
     <row r="41" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B41" s="17">
         <v>751</v>
@@ -2603,7 +2591,7 @@
     </row>
     <row r="42" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B42" s="17">
         <v>0</v>
@@ -2611,7 +2599,7 @@
     </row>
     <row r="43" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B43" s="17">
         <v>0</v>
@@ -2619,7 +2607,7 @@
     </row>
     <row r="44" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B44" s="17">
         <v>0</v>
@@ -2627,7 +2615,7 @@
     </row>
     <row r="45" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B45" s="17">
         <v>1</v>
@@ -2635,7 +2623,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B46" s="17">
         <v>862</v>
@@ -2643,7 +2631,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B47" s="17">
         <v>0</v>
@@ -2651,7 +2639,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B48" s="17">
         <v>0</v>
@@ -2659,7 +2647,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B49" s="17">
         <v>0</v>
@@ -2667,7 +2655,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B50" s="17">
         <v>1</v>
@@ -2706,13 +2694,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:Z27"/>
+  <dimension ref="A1:W26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2733,11 +2721,10 @@
     <col min="18" max="18" width="14" style="6" customWidth="1"/>
     <col min="19" max="20" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="21" max="23" width="14.42578125" style="6" customWidth="1"/>
-    <col min="24" max="26" width="15.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="9.140625" style="6"/>
+    <col min="24" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>6</v>
       </c>
@@ -2807,19 +2794,10 @@
       <c r="W1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>4</v>
@@ -2828,14 +2806,12 @@
         <v>0</v>
       </c>
       <c r="S2" s="10"/>
-      <c r="T2" s="10">
-        <v>50</v>
-      </c>
+      <c r="T2" s="10"/>
       <c r="U2" s="10"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>4</v>
@@ -2850,9 +2826,9 @@
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>4</v>
@@ -2868,9 +2844,9 @@
       <c r="U4" s="10"/>
       <c r="V4" s="10"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>
@@ -2886,9 +2862,9 @@
       <c r="U5" s="10"/>
       <c r="V5" s="10"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>4</v>
@@ -2904,9 +2880,9 @@
       <c r="U6" s="10"/>
       <c r="V6" s="10"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>4</v>
@@ -2946,31 +2922,36 @@
         <f>80*782/1660</f>
         <v>37.686746987951807</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="R7" s="6">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="D8" s="5">
+        <v>50</v>
+      </c>
       <c r="Q8" s="6">
+        <v>50</v>
+      </c>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10">
         <v>0</v>
       </c>
-      <c r="S8" s="10">
-        <v>100</v>
-      </c>
-      <c r="T8" s="10"/>
       <c r="U8" s="10"/>
       <c r="W8" s="10"/>
-      <c r="X8" s="10"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9" s="5">
         <v>50</v>
@@ -2983,34 +2964,30 @@
       <c r="U9" s="10">
         <v>0</v>
       </c>
+      <c r="V9" s="10"/>
       <c r="W9" s="10"/>
-      <c r="X9" s="10"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="5">
-        <v>50</v>
-      </c>
       <c r="Q10" s="6">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
       <c r="U10" s="10"/>
-      <c r="V10" s="10">
-        <v>0</v>
+      <c r="V10" s="6">
+        <v>99</v>
       </c>
       <c r="W10" s="10"/>
-      <c r="X10" s="10"/>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>4</v>
@@ -3021,172 +2998,161 @@
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
       <c r="U11" s="10"/>
-      <c r="W11" s="10">
+      <c r="V11" s="6">
         <v>99</v>
       </c>
-      <c r="X11" s="10"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="W11" s="10"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="Q12" s="6">
-        <v>0</v>
-      </c>
-      <c r="S12" s="10"/>
-      <c r="T12" s="10"/>
-      <c r="U12" s="10"/>
-      <c r="W12" s="10">
-        <v>99</v>
-      </c>
-      <c r="X12" s="10"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D12" s="5">
+        <v>1</v>
+      </c>
+      <c r="E12" s="11">
+        <v>1</v>
+      </c>
+      <c r="F12" s="11">
+        <v>25.481798063623799</v>
+      </c>
+      <c r="G12" s="11">
+        <v>28.584806362378998</v>
+      </c>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11">
+        <v>63.651452282157699</v>
+      </c>
+      <c r="J12" s="11">
+        <v>82.987551867219906</v>
+      </c>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11">
+        <v>100</v>
+      </c>
+      <c r="M12" s="11">
+        <v>104.647302904564</v>
+      </c>
+      <c r="N12" s="11">
+        <v>107.966804979253</v>
+      </c>
+      <c r="O12" s="11">
+        <v>111.203319502075</v>
+      </c>
+      <c r="P12" s="11">
+        <v>115.767634854772</v>
+      </c>
+      <c r="Q12" s="11">
+        <v>117.42738589211601</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="5">
-        <v>1</v>
-      </c>
-      <c r="E13" s="11">
-        <v>1</v>
-      </c>
-      <c r="F13" s="11">
-        <v>25.481798063623799</v>
-      </c>
-      <c r="G13" s="11">
-        <v>28.584806362378998</v>
-      </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11">
-        <v>63.651452282157699</v>
-      </c>
-      <c r="J13" s="11">
-        <v>82.987551867219906</v>
-      </c>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11">
-        <v>100</v>
-      </c>
-      <c r="M13" s="11">
-        <v>104.647302904564</v>
-      </c>
-      <c r="N13" s="11">
-        <v>107.966804979253</v>
-      </c>
-      <c r="O13" s="11">
-        <v>111.203319502075</v>
-      </c>
-      <c r="P13" s="11">
-        <v>115.767634854772</v>
-      </c>
-      <c r="Q13" s="11">
-        <v>117.42738589211601</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="J13" s="6">
+        <v>5.4</v>
+      </c>
+      <c r="K13" s="6">
+        <v>5.6</v>
+      </c>
+      <c r="N13" s="6">
+        <v>6</v>
+      </c>
+      <c r="O13" s="6">
+        <v>7.63</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J14" s="6">
-        <v>5.4</v>
-      </c>
-      <c r="K14" s="6">
-        <v>5.6</v>
-      </c>
-      <c r="N14" s="6">
-        <v>6</v>
-      </c>
-      <c r="O14" s="6">
-        <v>7.63</v>
+      <c r="I14" s="6">
+        <v>1</v>
       </c>
       <c r="Q14" s="6">
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I15" s="6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="Q15" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="W15" s="6">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I16" s="6">
-        <v>6</v>
-      </c>
-      <c r="Q16" s="6">
-        <v>10</v>
-      </c>
-      <c r="X16" s="10">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="Z16" s="6">
-        <f>Q16/2</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5">
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5">
         <v>63</v>
       </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+    </row>
+    <row r="19" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+    </row>
+    <row r="24" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="I24" s="8"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+    </row>
+    <row r="25" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I25" s="8"/>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
@@ -3197,7 +3163,7 @@
       <c r="P25" s="8"/>
       <c r="Q25" s="8"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I26" s="8"/>
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
@@ -3208,21 +3174,10 @@
       <c r="P26" s="8"/>
       <c r="Q26" s="8"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I27" s="8"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="8"/>
-    </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="3">
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:E7 E25:Q27">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:E7 E24:Q26">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Remove IPT code for open doors
... as explained in Slack post. Also some simplification to the input spreadsheet.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -2195,7 +2195,7 @@
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2694,13 +2694,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:W26"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2709,22 +2709,20 @@
     <col min="2" max="2" width="11" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="4" customWidth="1"/>
     <col min="4" max="4" width="11" style="5" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" style="6" customWidth="1"/>
-    <col min="10" max="12" width="7" style="6" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" style="6" customWidth="1"/>
-    <col min="14" max="15" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="7.85546875" style="6" customWidth="1"/>
-    <col min="18" max="18" width="14" style="6" customWidth="1"/>
-    <col min="19" max="20" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="14.42578125" style="6" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="6"/>
+    <col min="5" max="5" width="7.140625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" style="6" customWidth="1"/>
+    <col min="8" max="10" width="7" style="6" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="6" customWidth="1"/>
+    <col min="12" max="13" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="7.85546875" style="6" customWidth="1"/>
+    <col min="16" max="16" width="14" style="6" customWidth="1"/>
+    <col min="17" max="18" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="14.42578125" style="6" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>6</v>
       </c>
@@ -2738,149 +2736,143 @@
         <v>1920</v>
       </c>
       <c r="E1" s="1">
-        <v>1950</v>
+        <v>1989</v>
       </c>
       <c r="F1" s="1">
-        <v>1989</v>
+        <v>1994</v>
       </c>
       <c r="G1" s="1">
-        <v>1990</v>
+        <v>2000</v>
       </c>
       <c r="H1" s="1">
-        <v>1994</v>
+        <v>2006</v>
       </c>
       <c r="I1" s="1">
-        <v>2000</v>
+        <v>2008</v>
       </c>
       <c r="J1" s="1">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="K1" s="1">
-        <v>2008</v>
+        <v>2011</v>
       </c>
       <c r="L1" s="1">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="M1" s="1">
-        <v>2011</v>
+        <v>2013</v>
       </c>
       <c r="N1" s="1">
-        <v>2012</v>
+        <v>2014</v>
       </c>
       <c r="O1" s="1">
-        <v>2013</v>
-      </c>
-      <c r="P1" s="1">
-        <v>2014</v>
-      </c>
-      <c r="Q1" s="1">
         <v>2015</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="R1" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="W1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="6">
+      <c r="O2" s="6">
         <v>0</v>
       </c>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
       <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>39</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
       <c r="J3" s="6">
-        <v>0</v>
-      </c>
-      <c r="L3" s="6">
         <v>60</v>
       </c>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
       <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>40</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
       <c r="J4" s="6">
-        <v>0</v>
-      </c>
-      <c r="L4" s="6">
         <v>60</v>
       </c>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>77</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="6">
+      <c r="G5" s="6">
         <v>0</v>
       </c>
-      <c r="L5" s="6">
+      <c r="J5" s="6">
         <v>100</v>
       </c>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>76</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="6">
+      <c r="G6" s="6">
         <v>0</v>
       </c>
-      <c r="L6" s="6">
+      <c r="J6" s="6">
         <v>50</v>
       </c>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>41</v>
       </c>
@@ -2891,42 +2883,38 @@
         <v>0.5</v>
       </c>
       <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="6">
+      <c r="E7" s="6">
         <v>0</v>
       </c>
-      <c r="G7" s="6">
-        <v>5</v>
-      </c>
-      <c r="L7" s="6">
+      <c r="J7" s="6">
         <f>80*(1174/2649)</f>
         <v>35.454888637221593</v>
       </c>
-      <c r="M7" s="6">
+      <c r="K7" s="6">
         <f>80*(1077/2407)</f>
         <v>35.795596177814708</v>
       </c>
-      <c r="N7" s="6">
+      <c r="L7" s="6">
         <f>80*(1094/2280)</f>
         <v>38.385964912280699</v>
       </c>
-      <c r="O7" s="6">
+      <c r="M7" s="6">
         <f>80*(961/1932)</f>
         <v>39.792960662525878</v>
       </c>
-      <c r="P7" s="6">
+      <c r="N7" s="6">
         <f>80*(891/1872)</f>
         <v>38.076923076923073</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="O7" s="6">
         <f>80*782/1660</f>
         <v>37.686746987951807</v>
       </c>
-      <c r="R7" s="6">
+      <c r="P7" s="6">
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>42</v>
       </c>
@@ -2936,17 +2924,17 @@
       <c r="D8" s="5">
         <v>50</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="O8" s="6">
         <v>50</v>
       </c>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10">
+        <v>0</v>
+      </c>
       <c r="S8" s="10"/>
-      <c r="T8" s="10">
-        <v>0</v>
-      </c>
       <c r="U8" s="10"/>
-      <c r="W8" s="10"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>43</v>
       </c>
@@ -2956,54 +2944,54 @@
       <c r="D9" s="5">
         <v>50</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="O9" s="6">
         <v>50</v>
       </c>
-      <c r="S9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10">
+        <v>0</v>
+      </c>
       <c r="T9" s="10"/>
-      <c r="U9" s="10">
-        <v>0</v>
-      </c>
-      <c r="V9" s="10"/>
-      <c r="W9" s="10"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U9" s="10"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>54</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="O10" s="6">
         <v>0</v>
       </c>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
       <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
+      <c r="T10" s="6">
+        <v>99</v>
+      </c>
       <c r="U10" s="10"/>
-      <c r="V10" s="6">
-        <v>99</v>
-      </c>
-      <c r="W10" s="10"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>65</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="Q11" s="6">
+      <c r="O11" s="6">
         <v>0</v>
       </c>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
       <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
+      <c r="T11" s="6">
+        <v>99</v>
+      </c>
       <c r="U11" s="10"/>
-      <c r="V11" s="6">
-        <v>99</v>
-      </c>
-      <c r="W11" s="10"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>21</v>
       </c>
@@ -3014,96 +3002,90 @@
         <v>1</v>
       </c>
       <c r="E12" s="11">
-        <v>1</v>
-      </c>
-      <c r="F12" s="11">
         <v>25.481798063623799</v>
       </c>
+      <c r="F12" s="11"/>
       <c r="G12" s="11">
-        <v>28.584806362378998</v>
-      </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11">
         <v>63.651452282157699</v>
       </c>
+      <c r="H12" s="11">
+        <v>82.987551867219906</v>
+      </c>
+      <c r="I12" s="11"/>
       <c r="J12" s="11">
-        <v>82.987551867219906</v>
-      </c>
-      <c r="K12" s="11"/>
+        <v>100</v>
+      </c>
+      <c r="K12" s="11">
+        <v>104.647302904564</v>
+      </c>
       <c r="L12" s="11">
-        <v>100</v>
+        <v>107.966804979253</v>
       </c>
       <c r="M12" s="11">
-        <v>104.647302904564</v>
+        <v>111.203319502075</v>
       </c>
       <c r="N12" s="11">
-        <v>107.966804979253</v>
+        <v>115.767634854772</v>
       </c>
       <c r="O12" s="11">
-        <v>111.203319502075</v>
-      </c>
-      <c r="P12" s="11">
-        <v>115.767634854772</v>
-      </c>
-      <c r="Q12" s="11">
         <v>117.42738589211601</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J13" s="6">
+      <c r="H13" s="6">
         <v>5.4</v>
       </c>
-      <c r="K13" s="6">
+      <c r="I13" s="6">
         <v>5.6</v>
       </c>
-      <c r="N13" s="6">
+      <c r="L13" s="6">
         <v>6</v>
       </c>
+      <c r="M13" s="6">
+        <v>7.63</v>
+      </c>
       <c r="O13" s="6">
-        <v>7.63</v>
-      </c>
-      <c r="Q13" s="6">
         <v>8.4</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I14" s="6">
+      <c r="G14" s="6">
         <v>1</v>
       </c>
-      <c r="Q14" s="6">
+      <c r="O14" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I15" s="6">
+      <c r="G15" s="6">
         <v>6</v>
       </c>
-      <c r="Q15" s="6">
+      <c r="O15" s="6">
         <v>10</v>
       </c>
-      <c r="W15" s="6">
+      <c r="U15" s="6">
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>28</v>
       </c>
@@ -3111,11 +3093,11 @@
         <v>3</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="F16" s="5">
+        <v>63</v>
+      </c>
       <c r="G16" s="5"/>
-      <c r="H16" s="5">
-        <v>63</v>
-      </c>
+      <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
@@ -3123,10 +3105,8 @@
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-    </row>
-    <row r="19" spans="5:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -3138,46 +3118,44 @@
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-    </row>
-    <row r="24" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="I24" s="8"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
+    </row>
+    <row r="24" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="G24" s="8"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
       <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="8"/>
-    </row>
-    <row r="25" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="I25" s="8"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
+    </row>
+    <row r="25" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="G25" s="8"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
       <c r="N25" s="8"/>
       <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
-    </row>
-    <row r="26" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="I26" s="8"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
+    </row>
+    <row r="26" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="G26" s="8"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
       <c r="L26" s="8"/>
       <c r="M26" s="8"/>
       <c r="N26" s="8"/>
       <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
     </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="3">
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:E7 E24:Q26">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7 E24:O26">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
New code for a "DOTS contributor" replaces the old code for the "Open Doors" program
Similar approach, except applies to the case detection proportion (rather than the true rate) and no additional effect on IPT. Old code is still there as comments until confirmed with rest of team.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -150,9 +150,6 @@
     <t>int_perc_ngo_activities</t>
   </si>
   <si>
-    <t>int_perc_opendoors_activities</t>
-  </si>
-  <si>
     <t>Months of treatment x 4 weeks x 10 BNG per week x EUR exchange rate x treatment success rate</t>
   </si>
   <si>
@@ -283,6 +280,9 @@
   </si>
   <si>
     <t>econ_saturation_treatment_support_relative_mdr</t>
+  </si>
+  <si>
+    <t>int_perc_dots_contributor</t>
   </si>
 </sst>
 </file>
@@ -2195,7 +2195,7 @@
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2230,7 +2230,7 @@
     </row>
     <row r="3" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="18">
         <v>2</v>
@@ -2240,7 +2240,7 @@
     </row>
     <row r="4" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="18">
         <v>1920</v>
@@ -2250,7 +2250,7 @@
     </row>
     <row r="5" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="18">
         <v>1920</v>
@@ -2260,7 +2260,7 @@
     </row>
     <row r="6" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="18">
         <v>1.2</v>
@@ -2357,7 +2357,7 @@
     </row>
     <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" s="24">
         <v>1950</v>
@@ -2394,7 +2394,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" s="19">
         <v>0.6</v>
@@ -2402,7 +2402,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B20" s="19">
         <v>0.03</v>
@@ -2410,7 +2410,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B21" s="19">
         <v>0.03</v>
@@ -2418,18 +2418,18 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B22" s="19">
         <v>92</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" s="19">
         <v>0</v>
@@ -2437,7 +2437,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B24" s="19">
         <v>0</v>
@@ -2445,7 +2445,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B25" s="19">
         <v>0</v>
@@ -2453,7 +2453,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B26" s="19">
         <v>1</v>
@@ -2461,18 +2461,18 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B27" s="19">
         <v>857</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B28" s="19">
         <v>0</v>
@@ -2480,7 +2480,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B29" s="19">
         <v>0</v>
@@ -2488,7 +2488,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B30" s="19">
         <v>0</v>
@@ -2496,7 +2496,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B31" s="19">
         <v>1</v>
@@ -2504,19 +2504,19 @@
     </row>
     <row r="32" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B32" s="17">
         <f>1.02+67.12</f>
         <v>68.14</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B33" s="17">
         <v>0</v>
@@ -2524,18 +2524,18 @@
     </row>
     <row r="34" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B34" s="17">
         <v>8028</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B35" s="17">
         <v>1</v>
@@ -2543,7 +2543,7 @@
     </row>
     <row r="36" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B36" s="17">
         <v>1</v>
@@ -2551,7 +2551,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B37" s="26">
         <v>6094</v>
@@ -2559,7 +2559,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38" s="25">
         <v>0</v>
@@ -2567,7 +2567,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39" s="17">
         <v>0</v>
@@ -2575,7 +2575,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" s="17">
         <v>0.9</v>
@@ -2583,7 +2583,7 @@
     </row>
     <row r="41" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B41" s="17">
         <v>751</v>
@@ -2591,7 +2591,7 @@
     </row>
     <row r="42" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B42" s="17">
         <v>0</v>
@@ -2599,7 +2599,7 @@
     </row>
     <row r="43" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B43" s="17">
         <v>0</v>
@@ -2607,7 +2607,7 @@
     </row>
     <row r="44" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B44" s="17">
         <v>0</v>
@@ -2615,7 +2615,7 @@
     </row>
     <row r="45" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B45" s="17">
         <v>1</v>
@@ -2623,7 +2623,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B46" s="17">
         <v>862</v>
@@ -2631,7 +2631,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B47" s="17">
         <v>0</v>
@@ -2639,7 +2639,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B48" s="17">
         <v>0</v>
@@ -2647,7 +2647,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B49" s="17">
         <v>0</v>
@@ -2655,7 +2655,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B50" s="17">
         <v>1</v>
@@ -2696,11 +2696,11 @@
   </sheetPr>
   <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2838,7 +2838,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>
@@ -2856,7 +2856,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>4</v>
@@ -2879,9 +2879,6 @@
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="4">
-        <v>0.5</v>
-      </c>
       <c r="D7" s="22"/>
       <c r="E7" s="6">
         <v>0</v>
@@ -2919,7 +2916,7 @@
         <v>42</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8" s="5">
         <v>50</v>
@@ -2936,16 +2933,13 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="5">
-        <v>50</v>
-      </c>
       <c r="O9" s="6">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="Q9" s="10"/>
       <c r="R9" s="10"/>
@@ -2957,7 +2951,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>4</v>
@@ -2975,7 +2969,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>4</v>
@@ -3036,7 +3030,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H13" s="6">
         <v>5.4</v>
@@ -3059,7 +3053,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G14" s="6">
         <v>1</v>
@@ -3073,7 +3067,7 @@
         <v>27</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G15" s="6">
         <v>6</v>

</xml_diff>

<commit_message>
Implement riskgroup-specific ngo activities
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rragonnet\Google Drive\GitHub\AuTuMN\AuTuMN\autumn\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="612" windowWidth="16272" windowHeight="6300" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1895,8 +1900,8 @@
       <sheetName val="dropdown_lists"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
@@ -1946,7 +1951,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1981,7 +1986,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2195,22 +2200,22 @@
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.28515625" style="17" customWidth="1"/>
+    <col min="1" max="1" width="47.33203125" style="17" customWidth="1"/>
     <col min="2" max="2" width="18" style="19" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="17"/>
-    <col min="6" max="6" width="13.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="17"/>
+    <col min="3" max="5" width="9.109375" style="17"/>
+    <col min="6" max="6" width="13.88671875" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2218,7 +2223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
@@ -2228,7 +2233,7 @@
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
     </row>
-    <row r="3" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>50</v>
       </c>
@@ -2238,7 +2243,7 @@
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
     </row>
-    <row r="4" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>51</v>
       </c>
@@ -2248,7 +2253,7 @@
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
     </row>
-    <row r="5" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>52</v>
       </c>
@@ -2258,7 +2263,7 @@
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
     </row>
-    <row r="6" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>65</v>
       </c>
@@ -2268,7 +2273,7 @@
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
     </row>
-    <row r="7" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>11</v>
       </c>
@@ -2278,7 +2283,7 @@
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
     </row>
-    <row r="8" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>23</v>
       </c>
@@ -2291,7 +2296,7 @@
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
     </row>
-    <row r="9" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>12</v>
       </c>
@@ -2301,7 +2306,7 @@
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
     </row>
-    <row r="10" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>22</v>
       </c>
@@ -2309,7 +2314,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>24</v>
       </c>
@@ -2317,7 +2322,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>29</v>
       </c>
@@ -2329,7 +2334,7 @@
       <c r="D12" s="13"/>
       <c r="E12" s="17"/>
     </row>
-    <row r="13" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>30</v>
       </c>
@@ -2342,7 +2347,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="14" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>32</v>
       </c>
@@ -2355,7 +2360,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>66</v>
       </c>
@@ -2368,7 +2373,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>35</v>
       </c>
@@ -2376,7 +2381,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>36</v>
       </c>
@@ -2384,7 +2389,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>37</v>
       </c>
@@ -2392,7 +2397,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>67</v>
       </c>
@@ -2400,7 +2405,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>73</v>
       </c>
@@ -2408,7 +2413,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>74</v>
       </c>
@@ -2416,7 +2421,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>77</v>
       </c>
@@ -2427,7 +2432,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>78</v>
       </c>
@@ -2435,7 +2440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
         <v>79</v>
       </c>
@@ -2443,7 +2448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
         <v>80</v>
       </c>
@@ -2451,7 +2456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
         <v>81</v>
       </c>
@@ -2459,7 +2464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="17" t="s">
         <v>82</v>
       </c>
@@ -2470,7 +2475,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
         <v>83</v>
       </c>
@@ -2478,7 +2483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
         <v>84</v>
       </c>
@@ -2486,7 +2491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
         <v>85</v>
       </c>
@@ -2494,7 +2499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
         <v>86</v>
       </c>
@@ -2502,7 +2507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="17" t="s">
         <v>72</v>
       </c>
@@ -2514,7 +2519,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
         <v>71</v>
       </c>
@@ -2522,7 +2527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="17" t="s">
         <v>70</v>
       </c>
@@ -2533,7 +2538,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
         <v>69</v>
       </c>
@@ -2541,7 +2546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
         <v>68</v>
       </c>
@@ -2549,7 +2554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
         <v>46</v>
       </c>
@@ -2557,7 +2562,7 @@
         <v>6094</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="17" t="s">
         <v>47</v>
       </c>
@@ -2565,7 +2570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
         <v>48</v>
       </c>
@@ -2573,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
         <v>49</v>
       </c>
@@ -2581,7 +2586,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
         <v>54</v>
       </c>
@@ -2589,7 +2594,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
         <v>55</v>
       </c>
@@ -2597,7 +2602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
         <v>56</v>
       </c>
@@ -2605,7 +2610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
         <v>57</v>
       </c>
@@ -2613,7 +2618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="17" t="s">
         <v>58</v>
       </c>
@@ -2621,7 +2626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="17" t="s">
         <v>59</v>
       </c>
@@ -2629,7 +2634,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="17" t="s">
         <v>60</v>
       </c>
@@ -2637,7 +2642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="17" t="s">
         <v>61</v>
       </c>
@@ -2645,7 +2650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="17" t="s">
         <v>62</v>
       </c>
@@ -2653,7 +2658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="17" t="s">
         <v>63</v>
       </c>
@@ -2697,32 +2702,32 @@
   <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="57.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="57.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="11" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="4" customWidth="1"/>
     <col min="4" max="4" width="11" style="5" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="7.109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="7.5546875" style="6" customWidth="1"/>
     <col min="8" max="10" width="7" style="6" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="6" customWidth="1"/>
-    <col min="12" max="13" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="7.85546875" style="6" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="6" customWidth="1"/>
+    <col min="12" max="13" width="7.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="7.88671875" style="6" customWidth="1"/>
     <col min="16" max="16" width="14" style="6" customWidth="1"/>
-    <col min="17" max="18" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="14.42578125" style="6" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="6"/>
+    <col min="17" max="18" width="14.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="14.44140625" style="6" customWidth="1"/>
+    <col min="22" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>6</v>
       </c>
@@ -2787,7 +2792,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>38</v>
       </c>
@@ -2801,7 +2806,7 @@
       <c r="R2" s="10"/>
       <c r="S2" s="10"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>39</v>
       </c>
@@ -2818,7 +2823,7 @@
       <c r="R3" s="10"/>
       <c r="S3" s="10"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>40</v>
       </c>
@@ -2836,7 +2841,7 @@
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
         <v>76</v>
       </c>
@@ -2854,7 +2859,7 @@
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
         <v>75</v>
       </c>
@@ -2872,7 +2877,7 @@
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>41</v>
       </c>
@@ -2911,7 +2916,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
         <v>42</v>
       </c>
@@ -2921,17 +2926,22 @@
       <c r="D8" s="5">
         <v>50</v>
       </c>
+      <c r="E8" s="6">
+        <v>50</v>
+      </c>
       <c r="O8" s="6">
         <v>50</v>
       </c>
-      <c r="Q8" s="10"/>
+      <c r="Q8" s="10">
+        <v>100</v>
+      </c>
       <c r="R8" s="10">
         <v>0</v>
       </c>
       <c r="S8" s="10"/>
       <c r="U8" s="10"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
         <v>87</v>
       </c>
@@ -2949,7 +2959,7 @@
       <c r="T9" s="10"/>
       <c r="U9" s="10"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
         <v>53</v>
       </c>
@@ -2967,7 +2977,7 @@
       </c>
       <c r="U10" s="10"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
         <v>64</v>
       </c>
@@ -2985,7 +2995,7 @@
       </c>
       <c r="U11" s="10"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
         <v>21</v>
       </c>
@@ -3025,7 +3035,7 @@
         <v>117.42738589211601</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
         <v>25</v>
       </c>
@@ -3048,7 +3058,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>26</v>
       </c>
@@ -3062,7 +3072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
         <v>27</v>
       </c>
@@ -3079,7 +3089,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
         <v>28</v>
       </c>
@@ -3100,7 +3110,7 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="19" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -3113,7 +3123,7 @@
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
     </row>
-    <row r="24" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:15" x14ac:dyDescent="0.3">
       <c r="G24" s="8"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
@@ -3124,7 +3134,7 @@
       <c r="N24" s="8"/>
       <c r="O24" s="8"/>
     </row>
-    <row r="25" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:15" x14ac:dyDescent="0.3">
       <c r="G25" s="8"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
@@ -3135,7 +3145,7 @@
       <c r="N25" s="8"/>
       <c r="O25" s="8"/>
     </row>
-    <row r="26" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:15" x14ac:dyDescent="0.3">
       <c r="G26" s="8"/>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
@@ -3186,7 +3196,7 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">

</xml_diff>

<commit_message>
Make easier for NGO activities to be set to 100% at baseline
Prevent starting zero being added in data processing and make relevant adjustments to spreadsheets.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rragonnet\Google Drive\GitHub\AuTuMN\AuTuMN\autumn\xls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="612" windowWidth="16272" windowHeight="6300" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1951,7 +1946,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1986,7 +1981,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2204,15 +2199,15 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.33203125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="47.28515625" style="17" customWidth="1"/>
     <col min="2" max="2" width="18" style="19" customWidth="1"/>
-    <col min="3" max="5" width="9.109375" style="17"/>
-    <col min="6" max="6" width="13.88671875" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="17"/>
+    <col min="3" max="5" width="9.140625" style="17"/>
+    <col min="6" max="6" width="13.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -2702,29 +2697,29 @@
   <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q19" sqref="Q19"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="57.7109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="11" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="4" customWidth="1"/>
     <col min="4" max="4" width="11" style="5" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" style="6" customWidth="1"/>
     <col min="8" max="10" width="7" style="6" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" style="6" customWidth="1"/>
-    <col min="12" max="13" width="7.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="7.88671875" style="6" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="6" customWidth="1"/>
+    <col min="12" max="13" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="7.85546875" style="6" customWidth="1"/>
     <col min="16" max="16" width="14" style="6" customWidth="1"/>
-    <col min="17" max="18" width="14.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="14.44140625" style="6" customWidth="1"/>
-    <col min="22" max="16384" width="9.109375" style="6"/>
+    <col min="17" max="18" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="14.42578125" style="6" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -2923,14 +2918,8 @@
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="5">
-        <v>50</v>
-      </c>
-      <c r="E8" s="6">
-        <v>50</v>
-      </c>
       <c r="O8" s="6">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="Q8" s="10">
         <v>100</v>
@@ -3196,7 +3185,7 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">

</xml_diff>

<commit_message>
Rename NGO intervention to dots_groupcontributor for generality
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -147,9 +147,6 @@
     <t>int_perc_firstline_dst</t>
   </si>
   <si>
-    <t>int_perc_ngo_activities</t>
-  </si>
-  <si>
     <t>Months of treatment x 4 weeks x 10 BNG per week x EUR exchange rate x treatment success rate</t>
   </si>
   <si>
@@ -283,6 +280,9 @@
   </si>
   <si>
     <t>int_perc_dots_contributor</t>
+  </si>
+  <si>
+    <t>int_perc_dots_groupcontributor</t>
   </si>
 </sst>
 </file>
@@ -2230,7 +2230,7 @@
     </row>
     <row r="3" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="18">
         <v>2</v>
@@ -2240,7 +2240,7 @@
     </row>
     <row r="4" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="18">
         <v>1920</v>
@@ -2250,7 +2250,7 @@
     </row>
     <row r="5" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="18">
         <v>1920</v>
@@ -2260,7 +2260,7 @@
     </row>
     <row r="6" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" s="18">
         <v>1.2</v>
@@ -2357,7 +2357,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" s="24">
         <v>1950</v>
@@ -2394,7 +2394,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19" s="19">
         <v>0.6</v>
@@ -2402,7 +2402,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B20" s="19">
         <v>0.03</v>
@@ -2410,7 +2410,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B21" s="19">
         <v>0.03</v>
@@ -2418,18 +2418,18 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B22" s="19">
         <v>92</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B23" s="19">
         <v>0</v>
@@ -2437,7 +2437,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B24" s="19">
         <v>0</v>
@@ -2445,7 +2445,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B25" s="19">
         <v>0</v>
@@ -2453,7 +2453,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B26" s="19">
         <v>1</v>
@@ -2461,18 +2461,18 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B27" s="19">
         <v>857</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B28" s="19">
         <v>0</v>
@@ -2480,7 +2480,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B29" s="19">
         <v>0</v>
@@ -2488,7 +2488,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B30" s="19">
         <v>0</v>
@@ -2496,7 +2496,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B31" s="19">
         <v>1</v>
@@ -2504,19 +2504,19 @@
     </row>
     <row r="32" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B32" s="17">
         <f>1.02+67.12</f>
         <v>68.14</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B33" s="17">
         <v>0</v>
@@ -2524,18 +2524,18 @@
     </row>
     <row r="34" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B34" s="17">
         <v>8028</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B35" s="17">
         <v>1</v>
@@ -2543,7 +2543,7 @@
     </row>
     <row r="36" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B36" s="17">
         <v>1</v>
@@ -2551,7 +2551,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B37" s="26">
         <v>6094</v>
@@ -2559,7 +2559,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B38" s="25">
         <v>0</v>
@@ -2567,7 +2567,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B39" s="17">
         <v>0</v>
@@ -2575,7 +2575,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B40" s="17">
         <v>0.9</v>
@@ -2583,7 +2583,7 @@
     </row>
     <row r="41" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B41" s="17">
         <v>751</v>
@@ -2591,7 +2591,7 @@
     </row>
     <row r="42" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B42" s="17">
         <v>0</v>
@@ -2599,7 +2599,7 @@
     </row>
     <row r="43" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B43" s="17">
         <v>0</v>
@@ -2607,7 +2607,7 @@
     </row>
     <row r="44" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B44" s="17">
         <v>0</v>
@@ -2615,7 +2615,7 @@
     </row>
     <row r="45" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B45" s="17">
         <v>1</v>
@@ -2623,7 +2623,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B46" s="17">
         <v>862</v>
@@ -2631,7 +2631,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B47" s="17">
         <v>0</v>
@@ -2639,7 +2639,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B48" s="17">
         <v>0</v>
@@ -2647,7 +2647,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B49" s="17">
         <v>0</v>
@@ -2655,7 +2655,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B50" s="17">
         <v>1</v>
@@ -2700,7 +2700,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2838,7 +2838,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>
@@ -2856,7 +2856,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>4</v>
@@ -2913,7 +2913,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>4</v>
@@ -2932,7 +2932,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>4</v>
@@ -2950,7 +2950,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>4</v>
@@ -2968,7 +2968,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Update readme and Bulgaria sheet
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -2697,10 +2697,10 @@
   <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T11" sqref="T11"/>
+      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2882,28 +2882,10 @@
         <v>0</v>
       </c>
       <c r="J7" s="6">
-        <f>80*(1174/2649)</f>
-        <v>35.454888637221593</v>
-      </c>
-      <c r="K7" s="6">
-        <f>80*(1077/2407)</f>
-        <v>35.795596177814708</v>
-      </c>
-      <c r="L7" s="6">
-        <f>80*(1094/2280)</f>
-        <v>38.385964912280699</v>
-      </c>
-      <c r="M7" s="6">
-        <f>80*(961/1932)</f>
-        <v>39.792960662525878</v>
-      </c>
-      <c r="N7" s="6">
-        <f>80*(891/1872)</f>
-        <v>38.076923076923073</v>
+        <v>80</v>
       </c>
       <c r="O7" s="6">
-        <f>80*782/1660</f>
-        <v>37.686746987951807</v>
+        <v>86</v>
       </c>
       <c r="Q7" s="6">
         <v>95</v>
@@ -3061,10 +3043,10 @@
         <v>4</v>
       </c>
       <c r="G15" s="6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="O15" s="6">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U15" s="6">
         <v>5.0999999999999996</v>

</xml_diff>

<commit_message>
Really strange debug to population adjustment
Can't understand how the code as it stands would ever have run, but seems fixed now.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="89">
   <si>
     <t>parameter</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>int_perc_dots_groupcontributor</t>
+  </si>
+  <si>
+    <t>target_population</t>
   </si>
 </sst>
 </file>
@@ -1895,8 +1898,8 @@
       <sheetName val="dropdown_lists"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
@@ -2193,10 +2196,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2225,6 +2228,12 @@
       <c r="B2" s="13">
         <v>3</v>
       </c>
+      <c r="C2" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="D2" s="14">
+        <v>40</v>
+      </c>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
     </row>
@@ -2301,116 +2310,118 @@
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="23">
+        <v>7128000</v>
+      </c>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B11" s="19">
         <v>2.4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B12" s="16">
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
+    <row r="13" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B13" s="13">
         <f>20/12</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="17"/>
-    </row>
-    <row r="13" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="16">
-        <v>0.4</v>
-      </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="17" t="s">
-        <v>31</v>
-      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="17"/>
     </row>
     <row r="14" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="16">
-        <v>0.89</v>
+        <v>0.4</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="16">
+        <v>0.89</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B16" s="24">
         <v>1950</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="17" t="s">
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="17" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="19">
-        <v>1990</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="19">
-        <v>6</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="19">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="B19" s="19">
-        <v>0.6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B20" s="19">
-        <v>0.03</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B21" s="19">
         <v>0.03</v>
@@ -2418,26 +2429,26 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B22" s="19">
-        <v>92</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>42</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B23" s="19">
-        <v>0</v>
+        <v>92</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B24" s="19">
         <v>0</v>
@@ -2445,7 +2456,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25" s="19">
         <v>0</v>
@@ -2453,34 +2464,34 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B27" s="19">
-        <v>857</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B28" s="19">
-        <v>0</v>
+        <v>857</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B29" s="19">
         <v>0</v>
@@ -2488,7 +2499,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B30" s="19">
         <v>0</v>
@@ -2496,174 +2507,182 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="B31" s="19">
+      <c r="B32" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="17" t="s">
+    <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B32" s="17">
+      <c r="B33" s="17">
         <f>1.02+67.12</f>
         <v>68.14</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E33" s="14" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B33" s="17">
-        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B34" s="17">
-        <v>8028</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B35" s="17">
-        <v>1</v>
+        <v>8028</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B36" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B37" s="26">
-        <v>6094</v>
+        <v>67</v>
+      </c>
+      <c r="B37" s="17">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B38" s="25">
-        <v>0</v>
+        <v>45</v>
+      </c>
+      <c r="B38" s="26">
+        <v>6094</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B39" s="17">
+        <v>46</v>
+      </c>
+      <c r="B39" s="25">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B40" s="17">
+      <c r="B41" s="17">
         <v>0.9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41" s="17">
-        <v>751</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" s="17">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="17" t="s">
         <v>54</v>
-      </c>
-      <c r="B42" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="17" t="s">
-        <v>55</v>
       </c>
       <c r="B43" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B44" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B45" s="17">
+      <c r="B46" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="17" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B46" s="17">
+      <c r="B47" s="17">
         <v>862</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="17" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="17" t="s">
         <v>59</v>
-      </c>
-      <c r="B47" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="17" t="s">
-        <v>60</v>
       </c>
       <c r="B48" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B49" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B50" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B50" s="17">
+      <c r="B51" s="17">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9 F9:G9 B3">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B10 F9:G10 B3">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
@@ -2676,7 +2695,7 @@
       <formula2>1</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age unstratified" prompt="Some values you can replace the ones to the left with if you want a manual calibration for the model without age stratification." sqref="H1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15:D15 B4:B6">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16:D16 B4:B6">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
@@ -2684,7 +2703,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B12" unlockedFormula="1"/>
+    <ignoredError sqref="B13" unlockedFormula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2694,13 +2713,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2713,16 +2732,15 @@
     <col min="6" max="6" width="7.42578125" style="6" customWidth="1"/>
     <col min="7" max="7" width="7.5703125" style="6" customWidth="1"/>
     <col min="8" max="10" width="7" style="6" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="6" customWidth="1"/>
-    <col min="12" max="13" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="7.85546875" style="6" customWidth="1"/>
-    <col min="16" max="17" width="14" style="6" customWidth="1"/>
-    <col min="18" max="18" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="14.42578125" style="6" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="6"/>
+    <col min="11" max="12" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.85546875" style="6" customWidth="1"/>
+    <col min="14" max="15" width="14" style="6" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="14.42578125" style="6" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>6</v>
       </c>
@@ -2754,56 +2772,50 @@
         <v>2010</v>
       </c>
       <c r="K1" s="1">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="L1" s="1">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="M1" s="1">
-        <v>2013</v>
-      </c>
-      <c r="N1" s="1">
-        <v>2014</v>
-      </c>
-      <c r="O1" s="1">
         <v>2015</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="P1" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="6">
+      <c r="M2" s="6">
         <v>0</v>
       </c>
-      <c r="P2" s="6">
+      <c r="N2" s="6">
         <v>80</v>
       </c>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>39</v>
       </c>
@@ -2816,10 +2828,10 @@
       <c r="J3" s="6">
         <v>60</v>
       </c>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>40</v>
       </c>
@@ -2832,11 +2844,11 @@
       <c r="J4" s="6">
         <v>60</v>
       </c>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>75</v>
       </c>
@@ -2849,11 +2861,11 @@
       <c r="J5" s="6">
         <v>100</v>
       </c>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
       <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>74</v>
       </c>
@@ -2866,11 +2878,11 @@
       <c r="J6" s="6">
         <v>50</v>
       </c>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
       <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>41</v>
       </c>
@@ -2884,81 +2896,81 @@
       <c r="J7" s="6">
         <v>80</v>
       </c>
+      <c r="M7" s="6">
+        <v>86</v>
+      </c>
       <c r="O7" s="6">
-        <v>86</v>
-      </c>
-      <c r="Q7" s="6">
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>87</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O8" s="6">
+      <c r="M8" s="6">
         <v>100</v>
       </c>
-      <c r="R8" s="10">
+      <c r="P8" s="10">
         <v>0</v>
       </c>
+      <c r="Q8" s="10"/>
       <c r="S8" s="10"/>
-      <c r="U8" s="10"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>86</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O9" s="6">
+      <c r="M9" s="6">
         <v>100</v>
       </c>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10">
+        <v>0</v>
+      </c>
       <c r="R9" s="10"/>
-      <c r="S9" s="10">
-        <v>0</v>
-      </c>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S9" s="10"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>52</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O10" s="6">
+      <c r="M10" s="6">
         <v>0</v>
       </c>
-      <c r="R10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="6">
+        <v>99</v>
+      </c>
       <c r="S10" s="10"/>
-      <c r="T10" s="6">
-        <v>99</v>
-      </c>
-      <c r="U10" s="10"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>63</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O11" s="6">
+      <c r="M11" s="6">
         <v>0</v>
       </c>
-      <c r="R11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="6">
+        <v>99</v>
+      </c>
       <c r="S11" s="10"/>
-      <c r="T11" s="6">
-        <v>99</v>
-      </c>
-      <c r="U11" s="10"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>21</v>
       </c>
@@ -2983,22 +2995,16 @@
         <v>100</v>
       </c>
       <c r="K12" s="11">
-        <v>104.647302904564</v>
+        <v>107.966804979253</v>
       </c>
       <c r="L12" s="11">
-        <v>107.966804979253</v>
+        <v>111.203319502075</v>
       </c>
       <c r="M12" s="11">
-        <v>111.203319502075</v>
-      </c>
-      <c r="N12" s="11">
-        <v>115.767634854772</v>
-      </c>
-      <c r="O12" s="11">
         <v>117.42738589211601</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>25</v>
       </c>
@@ -3011,17 +3017,17 @@
       <c r="I13" s="6">
         <v>5.6</v>
       </c>
+      <c r="K13" s="6">
+        <v>6</v>
+      </c>
       <c r="L13" s="6">
-        <v>6</v>
+        <v>7.63</v>
       </c>
       <c r="M13" s="6">
-        <v>7.63</v>
-      </c>
-      <c r="O13" s="6">
         <v>8.4</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>26</v>
       </c>
@@ -3031,11 +3037,11 @@
       <c r="G14" s="6">
         <v>1</v>
       </c>
-      <c r="O14" s="6">
+      <c r="M14" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>27</v>
       </c>
@@ -3045,14 +3051,14 @@
       <c r="G15" s="6">
         <v>8</v>
       </c>
-      <c r="O15" s="6">
+      <c r="M15" s="6">
         <v>8</v>
       </c>
-      <c r="U15" s="6">
+      <c r="S15" s="6">
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>28</v>
       </c>
@@ -3070,10 +3076,8 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-    </row>
-    <row r="19" spans="5:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -3083,10 +3087,8 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-    </row>
-    <row r="24" spans="5:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="5:13" x14ac:dyDescent="0.25">
       <c r="G24" s="8"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
@@ -3094,10 +3096,8 @@
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-    </row>
-    <row r="25" spans="5:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="5:13" x14ac:dyDescent="0.25">
       <c r="G25" s="8"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
@@ -3105,10 +3105,8 @@
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-    </row>
-    <row r="26" spans="5:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="5:13" x14ac:dyDescent="0.25">
       <c r="G26" s="8"/>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
@@ -3116,13 +3114,11 @@
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
       <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
     </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="3">
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7 E24:O26">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7 E24:M26">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Add Tan's estimates for DST coverage
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -2198,8 +2198,8 @@
   </sheetPr>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2600,7 +2600,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
         <v>53</v>
       </c>
@@ -2713,13 +2713,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:S26"/>
+  <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2731,16 +2731,17 @@
     <col min="5" max="5" width="7.140625" style="6" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" style="6" customWidth="1"/>
     <col min="7" max="7" width="7.5703125" style="6" customWidth="1"/>
-    <col min="8" max="10" width="7" style="6" customWidth="1"/>
-    <col min="11" max="12" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.85546875" style="6" customWidth="1"/>
-    <col min="14" max="15" width="14" style="6" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="14.42578125" style="6" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="6"/>
+    <col min="8" max="12" width="7" style="6" customWidth="1"/>
+    <col min="13" max="14" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.42578125" style="6" customWidth="1"/>
+    <col min="16" max="16" width="7.85546875" style="6" customWidth="1"/>
+    <col min="17" max="18" width="14" style="6" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="14.42578125" style="6" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>6</v>
       </c>
@@ -2769,53 +2770,62 @@
         <v>2008</v>
       </c>
       <c r="J1" s="1">
+        <v>2009</v>
+      </c>
+      <c r="K1" s="1">
         <v>2010</v>
       </c>
-      <c r="K1" s="1">
+      <c r="L1" s="1">
+        <v>2011</v>
+      </c>
+      <c r="M1" s="1">
         <v>2012</v>
       </c>
-      <c r="L1" s="1">
+      <c r="N1" s="1">
         <v>2013</v>
       </c>
-      <c r="M1" s="1">
+      <c r="O1" s="1">
+        <v>2014</v>
+      </c>
+      <c r="P1" s="1">
         <v>2015</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="6">
+      <c r="P2" s="6">
         <v>0</v>
       </c>
-      <c r="N2" s="6">
+      <c r="Q2" s="6">
         <v>80</v>
       </c>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>39</v>
       </c>
@@ -2825,13 +2835,13 @@
       <c r="H3" s="6">
         <v>0</v>
       </c>
-      <c r="J3" s="6">
+      <c r="K3" s="6">
         <v>60</v>
       </c>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>40</v>
       </c>
@@ -2841,14 +2851,14 @@
       <c r="H4" s="6">
         <v>0</v>
       </c>
-      <c r="J4" s="6">
+      <c r="K4" s="6">
         <v>60</v>
       </c>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>75</v>
       </c>
@@ -2858,14 +2868,14 @@
       <c r="G5" s="6">
         <v>0</v>
       </c>
-      <c r="J5" s="6">
+      <c r="K5" s="6">
         <v>100</v>
       </c>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>74</v>
       </c>
@@ -2875,14 +2885,14 @@
       <c r="G6" s="6">
         <v>0</v>
       </c>
-      <c r="J6" s="6">
+      <c r="K6" s="6">
         <v>50</v>
       </c>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>41</v>
       </c>
@@ -2894,83 +2904,105 @@
         <v>0</v>
       </c>
       <c r="J7" s="6">
-        <v>80</v>
+        <f>844/1280*100</f>
+        <v>65.9375</v>
+      </c>
+      <c r="K7" s="6">
+        <f>966/1174*100</f>
+        <v>82.282793867120958</v>
+      </c>
+      <c r="L7" s="6">
+        <f>745/1077*100</f>
+        <v>69.173630454967508</v>
       </c>
       <c r="M7" s="6">
-        <v>86</v>
+        <f>829/1091*100</f>
+        <v>75.985334555453704</v>
+      </c>
+      <c r="N7" s="6">
+        <f>734/951*100</f>
+        <v>77.181913774973708</v>
       </c>
       <c r="O7" s="6">
+        <f>740/891*100</f>
+        <v>83.052749719416383</v>
+      </c>
+      <c r="P7" s="6">
+        <f>674/782*100</f>
+        <v>86.189258312020456</v>
+      </c>
+      <c r="R7" s="6">
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>87</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="M8" s="6">
+      <c r="P8" s="6">
         <v>100</v>
       </c>
-      <c r="P8" s="10">
+      <c r="S8" s="10">
         <v>0</v>
       </c>
-      <c r="Q8" s="10"/>
-      <c r="S8" s="10"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T8" s="10"/>
+      <c r="V8" s="10"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>86</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="M9" s="6">
+      <c r="P9" s="6">
         <v>100</v>
       </c>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10">
+      <c r="S9" s="10"/>
+      <c r="T9" s="10">
         <v>0</v>
       </c>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>52</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="M10" s="6">
+      <c r="P10" s="6">
         <v>0</v>
       </c>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="6">
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="6">
         <v>99</v>
       </c>
-      <c r="S10" s="10"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V10" s="10"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>63</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="M11" s="6">
+      <c r="P11" s="6">
         <v>0</v>
       </c>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="6">
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="6">
         <v>99</v>
       </c>
-      <c r="S11" s="10"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V11" s="10"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>21</v>
       </c>
@@ -2991,20 +3023,23 @@
         <v>82.987551867219906</v>
       </c>
       <c r="I12" s="11"/>
-      <c r="J12" s="11">
+      <c r="J12" s="11"/>
+      <c r="K12" s="11">
         <v>100</v>
       </c>
-      <c r="K12" s="11">
+      <c r="L12" s="11"/>
+      <c r="M12" s="11">
         <v>107.966804979253</v>
       </c>
-      <c r="L12" s="11">
+      <c r="N12" s="11">
         <v>111.203319502075</v>
       </c>
-      <c r="M12" s="11">
+      <c r="O12" s="11"/>
+      <c r="P12" s="11">
         <v>117.42738589211601</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>25</v>
       </c>
@@ -3017,17 +3052,17 @@
       <c r="I13" s="6">
         <v>5.6</v>
       </c>
-      <c r="K13" s="6">
+      <c r="M13" s="6">
         <v>6</v>
       </c>
-      <c r="L13" s="6">
+      <c r="N13" s="6">
         <v>7.63</v>
       </c>
-      <c r="M13" s="6">
+      <c r="P13" s="6">
         <v>8.4</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>26</v>
       </c>
@@ -3037,11 +3072,11 @@
       <c r="G14" s="6">
         <v>1</v>
       </c>
-      <c r="M14" s="6">
+      <c r="P14" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>27</v>
       </c>
@@ -3051,14 +3086,14 @@
       <c r="G15" s="6">
         <v>8</v>
       </c>
-      <c r="M15" s="6">
+      <c r="P15" s="6">
         <v>8</v>
       </c>
-      <c r="S15" s="6">
+      <c r="V15" s="6">
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>28</v>
       </c>
@@ -3076,8 +3111,11 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
-    </row>
-    <row r="19" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+    </row>
+    <row r="19" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -3087,38 +3125,50 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
-    </row>
-    <row r="24" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+    </row>
+    <row r="24" spans="5:16" x14ac:dyDescent="0.25">
       <c r="G24" s="8"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
-      <c r="J24" s="8"/>
+      <c r="J24" s="7"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
-    </row>
-    <row r="25" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+    </row>
+    <row r="25" spans="5:16" x14ac:dyDescent="0.25">
       <c r="G25" s="8"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
-      <c r="J25" s="8"/>
+      <c r="J25" s="7"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
-    </row>
-    <row r="26" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+    </row>
+    <row r="26" spans="5:16" x14ac:dyDescent="0.25">
       <c r="G26" s="8"/>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
-      <c r="J26" s="8"/>
+      <c r="J26" s="7"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
       <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
     </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="3">
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7 E24:M26">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7 E24:P26">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Update Bulgaria data spreadsheet
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdoan\Github\AuTuMN\autumn\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807" activeTab="1"/>
   </bookViews>
@@ -14,7 +19,7 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -291,7 +296,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -1949,7 +1954,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1982,9 +1987,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2017,6 +2039,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2446,7 +2485,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>77</v>
       </c>
@@ -2454,7 +2493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>78</v>
       </c>
@@ -2462,7 +2501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>79</v>
       </c>
@@ -2470,7 +2509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>80</v>
       </c>
@@ -2478,7 +2517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>81</v>
       </c>
@@ -2489,7 +2528,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>82</v>
       </c>
@@ -2497,7 +2536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>83</v>
       </c>
@@ -2505,7 +2544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>84</v>
       </c>
@@ -2513,7 +2552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>85</v>
       </c>
@@ -2521,7 +2560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
         <v>71</v>
       </c>
@@ -2533,7 +2572,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>70</v>
       </c>
@@ -2541,7 +2580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>69</v>
       </c>
@@ -2552,7 +2591,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
         <v>68</v>
       </c>
@@ -2560,7 +2599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>67</v>
       </c>
@@ -2568,7 +2607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
         <v>45</v>
       </c>
@@ -2576,7 +2615,7 @@
         <v>6094</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
         <v>46</v>
       </c>
@@ -2584,7 +2623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
         <v>47</v>
       </c>
@@ -2592,7 +2631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
         <v>48</v>
       </c>
@@ -2716,10 +2755,10 @@
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P8" sqref="P8"/>
+      <selection pane="bottomRight" activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2820,7 +2859,7 @@
         <v>0</v>
       </c>
       <c r="Q2" s="6">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="S2" s="10"/>
       <c r="T2" s="10"/>
@@ -2832,11 +2871,14 @@
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="6">
+      <c r="G3" s="6">
         <v>0</v>
       </c>
+      <c r="I3" s="6">
+        <v>60</v>
+      </c>
       <c r="K3" s="6">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="S3" s="10"/>
       <c r="T3" s="10"/>
@@ -2848,11 +2890,14 @@
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="6">
+      <c r="G4" s="6">
         <v>0</v>
       </c>
+      <c r="I4" s="6">
+        <v>60</v>
+      </c>
       <c r="K4" s="6">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
@@ -2961,7 +3006,9 @@
       <c r="P9" s="6">
         <v>100</v>
       </c>
-      <c r="S9" s="10"/>
+      <c r="S9" s="10">
+        <v>0</v>
+      </c>
       <c r="T9" s="10">
         <v>0</v>
       </c>
@@ -3184,7 +3231,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="382" yWindow="552" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[1]dropdown_lists!#REF!</xm:f>
+            <xm:f>'C:\Users\ntdoan\Github\AuTuMN\autumn\xls\[data_default.xlsx]dropdown_lists'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B7</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
Loose manual calibration for Bulgaria
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdoan\Github\AuTuMN\autumn\xls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="615" windowWidth="16275" windowHeight="6300" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -296,7 +291,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -1898,14 +1893,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="constants"/>
-      <sheetName val="time_variants"/>
       <sheetName val="dropdown_lists"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1954,7 +1945,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1987,26 +1978,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2039,23 +2013,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2237,8 +2194,8 @@
   </sheetPr>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2265,7 +2222,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="13">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="C2" s="14">
         <v>1.5</v>
@@ -2442,7 +2399,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>37</v>
       </c>
@@ -2450,7 +2407,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>66</v>
       </c>
@@ -2458,7 +2415,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>72</v>
       </c>
@@ -2466,7 +2423,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>73</v>
       </c>
@@ -2474,7 +2431,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>76</v>
       </c>
@@ -2752,13 +2709,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:V26"/>
+  <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R7" sqref="R7"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3162,19 +3119,31 @@
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
     </row>
-    <row r="19" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
+    <row r="18" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+    </row>
+    <row r="23" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="G23" s="8"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
     </row>
     <row r="24" spans="5:16" x14ac:dyDescent="0.25">
       <c r="G24" s="8"/>
@@ -3200,22 +3169,10 @@
       <c r="O25" s="8"/>
       <c r="P25" s="8"/>
     </row>
-    <row r="26" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="G26" s="8"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
-    </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="3">
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7 E24:P26">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7 E23:P25">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -3231,7 +3188,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="382" yWindow="552" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'C:\Users\ntdoan\Github\AuTuMN\autumn\xls\[data_default.xlsx]dropdown_lists'!#REF!</xm:f>
+            <xm:f>[1]dropdown_lists!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B7</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
Move DST coverage take-off from 1995 to 2008
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -307,7 +307,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -1180,7 +1180,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="662" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="662" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="662" applyFont="1"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1">
@@ -2700,10 +2700,10 @@
   <dimension ref="A1:W25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T11" sqref="T11"/>
+      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2897,7 +2897,7 @@
         <v>71</v>
       </c>
       <c r="D7" s="19"/>
-      <c r="E7" s="6">
+      <c r="I7" s="6">
         <v>0</v>
       </c>
       <c r="J7" s="6">

</xml_diff>

<commit_message>
Adjust initial population size following changes in demo data
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="6588" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="6588" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -2161,8 +2161,8 @@
   </sheetPr>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2269,7 +2269,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="20">
-        <v>10000000</v>
+        <v>7500000</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
@@ -2699,7 +2699,7 @@
   </sheetPr>
   <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
Change order of scenarios (Negative interventions at the end)
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="6588" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="6588" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -1153,7 +1153,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="662" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="3" xfId="662" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1189,6 +1189,11 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="661" applyFont="1"/>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="662" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="662" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="662" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="663">
@@ -2161,8 +2166,8 @@
   </sheetPr>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2190,13 +2195,16 @@
         <v>2</v>
       </c>
       <c r="B2" s="11">
-        <v>2.7122322346359198</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C2" s="14">
         <v>1.5</v>
       </c>
       <c r="D2" s="14">
         <v>40</v>
+      </c>
+      <c r="E2" s="14">
+        <v>2.7122322346359198</v>
       </c>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
@@ -2355,7 +2363,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="16">
-        <v>1990</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -2697,13 +2705,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:W25"/>
+  <dimension ref="A1:W34"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="Y23" sqref="Y23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2865,12 +2873,11 @@
       <c r="K5" s="6">
         <v>50</v>
       </c>
-      <c r="S5" s="9"/>
+      <c r="S5" s="9">
+        <v>100</v>
+      </c>
       <c r="T5" s="9"/>
       <c r="U5" s="9"/>
-      <c r="V5" s="6">
-        <v>100</v>
-      </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
@@ -2942,11 +2949,11 @@
       <c r="P8" s="6">
         <v>100</v>
       </c>
-      <c r="S8" s="9">
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="V8" s="9">
         <v>0</v>
       </c>
-      <c r="T8" s="9"/>
-      <c r="V8" s="9"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
@@ -2958,14 +2965,14 @@
       <c r="P9" s="6">
         <v>100</v>
       </c>
-      <c r="S9" s="9">
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9">
         <v>0</v>
       </c>
-      <c r="T9" s="9">
+      <c r="V9" s="9">
         <v>0</v>
       </c>
-      <c r="U9" s="9"/>
-      <c r="V9" s="9"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
@@ -2978,9 +2985,8 @@
         <v>0</v>
       </c>
       <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="6">
-        <v>99</v>
+      <c r="T10" s="9">
+        <v>100</v>
       </c>
       <c r="V10" s="9"/>
     </row>
@@ -2995,9 +3001,8 @@
         <v>0</v>
       </c>
       <c r="S11" s="9"/>
-      <c r="T11" s="9"/>
-      <c r="U11" s="6">
-        <v>99</v>
+      <c r="T11" s="9">
+        <v>100</v>
       </c>
       <c r="V11" s="9"/>
     </row>
@@ -3109,7 +3114,7 @@
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
     </row>
-    <row r="18" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:23" x14ac:dyDescent="0.3">
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -3123,25 +3128,84 @@
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
     </row>
-    <row r="23" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:23" x14ac:dyDescent="0.3">
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" spans="5:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:23" x14ac:dyDescent="0.3">
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
-    </row>
-    <row r="25" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="Q24" s="24"/>
+      <c r="R24" s="24"/>
+      <c r="S24" s="24"/>
+      <c r="T24" s="24"/>
+      <c r="U24" s="24"/>
+      <c r="V24" s="24"/>
+      <c r="W24" s="24"/>
+    </row>
+    <row r="25" spans="5:23" x14ac:dyDescent="0.3">
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="25"/>
+      <c r="S25" s="26"/>
+      <c r="T25" s="26"/>
+      <c r="U25" s="25"/>
+      <c r="V25" s="25"/>
+      <c r="W25" s="25"/>
+    </row>
+    <row r="26" spans="5:23" x14ac:dyDescent="0.3">
+      <c r="Q26" s="25"/>
+      <c r="R26" s="25"/>
+      <c r="S26" s="26"/>
+      <c r="T26" s="26"/>
+      <c r="U26" s="25"/>
+      <c r="V26" s="25"/>
+      <c r="W26" s="25"/>
+    </row>
+    <row r="27" spans="5:23" x14ac:dyDescent="0.3">
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
+      <c r="U27" s="9"/>
+    </row>
+    <row r="28" spans="5:23" x14ac:dyDescent="0.3">
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+    </row>
+    <row r="29" spans="5:23" x14ac:dyDescent="0.3">
+      <c r="S29" s="9"/>
+      <c r="T29" s="9"/>
+      <c r="U29" s="9"/>
+    </row>
+    <row r="31" spans="5:23" x14ac:dyDescent="0.3">
+      <c r="S31" s="9"/>
+      <c r="T31" s="9"/>
+      <c r="V31" s="9"/>
+    </row>
+    <row r="32" spans="5:23" x14ac:dyDescent="0.3">
+      <c r="S32" s="9"/>
+      <c r="T32" s="9"/>
+      <c r="U32" s="9"/>
+      <c r="V32" s="9"/>
+    </row>
+    <row r="33" spans="19:22" x14ac:dyDescent="0.3">
+      <c r="S33" s="9"/>
+      <c r="T33" s="9"/>
+      <c r="V33" s="9"/>
+    </row>
+    <row r="34" spans="19:22" x14ac:dyDescent="0.3">
+      <c r="S34" s="9"/>
+      <c r="T34" s="9"/>
+      <c r="V34" s="9"/>
     </row>
   </sheetData>
   <dataValidations count="3">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7 E23:E25 F23:F25 G23:G25 H23:H25 I23:I25 J23:J25 K23:K25 L23:L25 M23:M25 N23:N25 O23:O25 P23:P25" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7 E23:P25" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Fix economics for Firstline
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="6588" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15120" windowHeight="5772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -134,27 +134,12 @@
     <t>econ_saturation_treatment_support_relative_mdr</t>
   </si>
   <si>
-    <t>econ_unitcost_improve_dst</t>
-  </si>
-  <si>
     <t>Transportation of culture + cost per DST</t>
   </si>
   <si>
-    <t>econ_inflectioncost_improve_dst</t>
-  </si>
-  <si>
-    <t>econ_startupcost_improve_dst</t>
-  </si>
-  <si>
     <t>3 extra staff, 223 EUR per month salary, assuming 1 year to get everything up to speed</t>
   </si>
   <si>
-    <t>econ_startupduration_improve_dst</t>
-  </si>
-  <si>
-    <t>econ_saturation_improve_dst</t>
-  </si>
-  <si>
     <t>econ_unitcost_shortcourse_mdr</t>
   </si>
   <si>
@@ -300,6 +285,21 @@
   </si>
   <si>
     <t>scenario_7</t>
+  </si>
+  <si>
+    <t>econ_unitcost_firstline_dst</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_firstline_dst</t>
+  </si>
+  <si>
+    <t>econ_startupcost_firstline_dst</t>
+  </si>
+  <si>
+    <t>econ_startupduration_firstline_dst</t>
+  </si>
+  <si>
+    <t>econ_saturation_firstline_dst</t>
   </si>
 </sst>
 </file>
@@ -2166,8 +2166,8 @@
   </sheetPr>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2203,9 +2203,6 @@
       <c r="D2" s="14">
         <v>40</v>
       </c>
-      <c r="E2" s="14">
-        <v>2.7122322346359198</v>
-      </c>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
     </row>
@@ -2494,19 +2491,19 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
-        <v>37</v>
+        <v>88</v>
       </c>
       <c r="B33" s="14">
         <f>1.02+67.12</f>
         <v>68.14</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="B34" s="14">
         <v>0</v>
@@ -2514,18 +2511,18 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="B35" s="14">
         <v>8028</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="14" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="B36" s="14">
         <v>1</v>
@@ -2533,7 +2530,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="14" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="B37" s="14">
         <v>1</v>
@@ -2541,7 +2538,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="14" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B38" s="23">
         <v>6094</v>
@@ -2549,7 +2546,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="14" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B39" s="22">
         <v>0</v>
@@ -2557,7 +2554,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="14" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B40" s="14">
         <v>0</v>
@@ -2565,7 +2562,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="14" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B41" s="14">
         <v>0.9</v>
@@ -2573,7 +2570,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B42" s="14">
         <v>751</v>
@@ -2581,7 +2578,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B43" s="14">
         <v>0</v>
@@ -2589,7 +2586,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="14" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B44" s="14">
         <v>0</v>
@@ -2597,7 +2594,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="14" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B45" s="14">
         <v>0</v>
@@ -2605,7 +2602,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="14" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B46" s="14">
         <v>1</v>
@@ -2613,7 +2610,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="14" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B47" s="14">
         <v>862</v>
@@ -2621,7 +2618,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="14" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B48" s="14">
         <v>0</v>
@@ -2629,7 +2626,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="14" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B49" s="14">
         <v>0</v>
@@ -2637,7 +2634,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="14" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B50" s="14">
         <v>0</v>
@@ -2645,7 +2642,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="14" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B51" s="14">
         <v>1</v>
@@ -2653,7 +2650,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B52">
         <v>0.98131072044477996</v>
@@ -2661,7 +2658,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B53">
         <v>0.70077298513799691</v>
@@ -2669,7 +2666,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B54">
         <v>3.0599132140241752</v>
@@ -2707,11 +2704,11 @@
   </sheetPr>
   <dimension ref="A1:W34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y23" sqref="Y23"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2736,13 +2733,13 @@
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D1" s="1">
         <v>1920</v>
@@ -2784,33 +2781,33 @@
         <v>2015</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="W1" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="P2" s="6">
         <v>0</v>
@@ -2823,10 +2820,10 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G3" s="6">
         <v>0</v>
@@ -2842,10 +2839,10 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G4" s="6">
         <v>0</v>
@@ -2862,10 +2859,10 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G5" s="6">
         <v>0</v>
@@ -2881,10 +2878,10 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G6" s="6">
         <v>0</v>
@@ -2898,10 +2895,10 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D7" s="19"/>
       <c r="I7" s="6">
@@ -2941,10 +2938,10 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="P8" s="6">
         <v>100</v>
@@ -2957,10 +2954,10 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="P9" s="6">
         <v>100</v>
@@ -2976,10 +2973,10 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="P10" s="6">
         <v>0</v>
@@ -2992,10 +2989,10 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="P11" s="6">
         <v>0</v>
@@ -3008,10 +3005,10 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D12" s="5">
         <v>1</v>
@@ -3040,10 +3037,10 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H13" s="6">
         <v>5.4</v>
@@ -3063,10 +3060,10 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G14" s="6">
         <v>1</v>
@@ -3077,10 +3074,10 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G15" s="6">
         <v>8</v>
@@ -3094,10 +3091,10 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5">
@@ -3234,35 +3231,35 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add uncertainty ranges for Bulgaria interventions
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15120" windowHeight="5772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15120" windowHeight="5772" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -65,12 +65,6 @@
     <t>tb_timeperiod_ontreatment_mdr</t>
   </si>
   <si>
-    <t>program_prop_shortcourse_mdr_relativeduration</t>
-  </si>
-  <si>
-    <t>Proportional reduction in duration of MDR-TB treatment with short course treatment (also applies to duration of infectiousness)</t>
-  </si>
-  <si>
     <t>program_prop_treatment_success_shortcoursemdr</t>
   </si>
   <si>
@@ -300,6 +294,12 @@
   </si>
   <si>
     <t>econ_saturation_firstline_dst</t>
+  </si>
+  <si>
+    <t>scenario_15</t>
+  </si>
+  <si>
+    <t>int_timeperiod_shortcourse_mdr</t>
   </si>
 </sst>
 </file>
@@ -2166,8 +2166,8 @@
   </sheetPr>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A40" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2318,20 +2318,17 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="B14" s="13">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
-      <c r="E14" s="14" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" s="13">
         <v>0.89</v>
@@ -2339,12 +2336,12 @@
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" s="21">
         <v>1950</v>
@@ -2352,20 +2349,20 @@
       <c r="C16" s="21"/>
       <c r="D16" s="21"/>
       <c r="E16" s="14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B17" s="16">
-        <v>2010</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B18" s="16">
         <v>6</v>
@@ -2373,7 +2370,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" s="16">
         <v>13</v>
@@ -2381,7 +2378,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B20" s="16">
         <v>0.6</v>
@@ -2389,7 +2386,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21" s="16">
         <v>0.03</v>
@@ -2397,7 +2394,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B22" s="16">
         <v>0.03</v>
@@ -2405,18 +2402,18 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B23" s="16">
         <v>92</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B24" s="16">
         <v>0</v>
@@ -2424,7 +2421,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B25" s="16">
         <v>0</v>
@@ -2432,7 +2429,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B26" s="16">
         <v>0</v>
@@ -2440,7 +2437,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B27" s="16">
         <v>1</v>
@@ -2448,18 +2445,18 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B28" s="16">
         <v>857</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B29" s="16">
         <v>0</v>
@@ -2467,7 +2464,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B30" s="16">
         <v>0</v>
@@ -2475,7 +2472,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B31" s="16">
         <v>0</v>
@@ -2483,7 +2480,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B32" s="16">
         <v>1</v>
@@ -2491,19 +2488,19 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B33" s="14">
         <f>1.02+67.12</f>
         <v>68.14</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B34" s="14">
         <v>0</v>
@@ -2511,18 +2508,18 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B35" s="14">
         <v>8028</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B36" s="14">
         <v>1</v>
@@ -2530,7 +2527,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B37" s="14">
         <v>1</v>
@@ -2538,15 +2535,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B38" s="23">
-        <v>6094</v>
+        <f>6094-7861</f>
+        <v>-1767</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B39" s="22">
         <v>0</v>
@@ -2554,7 +2552,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B40" s="14">
         <v>0</v>
@@ -2562,7 +2560,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B41" s="14">
         <v>0.9</v>
@@ -2570,7 +2568,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B42" s="14">
         <v>751</v>
@@ -2578,7 +2576,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B43" s="14">
         <v>0</v>
@@ -2586,7 +2584,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B44" s="14">
         <v>0</v>
@@ -2594,7 +2592,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B45" s="14">
         <v>0</v>
@@ -2602,7 +2600,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B46" s="14">
         <v>1</v>
@@ -2610,7 +2608,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B47" s="14">
         <v>862</v>
@@ -2618,7 +2616,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B48" s="14">
         <v>0</v>
@@ -2626,7 +2624,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B49" s="14">
         <v>0</v>
@@ -2634,7 +2632,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B50" s="14">
         <v>0</v>
@@ -2642,7 +2640,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B51" s="14">
         <v>1</v>
@@ -2650,7 +2648,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B52">
         <v>0.98131072044477996</v>
@@ -2658,7 +2656,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B53">
         <v>0.70077298513799691</v>
@@ -2666,7 +2664,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B54">
         <v>3.0599132140241752</v>
@@ -2702,13 +2700,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:W34"/>
+  <dimension ref="A1:X34"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2726,20 +2724,19 @@
     <col min="16" max="16" width="7.88671875" style="6" customWidth="1"/>
     <col min="17" max="18" width="14" style="6" customWidth="1"/>
     <col min="19" max="19" width="14.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="14.44140625" style="6" customWidth="1"/>
-    <col min="23" max="23" width="9.109375" style="6" customWidth="1"/>
+    <col min="20" max="23" width="14.44140625" style="6" customWidth="1"/>
     <col min="24" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>56</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>58</v>
       </c>
       <c r="D1" s="1">
         <v>1920</v>
@@ -2781,33 +2778,36 @@
         <v>2015</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="P2" s="6">
         <v>0</v>
@@ -2818,12 +2818,12 @@
       <c r="S2" s="9"/>
       <c r="T2" s="9"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G3" s="6">
         <v>0</v>
@@ -2837,12 +2837,12 @@
       <c r="S3" s="9"/>
       <c r="T3" s="9"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G4" s="6">
         <v>0</v>
@@ -2857,12 +2857,12 @@
       <c r="T4" s="9"/>
       <c r="U4" s="9"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G5" s="6">
         <v>0</v>
@@ -2876,12 +2876,12 @@
       <c r="T5" s="9"/>
       <c r="U5" s="9"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G6" s="6">
         <v>0</v>
@@ -2893,12 +2893,12 @@
       <c r="T6" s="9"/>
       <c r="U6" s="9"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D7" s="19"/>
       <c r="I7" s="6">
@@ -2936,12 +2936,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="P8" s="6">
         <v>100</v>
@@ -2951,13 +2951,16 @@
       <c r="V8" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X8" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="P9" s="6">
         <v>100</v>
@@ -2970,13 +2973,16 @@
       <c r="V9" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="P10" s="6">
         <v>0</v>
@@ -2987,12 +2993,12 @@
       </c>
       <c r="V10" s="9"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="P11" s="6">
         <v>0</v>
@@ -3003,12 +3009,12 @@
       </c>
       <c r="V11" s="9"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D12" s="5">
         <v>1</v>
@@ -3035,12 +3041,12 @@
         <v>117.42738589211601</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H13" s="6">
         <v>5.4</v>
@@ -3058,12 +3064,12 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G14" s="6">
         <v>1</v>
@@ -3072,12 +3078,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G15" s="6">
         <v>8</v>
@@ -3089,12 +3095,12 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5">
@@ -3231,35 +3237,35 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move bulgaria-specific parameters to Bulgaria spreadsheet
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15120" windowHeight="5772" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15120" windowHeight="5772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="95">
   <si>
     <t>parameter</t>
   </si>
@@ -300,6 +300,12 @@
   </si>
   <si>
     <t>int_timeperiod_shortcourse_mdr</t>
+  </si>
+  <si>
+    <t>int_prop_detection_ngo_ruralpoor</t>
+  </si>
+  <si>
+    <t>int_prop_detection_dots_contributor</t>
   </si>
 </sst>
 </file>
@@ -1153,7 +1159,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="662" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="3" xfId="662" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1195,6 +1201,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="662" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="241"/>
   </cellXfs>
   <cellStyles count="663">
     <cellStyle name="Comma 2" xfId="614" xr:uid="{00000000-0005-0000-0000-000069020000}"/>
@@ -2164,10 +2171,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2401,35 +2408,49 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="16">
-        <v>92</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>25</v>
-      </c>
+      <c r="A23" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="27">
+        <v>0.25</v>
+      </c>
+      <c r="C23" s="27">
+        <v>0.15</v>
+      </c>
+      <c r="D23" s="27">
+        <v>0.35</v>
+      </c>
+      <c r="E23" s="27"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="16">
-        <v>0</v>
-      </c>
+      <c r="A24" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="27">
+        <v>0.08</v>
+      </c>
+      <c r="C24" s="27">
+        <v>0.05</v>
+      </c>
+      <c r="D24" s="27">
+        <v>0.12</v>
+      </c>
+      <c r="E24" s="27"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B25" s="16">
-        <v>0</v>
+        <v>92</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B26" s="16">
         <v>0</v>
@@ -2437,42 +2458,42 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B27" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B28" s="16">
-        <v>857</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B29" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B30" s="16">
-        <v>0</v>
+        <v>857</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B31" s="16">
         <v>0</v>
@@ -2480,119 +2501,119 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B32" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="B33" s="14">
+      <c r="B35" s="14">
         <f>1.02+67.12</f>
         <v>68.14</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E35" s="14" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B34" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B35" s="14">
-        <v>8028</v>
-      </c>
-      <c r="E35" s="14" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B36" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B37" s="14">
-        <v>1</v>
+        <v>8028</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="23">
+      <c r="B40" s="23">
         <f>6094-7861</f>
         <v>-1767</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B40" s="14">
-        <v>0</v>
-      </c>
-    </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41" s="14">
-        <v>0.9</v>
+        <v>38</v>
+      </c>
+      <c r="B41" s="22">
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B42" s="14">
-        <v>751</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B43" s="14">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B44" s="14">
-        <v>0</v>
+        <v>751</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B45" s="14">
         <v>0</v>
@@ -2600,92 +2621,122 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B46" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B47" s="14">
-        <v>862</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="14">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="14" t="s">
         <v>47</v>
-      </c>
-      <c r="B48" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B49" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="14" t="s">
-        <v>49</v>
       </c>
       <c r="B50" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B51" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="14">
+      <c r="B53" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>51</v>
       </c>
-      <c r="B52">
+      <c r="B54">
         <v>0.98131072044477996</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>52</v>
       </c>
-      <c r="B53">
+      <c r="B55">
         <v>0.70077298513799691</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>53</v>
       </c>
-      <c r="B54">
+      <c r="B56">
         <v>3.0599132140241752</v>
       </c>
+    </row>
+    <row r="59" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="14"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+    </row>
+    <row r="60" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="14"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 B9:B10 F9:F10 G9:G10" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 B9:B10 F9:G10" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 F2:F6 G2:G6" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 F2:G6" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7 F7:F8 G7:G8" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7 F7:G8" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age unstratified" prompt="Some values you can replace the ones to the left with if you want a manual calibration for the model without age stratification." sqref="H1" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B6 B16 C16 D16" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B6 B16:D16" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
@@ -2702,11 +2753,11 @@
   </sheetPr>
   <dimension ref="A1:X34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Bulgaria manual calibration with heterogenous mixing
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -2170,7 +2170,7 @@
   <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2198,7 +2198,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="9">
-        <v>10.5</v>
+        <v>2</v>
       </c>
       <c r="C2" s="12">
         <v>1.5</v>
@@ -2224,7 +2224,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="13">
-        <v>1860</v>
+        <v>1900</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -2347,7 +2347,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="19">
-        <v>1973</v>
+        <v>1960</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>

</xml_diff>

<commit_message>
Make MCMC adjustments  for Bulgaria run
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -2170,7 +2170,7 @@
   <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2181,8 +2181,8 @@
     <col min="6" max="6" width="13.88671875" style="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.88671875" style="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.109375" style="12" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="12"/>
+    <col min="9" max="11" width="9.109375" style="12" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -2201,10 +2201,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="12">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="D2" s="12">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -2347,7 +2347,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="19">
-        <v>1960</v>
+        <v>1961</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
@@ -2758,8 +2758,8 @@
     <col min="17" max="18" width="14" style="23" customWidth="1"/>
     <col min="19" max="19" width="14.44140625" style="23" bestFit="1" customWidth="1"/>
     <col min="20" max="23" width="14.44140625" style="23" customWidth="1"/>
-    <col min="24" max="24" width="9.109375" style="23" customWidth="1"/>
-    <col min="25" max="16384" width="9.109375" style="23"/>
+    <col min="24" max="25" width="9.109375" style="23" customWidth="1"/>
+    <col min="26" max="16384" width="9.109375" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Change saturation from 100% to 110% for Tx_support and ambulatory_care interventions
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rragonnet\Google Drive\GitHub\AuTuMN\AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FCD42E2D-DADC-468F-8C95-EE98A3FE090E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EE5CF711-BB06-4A23-9993-D3CDF59402AC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15120" windowHeight="5772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2176,8 +2176,8 @@
   </sheetPr>
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2480,7 +2480,7 @@
         <v>32</v>
       </c>
       <c r="B29" s="14">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -2523,7 +2523,7 @@
         <v>37</v>
       </c>
       <c r="B34" s="14">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -2646,7 +2646,7 @@
         <v>53</v>
       </c>
       <c r="B48" s="12">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -2689,7 +2689,7 @@
         <v>58</v>
       </c>
       <c r="B53" s="12">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -2749,10 +2749,10 @@
   <dimension ref="A1:X34"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S3" sqref="S3"/>
+      <selection pane="bottomRight" activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Increase Bulgaria mortality reporting to 100%
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rragonnet\Google Drive\GitHub\AuTuMN\AuTuMN\autumn\xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Documents\AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0641327F-B46E-4518-808C-34F84DE052A8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10356" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10350"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
     <sheet name="time_variants" sheetId="2" r:id="rId2"/>
     <sheet name="dropdown_lists" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -318,7 +317,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -1207,669 +1206,669 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="241"/>
   </cellXfs>
   <cellStyles count="663">
-    <cellStyle name="Comma 2" xfId="614" xr:uid="{00000000-0005-0000-0000-000066020000}"/>
-    <cellStyle name="Comma 2 2" xfId="626" xr:uid="{00000000-0005-0000-0000-000072020000}"/>
-    <cellStyle name="Input 2" xfId="378" xr:uid="{00000000-0005-0000-0000-00007A010000}"/>
+    <cellStyle name="Comma 2" xfId="614"/>
+    <cellStyle name="Comma 2 2" xfId="626"/>
+    <cellStyle name="Input 2" xfId="378"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="545" xr:uid="{00000000-0005-0000-0000-000021020000}"/>
-    <cellStyle name="Normal 2" xfId="449" xr:uid="{00000000-0005-0000-0000-0000C1010000}"/>
-    <cellStyle name="Normal 2 2" xfId="439" xr:uid="{00000000-0005-0000-0000-0000B7010000}"/>
-    <cellStyle name="Normal 3" xfId="448" xr:uid="{00000000-0005-0000-0000-0000C0010000}"/>
-    <cellStyle name="Normal 3 2" xfId="500" xr:uid="{00000000-0005-0000-0000-0000F4010000}"/>
-    <cellStyle name="Normal 4" xfId="451" xr:uid="{00000000-0005-0000-0000-0000C3010000}"/>
-    <cellStyle name="Normal 4 2" xfId="81" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
-    <cellStyle name="Normal 5" xfId="450" xr:uid="{00000000-0005-0000-0000-0000C2010000}"/>
-    <cellStyle name="Normal 5 2" xfId="242" xr:uid="{00000000-0005-0000-0000-0000F2000000}"/>
-    <cellStyle name="Normal 6" xfId="453" xr:uid="{00000000-0005-0000-0000-0000C5010000}"/>
-    <cellStyle name="Normal 6 10" xfId="41" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="Normal 6 10 2" xfId="121" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
-    <cellStyle name="Normal 6 10 2 2" xfId="168" xr:uid="{00000000-0005-0000-0000-0000A8000000}"/>
-    <cellStyle name="Normal 6 10 2 3" xfId="167" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
-    <cellStyle name="Normal 6 10 3" xfId="118" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
-    <cellStyle name="Normal 6 10 4" xfId="117" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
-    <cellStyle name="Normal 6 11" xfId="40" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="Normal 6 11 2" xfId="251" xr:uid="{00000000-0005-0000-0000-0000FB000000}"/>
-    <cellStyle name="Normal 6 11 2 2" xfId="421" xr:uid="{00000000-0005-0000-0000-0000A5010000}"/>
-    <cellStyle name="Normal 6 11 2 3" xfId="422" xr:uid="{00000000-0005-0000-0000-0000A6010000}"/>
-    <cellStyle name="Normal 6 11 3" xfId="252" xr:uid="{00000000-0005-0000-0000-0000FC000000}"/>
-    <cellStyle name="Normal 6 11 4" xfId="250" xr:uid="{00000000-0005-0000-0000-0000FA000000}"/>
-    <cellStyle name="Normal 6 12" xfId="43" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="Normal 6 12 2" xfId="227" xr:uid="{00000000-0005-0000-0000-0000E3000000}"/>
-    <cellStyle name="Normal 6 12 2 2" xfId="181" xr:uid="{00000000-0005-0000-0000-0000B5000000}"/>
-    <cellStyle name="Normal 6 12 2 3" xfId="180" xr:uid="{00000000-0005-0000-0000-0000B4000000}"/>
-    <cellStyle name="Normal 6 12 3" xfId="226" xr:uid="{00000000-0005-0000-0000-0000E2000000}"/>
-    <cellStyle name="Normal 6 12 4" xfId="225" xr:uid="{00000000-0005-0000-0000-0000E1000000}"/>
-    <cellStyle name="Normal 6 13" xfId="42" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="Normal 6 13 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="Normal 6 13 2 2" xfId="503" xr:uid="{00000000-0005-0000-0000-0000F7010000}"/>
-    <cellStyle name="Normal 6 13 2 3" xfId="504" xr:uid="{00000000-0005-0000-0000-0000F8010000}"/>
-    <cellStyle name="Normal 6 13 3" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Normal 6 13 4" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="Normal 6 14" xfId="45" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="Normal 6 14 2" xfId="337" xr:uid="{00000000-0005-0000-0000-000051010000}"/>
-    <cellStyle name="Normal 6 14 2 2" xfId="76" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
-    <cellStyle name="Normal 6 14 2 3" xfId="75" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Normal 6 14 3" xfId="336" xr:uid="{00000000-0005-0000-0000-000050010000}"/>
-    <cellStyle name="Normal 6 14 4" xfId="338" xr:uid="{00000000-0005-0000-0000-000052010000}"/>
-    <cellStyle name="Normal 6 15" xfId="44" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="Normal 6 15 2" xfId="130" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
-    <cellStyle name="Normal 6 15 3" xfId="131" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
-    <cellStyle name="Normal 6 16" xfId="47" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="Normal 6 17" xfId="46" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="Normal 6 2" xfId="315" xr:uid="{00000000-0005-0000-0000-00003B010000}"/>
-    <cellStyle name="Normal 6 2 10" xfId="233" xr:uid="{00000000-0005-0000-0000-0000E9000000}"/>
-    <cellStyle name="Normal 6 2 11" xfId="232" xr:uid="{00000000-0005-0000-0000-0000E8000000}"/>
-    <cellStyle name="Normal 6 2 2" xfId="578" xr:uid="{00000000-0005-0000-0000-000042020000}"/>
-    <cellStyle name="Normal 6 2 2 10" xfId="528" xr:uid="{00000000-0005-0000-0000-000010020000}"/>
-    <cellStyle name="Normal 6 2 2 2" xfId="465" xr:uid="{00000000-0005-0000-0000-0000D1010000}"/>
-    <cellStyle name="Normal 6 2 2 2 2" xfId="485" xr:uid="{00000000-0005-0000-0000-0000E5010000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 2" xfId="512" xr:uid="{00000000-0005-0000-0000-000000020000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 2 2" xfId="329" xr:uid="{00000000-0005-0000-0000-000049010000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 2 3" xfId="328" xr:uid="{00000000-0005-0000-0000-000048010000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 4" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 3" xfId="511" xr:uid="{00000000-0005-0000-0000-0000FF010000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 2" xfId="218" xr:uid="{00000000-0005-0000-0000-0000DA000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 2 2" xfId="67" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 2 3" xfId="68" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 3" xfId="219" xr:uid="{00000000-0005-0000-0000-0000DB000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 4" xfId="220" xr:uid="{00000000-0005-0000-0000-0000DC000000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 4" xfId="309" xr:uid="{00000000-0005-0000-0000-000035010000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 4 2" xfId="437" xr:uid="{00000000-0005-0000-0000-0000B5010000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 4 3" xfId="436" xr:uid="{00000000-0005-0000-0000-0000B4010000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 5" xfId="260" xr:uid="{00000000-0005-0000-0000-000004010000}"/>
-    <cellStyle name="Normal 6 2 2 2 2 6" xfId="508" xr:uid="{00000000-0005-0000-0000-0000FC010000}"/>
-    <cellStyle name="Normal 6 2 2 2 3" xfId="191" xr:uid="{00000000-0005-0000-0000-0000BF000000}"/>
-    <cellStyle name="Normal 6 2 2 2 3 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="Normal 6 2 2 2 3 2 2" xfId="496" xr:uid="{00000000-0005-0000-0000-0000F0010000}"/>
-    <cellStyle name="Normal 6 2 2 2 3 2 3" xfId="497" xr:uid="{00000000-0005-0000-0000-0000F1010000}"/>
-    <cellStyle name="Normal 6 2 2 2 3 3" xfId="57" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="Normal 6 2 2 2 3 4" xfId="54" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="Normal 6 2 2 2 4" xfId="178" xr:uid="{00000000-0005-0000-0000-0000B2000000}"/>
-    <cellStyle name="Normal 6 2 2 2 4 2" xfId="385" xr:uid="{00000000-0005-0000-0000-000081010000}"/>
-    <cellStyle name="Normal 6 2 2 2 4 2 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="Normal 6 2 2 2 4 2 3" xfId="71" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="Normal 6 2 2 2 4 3" xfId="384" xr:uid="{00000000-0005-0000-0000-000080010000}"/>
-    <cellStyle name="Normal 6 2 2 2 4 4" xfId="389" xr:uid="{00000000-0005-0000-0000-000085010000}"/>
-    <cellStyle name="Normal 6 2 2 2 5" xfId="177" xr:uid="{00000000-0005-0000-0000-0000B1000000}"/>
-    <cellStyle name="Normal 6 2 2 2 5 2" xfId="592" xr:uid="{00000000-0005-0000-0000-000050020000}"/>
-    <cellStyle name="Normal 6 2 2 2 5 3" xfId="593" xr:uid="{00000000-0005-0000-0000-000051020000}"/>
-    <cellStyle name="Normal 6 2 2 2 6" xfId="483" xr:uid="{00000000-0005-0000-0000-0000E3010000}"/>
-    <cellStyle name="Normal 6 2 2 2 7" xfId="482" xr:uid="{00000000-0005-0000-0000-0000E2010000}"/>
-    <cellStyle name="Normal 6 2 2 3" xfId="464" xr:uid="{00000000-0005-0000-0000-0000D0010000}"/>
-    <cellStyle name="Normal 6 2 2 3 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="Normal 6 2 2 3 2 2" xfId="230" xr:uid="{00000000-0005-0000-0000-0000E6000000}"/>
-    <cellStyle name="Normal 6 2 2 3 2 2 2" xfId="560" xr:uid="{00000000-0005-0000-0000-000030020000}"/>
-    <cellStyle name="Normal 6 2 2 3 2 2 3" xfId="561" xr:uid="{00000000-0005-0000-0000-000031020000}"/>
-    <cellStyle name="Normal 6 2 2 3 2 3" xfId="231" xr:uid="{00000000-0005-0000-0000-0000E7000000}"/>
-    <cellStyle name="Normal 6 2 2 3 2 4" xfId="228" xr:uid="{00000000-0005-0000-0000-0000E4000000}"/>
-    <cellStyle name="Normal 6 2 2 3 3" xfId="25" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="Normal 6 2 2 3 3 2" xfId="31" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="Normal 6 2 2 3 3 2 2" xfId="133" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
-    <cellStyle name="Normal 6 2 2 3 3 2 3" xfId="132" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
-    <cellStyle name="Normal 6 2 2 3 3 3" xfId="30" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="Normal 6 2 2 3 3 4" xfId="27" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="Normal 6 2 2 3 4" xfId="20" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="Normal 6 2 2 3 4 2" xfId="193" xr:uid="{00000000-0005-0000-0000-0000C1000000}"/>
-    <cellStyle name="Normal 6 2 2 3 4 3" xfId="194" xr:uid="{00000000-0005-0000-0000-0000C2000000}"/>
-    <cellStyle name="Normal 6 2 2 3 5" xfId="21" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="Normal 6 2 2 3 6" xfId="22" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="Normal 6 2 2 4" xfId="467" xr:uid="{00000000-0005-0000-0000-0000D3010000}"/>
-    <cellStyle name="Normal 6 2 2 4 2" xfId="206" xr:uid="{00000000-0005-0000-0000-0000CE000000}"/>
-    <cellStyle name="Normal 6 2 2 4 2 2" xfId="143" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
-    <cellStyle name="Normal 6 2 2 4 2 3" xfId="544" xr:uid="{00000000-0005-0000-0000-000020020000}"/>
-    <cellStyle name="Normal 6 2 2 4 3" xfId="205" xr:uid="{00000000-0005-0000-0000-0000CD000000}"/>
-    <cellStyle name="Normal 6 2 2 4 4" xfId="533" xr:uid="{00000000-0005-0000-0000-000015020000}"/>
-    <cellStyle name="Normal 6 2 2 5" xfId="466" xr:uid="{00000000-0005-0000-0000-0000D2010000}"/>
-    <cellStyle name="Normal 6 2 2 5 2" xfId="405" xr:uid="{00000000-0005-0000-0000-000095010000}"/>
-    <cellStyle name="Normal 6 2 2 5 2 2" xfId="248" xr:uid="{00000000-0005-0000-0000-0000F8000000}"/>
-    <cellStyle name="Normal 6 2 2 5 2 3" xfId="249" xr:uid="{00000000-0005-0000-0000-0000F9000000}"/>
-    <cellStyle name="Normal 6 2 2 5 3" xfId="406" xr:uid="{00000000-0005-0000-0000-000096010000}"/>
-    <cellStyle name="Normal 6 2 2 5 4" xfId="408" xr:uid="{00000000-0005-0000-0000-000098010000}"/>
-    <cellStyle name="Normal 6 2 2 6" xfId="469" xr:uid="{00000000-0005-0000-0000-0000D5010000}"/>
-    <cellStyle name="Normal 6 2 2 6 2" xfId="602" xr:uid="{00000000-0005-0000-0000-00005A020000}"/>
-    <cellStyle name="Normal 6 2 2 6 2 2" xfId="590" xr:uid="{00000000-0005-0000-0000-00004E020000}"/>
-    <cellStyle name="Normal 6 2 2 6 2 3" xfId="589" xr:uid="{00000000-0005-0000-0000-00004D020000}"/>
-    <cellStyle name="Normal 6 2 2 6 3" xfId="601" xr:uid="{00000000-0005-0000-0000-000059020000}"/>
-    <cellStyle name="Normal 6 2 2 6 4" xfId="603" xr:uid="{00000000-0005-0000-0000-00005B020000}"/>
-    <cellStyle name="Normal 6 2 2 7" xfId="468" xr:uid="{00000000-0005-0000-0000-0000D4010000}"/>
-    <cellStyle name="Normal 6 2 2 7 2" xfId="156" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
-    <cellStyle name="Normal 6 2 2 7 2 2" xfId="262" xr:uid="{00000000-0005-0000-0000-000006010000}"/>
-    <cellStyle name="Normal 6 2 2 7 2 3" xfId="263" xr:uid="{00000000-0005-0000-0000-000007010000}"/>
-    <cellStyle name="Normal 6 2 2 7 3" xfId="157" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
-    <cellStyle name="Normal 6 2 2 7 4" xfId="158" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
-    <cellStyle name="Normal 6 2 2 8" xfId="101" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
-    <cellStyle name="Normal 6 2 2 8 2" xfId="349" xr:uid="{00000000-0005-0000-0000-00005D010000}"/>
-    <cellStyle name="Normal 6 2 2 8 3" xfId="348" xr:uid="{00000000-0005-0000-0000-00005C010000}"/>
-    <cellStyle name="Normal 6 2 2 9" xfId="99" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
-    <cellStyle name="Normal 6 2 3" xfId="577" xr:uid="{00000000-0005-0000-0000-000041020000}"/>
-    <cellStyle name="Normal 6 2 3 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="Normal 6 2 3 2 2" xfId="294" xr:uid="{00000000-0005-0000-0000-000026010000}"/>
-    <cellStyle name="Normal 6 2 3 2 2 2" xfId="360" xr:uid="{00000000-0005-0000-0000-000068010000}"/>
-    <cellStyle name="Normal 6 2 3 2 2 2 2" xfId="526" xr:uid="{00000000-0005-0000-0000-00000E020000}"/>
-    <cellStyle name="Normal 6 2 3 2 2 2 3" xfId="527" xr:uid="{00000000-0005-0000-0000-00000F020000}"/>
-    <cellStyle name="Normal 6 2 3 2 2 3" xfId="361" xr:uid="{00000000-0005-0000-0000-000069010000}"/>
-    <cellStyle name="Normal 6 2 3 2 2 4" xfId="355" xr:uid="{00000000-0005-0000-0000-000063010000}"/>
-    <cellStyle name="Normal 6 2 3 2 3" xfId="295" xr:uid="{00000000-0005-0000-0000-000027010000}"/>
-    <cellStyle name="Normal 6 2 3 2 3 2" xfId="173" xr:uid="{00000000-0005-0000-0000-0000AD000000}"/>
-    <cellStyle name="Normal 6 2 3 2 3 2 2" xfId="443" xr:uid="{00000000-0005-0000-0000-0000BB010000}"/>
-    <cellStyle name="Normal 6 2 3 2 3 2 3" xfId="442" xr:uid="{00000000-0005-0000-0000-0000BA010000}"/>
-    <cellStyle name="Normal 6 2 3 2 3 3" xfId="172" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
-    <cellStyle name="Normal 6 2 3 2 3 4" xfId="169" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
-    <cellStyle name="Normal 6 2 3 2 4" xfId="289" xr:uid="{00000000-0005-0000-0000-000021010000}"/>
-    <cellStyle name="Normal 6 2 3 2 4 2" xfId="213" xr:uid="{00000000-0005-0000-0000-0000D5000000}"/>
-    <cellStyle name="Normal 6 2 3 2 4 3" xfId="214" xr:uid="{00000000-0005-0000-0000-0000D6000000}"/>
-    <cellStyle name="Normal 6 2 3 2 5" xfId="290" xr:uid="{00000000-0005-0000-0000-000022010000}"/>
-    <cellStyle name="Normal 6 2 3 2 6" xfId="291" xr:uid="{00000000-0005-0000-0000-000023010000}"/>
-    <cellStyle name="Normal 6 2 3 3" xfId="13" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="Normal 6 2 3 3 2" xfId="84" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
-    <cellStyle name="Normal 6 2 3 3 2 2" xfId="543" xr:uid="{00000000-0005-0000-0000-00001F020000}"/>
-    <cellStyle name="Normal 6 2 3 3 2 3" xfId="542" xr:uid="{00000000-0005-0000-0000-00001E020000}"/>
-    <cellStyle name="Normal 6 2 3 3 3" xfId="83" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
-    <cellStyle name="Normal 6 2 3 3 4" xfId="82" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="Normal 6 2 3 4" xfId="14" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="Normal 6 2 3 4 2" xfId="216" xr:uid="{00000000-0005-0000-0000-0000D8000000}"/>
-    <cellStyle name="Normal 6 2 3 4 2 2" xfId="660" xr:uid="{00000000-0005-0000-0000-000094020000}"/>
-    <cellStyle name="Normal 6 2 3 4 2 3" xfId="661" xr:uid="{00000000-0005-0000-0000-000095020000}"/>
-    <cellStyle name="Normal 6 2 3 4 3" xfId="55" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="Normal 6 2 3 4 4" xfId="223" xr:uid="{00000000-0005-0000-0000-0000DF000000}"/>
-    <cellStyle name="Normal 6 2 3 5" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="Normal 6 2 3 5 2" xfId="506" xr:uid="{00000000-0005-0000-0000-0000FA010000}"/>
-    <cellStyle name="Normal 6 2 3 5 3" xfId="505" xr:uid="{00000000-0005-0000-0000-0000F9010000}"/>
-    <cellStyle name="Normal 6 2 3 6" xfId="69" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="Normal 6 2 3 7" xfId="72" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
-    <cellStyle name="Normal 6 2 4" xfId="331" xr:uid="{00000000-0005-0000-0000-00004B010000}"/>
-    <cellStyle name="Normal 6 2 4 2" xfId="400" xr:uid="{00000000-0005-0000-0000-000090010000}"/>
-    <cellStyle name="Normal 6 2 4 2 2" xfId="256" xr:uid="{00000000-0005-0000-0000-000000010000}"/>
-    <cellStyle name="Normal 6 2 4 2 2 2" xfId="274" xr:uid="{00000000-0005-0000-0000-000012010000}"/>
-    <cellStyle name="Normal 6 2 4 2 2 3" xfId="270" xr:uid="{00000000-0005-0000-0000-00000E010000}"/>
-    <cellStyle name="Normal 6 2 4 2 3" xfId="255" xr:uid="{00000000-0005-0000-0000-0000FF000000}"/>
-    <cellStyle name="Normal 6 2 4 2 4" xfId="257" xr:uid="{00000000-0005-0000-0000-000001010000}"/>
-    <cellStyle name="Normal 6 2 4 3" xfId="399" xr:uid="{00000000-0005-0000-0000-00008F010000}"/>
-    <cellStyle name="Normal 6 2 4 3 2" xfId="458" xr:uid="{00000000-0005-0000-0000-0000CA010000}"/>
-    <cellStyle name="Normal 6 2 4 3 2 2" xfId="150" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
-    <cellStyle name="Normal 6 2 4 3 2 3" xfId="151" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
-    <cellStyle name="Normal 6 2 4 3 3" xfId="459" xr:uid="{00000000-0005-0000-0000-0000CB010000}"/>
-    <cellStyle name="Normal 6 2 4 3 4" xfId="463" xr:uid="{00000000-0005-0000-0000-0000CF010000}"/>
-    <cellStyle name="Normal 6 2 4 4" xfId="398" xr:uid="{00000000-0005-0000-0000-00008E010000}"/>
-    <cellStyle name="Normal 6 2 4 4 2" xfId="522" xr:uid="{00000000-0005-0000-0000-00000A020000}"/>
-    <cellStyle name="Normal 6 2 4 4 3" xfId="521" xr:uid="{00000000-0005-0000-0000-000009020000}"/>
-    <cellStyle name="Normal 6 2 4 5" xfId="397" xr:uid="{00000000-0005-0000-0000-00008D010000}"/>
-    <cellStyle name="Normal 6 2 4 6" xfId="396" xr:uid="{00000000-0005-0000-0000-00008C010000}"/>
-    <cellStyle name="Normal 6 2 5" xfId="330" xr:uid="{00000000-0005-0000-0000-00004A010000}"/>
-    <cellStyle name="Normal 6 2 5 2" xfId="569" xr:uid="{00000000-0005-0000-0000-000039020000}"/>
-    <cellStyle name="Normal 6 2 5 2 2" xfId="376" xr:uid="{00000000-0005-0000-0000-000078010000}"/>
-    <cellStyle name="Normal 6 2 5 2 3" xfId="377" xr:uid="{00000000-0005-0000-0000-000079010000}"/>
-    <cellStyle name="Normal 6 2 5 3" xfId="570" xr:uid="{00000000-0005-0000-0000-00003A020000}"/>
-    <cellStyle name="Normal 6 2 5 4" xfId="568" xr:uid="{00000000-0005-0000-0000-000038020000}"/>
-    <cellStyle name="Normal 6 2 6" xfId="333" xr:uid="{00000000-0005-0000-0000-00004D010000}"/>
-    <cellStyle name="Normal 6 2 6 2" xfId="632" xr:uid="{00000000-0005-0000-0000-000078020000}"/>
-    <cellStyle name="Normal 6 2 6 2 2" xfId="175" xr:uid="{00000000-0005-0000-0000-0000AF000000}"/>
-    <cellStyle name="Normal 6 2 6 2 3" xfId="174" xr:uid="{00000000-0005-0000-0000-0000AE000000}"/>
-    <cellStyle name="Normal 6 2 6 3" xfId="631" xr:uid="{00000000-0005-0000-0000-000077020000}"/>
-    <cellStyle name="Normal 6 2 6 4" xfId="630" xr:uid="{00000000-0005-0000-0000-000076020000}"/>
-    <cellStyle name="Normal 6 2 7" xfId="332" xr:uid="{00000000-0005-0000-0000-00004C010000}"/>
-    <cellStyle name="Normal 6 2 7 2" xfId="195" xr:uid="{00000000-0005-0000-0000-0000C3000000}"/>
-    <cellStyle name="Normal 6 2 7 2 2" xfId="635" xr:uid="{00000000-0005-0000-0000-00007B020000}"/>
-    <cellStyle name="Normal 6 2 7 2 3" xfId="636" xr:uid="{00000000-0005-0000-0000-00007C020000}"/>
-    <cellStyle name="Normal 6 2 7 3" xfId="196" xr:uid="{00000000-0005-0000-0000-0000C4000000}"/>
-    <cellStyle name="Normal 6 2 7 4" xfId="427" xr:uid="{00000000-0005-0000-0000-0000AB010000}"/>
-    <cellStyle name="Normal 6 2 8" xfId="335" xr:uid="{00000000-0005-0000-0000-00004F010000}"/>
-    <cellStyle name="Normal 6 2 8 2" xfId="474" xr:uid="{00000000-0005-0000-0000-0000DA010000}"/>
-    <cellStyle name="Normal 6 2 8 2 2" xfId="524" xr:uid="{00000000-0005-0000-0000-00000C020000}"/>
-    <cellStyle name="Normal 6 2 8 2 3" xfId="523" xr:uid="{00000000-0005-0000-0000-00000B020000}"/>
-    <cellStyle name="Normal 6 2 8 3" xfId="473" xr:uid="{00000000-0005-0000-0000-0000D9010000}"/>
-    <cellStyle name="Normal 6 2 8 4" xfId="479" xr:uid="{00000000-0005-0000-0000-0000DF010000}"/>
-    <cellStyle name="Normal 6 2 9" xfId="334" xr:uid="{00000000-0005-0000-0000-00004E010000}"/>
-    <cellStyle name="Normal 6 2 9 2" xfId="26" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="Normal 6 2 9 3" xfId="98" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
-    <cellStyle name="Normal 6 3" xfId="314" xr:uid="{00000000-0005-0000-0000-00003A010000}"/>
-    <cellStyle name="Normal 6 3 10" xfId="183" xr:uid="{00000000-0005-0000-0000-0000B7000000}"/>
-    <cellStyle name="Normal 6 3 2" xfId="548" xr:uid="{00000000-0005-0000-0000-000024020000}"/>
-    <cellStyle name="Normal 6 3 2 2" xfId="207" xr:uid="{00000000-0005-0000-0000-0000CF000000}"/>
-    <cellStyle name="Normal 6 3 2 2 2" xfId="237" xr:uid="{00000000-0005-0000-0000-0000ED000000}"/>
-    <cellStyle name="Normal 6 3 2 2 2 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="Normal 6 3 2 2 2 2 2" xfId="89" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
-    <cellStyle name="Normal 6 3 2 2 2 2 3" xfId="90" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
-    <cellStyle name="Normal 6 3 2 2 2 3" xfId="51" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="Normal 6 3 2 2 2 4" xfId="48" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="Normal 6 3 2 2 3" xfId="238" xr:uid="{00000000-0005-0000-0000-0000EE000000}"/>
-    <cellStyle name="Normal 6 3 2 2 3 2" xfId="499" xr:uid="{00000000-0005-0000-0000-0000F3010000}"/>
-    <cellStyle name="Normal 6 3 2 2 3 2 2" xfId="288" xr:uid="{00000000-0005-0000-0000-000020010000}"/>
-    <cellStyle name="Normal 6 3 2 2 3 2 3" xfId="287" xr:uid="{00000000-0005-0000-0000-00001F010000}"/>
-    <cellStyle name="Normal 6 3 2 2 3 3" xfId="498" xr:uid="{00000000-0005-0000-0000-0000F2010000}"/>
-    <cellStyle name="Normal 6 3 2 2 3 4" xfId="495" xr:uid="{00000000-0005-0000-0000-0000EF010000}"/>
-    <cellStyle name="Normal 6 3 2 2 4" xfId="234" xr:uid="{00000000-0005-0000-0000-0000EA000000}"/>
-    <cellStyle name="Normal 6 3 2 2 4 2" xfId="612" xr:uid="{00000000-0005-0000-0000-000064020000}"/>
-    <cellStyle name="Normal 6 3 2 2 4 3" xfId="613" xr:uid="{00000000-0005-0000-0000-000065020000}"/>
-    <cellStyle name="Normal 6 3 2 2 5" xfId="235" xr:uid="{00000000-0005-0000-0000-0000EB000000}"/>
-    <cellStyle name="Normal 6 3 2 2 6" xfId="236" xr:uid="{00000000-0005-0000-0000-0000EC000000}"/>
-    <cellStyle name="Normal 6 3 2 3" xfId="208" xr:uid="{00000000-0005-0000-0000-0000D0000000}"/>
-    <cellStyle name="Normal 6 3 2 3 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Normal 6 3 2 3 2 2" xfId="394" xr:uid="{00000000-0005-0000-0000-00008A010000}"/>
-    <cellStyle name="Normal 6 3 2 3 2 3" xfId="393" xr:uid="{00000000-0005-0000-0000-000089010000}"/>
-    <cellStyle name="Normal 6 3 2 3 3" xfId="36" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="Normal 6 3 2 3 4" xfId="35" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="Normal 6 3 2 4" xfId="209" xr:uid="{00000000-0005-0000-0000-0000D1000000}"/>
-    <cellStyle name="Normal 6 3 2 4 2" xfId="627" xr:uid="{00000000-0005-0000-0000-000073020000}"/>
-    <cellStyle name="Normal 6 3 2 4 2 2" xfId="486" xr:uid="{00000000-0005-0000-0000-0000E6010000}"/>
-    <cellStyle name="Normal 6 3 2 4 2 3" xfId="487" xr:uid="{00000000-0005-0000-0000-0000E7010000}"/>
-    <cellStyle name="Normal 6 3 2 4 3" xfId="628" xr:uid="{00000000-0005-0000-0000-000074020000}"/>
-    <cellStyle name="Normal 6 3 2 4 4" xfId="629" xr:uid="{00000000-0005-0000-0000-000075020000}"/>
-    <cellStyle name="Normal 6 3 2 5" xfId="210" xr:uid="{00000000-0005-0000-0000-0000D2000000}"/>
-    <cellStyle name="Normal 6 3 2 5 2" xfId="431" xr:uid="{00000000-0005-0000-0000-0000AF010000}"/>
-    <cellStyle name="Normal 6 3 2 5 3" xfId="430" xr:uid="{00000000-0005-0000-0000-0000AE010000}"/>
-    <cellStyle name="Normal 6 3 2 6" xfId="211" xr:uid="{00000000-0005-0000-0000-0000D3000000}"/>
-    <cellStyle name="Normal 6 3 2 7" xfId="212" xr:uid="{00000000-0005-0000-0000-0000D4000000}"/>
-    <cellStyle name="Normal 6 3 3" xfId="549" xr:uid="{00000000-0005-0000-0000-000025020000}"/>
-    <cellStyle name="Normal 6 3 3 2" xfId="645" xr:uid="{00000000-0005-0000-0000-000085020000}"/>
-    <cellStyle name="Normal 6 3 3 2 2" xfId="558" xr:uid="{00000000-0005-0000-0000-00002E020000}"/>
-    <cellStyle name="Normal 6 3 3 2 2 2" xfId="190" xr:uid="{00000000-0005-0000-0000-0000BE000000}"/>
-    <cellStyle name="Normal 6 3 3 2 2 3" xfId="189" xr:uid="{00000000-0005-0000-0000-0000BD000000}"/>
-    <cellStyle name="Normal 6 3 3 2 3" xfId="557" xr:uid="{00000000-0005-0000-0000-00002D020000}"/>
-    <cellStyle name="Normal 6 3 3 2 4" xfId="556" xr:uid="{00000000-0005-0000-0000-00002C020000}"/>
-    <cellStyle name="Normal 6 3 3 3" xfId="644" xr:uid="{00000000-0005-0000-0000-000084020000}"/>
-    <cellStyle name="Normal 6 3 3 3 2" xfId="114" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
-    <cellStyle name="Normal 6 3 3 3 2 2" xfId="653" xr:uid="{00000000-0005-0000-0000-00008D020000}"/>
-    <cellStyle name="Normal 6 3 3 3 2 3" xfId="654" xr:uid="{00000000-0005-0000-0000-00008E020000}"/>
-    <cellStyle name="Normal 6 3 3 3 3" xfId="115" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
-    <cellStyle name="Normal 6 3 3 3 4" xfId="112" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
-    <cellStyle name="Normal 6 3 3 4" xfId="647" xr:uid="{00000000-0005-0000-0000-000087020000}"/>
-    <cellStyle name="Normal 6 3 3 4 2" xfId="317" xr:uid="{00000000-0005-0000-0000-00003D010000}"/>
-    <cellStyle name="Normal 6 3 3 4 3" xfId="316" xr:uid="{00000000-0005-0000-0000-00003C010000}"/>
-    <cellStyle name="Normal 6 3 3 5" xfId="646" xr:uid="{00000000-0005-0000-0000-000086020000}"/>
-    <cellStyle name="Normal 6 3 3 6" xfId="648" xr:uid="{00000000-0005-0000-0000-000088020000}"/>
-    <cellStyle name="Normal 6 3 4" xfId="550" xr:uid="{00000000-0005-0000-0000-000026020000}"/>
-    <cellStyle name="Normal 6 3 4 2" xfId="160" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
-    <cellStyle name="Normal 6 3 4 2 2" xfId="470" xr:uid="{00000000-0005-0000-0000-0000D6010000}"/>
-    <cellStyle name="Normal 6 3 4 2 3" xfId="471" xr:uid="{00000000-0005-0000-0000-0000D7010000}"/>
-    <cellStyle name="Normal 6 3 4 3" xfId="164" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
-    <cellStyle name="Normal 6 3 4 4" xfId="155" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
-    <cellStyle name="Normal 6 3 5" xfId="551" xr:uid="{00000000-0005-0000-0000-000027020000}"/>
-    <cellStyle name="Normal 6 3 5 2" xfId="493" xr:uid="{00000000-0005-0000-0000-0000ED010000}"/>
-    <cellStyle name="Normal 6 3 5 2 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="Normal 6 3 5 2 3" xfId="52" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="Normal 6 3 5 3" xfId="492" xr:uid="{00000000-0005-0000-0000-0000EC010000}"/>
-    <cellStyle name="Normal 6 3 5 4" xfId="491" xr:uid="{00000000-0005-0000-0000-0000EB010000}"/>
-    <cellStyle name="Normal 6 3 6" xfId="552" xr:uid="{00000000-0005-0000-0000-000028020000}"/>
-    <cellStyle name="Normal 6 3 6 2" xfId="323" xr:uid="{00000000-0005-0000-0000-000043010000}"/>
-    <cellStyle name="Normal 6 3 6 2 2" xfId="153" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
-    <cellStyle name="Normal 6 3 6 2 3" xfId="154" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
-    <cellStyle name="Normal 6 3 6 3" xfId="324" xr:uid="{00000000-0005-0000-0000-000044010000}"/>
-    <cellStyle name="Normal 6 3 6 4" xfId="322" xr:uid="{00000000-0005-0000-0000-000042010000}"/>
-    <cellStyle name="Normal 6 3 7" xfId="553" xr:uid="{00000000-0005-0000-0000-000029020000}"/>
-    <cellStyle name="Normal 6 3 7 2" xfId="111" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
-    <cellStyle name="Normal 6 3 7 2 2" xfId="347" xr:uid="{00000000-0005-0000-0000-00005B010000}"/>
-    <cellStyle name="Normal 6 3 7 2 3" xfId="346" xr:uid="{00000000-0005-0000-0000-00005A010000}"/>
-    <cellStyle name="Normal 6 3 7 3" xfId="110" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
-    <cellStyle name="Normal 6 3 7 4" xfId="109" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
-    <cellStyle name="Normal 6 3 8" xfId="501" xr:uid="{00000000-0005-0000-0000-0000F5010000}"/>
-    <cellStyle name="Normal 6 3 8 2" xfId="305" xr:uid="{00000000-0005-0000-0000-000031010000}"/>
-    <cellStyle name="Normal 6 3 8 3" xfId="306" xr:uid="{00000000-0005-0000-0000-000032010000}"/>
-    <cellStyle name="Normal 6 3 9" xfId="502" xr:uid="{00000000-0005-0000-0000-0000F6010000}"/>
-    <cellStyle name="Normal 6 4" xfId="311" xr:uid="{00000000-0005-0000-0000-000037010000}"/>
-    <cellStyle name="Normal 6 4 10" xfId="100" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
-    <cellStyle name="Normal 6 4 2" xfId="92" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
-    <cellStyle name="Normal 6 4 2 2" xfId="140" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
-    <cellStyle name="Normal 6 4 2 2 2" xfId="375" xr:uid="{00000000-0005-0000-0000-000077010000}"/>
-    <cellStyle name="Normal 6 4 2 2 2 2" xfId="267" xr:uid="{00000000-0005-0000-0000-00000B010000}"/>
-    <cellStyle name="Normal 6 4 2 2 2 2 2" xfId="382" xr:uid="{00000000-0005-0000-0000-00007E010000}"/>
-    <cellStyle name="Normal 6 4 2 2 2 2 3" xfId="381" xr:uid="{00000000-0005-0000-0000-00007D010000}"/>
-    <cellStyle name="Normal 6 4 2 2 2 3" xfId="266" xr:uid="{00000000-0005-0000-0000-00000A010000}"/>
-    <cellStyle name="Normal 6 4 2 2 2 4" xfId="268" xr:uid="{00000000-0005-0000-0000-00000C010000}"/>
-    <cellStyle name="Normal 6 4 2 2 3" xfId="395" xr:uid="{00000000-0005-0000-0000-00008B010000}"/>
-    <cellStyle name="Normal 6 4 2 2 3 2" xfId="480" xr:uid="{00000000-0005-0000-0000-0000E0010000}"/>
-    <cellStyle name="Normal 6 4 2 2 3 2 2" xfId="187" xr:uid="{00000000-0005-0000-0000-0000BB000000}"/>
-    <cellStyle name="Normal 6 4 2 2 3 2 3" xfId="188" xr:uid="{00000000-0005-0000-0000-0000BC000000}"/>
-    <cellStyle name="Normal 6 4 2 2 3 3" xfId="481" xr:uid="{00000000-0005-0000-0000-0000E1010000}"/>
-    <cellStyle name="Normal 6 4 2 2 3 4" xfId="484" xr:uid="{00000000-0005-0000-0000-0000E4010000}"/>
-    <cellStyle name="Normal 6 4 2 2 4" xfId="402" xr:uid="{00000000-0005-0000-0000-000092010000}"/>
-    <cellStyle name="Normal 6 4 2 2 4 2" xfId="429" xr:uid="{00000000-0005-0000-0000-0000AD010000}"/>
-    <cellStyle name="Normal 6 4 2 2 4 3" xfId="428" xr:uid="{00000000-0005-0000-0000-0000AC010000}"/>
-    <cellStyle name="Normal 6 4 2 2 5" xfId="401" xr:uid="{00000000-0005-0000-0000-000091010000}"/>
-    <cellStyle name="Normal 6 4 2 2 6" xfId="379" xr:uid="{00000000-0005-0000-0000-00007B010000}"/>
-    <cellStyle name="Normal 6 4 2 3" xfId="139" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
-    <cellStyle name="Normal 6 4 2 3 2" xfId="587" xr:uid="{00000000-0005-0000-0000-00004B020000}"/>
-    <cellStyle name="Normal 6 4 2 3 2 2" xfId="655" xr:uid="{00000000-0005-0000-0000-00008F020000}"/>
-    <cellStyle name="Normal 6 4 2 3 2 3" xfId="656" xr:uid="{00000000-0005-0000-0000-000090020000}"/>
-    <cellStyle name="Normal 6 4 2 3 3" xfId="588" xr:uid="{00000000-0005-0000-0000-00004C020000}"/>
-    <cellStyle name="Normal 6 4 2 3 4" xfId="591" xr:uid="{00000000-0005-0000-0000-00004F020000}"/>
-    <cellStyle name="Normal 6 4 2 4" xfId="138" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
-    <cellStyle name="Normal 6 4 2 4 2" xfId="623" xr:uid="{00000000-0005-0000-0000-00006F020000}"/>
-    <cellStyle name="Normal 6 4 2 4 2 2" xfId="605" xr:uid="{00000000-0005-0000-0000-00005D020000}"/>
-    <cellStyle name="Normal 6 4 2 4 2 3" xfId="604" xr:uid="{00000000-0005-0000-0000-00005C020000}"/>
-    <cellStyle name="Normal 6 4 2 4 3" xfId="622" xr:uid="{00000000-0005-0000-0000-00006E020000}"/>
-    <cellStyle name="Normal 6 4 2 4 4" xfId="621" xr:uid="{00000000-0005-0000-0000-00006D020000}"/>
-    <cellStyle name="Normal 6 4 2 5" xfId="137" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
-    <cellStyle name="Normal 6 4 2 5 2" xfId="184" xr:uid="{00000000-0005-0000-0000-0000B8000000}"/>
-    <cellStyle name="Normal 6 4 2 5 3" xfId="185" xr:uid="{00000000-0005-0000-0000-0000B9000000}"/>
-    <cellStyle name="Normal 6 4 2 6" xfId="136" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
-    <cellStyle name="Normal 6 4 2 7" xfId="135" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
-    <cellStyle name="Normal 6 4 3" xfId="91" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
-    <cellStyle name="Normal 6 4 3 2" xfId="342" xr:uid="{00000000-0005-0000-0000-000056010000}"/>
-    <cellStyle name="Normal 6 4 3 2 2" xfId="200" xr:uid="{00000000-0005-0000-0000-0000C8000000}"/>
-    <cellStyle name="Normal 6 4 3 2 2 2" xfId="127" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
-    <cellStyle name="Normal 6 4 3 2 2 3" xfId="128" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
-    <cellStyle name="Normal 6 4 3 2 3" xfId="201" xr:uid="{00000000-0005-0000-0000-0000C9000000}"/>
-    <cellStyle name="Normal 6 4 3 2 4" xfId="204" xr:uid="{00000000-0005-0000-0000-0000CC000000}"/>
-    <cellStyle name="Normal 6 4 3 3" xfId="343" xr:uid="{00000000-0005-0000-0000-000057010000}"/>
-    <cellStyle name="Normal 6 4 3 3 2" xfId="643" xr:uid="{00000000-0005-0000-0000-000083020000}"/>
-    <cellStyle name="Normal 6 4 3 3 2 2" xfId="298" xr:uid="{00000000-0005-0000-0000-00002A010000}"/>
-    <cellStyle name="Normal 6 4 3 3 2 3" xfId="297" xr:uid="{00000000-0005-0000-0000-000029010000}"/>
-    <cellStyle name="Normal 6 4 3 3 3" xfId="642" xr:uid="{00000000-0005-0000-0000-000082020000}"/>
-    <cellStyle name="Normal 6 4 3 3 4" xfId="583" xr:uid="{00000000-0005-0000-0000-000047020000}"/>
-    <cellStyle name="Normal 6 4 3 4" xfId="340" xr:uid="{00000000-0005-0000-0000-000054010000}"/>
-    <cellStyle name="Normal 6 4 3 4 2" xfId="444" xr:uid="{00000000-0005-0000-0000-0000BC010000}"/>
-    <cellStyle name="Normal 6 4 3 4 3" xfId="445" xr:uid="{00000000-0005-0000-0000-0000BD010000}"/>
-    <cellStyle name="Normal 6 4 3 5" xfId="341" xr:uid="{00000000-0005-0000-0000-000055010000}"/>
-    <cellStyle name="Normal 6 4 3 6" xfId="339" xr:uid="{00000000-0005-0000-0000-000053010000}"/>
-    <cellStyle name="Normal 6 4 4" xfId="441" xr:uid="{00000000-0005-0000-0000-0000B9010000}"/>
-    <cellStyle name="Normal 6 4 4 2" xfId="292" xr:uid="{00000000-0005-0000-0000-000024010000}"/>
-    <cellStyle name="Normal 6 4 4 2 2" xfId="247" xr:uid="{00000000-0005-0000-0000-0000F7000000}"/>
-    <cellStyle name="Normal 6 4 4 2 3" xfId="246" xr:uid="{00000000-0005-0000-0000-0000F6000000}"/>
-    <cellStyle name="Normal 6 4 4 3" xfId="412" xr:uid="{00000000-0005-0000-0000-00009C010000}"/>
-    <cellStyle name="Normal 6 4 4 4" xfId="293" xr:uid="{00000000-0005-0000-0000-000025010000}"/>
-    <cellStyle name="Normal 6 4 5" xfId="440" xr:uid="{00000000-0005-0000-0000-0000B8010000}"/>
-    <cellStyle name="Normal 6 4 5 2" xfId="460" xr:uid="{00000000-0005-0000-0000-0000CC010000}"/>
-    <cellStyle name="Normal 6 4 5 2 2" xfId="517" xr:uid="{00000000-0005-0000-0000-000005020000}"/>
-    <cellStyle name="Normal 6 4 5 2 3" xfId="520" xr:uid="{00000000-0005-0000-0000-000008020000}"/>
-    <cellStyle name="Normal 6 4 5 3" xfId="461" xr:uid="{00000000-0005-0000-0000-0000CD010000}"/>
-    <cellStyle name="Normal 6 4 5 4" xfId="462" xr:uid="{00000000-0005-0000-0000-0000CE010000}"/>
-    <cellStyle name="Normal 6 4 6" xfId="88" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="Normal 6 4 6 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal 6 4 6 2 2" xfId="595" xr:uid="{00000000-0005-0000-0000-000053020000}"/>
-    <cellStyle name="Normal 6 4 6 2 3" xfId="594" xr:uid="{00000000-0005-0000-0000-000052020000}"/>
-    <cellStyle name="Normal 6 4 6 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Normal 6 4 6 4" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Normal 6 4 7" xfId="87" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Normal 6 4 7 2" xfId="221" xr:uid="{00000000-0005-0000-0000-0000DD000000}"/>
-    <cellStyle name="Normal 6 4 7 2 2" xfId="403" xr:uid="{00000000-0005-0000-0000-000093010000}"/>
-    <cellStyle name="Normal 6 4 7 2 3" xfId="404" xr:uid="{00000000-0005-0000-0000-000094010000}"/>
-    <cellStyle name="Normal 6 4 7 3" xfId="222" xr:uid="{00000000-0005-0000-0000-0000DE000000}"/>
-    <cellStyle name="Normal 6 4 7 4" xfId="224" xr:uid="{00000000-0005-0000-0000-0000E0000000}"/>
-    <cellStyle name="Normal 6 4 8" xfId="97" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
-    <cellStyle name="Normal 6 4 8 2" xfId="95" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="Normal 6 4 8 3" xfId="380" xr:uid="{00000000-0005-0000-0000-00007C010000}"/>
-    <cellStyle name="Normal 6 4 9" xfId="96" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
-    <cellStyle name="Normal 6 5" xfId="310" xr:uid="{00000000-0005-0000-0000-000036010000}"/>
-    <cellStyle name="Normal 6 5 2" xfId="285" xr:uid="{00000000-0005-0000-0000-00001D010000}"/>
-    <cellStyle name="Normal 6 5 2 2" xfId="534" xr:uid="{00000000-0005-0000-0000-000016020000}"/>
-    <cellStyle name="Normal 6 5 2 2 2" xfId="182" xr:uid="{00000000-0005-0000-0000-0000B6000000}"/>
-    <cellStyle name="Normal 6 5 2 2 2 2" xfId="258" xr:uid="{00000000-0005-0000-0000-000002010000}"/>
-    <cellStyle name="Normal 6 5 2 2 2 2 2" xfId="546" xr:uid="{00000000-0005-0000-0000-000022020000}"/>
-    <cellStyle name="Normal 6 5 2 2 2 2 3" xfId="547" xr:uid="{00000000-0005-0000-0000-000023020000}"/>
-    <cellStyle name="Normal 6 5 2 2 2 3" xfId="259" xr:uid="{00000000-0005-0000-0000-000003010000}"/>
-    <cellStyle name="Normal 6 5 2 2 2 4" xfId="261" xr:uid="{00000000-0005-0000-0000-000005010000}"/>
-    <cellStyle name="Normal 6 5 2 2 3" xfId="417" xr:uid="{00000000-0005-0000-0000-0000A1010000}"/>
-    <cellStyle name="Normal 6 5 2 2 3 2" xfId="302" xr:uid="{00000000-0005-0000-0000-00002E010000}"/>
-    <cellStyle name="Normal 6 5 2 2 3 2 2" xfId="107" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
-    <cellStyle name="Normal 6 5 2 2 3 2 3" xfId="106" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
-    <cellStyle name="Normal 6 5 2 2 3 3" xfId="301" xr:uid="{00000000-0005-0000-0000-00002D010000}"/>
-    <cellStyle name="Normal 6 5 2 2 3 4" xfId="79" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="Normal 6 5 2 2 4" xfId="253" xr:uid="{00000000-0005-0000-0000-0000FD000000}"/>
-    <cellStyle name="Normal 6 5 2 2 4 2" xfId="419" xr:uid="{00000000-0005-0000-0000-0000A3010000}"/>
-    <cellStyle name="Normal 6 5 2 2 4 3" xfId="420" xr:uid="{00000000-0005-0000-0000-0000A4010000}"/>
-    <cellStyle name="Normal 6 5 2 2 5" xfId="254" xr:uid="{00000000-0005-0000-0000-0000FE000000}"/>
-    <cellStyle name="Normal 6 5 2 2 6" xfId="192" xr:uid="{00000000-0005-0000-0000-0000C0000000}"/>
-    <cellStyle name="Normal 6 5 2 3" xfId="535" xr:uid="{00000000-0005-0000-0000-000017020000}"/>
-    <cellStyle name="Normal 6 5 2 3 2" xfId="649" xr:uid="{00000000-0005-0000-0000-000089020000}"/>
-    <cellStyle name="Normal 6 5 2 3 2 2" xfId="370" xr:uid="{00000000-0005-0000-0000-000072010000}"/>
-    <cellStyle name="Normal 6 5 2 3 2 3" xfId="369" xr:uid="{00000000-0005-0000-0000-000071010000}"/>
-    <cellStyle name="Normal 6 5 2 3 3" xfId="70" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="Normal 6 5 2 3 4" xfId="276" xr:uid="{00000000-0005-0000-0000-000014010000}"/>
-    <cellStyle name="Normal 6 5 2 4" xfId="532" xr:uid="{00000000-0005-0000-0000-000014020000}"/>
-    <cellStyle name="Normal 6 5 2 4 2" xfId="518" xr:uid="{00000000-0005-0000-0000-000006020000}"/>
-    <cellStyle name="Normal 6 5 2 4 2 2" xfId="633" xr:uid="{00000000-0005-0000-0000-000079020000}"/>
-    <cellStyle name="Normal 6 5 2 4 2 3" xfId="634" xr:uid="{00000000-0005-0000-0000-00007A020000}"/>
-    <cellStyle name="Normal 6 5 2 4 3" xfId="519" xr:uid="{00000000-0005-0000-0000-000007020000}"/>
-    <cellStyle name="Normal 6 5 2 4 4" xfId="514" xr:uid="{00000000-0005-0000-0000-000002020000}"/>
-    <cellStyle name="Normal 6 5 2 5" xfId="447" xr:uid="{00000000-0005-0000-0000-0000BF010000}"/>
-    <cellStyle name="Normal 6 5 2 5 2" xfId="304" xr:uid="{00000000-0005-0000-0000-000030010000}"/>
-    <cellStyle name="Normal 6 5 2 5 3" xfId="303" xr:uid="{00000000-0005-0000-0000-00002F010000}"/>
-    <cellStyle name="Normal 6 5 2 6" xfId="530" xr:uid="{00000000-0005-0000-0000-000012020000}"/>
-    <cellStyle name="Normal 6 5 2 7" xfId="531" xr:uid="{00000000-0005-0000-0000-000013020000}"/>
-    <cellStyle name="Normal 6 5 3" xfId="286" xr:uid="{00000000-0005-0000-0000-00001E010000}"/>
-    <cellStyle name="Normal 6 5 3 2" xfId="321" xr:uid="{00000000-0005-0000-0000-000041010000}"/>
-    <cellStyle name="Normal 6 5 3 2 2" xfId="134" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
-    <cellStyle name="Normal 6 5 3 2 2 2" xfId="600" xr:uid="{00000000-0005-0000-0000-000058020000}"/>
-    <cellStyle name="Normal 6 5 3 2 2 3" xfId="599" xr:uid="{00000000-0005-0000-0000-000057020000}"/>
-    <cellStyle name="Normal 6 5 3 2 3" xfId="229" xr:uid="{00000000-0005-0000-0000-0000E5000000}"/>
-    <cellStyle name="Normal 6 5 3 2 4" xfId="472" xr:uid="{00000000-0005-0000-0000-0000D8010000}"/>
-    <cellStyle name="Normal 6 5 3 3" xfId="320" xr:uid="{00000000-0005-0000-0000-000040010000}"/>
-    <cellStyle name="Normal 6 5 3 3 2" xfId="32" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="Normal 6 5 3 3 2 2" xfId="423" xr:uid="{00000000-0005-0000-0000-0000A7010000}"/>
-    <cellStyle name="Normal 6 5 3 3 2 3" xfId="424" xr:uid="{00000000-0005-0000-0000-0000A8010000}"/>
-    <cellStyle name="Normal 6 5 3 3 3" xfId="34" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="Normal 6 5 3 3 4" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Normal 6 5 3 4" xfId="319" xr:uid="{00000000-0005-0000-0000-00003F010000}"/>
-    <cellStyle name="Normal 6 5 3 4 2" xfId="94" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
-    <cellStyle name="Normal 6 5 3 4 3" xfId="93" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="Normal 6 5 3 5" xfId="318" xr:uid="{00000000-0005-0000-0000-00003E010000}"/>
-    <cellStyle name="Normal 6 5 3 6" xfId="525" xr:uid="{00000000-0005-0000-0000-00000D020000}"/>
-    <cellStyle name="Normal 6 5 4" xfId="283" xr:uid="{00000000-0005-0000-0000-00001B010000}"/>
-    <cellStyle name="Normal 6 5 4 2" xfId="582" xr:uid="{00000000-0005-0000-0000-000046020000}"/>
-    <cellStyle name="Normal 6 5 4 2 2" xfId="478" xr:uid="{00000000-0005-0000-0000-0000DE010000}"/>
-    <cellStyle name="Normal 6 5 4 2 3" xfId="639" xr:uid="{00000000-0005-0000-0000-00007F020000}"/>
-    <cellStyle name="Normal 6 5 4 3" xfId="197" xr:uid="{00000000-0005-0000-0000-0000C5000000}"/>
-    <cellStyle name="Normal 6 5 4 4" xfId="584" xr:uid="{00000000-0005-0000-0000-000048020000}"/>
-    <cellStyle name="Normal 6 5 5" xfId="284" xr:uid="{00000000-0005-0000-0000-00001C010000}"/>
-    <cellStyle name="Normal 6 5 5 2" xfId="387" xr:uid="{00000000-0005-0000-0000-000083010000}"/>
-    <cellStyle name="Normal 6 5 5 2 2" xfId="119" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
-    <cellStyle name="Normal 6 5 5 2 3" xfId="33" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Normal 6 5 5 3" xfId="386" xr:uid="{00000000-0005-0000-0000-000082010000}"/>
-    <cellStyle name="Normal 6 5 5 4" xfId="388" xr:uid="{00000000-0005-0000-0000-000084010000}"/>
-    <cellStyle name="Normal 6 5 6" xfId="281" xr:uid="{00000000-0005-0000-0000-000019010000}"/>
-    <cellStyle name="Normal 6 5 6 2" xfId="74" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="Normal 6 5 6 3" xfId="356" xr:uid="{00000000-0005-0000-0000-000064010000}"/>
-    <cellStyle name="Normal 6 5 7" xfId="282" xr:uid="{00000000-0005-0000-0000-00001A010000}"/>
-    <cellStyle name="Normal 6 5 8" xfId="280" xr:uid="{00000000-0005-0000-0000-000018010000}"/>
-    <cellStyle name="Normal 6 6" xfId="313" xr:uid="{00000000-0005-0000-0000-000039010000}"/>
-    <cellStyle name="Normal 6 6 2" xfId="326" xr:uid="{00000000-0005-0000-0000-000046010000}"/>
-    <cellStyle name="Normal 6 6 2 2" xfId="245" xr:uid="{00000000-0005-0000-0000-0000F5000000}"/>
-    <cellStyle name="Normal 6 6 2 2 2" xfId="64" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="Normal 6 6 2 2 2 2" xfId="618" xr:uid="{00000000-0005-0000-0000-00006A020000}"/>
-    <cellStyle name="Normal 6 6 2 2 2 2 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="Normal 6 6 2 2 2 2 3" xfId="515" xr:uid="{00000000-0005-0000-0000-000003020000}"/>
-    <cellStyle name="Normal 6 6 2 2 2 3" xfId="617" xr:uid="{00000000-0005-0000-0000-000069020000}"/>
-    <cellStyle name="Normal 6 6 2 2 2 4" xfId="619" xr:uid="{00000000-0005-0000-0000-00006B020000}"/>
-    <cellStyle name="Normal 6 6 2 2 3" xfId="113" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
-    <cellStyle name="Normal 6 6 2 2 3 2" xfId="116" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
-    <cellStyle name="Normal 6 6 2 2 3 2 2" xfId="456" xr:uid="{00000000-0005-0000-0000-0000C8010000}"/>
-    <cellStyle name="Normal 6 6 2 2 3 2 3" xfId="457" xr:uid="{00000000-0005-0000-0000-0000C9010000}"/>
-    <cellStyle name="Normal 6 6 2 2 3 3" xfId="296" xr:uid="{00000000-0005-0000-0000-000028010000}"/>
-    <cellStyle name="Normal 6 6 2 2 3 4" xfId="176" xr:uid="{00000000-0005-0000-0000-0000B0000000}"/>
-    <cellStyle name="Normal 6 6 2 2 4" xfId="80" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="Normal 6 6 2 2 4 2" xfId="199" xr:uid="{00000000-0005-0000-0000-0000C7000000}"/>
-    <cellStyle name="Normal 6 6 2 2 4 3" xfId="198" xr:uid="{00000000-0005-0000-0000-0000C6000000}"/>
-    <cellStyle name="Normal 6 6 2 2 5" xfId="77" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="Normal 6 6 2 2 6" xfId="129" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
-    <cellStyle name="Normal 6 6 2 3" xfId="163" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
-    <cellStyle name="Normal 6 6 2 3 2" xfId="662" xr:uid="{00000000-0005-0000-0000-000096020000}"/>
-    <cellStyle name="Normal 6 6 2 3 2 2" xfId="278" xr:uid="{00000000-0005-0000-0000-000016010000}"/>
-    <cellStyle name="Normal 6 6 2 3 2 3" xfId="279" xr:uid="{00000000-0005-0000-0000-000017010000}"/>
-    <cellStyle name="Normal 6 6 2 3 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal 6 6 2 3 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 6 6 2 4" xfId="586" xr:uid="{00000000-0005-0000-0000-00004A020000}"/>
-    <cellStyle name="Normal 6 6 2 4 2" xfId="581" xr:uid="{00000000-0005-0000-0000-000045020000}"/>
-    <cellStyle name="Normal 6 6 2 4 2 2" xfId="383" xr:uid="{00000000-0005-0000-0000-00007F010000}"/>
-    <cellStyle name="Normal 6 6 2 4 2 3" xfId="516" xr:uid="{00000000-0005-0000-0000-000004020000}"/>
-    <cellStyle name="Normal 6 6 2 4 3" xfId="580" xr:uid="{00000000-0005-0000-0000-000044020000}"/>
-    <cellStyle name="Normal 6 6 2 4 4" xfId="579" xr:uid="{00000000-0005-0000-0000-000043020000}"/>
-    <cellStyle name="Normal 6 6 2 5" xfId="159" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
-    <cellStyle name="Normal 6 6 2 5 2" xfId="141" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
-    <cellStyle name="Normal 6 6 2 5 3" xfId="142" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
-    <cellStyle name="Normal 6 6 2 6" xfId="162" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
-    <cellStyle name="Normal 6 6 2 7" xfId="161" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
-    <cellStyle name="Normal 6 6 3" xfId="325" xr:uid="{00000000-0005-0000-0000-000045010000}"/>
-    <cellStyle name="Normal 6 6 3 2" xfId="374" xr:uid="{00000000-0005-0000-0000-000076010000}"/>
-    <cellStyle name="Normal 6 6 3 2 2" xfId="275" xr:uid="{00000000-0005-0000-0000-000013010000}"/>
-    <cellStyle name="Normal 6 6 3 2 2 2" xfId="410" xr:uid="{00000000-0005-0000-0000-00009A010000}"/>
-    <cellStyle name="Normal 6 6 3 2 2 3" xfId="411" xr:uid="{00000000-0005-0000-0000-00009B010000}"/>
-    <cellStyle name="Normal 6 6 3 2 3" xfId="362" xr:uid="{00000000-0005-0000-0000-00006A010000}"/>
-    <cellStyle name="Normal 6 6 3 2 4" xfId="277" xr:uid="{00000000-0005-0000-0000-000015010000}"/>
-    <cellStyle name="Normal 6 6 3 3" xfId="186" xr:uid="{00000000-0005-0000-0000-0000BA000000}"/>
-    <cellStyle name="Normal 6 6 3 3 2" xfId="105" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
-    <cellStyle name="Normal 6 6 3 3 2 2" xfId="300" xr:uid="{00000000-0005-0000-0000-00002C010000}"/>
-    <cellStyle name="Normal 6 6 3 3 2 3" xfId="299" xr:uid="{00000000-0005-0000-0000-00002B010000}"/>
-    <cellStyle name="Normal 6 6 3 3 3" xfId="104" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
-    <cellStyle name="Normal 6 6 3 3 4" xfId="574" xr:uid="{00000000-0005-0000-0000-00003E020000}"/>
-    <cellStyle name="Normal 6 6 3 4" xfId="371" xr:uid="{00000000-0005-0000-0000-000073010000}"/>
-    <cellStyle name="Normal 6 6 3 4 2" xfId="391" xr:uid="{00000000-0005-0000-0000-000087010000}"/>
-    <cellStyle name="Normal 6 6 3 4 3" xfId="392" xr:uid="{00000000-0005-0000-0000-000088010000}"/>
-    <cellStyle name="Normal 6 6 3 5" xfId="372" xr:uid="{00000000-0005-0000-0000-000074010000}"/>
-    <cellStyle name="Normal 6 6 3 6" xfId="373" xr:uid="{00000000-0005-0000-0000-000075010000}"/>
-    <cellStyle name="Normal 6 6 4" xfId="108" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
-    <cellStyle name="Normal 6 6 4 2" xfId="435" xr:uid="{00000000-0005-0000-0000-0000B3010000}"/>
-    <cellStyle name="Normal 6 6 4 2 2" xfId="433" xr:uid="{00000000-0005-0000-0000-0000B1010000}"/>
-    <cellStyle name="Normal 6 6 4 2 3" xfId="432" xr:uid="{00000000-0005-0000-0000-0000B0010000}"/>
-    <cellStyle name="Normal 6 6 4 3" xfId="434" xr:uid="{00000000-0005-0000-0000-0000B2010000}"/>
-    <cellStyle name="Normal 6 6 4 4" xfId="438" xr:uid="{00000000-0005-0000-0000-0000B6010000}"/>
-    <cellStyle name="Normal 6 6 5" xfId="585" xr:uid="{00000000-0005-0000-0000-000049020000}"/>
-    <cellStyle name="Normal 6 6 5 2" xfId="596" xr:uid="{00000000-0005-0000-0000-000054020000}"/>
-    <cellStyle name="Normal 6 6 5 2 2" xfId="554" xr:uid="{00000000-0005-0000-0000-00002A020000}"/>
-    <cellStyle name="Normal 6 6 5 2 3" xfId="555" xr:uid="{00000000-0005-0000-0000-00002B020000}"/>
-    <cellStyle name="Normal 6 6 5 3" xfId="597" xr:uid="{00000000-0005-0000-0000-000055020000}"/>
-    <cellStyle name="Normal 6 6 5 4" xfId="598" xr:uid="{00000000-0005-0000-0000-000056020000}"/>
-    <cellStyle name="Normal 6 6 6" xfId="616" xr:uid="{00000000-0005-0000-0000-000068020000}"/>
-    <cellStyle name="Normal 6 6 6 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="Normal 6 6 6 3" xfId="28" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="Normal 6 6 7" xfId="507" xr:uid="{00000000-0005-0000-0000-0000FB010000}"/>
-    <cellStyle name="Normal 6 6 8" xfId="513" xr:uid="{00000000-0005-0000-0000-000001020000}"/>
-    <cellStyle name="Normal 6 7" xfId="312" xr:uid="{00000000-0005-0000-0000-000038010000}"/>
-    <cellStyle name="Normal 6 7 2" xfId="65" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
-    <cellStyle name="Normal 6 7 2 2" xfId="610" xr:uid="{00000000-0005-0000-0000-000062020000}"/>
-    <cellStyle name="Normal 6 7 2 2 2" xfId="122" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
-    <cellStyle name="Normal 6 7 2 2 2 2" xfId="615" xr:uid="{00000000-0005-0000-0000-000067020000}"/>
-    <cellStyle name="Normal 6 7 2 2 2 2 2" xfId="243" xr:uid="{00000000-0005-0000-0000-0000F3000000}"/>
-    <cellStyle name="Normal 6 7 2 2 2 2 3" xfId="244" xr:uid="{00000000-0005-0000-0000-0000F4000000}"/>
-    <cellStyle name="Normal 6 7 2 2 2 3" xfId="120" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
-    <cellStyle name="Normal 6 7 2 2 2 4" xfId="562" xr:uid="{00000000-0005-0000-0000-000032020000}"/>
-    <cellStyle name="Normal 6 7 2 2 3" xfId="123" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
-    <cellStyle name="Normal 6 7 2 2 3 2" xfId="358" xr:uid="{00000000-0005-0000-0000-000066010000}"/>
-    <cellStyle name="Normal 6 7 2 2 3 2 2" xfId="390" xr:uid="{00000000-0005-0000-0000-000086010000}"/>
-    <cellStyle name="Normal 6 7 2 2 3 2 3" xfId="144" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
-    <cellStyle name="Normal 6 7 2 2 3 3" xfId="357" xr:uid="{00000000-0005-0000-0000-000065010000}"/>
-    <cellStyle name="Normal 6 7 2 2 3 4" xfId="359" xr:uid="{00000000-0005-0000-0000-000067010000}"/>
-    <cellStyle name="Normal 6 7 2 2 4" xfId="124" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
-    <cellStyle name="Normal 6 7 2 2 4 2" xfId="170" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
-    <cellStyle name="Normal 6 7 2 2 4 3" xfId="171" xr:uid="{00000000-0005-0000-0000-0000AB000000}"/>
-    <cellStyle name="Normal 6 7 2 2 5" xfId="125" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
-    <cellStyle name="Normal 6 7 2 2 6" xfId="126" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
-    <cellStyle name="Normal 6 7 2 3" xfId="611" xr:uid="{00000000-0005-0000-0000-000063020000}"/>
-    <cellStyle name="Normal 6 7 2 3 2" xfId="572" xr:uid="{00000000-0005-0000-0000-00003C020000}"/>
-    <cellStyle name="Normal 6 7 2 3 2 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="Normal 6 7 2 3 2 3" xfId="327" xr:uid="{00000000-0005-0000-0000-000047010000}"/>
-    <cellStyle name="Normal 6 7 2 3 3" xfId="571" xr:uid="{00000000-0005-0000-0000-00003B020000}"/>
-    <cellStyle name="Normal 6 7 2 3 4" xfId="573" xr:uid="{00000000-0005-0000-0000-00003D020000}"/>
-    <cellStyle name="Normal 6 7 2 4" xfId="606" xr:uid="{00000000-0005-0000-0000-00005E020000}"/>
-    <cellStyle name="Normal 6 7 2 4 2" xfId="272" xr:uid="{00000000-0005-0000-0000-000010010000}"/>
-    <cellStyle name="Normal 6 7 2 4 2 2" xfId="179" xr:uid="{00000000-0005-0000-0000-0000B3000000}"/>
-    <cellStyle name="Normal 6 7 2 4 2 3" xfId="536" xr:uid="{00000000-0005-0000-0000-000018020000}"/>
-    <cellStyle name="Normal 6 7 2 4 3" xfId="273" xr:uid="{00000000-0005-0000-0000-000011010000}"/>
-    <cellStyle name="Normal 6 7 2 4 4" xfId="271" xr:uid="{00000000-0005-0000-0000-00000F010000}"/>
-    <cellStyle name="Normal 6 7 2 5" xfId="607" xr:uid="{00000000-0005-0000-0000-00005F020000}"/>
-    <cellStyle name="Normal 6 7 2 5 2" xfId="86" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
-    <cellStyle name="Normal 6 7 2 5 3" xfId="85" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
-    <cellStyle name="Normal 6 7 2 6" xfId="608" xr:uid="{00000000-0005-0000-0000-000060020000}"/>
-    <cellStyle name="Normal 6 7 2 7" xfId="609" xr:uid="{00000000-0005-0000-0000-000061020000}"/>
-    <cellStyle name="Normal 6 7 3" xfId="66" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
-    <cellStyle name="Normal 6 7 3 2" xfId="409" xr:uid="{00000000-0005-0000-0000-000099010000}"/>
-    <cellStyle name="Normal 6 7 3 2 2" xfId="476" xr:uid="{00000000-0005-0000-0000-0000DC010000}"/>
-    <cellStyle name="Normal 6 7 3 2 2 2" xfId="353" xr:uid="{00000000-0005-0000-0000-000061010000}"/>
-    <cellStyle name="Normal 6 7 3 2 2 3" xfId="352" xr:uid="{00000000-0005-0000-0000-000060010000}"/>
-    <cellStyle name="Normal 6 7 3 2 3" xfId="475" xr:uid="{00000000-0005-0000-0000-0000DB010000}"/>
-    <cellStyle name="Normal 6 7 3 2 4" xfId="477" xr:uid="{00000000-0005-0000-0000-0000DD010000}"/>
-    <cellStyle name="Normal 6 7 3 3" xfId="418" xr:uid="{00000000-0005-0000-0000-0000A2010000}"/>
-    <cellStyle name="Normal 6 7 3 3 2" xfId="650" xr:uid="{00000000-0005-0000-0000-00008A020000}"/>
-    <cellStyle name="Normal 6 7 3 3 2 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="Normal 6 7 3 3 2 3" xfId="23" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="Normal 6 7 3 3 3" xfId="651" xr:uid="{00000000-0005-0000-0000-00008B020000}"/>
-    <cellStyle name="Normal 6 7 3 3 4" xfId="652" xr:uid="{00000000-0005-0000-0000-00008C020000}"/>
-    <cellStyle name="Normal 6 7 3 4" xfId="414" xr:uid="{00000000-0005-0000-0000-00009E010000}"/>
-    <cellStyle name="Normal 6 7 3 4 2" xfId="563" xr:uid="{00000000-0005-0000-0000-000033020000}"/>
-    <cellStyle name="Normal 6 7 3 4 3" xfId="620" xr:uid="{00000000-0005-0000-0000-00006C020000}"/>
-    <cellStyle name="Normal 6 7 3 5" xfId="413" xr:uid="{00000000-0005-0000-0000-00009D010000}"/>
-    <cellStyle name="Normal 6 7 3 6" xfId="407" xr:uid="{00000000-0005-0000-0000-000097010000}"/>
-    <cellStyle name="Normal 6 7 4" xfId="60" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="Normal 6 7 4 2" xfId="166" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
-    <cellStyle name="Normal 6 7 4 2 2" xfId="509" xr:uid="{00000000-0005-0000-0000-0000FD010000}"/>
-    <cellStyle name="Normal 6 7 4 2 3" xfId="510" xr:uid="{00000000-0005-0000-0000-0000FE010000}"/>
-    <cellStyle name="Normal 6 7 4 3" xfId="490" xr:uid="{00000000-0005-0000-0000-0000EA010000}"/>
-    <cellStyle name="Normal 6 7 4 4" xfId="494" xr:uid="{00000000-0005-0000-0000-0000EE010000}"/>
-    <cellStyle name="Normal 6 7 5" xfId="61" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
-    <cellStyle name="Normal 6 7 5 2" xfId="638" xr:uid="{00000000-0005-0000-0000-00007E020000}"/>
-    <cellStyle name="Normal 6 7 5 2 2" xfId="152" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
-    <cellStyle name="Normal 6 7 5 2 3" xfId="38" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="Normal 6 7 5 3" xfId="637" xr:uid="{00000000-0005-0000-0000-00007D020000}"/>
-    <cellStyle name="Normal 6 7 5 4" xfId="641" xr:uid="{00000000-0005-0000-0000-000081020000}"/>
-    <cellStyle name="Normal 6 7 6" xfId="62" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
-    <cellStyle name="Normal 6 7 6 2" xfId="415" xr:uid="{00000000-0005-0000-0000-00009F010000}"/>
-    <cellStyle name="Normal 6 7 6 3" xfId="416" xr:uid="{00000000-0005-0000-0000-0000A0010000}"/>
-    <cellStyle name="Normal 6 7 7" xfId="63" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
-    <cellStyle name="Normal 6 7 8" xfId="59" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="Normal 6 8" xfId="308" xr:uid="{00000000-0005-0000-0000-000034010000}"/>
-    <cellStyle name="Normal 6 8 2" xfId="364" xr:uid="{00000000-0005-0000-0000-00006C010000}"/>
-    <cellStyle name="Normal 6 8 2 2" xfId="146" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
-    <cellStyle name="Normal 6 8 2 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal 6 8 2 2 2 2" xfId="345" xr:uid="{00000000-0005-0000-0000-000059010000}"/>
-    <cellStyle name="Normal 6 8 2 2 2 3" xfId="344" xr:uid="{00000000-0005-0000-0000-000058010000}"/>
-    <cellStyle name="Normal 6 8 2 2 3" xfId="18" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Normal 6 8 2 2 4" xfId="575" xr:uid="{00000000-0005-0000-0000-00003F020000}"/>
-    <cellStyle name="Normal 6 8 2 3" xfId="145" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
-    <cellStyle name="Normal 6 8 2 3 2" xfId="240" xr:uid="{00000000-0005-0000-0000-0000F0000000}"/>
-    <cellStyle name="Normal 6 8 2 3 2 2" xfId="202" xr:uid="{00000000-0005-0000-0000-0000CA000000}"/>
-    <cellStyle name="Normal 6 8 2 3 2 3" xfId="203" xr:uid="{00000000-0005-0000-0000-0000CB000000}"/>
-    <cellStyle name="Normal 6 8 2 3 3" xfId="241" xr:uid="{00000000-0005-0000-0000-0000F1000000}"/>
-    <cellStyle name="Normal 6 8 2 3 4" xfId="239" xr:uid="{00000000-0005-0000-0000-0000EF000000}"/>
-    <cellStyle name="Normal 6 8 2 4" xfId="149" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
-    <cellStyle name="Normal 6 8 2 4 2" xfId="625" xr:uid="{00000000-0005-0000-0000-000071020000}"/>
-    <cellStyle name="Normal 6 8 2 4 3" xfId="624" xr:uid="{00000000-0005-0000-0000-000070020000}"/>
-    <cellStyle name="Normal 6 8 2 5" xfId="148" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
-    <cellStyle name="Normal 6 8 2 6" xfId="147" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
-    <cellStyle name="Normal 6 8 3" xfId="363" xr:uid="{00000000-0005-0000-0000-00006B010000}"/>
-    <cellStyle name="Normal 6 8 3 2" xfId="350" xr:uid="{00000000-0005-0000-0000-00005E010000}"/>
-    <cellStyle name="Normal 6 8 3 2 2" xfId="488" xr:uid="{00000000-0005-0000-0000-0000E8010000}"/>
-    <cellStyle name="Normal 6 8 3 2 3" xfId="489" xr:uid="{00000000-0005-0000-0000-0000E9010000}"/>
-    <cellStyle name="Normal 6 8 3 3" xfId="351" xr:uid="{00000000-0005-0000-0000-00005F010000}"/>
-    <cellStyle name="Normal 6 8 3 4" xfId="354" xr:uid="{00000000-0005-0000-0000-000062010000}"/>
-    <cellStyle name="Normal 6 8 4" xfId="368" xr:uid="{00000000-0005-0000-0000-000070010000}"/>
-    <cellStyle name="Normal 6 8 4 2" xfId="565" xr:uid="{00000000-0005-0000-0000-000035020000}"/>
-    <cellStyle name="Normal 6 8 4 2 2" xfId="165" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
-    <cellStyle name="Normal 6 8 4 2 3" xfId="446" xr:uid="{00000000-0005-0000-0000-0000BE010000}"/>
-    <cellStyle name="Normal 6 8 4 3" xfId="564" xr:uid="{00000000-0005-0000-0000-000034020000}"/>
-    <cellStyle name="Normal 6 8 4 4" xfId="559" xr:uid="{00000000-0005-0000-0000-00002F020000}"/>
-    <cellStyle name="Normal 6 8 5" xfId="367" xr:uid="{00000000-0005-0000-0000-00006F010000}"/>
-    <cellStyle name="Normal 6 8 5 2" xfId="102" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
-    <cellStyle name="Normal 6 8 5 3" xfId="103" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
-    <cellStyle name="Normal 6 8 6" xfId="366" xr:uid="{00000000-0005-0000-0000-00006E010000}"/>
-    <cellStyle name="Normal 6 8 7" xfId="365" xr:uid="{00000000-0005-0000-0000-00006D010000}"/>
-    <cellStyle name="Normal 6 9" xfId="307" xr:uid="{00000000-0005-0000-0000-000033010000}"/>
-    <cellStyle name="Normal 6 9 2" xfId="537" xr:uid="{00000000-0005-0000-0000-000019020000}"/>
-    <cellStyle name="Normal 6 9 2 2" xfId="215" xr:uid="{00000000-0005-0000-0000-0000D7000000}"/>
-    <cellStyle name="Normal 6 9 2 2 2" xfId="264" xr:uid="{00000000-0005-0000-0000-000008010000}"/>
-    <cellStyle name="Normal 6 9 2 2 3" xfId="265" xr:uid="{00000000-0005-0000-0000-000009010000}"/>
-    <cellStyle name="Normal 6 9 2 3" xfId="566" xr:uid="{00000000-0005-0000-0000-000036020000}"/>
-    <cellStyle name="Normal 6 9 2 4" xfId="217" xr:uid="{00000000-0005-0000-0000-0000D9000000}"/>
-    <cellStyle name="Normal 6 9 3" xfId="538" xr:uid="{00000000-0005-0000-0000-00001A020000}"/>
-    <cellStyle name="Normal 6 9 3 2" xfId="658" xr:uid="{00000000-0005-0000-0000-000092020000}"/>
-    <cellStyle name="Normal 6 9 3 2 2" xfId="426" xr:uid="{00000000-0005-0000-0000-0000AA010000}"/>
-    <cellStyle name="Normal 6 9 3 2 3" xfId="425" xr:uid="{00000000-0005-0000-0000-0000A9010000}"/>
-    <cellStyle name="Normal 6 9 3 3" xfId="657" xr:uid="{00000000-0005-0000-0000-000091020000}"/>
-    <cellStyle name="Normal 6 9 3 4" xfId="659" xr:uid="{00000000-0005-0000-0000-000093020000}"/>
-    <cellStyle name="Normal 6 9 4" xfId="540" xr:uid="{00000000-0005-0000-0000-00001C020000}"/>
-    <cellStyle name="Normal 6 9 4 2" xfId="640" xr:uid="{00000000-0005-0000-0000-000080020000}"/>
-    <cellStyle name="Normal 6 9 4 3" xfId="567" xr:uid="{00000000-0005-0000-0000-000037020000}"/>
-    <cellStyle name="Normal 6 9 5" xfId="541" xr:uid="{00000000-0005-0000-0000-00001D020000}"/>
-    <cellStyle name="Normal 6 9 6" xfId="539" xr:uid="{00000000-0005-0000-0000-00001B020000}"/>
-    <cellStyle name="Normal 7" xfId="452" xr:uid="{00000000-0005-0000-0000-0000C4010000}"/>
-    <cellStyle name="Normal 7 2" xfId="529" xr:uid="{00000000-0005-0000-0000-000011020000}"/>
-    <cellStyle name="Normal 8" xfId="455" xr:uid="{00000000-0005-0000-0000-0000C7010000}"/>
-    <cellStyle name="Normal 8 2" xfId="576" xr:uid="{00000000-0005-0000-0000-000040020000}"/>
-    <cellStyle name="Normal 9" xfId="454" xr:uid="{00000000-0005-0000-0000-0000C6010000}"/>
-    <cellStyle name="Normal 9 2" xfId="58" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="Percent 2" xfId="269" xr:uid="{00000000-0005-0000-0000-00000D010000}"/>
-    <cellStyle name="Percent 2 2" xfId="78" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Normal 10" xfId="545"/>
+    <cellStyle name="Normal 2" xfId="449"/>
+    <cellStyle name="Normal 2 2" xfId="439"/>
+    <cellStyle name="Normal 3" xfId="448"/>
+    <cellStyle name="Normal 3 2" xfId="500"/>
+    <cellStyle name="Normal 4" xfId="451"/>
+    <cellStyle name="Normal 4 2" xfId="81"/>
+    <cellStyle name="Normal 5" xfId="450"/>
+    <cellStyle name="Normal 5 2" xfId="242"/>
+    <cellStyle name="Normal 6" xfId="453"/>
+    <cellStyle name="Normal 6 10" xfId="41"/>
+    <cellStyle name="Normal 6 10 2" xfId="121"/>
+    <cellStyle name="Normal 6 10 2 2" xfId="168"/>
+    <cellStyle name="Normal 6 10 2 3" xfId="167"/>
+    <cellStyle name="Normal 6 10 3" xfId="118"/>
+    <cellStyle name="Normal 6 10 4" xfId="117"/>
+    <cellStyle name="Normal 6 11" xfId="40"/>
+    <cellStyle name="Normal 6 11 2" xfId="251"/>
+    <cellStyle name="Normal 6 11 2 2" xfId="421"/>
+    <cellStyle name="Normal 6 11 2 3" xfId="422"/>
+    <cellStyle name="Normal 6 11 3" xfId="252"/>
+    <cellStyle name="Normal 6 11 4" xfId="250"/>
+    <cellStyle name="Normal 6 12" xfId="43"/>
+    <cellStyle name="Normal 6 12 2" xfId="227"/>
+    <cellStyle name="Normal 6 12 2 2" xfId="181"/>
+    <cellStyle name="Normal 6 12 2 3" xfId="180"/>
+    <cellStyle name="Normal 6 12 3" xfId="226"/>
+    <cellStyle name="Normal 6 12 4" xfId="225"/>
+    <cellStyle name="Normal 6 13" xfId="42"/>
+    <cellStyle name="Normal 6 13 2" xfId="16"/>
+    <cellStyle name="Normal 6 13 2 2" xfId="503"/>
+    <cellStyle name="Normal 6 13 2 3" xfId="504"/>
+    <cellStyle name="Normal 6 13 3" xfId="17"/>
+    <cellStyle name="Normal 6 13 4" xfId="11"/>
+    <cellStyle name="Normal 6 14" xfId="45"/>
+    <cellStyle name="Normal 6 14 2" xfId="337"/>
+    <cellStyle name="Normal 6 14 2 2" xfId="76"/>
+    <cellStyle name="Normal 6 14 2 3" xfId="75"/>
+    <cellStyle name="Normal 6 14 3" xfId="336"/>
+    <cellStyle name="Normal 6 14 4" xfId="338"/>
+    <cellStyle name="Normal 6 15" xfId="44"/>
+    <cellStyle name="Normal 6 15 2" xfId="130"/>
+    <cellStyle name="Normal 6 15 3" xfId="131"/>
+    <cellStyle name="Normal 6 16" xfId="47"/>
+    <cellStyle name="Normal 6 17" xfId="46"/>
+    <cellStyle name="Normal 6 2" xfId="315"/>
+    <cellStyle name="Normal 6 2 10" xfId="233"/>
+    <cellStyle name="Normal 6 2 11" xfId="232"/>
+    <cellStyle name="Normal 6 2 2" xfId="578"/>
+    <cellStyle name="Normal 6 2 2 10" xfId="528"/>
+    <cellStyle name="Normal 6 2 2 2" xfId="465"/>
+    <cellStyle name="Normal 6 2 2 2 2" xfId="485"/>
+    <cellStyle name="Normal 6 2 2 2 2 2" xfId="512"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 2" xfId="7"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 2 2" xfId="329"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 2 3" xfId="328"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 3" xfId="6"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 4" xfId="8"/>
+    <cellStyle name="Normal 6 2 2 2 2 3" xfId="511"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 2" xfId="218"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 2 2" xfId="67"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 2 3" xfId="68"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 3" xfId="219"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 4" xfId="220"/>
+    <cellStyle name="Normal 6 2 2 2 2 4" xfId="309"/>
+    <cellStyle name="Normal 6 2 2 2 2 4 2" xfId="437"/>
+    <cellStyle name="Normal 6 2 2 2 2 4 3" xfId="436"/>
+    <cellStyle name="Normal 6 2 2 2 2 5" xfId="260"/>
+    <cellStyle name="Normal 6 2 2 2 2 6" xfId="508"/>
+    <cellStyle name="Normal 6 2 2 2 3" xfId="191"/>
+    <cellStyle name="Normal 6 2 2 2 3 2" xfId="56"/>
+    <cellStyle name="Normal 6 2 2 2 3 2 2" xfId="496"/>
+    <cellStyle name="Normal 6 2 2 2 3 2 3" xfId="497"/>
+    <cellStyle name="Normal 6 2 2 2 3 3" xfId="57"/>
+    <cellStyle name="Normal 6 2 2 2 3 4" xfId="54"/>
+    <cellStyle name="Normal 6 2 2 2 4" xfId="178"/>
+    <cellStyle name="Normal 6 2 2 2 4 2" xfId="385"/>
+    <cellStyle name="Normal 6 2 2 2 4 2 2" xfId="73"/>
+    <cellStyle name="Normal 6 2 2 2 4 2 3" xfId="71"/>
+    <cellStyle name="Normal 6 2 2 2 4 3" xfId="384"/>
+    <cellStyle name="Normal 6 2 2 2 4 4" xfId="389"/>
+    <cellStyle name="Normal 6 2 2 2 5" xfId="177"/>
+    <cellStyle name="Normal 6 2 2 2 5 2" xfId="592"/>
+    <cellStyle name="Normal 6 2 2 2 5 3" xfId="593"/>
+    <cellStyle name="Normal 6 2 2 2 6" xfId="483"/>
+    <cellStyle name="Normal 6 2 2 2 7" xfId="482"/>
+    <cellStyle name="Normal 6 2 2 3" xfId="464"/>
+    <cellStyle name="Normal 6 2 2 3 2" xfId="24"/>
+    <cellStyle name="Normal 6 2 2 3 2 2" xfId="230"/>
+    <cellStyle name="Normal 6 2 2 3 2 2 2" xfId="560"/>
+    <cellStyle name="Normal 6 2 2 3 2 2 3" xfId="561"/>
+    <cellStyle name="Normal 6 2 2 3 2 3" xfId="231"/>
+    <cellStyle name="Normal 6 2 2 3 2 4" xfId="228"/>
+    <cellStyle name="Normal 6 2 2 3 3" xfId="25"/>
+    <cellStyle name="Normal 6 2 2 3 3 2" xfId="31"/>
+    <cellStyle name="Normal 6 2 2 3 3 2 2" xfId="133"/>
+    <cellStyle name="Normal 6 2 2 3 3 2 3" xfId="132"/>
+    <cellStyle name="Normal 6 2 2 3 3 3" xfId="30"/>
+    <cellStyle name="Normal 6 2 2 3 3 4" xfId="27"/>
+    <cellStyle name="Normal 6 2 2 3 4" xfId="20"/>
+    <cellStyle name="Normal 6 2 2 3 4 2" xfId="193"/>
+    <cellStyle name="Normal 6 2 2 3 4 3" xfId="194"/>
+    <cellStyle name="Normal 6 2 2 3 5" xfId="21"/>
+    <cellStyle name="Normal 6 2 2 3 6" xfId="22"/>
+    <cellStyle name="Normal 6 2 2 4" xfId="467"/>
+    <cellStyle name="Normal 6 2 2 4 2" xfId="206"/>
+    <cellStyle name="Normal 6 2 2 4 2 2" xfId="143"/>
+    <cellStyle name="Normal 6 2 2 4 2 3" xfId="544"/>
+    <cellStyle name="Normal 6 2 2 4 3" xfId="205"/>
+    <cellStyle name="Normal 6 2 2 4 4" xfId="533"/>
+    <cellStyle name="Normal 6 2 2 5" xfId="466"/>
+    <cellStyle name="Normal 6 2 2 5 2" xfId="405"/>
+    <cellStyle name="Normal 6 2 2 5 2 2" xfId="248"/>
+    <cellStyle name="Normal 6 2 2 5 2 3" xfId="249"/>
+    <cellStyle name="Normal 6 2 2 5 3" xfId="406"/>
+    <cellStyle name="Normal 6 2 2 5 4" xfId="408"/>
+    <cellStyle name="Normal 6 2 2 6" xfId="469"/>
+    <cellStyle name="Normal 6 2 2 6 2" xfId="602"/>
+    <cellStyle name="Normal 6 2 2 6 2 2" xfId="590"/>
+    <cellStyle name="Normal 6 2 2 6 2 3" xfId="589"/>
+    <cellStyle name="Normal 6 2 2 6 3" xfId="601"/>
+    <cellStyle name="Normal 6 2 2 6 4" xfId="603"/>
+    <cellStyle name="Normal 6 2 2 7" xfId="468"/>
+    <cellStyle name="Normal 6 2 2 7 2" xfId="156"/>
+    <cellStyle name="Normal 6 2 2 7 2 2" xfId="262"/>
+    <cellStyle name="Normal 6 2 2 7 2 3" xfId="263"/>
+    <cellStyle name="Normal 6 2 2 7 3" xfId="157"/>
+    <cellStyle name="Normal 6 2 2 7 4" xfId="158"/>
+    <cellStyle name="Normal 6 2 2 8" xfId="101"/>
+    <cellStyle name="Normal 6 2 2 8 2" xfId="349"/>
+    <cellStyle name="Normal 6 2 2 8 3" xfId="348"/>
+    <cellStyle name="Normal 6 2 2 9" xfId="99"/>
+    <cellStyle name="Normal 6 2 3" xfId="577"/>
+    <cellStyle name="Normal 6 2 3 2" xfId="12"/>
+    <cellStyle name="Normal 6 2 3 2 2" xfId="294"/>
+    <cellStyle name="Normal 6 2 3 2 2 2" xfId="360"/>
+    <cellStyle name="Normal 6 2 3 2 2 2 2" xfId="526"/>
+    <cellStyle name="Normal 6 2 3 2 2 2 3" xfId="527"/>
+    <cellStyle name="Normal 6 2 3 2 2 3" xfId="361"/>
+    <cellStyle name="Normal 6 2 3 2 2 4" xfId="355"/>
+    <cellStyle name="Normal 6 2 3 2 3" xfId="295"/>
+    <cellStyle name="Normal 6 2 3 2 3 2" xfId="173"/>
+    <cellStyle name="Normal 6 2 3 2 3 2 2" xfId="443"/>
+    <cellStyle name="Normal 6 2 3 2 3 2 3" xfId="442"/>
+    <cellStyle name="Normal 6 2 3 2 3 3" xfId="172"/>
+    <cellStyle name="Normal 6 2 3 2 3 4" xfId="169"/>
+    <cellStyle name="Normal 6 2 3 2 4" xfId="289"/>
+    <cellStyle name="Normal 6 2 3 2 4 2" xfId="213"/>
+    <cellStyle name="Normal 6 2 3 2 4 3" xfId="214"/>
+    <cellStyle name="Normal 6 2 3 2 5" xfId="290"/>
+    <cellStyle name="Normal 6 2 3 2 6" xfId="291"/>
+    <cellStyle name="Normal 6 2 3 3" xfId="13"/>
+    <cellStyle name="Normal 6 2 3 3 2" xfId="84"/>
+    <cellStyle name="Normal 6 2 3 3 2 2" xfId="543"/>
+    <cellStyle name="Normal 6 2 3 3 2 3" xfId="542"/>
+    <cellStyle name="Normal 6 2 3 3 3" xfId="83"/>
+    <cellStyle name="Normal 6 2 3 3 4" xfId="82"/>
+    <cellStyle name="Normal 6 2 3 4" xfId="14"/>
+    <cellStyle name="Normal 6 2 3 4 2" xfId="216"/>
+    <cellStyle name="Normal 6 2 3 4 2 2" xfId="660"/>
+    <cellStyle name="Normal 6 2 3 4 2 3" xfId="661"/>
+    <cellStyle name="Normal 6 2 3 4 3" xfId="55"/>
+    <cellStyle name="Normal 6 2 3 4 4" xfId="223"/>
+    <cellStyle name="Normal 6 2 3 5" xfId="15"/>
+    <cellStyle name="Normal 6 2 3 5 2" xfId="506"/>
+    <cellStyle name="Normal 6 2 3 5 3" xfId="505"/>
+    <cellStyle name="Normal 6 2 3 6" xfId="69"/>
+    <cellStyle name="Normal 6 2 3 7" xfId="72"/>
+    <cellStyle name="Normal 6 2 4" xfId="331"/>
+    <cellStyle name="Normal 6 2 4 2" xfId="400"/>
+    <cellStyle name="Normal 6 2 4 2 2" xfId="256"/>
+    <cellStyle name="Normal 6 2 4 2 2 2" xfId="274"/>
+    <cellStyle name="Normal 6 2 4 2 2 3" xfId="270"/>
+    <cellStyle name="Normal 6 2 4 2 3" xfId="255"/>
+    <cellStyle name="Normal 6 2 4 2 4" xfId="257"/>
+    <cellStyle name="Normal 6 2 4 3" xfId="399"/>
+    <cellStyle name="Normal 6 2 4 3 2" xfId="458"/>
+    <cellStyle name="Normal 6 2 4 3 2 2" xfId="150"/>
+    <cellStyle name="Normal 6 2 4 3 2 3" xfId="151"/>
+    <cellStyle name="Normal 6 2 4 3 3" xfId="459"/>
+    <cellStyle name="Normal 6 2 4 3 4" xfId="463"/>
+    <cellStyle name="Normal 6 2 4 4" xfId="398"/>
+    <cellStyle name="Normal 6 2 4 4 2" xfId="522"/>
+    <cellStyle name="Normal 6 2 4 4 3" xfId="521"/>
+    <cellStyle name="Normal 6 2 4 5" xfId="397"/>
+    <cellStyle name="Normal 6 2 4 6" xfId="396"/>
+    <cellStyle name="Normal 6 2 5" xfId="330"/>
+    <cellStyle name="Normal 6 2 5 2" xfId="569"/>
+    <cellStyle name="Normal 6 2 5 2 2" xfId="376"/>
+    <cellStyle name="Normal 6 2 5 2 3" xfId="377"/>
+    <cellStyle name="Normal 6 2 5 3" xfId="570"/>
+    <cellStyle name="Normal 6 2 5 4" xfId="568"/>
+    <cellStyle name="Normal 6 2 6" xfId="333"/>
+    <cellStyle name="Normal 6 2 6 2" xfId="632"/>
+    <cellStyle name="Normal 6 2 6 2 2" xfId="175"/>
+    <cellStyle name="Normal 6 2 6 2 3" xfId="174"/>
+    <cellStyle name="Normal 6 2 6 3" xfId="631"/>
+    <cellStyle name="Normal 6 2 6 4" xfId="630"/>
+    <cellStyle name="Normal 6 2 7" xfId="332"/>
+    <cellStyle name="Normal 6 2 7 2" xfId="195"/>
+    <cellStyle name="Normal 6 2 7 2 2" xfId="635"/>
+    <cellStyle name="Normal 6 2 7 2 3" xfId="636"/>
+    <cellStyle name="Normal 6 2 7 3" xfId="196"/>
+    <cellStyle name="Normal 6 2 7 4" xfId="427"/>
+    <cellStyle name="Normal 6 2 8" xfId="335"/>
+    <cellStyle name="Normal 6 2 8 2" xfId="474"/>
+    <cellStyle name="Normal 6 2 8 2 2" xfId="524"/>
+    <cellStyle name="Normal 6 2 8 2 3" xfId="523"/>
+    <cellStyle name="Normal 6 2 8 3" xfId="473"/>
+    <cellStyle name="Normal 6 2 8 4" xfId="479"/>
+    <cellStyle name="Normal 6 2 9" xfId="334"/>
+    <cellStyle name="Normal 6 2 9 2" xfId="26"/>
+    <cellStyle name="Normal 6 2 9 3" xfId="98"/>
+    <cellStyle name="Normal 6 3" xfId="314"/>
+    <cellStyle name="Normal 6 3 10" xfId="183"/>
+    <cellStyle name="Normal 6 3 2" xfId="548"/>
+    <cellStyle name="Normal 6 3 2 2" xfId="207"/>
+    <cellStyle name="Normal 6 3 2 2 2" xfId="237"/>
+    <cellStyle name="Normal 6 3 2 2 2 2" xfId="50"/>
+    <cellStyle name="Normal 6 3 2 2 2 2 2" xfId="89"/>
+    <cellStyle name="Normal 6 3 2 2 2 2 3" xfId="90"/>
+    <cellStyle name="Normal 6 3 2 2 2 3" xfId="51"/>
+    <cellStyle name="Normal 6 3 2 2 2 4" xfId="48"/>
+    <cellStyle name="Normal 6 3 2 2 3" xfId="238"/>
+    <cellStyle name="Normal 6 3 2 2 3 2" xfId="499"/>
+    <cellStyle name="Normal 6 3 2 2 3 2 2" xfId="288"/>
+    <cellStyle name="Normal 6 3 2 2 3 2 3" xfId="287"/>
+    <cellStyle name="Normal 6 3 2 2 3 3" xfId="498"/>
+    <cellStyle name="Normal 6 3 2 2 3 4" xfId="495"/>
+    <cellStyle name="Normal 6 3 2 2 4" xfId="234"/>
+    <cellStyle name="Normal 6 3 2 2 4 2" xfId="612"/>
+    <cellStyle name="Normal 6 3 2 2 4 3" xfId="613"/>
+    <cellStyle name="Normal 6 3 2 2 5" xfId="235"/>
+    <cellStyle name="Normal 6 3 2 2 6" xfId="236"/>
+    <cellStyle name="Normal 6 3 2 3" xfId="208"/>
+    <cellStyle name="Normal 6 3 2 3 2" xfId="37"/>
+    <cellStyle name="Normal 6 3 2 3 2 2" xfId="394"/>
+    <cellStyle name="Normal 6 3 2 3 2 3" xfId="393"/>
+    <cellStyle name="Normal 6 3 2 3 3" xfId="36"/>
+    <cellStyle name="Normal 6 3 2 3 4" xfId="35"/>
+    <cellStyle name="Normal 6 3 2 4" xfId="209"/>
+    <cellStyle name="Normal 6 3 2 4 2" xfId="627"/>
+    <cellStyle name="Normal 6 3 2 4 2 2" xfId="486"/>
+    <cellStyle name="Normal 6 3 2 4 2 3" xfId="487"/>
+    <cellStyle name="Normal 6 3 2 4 3" xfId="628"/>
+    <cellStyle name="Normal 6 3 2 4 4" xfId="629"/>
+    <cellStyle name="Normal 6 3 2 5" xfId="210"/>
+    <cellStyle name="Normal 6 3 2 5 2" xfId="431"/>
+    <cellStyle name="Normal 6 3 2 5 3" xfId="430"/>
+    <cellStyle name="Normal 6 3 2 6" xfId="211"/>
+    <cellStyle name="Normal 6 3 2 7" xfId="212"/>
+    <cellStyle name="Normal 6 3 3" xfId="549"/>
+    <cellStyle name="Normal 6 3 3 2" xfId="645"/>
+    <cellStyle name="Normal 6 3 3 2 2" xfId="558"/>
+    <cellStyle name="Normal 6 3 3 2 2 2" xfId="190"/>
+    <cellStyle name="Normal 6 3 3 2 2 3" xfId="189"/>
+    <cellStyle name="Normal 6 3 3 2 3" xfId="557"/>
+    <cellStyle name="Normal 6 3 3 2 4" xfId="556"/>
+    <cellStyle name="Normal 6 3 3 3" xfId="644"/>
+    <cellStyle name="Normal 6 3 3 3 2" xfId="114"/>
+    <cellStyle name="Normal 6 3 3 3 2 2" xfId="653"/>
+    <cellStyle name="Normal 6 3 3 3 2 3" xfId="654"/>
+    <cellStyle name="Normal 6 3 3 3 3" xfId="115"/>
+    <cellStyle name="Normal 6 3 3 3 4" xfId="112"/>
+    <cellStyle name="Normal 6 3 3 4" xfId="647"/>
+    <cellStyle name="Normal 6 3 3 4 2" xfId="317"/>
+    <cellStyle name="Normal 6 3 3 4 3" xfId="316"/>
+    <cellStyle name="Normal 6 3 3 5" xfId="646"/>
+    <cellStyle name="Normal 6 3 3 6" xfId="648"/>
+    <cellStyle name="Normal 6 3 4" xfId="550"/>
+    <cellStyle name="Normal 6 3 4 2" xfId="160"/>
+    <cellStyle name="Normal 6 3 4 2 2" xfId="470"/>
+    <cellStyle name="Normal 6 3 4 2 3" xfId="471"/>
+    <cellStyle name="Normal 6 3 4 3" xfId="164"/>
+    <cellStyle name="Normal 6 3 4 4" xfId="155"/>
+    <cellStyle name="Normal 6 3 5" xfId="551"/>
+    <cellStyle name="Normal 6 3 5 2" xfId="493"/>
+    <cellStyle name="Normal 6 3 5 2 2" xfId="53"/>
+    <cellStyle name="Normal 6 3 5 2 3" xfId="52"/>
+    <cellStyle name="Normal 6 3 5 3" xfId="492"/>
+    <cellStyle name="Normal 6 3 5 4" xfId="491"/>
+    <cellStyle name="Normal 6 3 6" xfId="552"/>
+    <cellStyle name="Normal 6 3 6 2" xfId="323"/>
+    <cellStyle name="Normal 6 3 6 2 2" xfId="153"/>
+    <cellStyle name="Normal 6 3 6 2 3" xfId="154"/>
+    <cellStyle name="Normal 6 3 6 3" xfId="324"/>
+    <cellStyle name="Normal 6 3 6 4" xfId="322"/>
+    <cellStyle name="Normal 6 3 7" xfId="553"/>
+    <cellStyle name="Normal 6 3 7 2" xfId="111"/>
+    <cellStyle name="Normal 6 3 7 2 2" xfId="347"/>
+    <cellStyle name="Normal 6 3 7 2 3" xfId="346"/>
+    <cellStyle name="Normal 6 3 7 3" xfId="110"/>
+    <cellStyle name="Normal 6 3 7 4" xfId="109"/>
+    <cellStyle name="Normal 6 3 8" xfId="501"/>
+    <cellStyle name="Normal 6 3 8 2" xfId="305"/>
+    <cellStyle name="Normal 6 3 8 3" xfId="306"/>
+    <cellStyle name="Normal 6 3 9" xfId="502"/>
+    <cellStyle name="Normal 6 4" xfId="311"/>
+    <cellStyle name="Normal 6 4 10" xfId="100"/>
+    <cellStyle name="Normal 6 4 2" xfId="92"/>
+    <cellStyle name="Normal 6 4 2 2" xfId="140"/>
+    <cellStyle name="Normal 6 4 2 2 2" xfId="375"/>
+    <cellStyle name="Normal 6 4 2 2 2 2" xfId="267"/>
+    <cellStyle name="Normal 6 4 2 2 2 2 2" xfId="382"/>
+    <cellStyle name="Normal 6 4 2 2 2 2 3" xfId="381"/>
+    <cellStyle name="Normal 6 4 2 2 2 3" xfId="266"/>
+    <cellStyle name="Normal 6 4 2 2 2 4" xfId="268"/>
+    <cellStyle name="Normal 6 4 2 2 3" xfId="395"/>
+    <cellStyle name="Normal 6 4 2 2 3 2" xfId="480"/>
+    <cellStyle name="Normal 6 4 2 2 3 2 2" xfId="187"/>
+    <cellStyle name="Normal 6 4 2 2 3 2 3" xfId="188"/>
+    <cellStyle name="Normal 6 4 2 2 3 3" xfId="481"/>
+    <cellStyle name="Normal 6 4 2 2 3 4" xfId="484"/>
+    <cellStyle name="Normal 6 4 2 2 4" xfId="402"/>
+    <cellStyle name="Normal 6 4 2 2 4 2" xfId="429"/>
+    <cellStyle name="Normal 6 4 2 2 4 3" xfId="428"/>
+    <cellStyle name="Normal 6 4 2 2 5" xfId="401"/>
+    <cellStyle name="Normal 6 4 2 2 6" xfId="379"/>
+    <cellStyle name="Normal 6 4 2 3" xfId="139"/>
+    <cellStyle name="Normal 6 4 2 3 2" xfId="587"/>
+    <cellStyle name="Normal 6 4 2 3 2 2" xfId="655"/>
+    <cellStyle name="Normal 6 4 2 3 2 3" xfId="656"/>
+    <cellStyle name="Normal 6 4 2 3 3" xfId="588"/>
+    <cellStyle name="Normal 6 4 2 3 4" xfId="591"/>
+    <cellStyle name="Normal 6 4 2 4" xfId="138"/>
+    <cellStyle name="Normal 6 4 2 4 2" xfId="623"/>
+    <cellStyle name="Normal 6 4 2 4 2 2" xfId="605"/>
+    <cellStyle name="Normal 6 4 2 4 2 3" xfId="604"/>
+    <cellStyle name="Normal 6 4 2 4 3" xfId="622"/>
+    <cellStyle name="Normal 6 4 2 4 4" xfId="621"/>
+    <cellStyle name="Normal 6 4 2 5" xfId="137"/>
+    <cellStyle name="Normal 6 4 2 5 2" xfId="184"/>
+    <cellStyle name="Normal 6 4 2 5 3" xfId="185"/>
+    <cellStyle name="Normal 6 4 2 6" xfId="136"/>
+    <cellStyle name="Normal 6 4 2 7" xfId="135"/>
+    <cellStyle name="Normal 6 4 3" xfId="91"/>
+    <cellStyle name="Normal 6 4 3 2" xfId="342"/>
+    <cellStyle name="Normal 6 4 3 2 2" xfId="200"/>
+    <cellStyle name="Normal 6 4 3 2 2 2" xfId="127"/>
+    <cellStyle name="Normal 6 4 3 2 2 3" xfId="128"/>
+    <cellStyle name="Normal 6 4 3 2 3" xfId="201"/>
+    <cellStyle name="Normal 6 4 3 2 4" xfId="204"/>
+    <cellStyle name="Normal 6 4 3 3" xfId="343"/>
+    <cellStyle name="Normal 6 4 3 3 2" xfId="643"/>
+    <cellStyle name="Normal 6 4 3 3 2 2" xfId="298"/>
+    <cellStyle name="Normal 6 4 3 3 2 3" xfId="297"/>
+    <cellStyle name="Normal 6 4 3 3 3" xfId="642"/>
+    <cellStyle name="Normal 6 4 3 3 4" xfId="583"/>
+    <cellStyle name="Normal 6 4 3 4" xfId="340"/>
+    <cellStyle name="Normal 6 4 3 4 2" xfId="444"/>
+    <cellStyle name="Normal 6 4 3 4 3" xfId="445"/>
+    <cellStyle name="Normal 6 4 3 5" xfId="341"/>
+    <cellStyle name="Normal 6 4 3 6" xfId="339"/>
+    <cellStyle name="Normal 6 4 4" xfId="441"/>
+    <cellStyle name="Normal 6 4 4 2" xfId="292"/>
+    <cellStyle name="Normal 6 4 4 2 2" xfId="247"/>
+    <cellStyle name="Normal 6 4 4 2 3" xfId="246"/>
+    <cellStyle name="Normal 6 4 4 3" xfId="412"/>
+    <cellStyle name="Normal 6 4 4 4" xfId="293"/>
+    <cellStyle name="Normal 6 4 5" xfId="440"/>
+    <cellStyle name="Normal 6 4 5 2" xfId="460"/>
+    <cellStyle name="Normal 6 4 5 2 2" xfId="517"/>
+    <cellStyle name="Normal 6 4 5 2 3" xfId="520"/>
+    <cellStyle name="Normal 6 4 5 3" xfId="461"/>
+    <cellStyle name="Normal 6 4 5 4" xfId="462"/>
+    <cellStyle name="Normal 6 4 6" xfId="88"/>
+    <cellStyle name="Normal 6 4 6 2" xfId="5"/>
+    <cellStyle name="Normal 6 4 6 2 2" xfId="595"/>
+    <cellStyle name="Normal 6 4 6 2 3" xfId="594"/>
+    <cellStyle name="Normal 6 4 6 3" xfId="4"/>
+    <cellStyle name="Normal 6 4 6 4" xfId="10"/>
+    <cellStyle name="Normal 6 4 7" xfId="87"/>
+    <cellStyle name="Normal 6 4 7 2" xfId="221"/>
+    <cellStyle name="Normal 6 4 7 2 2" xfId="403"/>
+    <cellStyle name="Normal 6 4 7 2 3" xfId="404"/>
+    <cellStyle name="Normal 6 4 7 3" xfId="222"/>
+    <cellStyle name="Normal 6 4 7 4" xfId="224"/>
+    <cellStyle name="Normal 6 4 8" xfId="97"/>
+    <cellStyle name="Normal 6 4 8 2" xfId="95"/>
+    <cellStyle name="Normal 6 4 8 3" xfId="380"/>
+    <cellStyle name="Normal 6 4 9" xfId="96"/>
+    <cellStyle name="Normal 6 5" xfId="310"/>
+    <cellStyle name="Normal 6 5 2" xfId="285"/>
+    <cellStyle name="Normal 6 5 2 2" xfId="534"/>
+    <cellStyle name="Normal 6 5 2 2 2" xfId="182"/>
+    <cellStyle name="Normal 6 5 2 2 2 2" xfId="258"/>
+    <cellStyle name="Normal 6 5 2 2 2 2 2" xfId="546"/>
+    <cellStyle name="Normal 6 5 2 2 2 2 3" xfId="547"/>
+    <cellStyle name="Normal 6 5 2 2 2 3" xfId="259"/>
+    <cellStyle name="Normal 6 5 2 2 2 4" xfId="261"/>
+    <cellStyle name="Normal 6 5 2 2 3" xfId="417"/>
+    <cellStyle name="Normal 6 5 2 2 3 2" xfId="302"/>
+    <cellStyle name="Normal 6 5 2 2 3 2 2" xfId="107"/>
+    <cellStyle name="Normal 6 5 2 2 3 2 3" xfId="106"/>
+    <cellStyle name="Normal 6 5 2 2 3 3" xfId="301"/>
+    <cellStyle name="Normal 6 5 2 2 3 4" xfId="79"/>
+    <cellStyle name="Normal 6 5 2 2 4" xfId="253"/>
+    <cellStyle name="Normal 6 5 2 2 4 2" xfId="419"/>
+    <cellStyle name="Normal 6 5 2 2 4 3" xfId="420"/>
+    <cellStyle name="Normal 6 5 2 2 5" xfId="254"/>
+    <cellStyle name="Normal 6 5 2 2 6" xfId="192"/>
+    <cellStyle name="Normal 6 5 2 3" xfId="535"/>
+    <cellStyle name="Normal 6 5 2 3 2" xfId="649"/>
+    <cellStyle name="Normal 6 5 2 3 2 2" xfId="370"/>
+    <cellStyle name="Normal 6 5 2 3 2 3" xfId="369"/>
+    <cellStyle name="Normal 6 5 2 3 3" xfId="70"/>
+    <cellStyle name="Normal 6 5 2 3 4" xfId="276"/>
+    <cellStyle name="Normal 6 5 2 4" xfId="532"/>
+    <cellStyle name="Normal 6 5 2 4 2" xfId="518"/>
+    <cellStyle name="Normal 6 5 2 4 2 2" xfId="633"/>
+    <cellStyle name="Normal 6 5 2 4 2 3" xfId="634"/>
+    <cellStyle name="Normal 6 5 2 4 3" xfId="519"/>
+    <cellStyle name="Normal 6 5 2 4 4" xfId="514"/>
+    <cellStyle name="Normal 6 5 2 5" xfId="447"/>
+    <cellStyle name="Normal 6 5 2 5 2" xfId="304"/>
+    <cellStyle name="Normal 6 5 2 5 3" xfId="303"/>
+    <cellStyle name="Normal 6 5 2 6" xfId="530"/>
+    <cellStyle name="Normal 6 5 2 7" xfId="531"/>
+    <cellStyle name="Normal 6 5 3" xfId="286"/>
+    <cellStyle name="Normal 6 5 3 2" xfId="321"/>
+    <cellStyle name="Normal 6 5 3 2 2" xfId="134"/>
+    <cellStyle name="Normal 6 5 3 2 2 2" xfId="600"/>
+    <cellStyle name="Normal 6 5 3 2 2 3" xfId="599"/>
+    <cellStyle name="Normal 6 5 3 2 3" xfId="229"/>
+    <cellStyle name="Normal 6 5 3 2 4" xfId="472"/>
+    <cellStyle name="Normal 6 5 3 3" xfId="320"/>
+    <cellStyle name="Normal 6 5 3 3 2" xfId="32"/>
+    <cellStyle name="Normal 6 5 3 3 2 2" xfId="423"/>
+    <cellStyle name="Normal 6 5 3 3 2 3" xfId="424"/>
+    <cellStyle name="Normal 6 5 3 3 3" xfId="34"/>
+    <cellStyle name="Normal 6 5 3 3 4" xfId="9"/>
+    <cellStyle name="Normal 6 5 3 4" xfId="319"/>
+    <cellStyle name="Normal 6 5 3 4 2" xfId="94"/>
+    <cellStyle name="Normal 6 5 3 4 3" xfId="93"/>
+    <cellStyle name="Normal 6 5 3 5" xfId="318"/>
+    <cellStyle name="Normal 6 5 3 6" xfId="525"/>
+    <cellStyle name="Normal 6 5 4" xfId="283"/>
+    <cellStyle name="Normal 6 5 4 2" xfId="582"/>
+    <cellStyle name="Normal 6 5 4 2 2" xfId="478"/>
+    <cellStyle name="Normal 6 5 4 2 3" xfId="639"/>
+    <cellStyle name="Normal 6 5 4 3" xfId="197"/>
+    <cellStyle name="Normal 6 5 4 4" xfId="584"/>
+    <cellStyle name="Normal 6 5 5" xfId="284"/>
+    <cellStyle name="Normal 6 5 5 2" xfId="387"/>
+    <cellStyle name="Normal 6 5 5 2 2" xfId="119"/>
+    <cellStyle name="Normal 6 5 5 2 3" xfId="33"/>
+    <cellStyle name="Normal 6 5 5 3" xfId="386"/>
+    <cellStyle name="Normal 6 5 5 4" xfId="388"/>
+    <cellStyle name="Normal 6 5 6" xfId="281"/>
+    <cellStyle name="Normal 6 5 6 2" xfId="74"/>
+    <cellStyle name="Normal 6 5 6 3" xfId="356"/>
+    <cellStyle name="Normal 6 5 7" xfId="282"/>
+    <cellStyle name="Normal 6 5 8" xfId="280"/>
+    <cellStyle name="Normal 6 6" xfId="313"/>
+    <cellStyle name="Normal 6 6 2" xfId="326"/>
+    <cellStyle name="Normal 6 6 2 2" xfId="245"/>
+    <cellStyle name="Normal 6 6 2 2 2" xfId="64"/>
+    <cellStyle name="Normal 6 6 2 2 2 2" xfId="618"/>
+    <cellStyle name="Normal 6 6 2 2 2 2 2" xfId="39"/>
+    <cellStyle name="Normal 6 6 2 2 2 2 3" xfId="515"/>
+    <cellStyle name="Normal 6 6 2 2 2 3" xfId="617"/>
+    <cellStyle name="Normal 6 6 2 2 2 4" xfId="619"/>
+    <cellStyle name="Normal 6 6 2 2 3" xfId="113"/>
+    <cellStyle name="Normal 6 6 2 2 3 2" xfId="116"/>
+    <cellStyle name="Normal 6 6 2 2 3 2 2" xfId="456"/>
+    <cellStyle name="Normal 6 6 2 2 3 2 3" xfId="457"/>
+    <cellStyle name="Normal 6 6 2 2 3 3" xfId="296"/>
+    <cellStyle name="Normal 6 6 2 2 3 4" xfId="176"/>
+    <cellStyle name="Normal 6 6 2 2 4" xfId="80"/>
+    <cellStyle name="Normal 6 6 2 2 4 2" xfId="199"/>
+    <cellStyle name="Normal 6 6 2 2 4 3" xfId="198"/>
+    <cellStyle name="Normal 6 6 2 2 5" xfId="77"/>
+    <cellStyle name="Normal 6 6 2 2 6" xfId="129"/>
+    <cellStyle name="Normal 6 6 2 3" xfId="163"/>
+    <cellStyle name="Normal 6 6 2 3 2" xfId="662"/>
+    <cellStyle name="Normal 6 6 2 3 2 2" xfId="278"/>
+    <cellStyle name="Normal 6 6 2 3 2 3" xfId="279"/>
+    <cellStyle name="Normal 6 6 2 3 3" xfId="1"/>
+    <cellStyle name="Normal 6 6 2 3 4" xfId="2"/>
+    <cellStyle name="Normal 6 6 2 4" xfId="586"/>
+    <cellStyle name="Normal 6 6 2 4 2" xfId="581"/>
+    <cellStyle name="Normal 6 6 2 4 2 2" xfId="383"/>
+    <cellStyle name="Normal 6 6 2 4 2 3" xfId="516"/>
+    <cellStyle name="Normal 6 6 2 4 3" xfId="580"/>
+    <cellStyle name="Normal 6 6 2 4 4" xfId="579"/>
+    <cellStyle name="Normal 6 6 2 5" xfId="159"/>
+    <cellStyle name="Normal 6 6 2 5 2" xfId="141"/>
+    <cellStyle name="Normal 6 6 2 5 3" xfId="142"/>
+    <cellStyle name="Normal 6 6 2 6" xfId="162"/>
+    <cellStyle name="Normal 6 6 2 7" xfId="161"/>
+    <cellStyle name="Normal 6 6 3" xfId="325"/>
+    <cellStyle name="Normal 6 6 3 2" xfId="374"/>
+    <cellStyle name="Normal 6 6 3 2 2" xfId="275"/>
+    <cellStyle name="Normal 6 6 3 2 2 2" xfId="410"/>
+    <cellStyle name="Normal 6 6 3 2 2 3" xfId="411"/>
+    <cellStyle name="Normal 6 6 3 2 3" xfId="362"/>
+    <cellStyle name="Normal 6 6 3 2 4" xfId="277"/>
+    <cellStyle name="Normal 6 6 3 3" xfId="186"/>
+    <cellStyle name="Normal 6 6 3 3 2" xfId="105"/>
+    <cellStyle name="Normal 6 6 3 3 2 2" xfId="300"/>
+    <cellStyle name="Normal 6 6 3 3 2 3" xfId="299"/>
+    <cellStyle name="Normal 6 6 3 3 3" xfId="104"/>
+    <cellStyle name="Normal 6 6 3 3 4" xfId="574"/>
+    <cellStyle name="Normal 6 6 3 4" xfId="371"/>
+    <cellStyle name="Normal 6 6 3 4 2" xfId="391"/>
+    <cellStyle name="Normal 6 6 3 4 3" xfId="392"/>
+    <cellStyle name="Normal 6 6 3 5" xfId="372"/>
+    <cellStyle name="Normal 6 6 3 6" xfId="373"/>
+    <cellStyle name="Normal 6 6 4" xfId="108"/>
+    <cellStyle name="Normal 6 6 4 2" xfId="435"/>
+    <cellStyle name="Normal 6 6 4 2 2" xfId="433"/>
+    <cellStyle name="Normal 6 6 4 2 3" xfId="432"/>
+    <cellStyle name="Normal 6 6 4 3" xfId="434"/>
+    <cellStyle name="Normal 6 6 4 4" xfId="438"/>
+    <cellStyle name="Normal 6 6 5" xfId="585"/>
+    <cellStyle name="Normal 6 6 5 2" xfId="596"/>
+    <cellStyle name="Normal 6 6 5 2 2" xfId="554"/>
+    <cellStyle name="Normal 6 6 5 2 3" xfId="555"/>
+    <cellStyle name="Normal 6 6 5 3" xfId="597"/>
+    <cellStyle name="Normal 6 6 5 4" xfId="598"/>
+    <cellStyle name="Normal 6 6 6" xfId="616"/>
+    <cellStyle name="Normal 6 6 6 2" xfId="29"/>
+    <cellStyle name="Normal 6 6 6 3" xfId="28"/>
+    <cellStyle name="Normal 6 6 7" xfId="507"/>
+    <cellStyle name="Normal 6 6 8" xfId="513"/>
+    <cellStyle name="Normal 6 7" xfId="312"/>
+    <cellStyle name="Normal 6 7 2" xfId="65"/>
+    <cellStyle name="Normal 6 7 2 2" xfId="610"/>
+    <cellStyle name="Normal 6 7 2 2 2" xfId="122"/>
+    <cellStyle name="Normal 6 7 2 2 2 2" xfId="615"/>
+    <cellStyle name="Normal 6 7 2 2 2 2 2" xfId="243"/>
+    <cellStyle name="Normal 6 7 2 2 2 2 3" xfId="244"/>
+    <cellStyle name="Normal 6 7 2 2 2 3" xfId="120"/>
+    <cellStyle name="Normal 6 7 2 2 2 4" xfId="562"/>
+    <cellStyle name="Normal 6 7 2 2 3" xfId="123"/>
+    <cellStyle name="Normal 6 7 2 2 3 2" xfId="358"/>
+    <cellStyle name="Normal 6 7 2 2 3 2 2" xfId="390"/>
+    <cellStyle name="Normal 6 7 2 2 3 2 3" xfId="144"/>
+    <cellStyle name="Normal 6 7 2 2 3 3" xfId="357"/>
+    <cellStyle name="Normal 6 7 2 2 3 4" xfId="359"/>
+    <cellStyle name="Normal 6 7 2 2 4" xfId="124"/>
+    <cellStyle name="Normal 6 7 2 2 4 2" xfId="170"/>
+    <cellStyle name="Normal 6 7 2 2 4 3" xfId="171"/>
+    <cellStyle name="Normal 6 7 2 2 5" xfId="125"/>
+    <cellStyle name="Normal 6 7 2 2 6" xfId="126"/>
+    <cellStyle name="Normal 6 7 2 3" xfId="611"/>
+    <cellStyle name="Normal 6 7 2 3 2" xfId="572"/>
+    <cellStyle name="Normal 6 7 2 3 2 2" xfId="49"/>
+    <cellStyle name="Normal 6 7 2 3 2 3" xfId="327"/>
+    <cellStyle name="Normal 6 7 2 3 3" xfId="571"/>
+    <cellStyle name="Normal 6 7 2 3 4" xfId="573"/>
+    <cellStyle name="Normal 6 7 2 4" xfId="606"/>
+    <cellStyle name="Normal 6 7 2 4 2" xfId="272"/>
+    <cellStyle name="Normal 6 7 2 4 2 2" xfId="179"/>
+    <cellStyle name="Normal 6 7 2 4 2 3" xfId="536"/>
+    <cellStyle name="Normal 6 7 2 4 3" xfId="273"/>
+    <cellStyle name="Normal 6 7 2 4 4" xfId="271"/>
+    <cellStyle name="Normal 6 7 2 5" xfId="607"/>
+    <cellStyle name="Normal 6 7 2 5 2" xfId="86"/>
+    <cellStyle name="Normal 6 7 2 5 3" xfId="85"/>
+    <cellStyle name="Normal 6 7 2 6" xfId="608"/>
+    <cellStyle name="Normal 6 7 2 7" xfId="609"/>
+    <cellStyle name="Normal 6 7 3" xfId="66"/>
+    <cellStyle name="Normal 6 7 3 2" xfId="409"/>
+    <cellStyle name="Normal 6 7 3 2 2" xfId="476"/>
+    <cellStyle name="Normal 6 7 3 2 2 2" xfId="353"/>
+    <cellStyle name="Normal 6 7 3 2 2 3" xfId="352"/>
+    <cellStyle name="Normal 6 7 3 2 3" xfId="475"/>
+    <cellStyle name="Normal 6 7 3 2 4" xfId="477"/>
+    <cellStyle name="Normal 6 7 3 3" xfId="418"/>
+    <cellStyle name="Normal 6 7 3 3 2" xfId="650"/>
+    <cellStyle name="Normal 6 7 3 3 2 2" xfId="19"/>
+    <cellStyle name="Normal 6 7 3 3 2 3" xfId="23"/>
+    <cellStyle name="Normal 6 7 3 3 3" xfId="651"/>
+    <cellStyle name="Normal 6 7 3 3 4" xfId="652"/>
+    <cellStyle name="Normal 6 7 3 4" xfId="414"/>
+    <cellStyle name="Normal 6 7 3 4 2" xfId="563"/>
+    <cellStyle name="Normal 6 7 3 4 3" xfId="620"/>
+    <cellStyle name="Normal 6 7 3 5" xfId="413"/>
+    <cellStyle name="Normal 6 7 3 6" xfId="407"/>
+    <cellStyle name="Normal 6 7 4" xfId="60"/>
+    <cellStyle name="Normal 6 7 4 2" xfId="166"/>
+    <cellStyle name="Normal 6 7 4 2 2" xfId="509"/>
+    <cellStyle name="Normal 6 7 4 2 3" xfId="510"/>
+    <cellStyle name="Normal 6 7 4 3" xfId="490"/>
+    <cellStyle name="Normal 6 7 4 4" xfId="494"/>
+    <cellStyle name="Normal 6 7 5" xfId="61"/>
+    <cellStyle name="Normal 6 7 5 2" xfId="638"/>
+    <cellStyle name="Normal 6 7 5 2 2" xfId="152"/>
+    <cellStyle name="Normal 6 7 5 2 3" xfId="38"/>
+    <cellStyle name="Normal 6 7 5 3" xfId="637"/>
+    <cellStyle name="Normal 6 7 5 4" xfId="641"/>
+    <cellStyle name="Normal 6 7 6" xfId="62"/>
+    <cellStyle name="Normal 6 7 6 2" xfId="415"/>
+    <cellStyle name="Normal 6 7 6 3" xfId="416"/>
+    <cellStyle name="Normal 6 7 7" xfId="63"/>
+    <cellStyle name="Normal 6 7 8" xfId="59"/>
+    <cellStyle name="Normal 6 8" xfId="308"/>
+    <cellStyle name="Normal 6 8 2" xfId="364"/>
+    <cellStyle name="Normal 6 8 2 2" xfId="146"/>
+    <cellStyle name="Normal 6 8 2 2 2" xfId="3"/>
+    <cellStyle name="Normal 6 8 2 2 2 2" xfId="345"/>
+    <cellStyle name="Normal 6 8 2 2 2 3" xfId="344"/>
+    <cellStyle name="Normal 6 8 2 2 3" xfId="18"/>
+    <cellStyle name="Normal 6 8 2 2 4" xfId="575"/>
+    <cellStyle name="Normal 6 8 2 3" xfId="145"/>
+    <cellStyle name="Normal 6 8 2 3 2" xfId="240"/>
+    <cellStyle name="Normal 6 8 2 3 2 2" xfId="202"/>
+    <cellStyle name="Normal 6 8 2 3 2 3" xfId="203"/>
+    <cellStyle name="Normal 6 8 2 3 3" xfId="241"/>
+    <cellStyle name="Normal 6 8 2 3 4" xfId="239"/>
+    <cellStyle name="Normal 6 8 2 4" xfId="149"/>
+    <cellStyle name="Normal 6 8 2 4 2" xfId="625"/>
+    <cellStyle name="Normal 6 8 2 4 3" xfId="624"/>
+    <cellStyle name="Normal 6 8 2 5" xfId="148"/>
+    <cellStyle name="Normal 6 8 2 6" xfId="147"/>
+    <cellStyle name="Normal 6 8 3" xfId="363"/>
+    <cellStyle name="Normal 6 8 3 2" xfId="350"/>
+    <cellStyle name="Normal 6 8 3 2 2" xfId="488"/>
+    <cellStyle name="Normal 6 8 3 2 3" xfId="489"/>
+    <cellStyle name="Normal 6 8 3 3" xfId="351"/>
+    <cellStyle name="Normal 6 8 3 4" xfId="354"/>
+    <cellStyle name="Normal 6 8 4" xfId="368"/>
+    <cellStyle name="Normal 6 8 4 2" xfId="565"/>
+    <cellStyle name="Normal 6 8 4 2 2" xfId="165"/>
+    <cellStyle name="Normal 6 8 4 2 3" xfId="446"/>
+    <cellStyle name="Normal 6 8 4 3" xfId="564"/>
+    <cellStyle name="Normal 6 8 4 4" xfId="559"/>
+    <cellStyle name="Normal 6 8 5" xfId="367"/>
+    <cellStyle name="Normal 6 8 5 2" xfId="102"/>
+    <cellStyle name="Normal 6 8 5 3" xfId="103"/>
+    <cellStyle name="Normal 6 8 6" xfId="366"/>
+    <cellStyle name="Normal 6 8 7" xfId="365"/>
+    <cellStyle name="Normal 6 9" xfId="307"/>
+    <cellStyle name="Normal 6 9 2" xfId="537"/>
+    <cellStyle name="Normal 6 9 2 2" xfId="215"/>
+    <cellStyle name="Normal 6 9 2 2 2" xfId="264"/>
+    <cellStyle name="Normal 6 9 2 2 3" xfId="265"/>
+    <cellStyle name="Normal 6 9 2 3" xfId="566"/>
+    <cellStyle name="Normal 6 9 2 4" xfId="217"/>
+    <cellStyle name="Normal 6 9 3" xfId="538"/>
+    <cellStyle name="Normal 6 9 3 2" xfId="658"/>
+    <cellStyle name="Normal 6 9 3 2 2" xfId="426"/>
+    <cellStyle name="Normal 6 9 3 2 3" xfId="425"/>
+    <cellStyle name="Normal 6 9 3 3" xfId="657"/>
+    <cellStyle name="Normal 6 9 3 4" xfId="659"/>
+    <cellStyle name="Normal 6 9 4" xfId="540"/>
+    <cellStyle name="Normal 6 9 4 2" xfId="640"/>
+    <cellStyle name="Normal 6 9 4 3" xfId="567"/>
+    <cellStyle name="Normal 6 9 5" xfId="541"/>
+    <cellStyle name="Normal 6 9 6" xfId="539"/>
+    <cellStyle name="Normal 7" xfId="452"/>
+    <cellStyle name="Normal 7 2" xfId="529"/>
+    <cellStyle name="Normal 8" xfId="455"/>
+    <cellStyle name="Normal 8 2" xfId="576"/>
+    <cellStyle name="Normal 9" xfId="454"/>
+    <cellStyle name="Normal 9 2" xfId="58"/>
+    <cellStyle name="Percent 2" xfId="269"/>
+    <cellStyle name="Percent 2 2" xfId="78"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2170,29 +2169,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.33203125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="47.28515625" style="12" customWidth="1"/>
     <col min="2" max="2" width="18" style="14" customWidth="1"/>
-    <col min="3" max="5" width="9.109375" style="12" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="9.109375" style="12" customWidth="1"/>
-    <col min="14" max="16384" width="9.109375" style="12"/>
+    <col min="3" max="5" width="9.140625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="9.140625" style="12" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2200,7 +2199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -2216,7 +2215,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>3</v>
       </c>
@@ -2226,7 +2225,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>4</v>
       </c>
@@ -2236,7 +2235,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
@@ -2246,7 +2245,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>6</v>
       </c>
@@ -2256,17 +2255,17 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="11">
-        <v>0.14000000000000001</v>
+        <v>1</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>8</v>
       </c>
@@ -2279,7 +2278,7 @@
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>9</v>
       </c>
@@ -2289,7 +2288,7 @@
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>10</v>
       </c>
@@ -2299,7 +2298,7 @@
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>11</v>
       </c>
@@ -2307,7 +2306,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>12</v>
       </c>
@@ -2315,7 +2314,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>13</v>
       </c>
@@ -2326,7 +2325,7 @@
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>14</v>
       </c>
@@ -2336,7 +2335,7 @@
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>15</v>
       </c>
@@ -2349,7 +2348,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>17</v>
       </c>
@@ -2362,7 +2361,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>19</v>
       </c>
@@ -2370,7 +2369,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>20</v>
       </c>
@@ -2378,7 +2377,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>21</v>
       </c>
@@ -2386,7 +2385,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>22</v>
       </c>
@@ -2394,7 +2393,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>23</v>
       </c>
@@ -2402,7 +2401,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>24</v>
       </c>
@@ -2410,7 +2409,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>25</v>
       </c>
@@ -2425,7 +2424,7 @@
       </c>
       <c r="E23" s="25"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>26</v>
       </c>
@@ -2440,7 +2439,7 @@
       </c>
       <c r="E24" s="25"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>27</v>
       </c>
@@ -2451,7 +2450,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>29</v>
       </c>
@@ -2459,7 +2458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>30</v>
       </c>
@@ -2467,7 +2466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>31</v>
       </c>
@@ -2475,7 +2474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>32</v>
       </c>
@@ -2483,7 +2482,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>33</v>
       </c>
@@ -2494,7 +2493,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>34</v>
       </c>
@@ -2502,7 +2501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>35</v>
       </c>
@@ -2510,7 +2509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>36</v>
       </c>
@@ -2518,7 +2517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>37</v>
       </c>
@@ -2526,7 +2525,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>38</v>
       </c>
@@ -2538,7 +2537,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>40</v>
       </c>
@@ -2546,7 +2545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>41</v>
       </c>
@@ -2557,7 +2556,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>43</v>
       </c>
@@ -2565,7 +2564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>44</v>
       </c>
@@ -2573,7 +2572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>45</v>
       </c>
@@ -2582,7 +2581,7 @@
         <v>-1767</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>46</v>
       </c>
@@ -2590,7 +2589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>47</v>
       </c>
@@ -2598,7 +2597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>48</v>
       </c>
@@ -2606,7 +2605,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>49</v>
       </c>
@@ -2617,7 +2616,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>51</v>
       </c>
@@ -2625,7 +2624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>52</v>
       </c>
@@ -2633,7 +2632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>53</v>
       </c>
@@ -2641,7 +2640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>54</v>
       </c>
@@ -2649,7 +2648,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>55</v>
       </c>
@@ -2660,7 +2659,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>57</v>
       </c>
@@ -2668,7 +2667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
         <v>58</v>
       </c>
@@ -2676,7 +2675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>59</v>
       </c>
@@ -2684,7 +2683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>60</v>
       </c>
@@ -2692,7 +2691,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>61</v>
       </c>
@@ -2700,7 +2699,7 @@
         <v>0.57773922585488524</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>62</v>
       </c>
@@ -2708,7 +2707,7 @@
         <v>0.72388695785815904</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>63</v>
       </c>
@@ -2718,20 +2717,20 @@
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="B3:B10 F9:F10 G9:G10" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="B3:B10 F9:F10 G9:G10">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B2 F2:F6 G2:G6" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B2 F2:F6 G2:G6">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B7 F7:F8 G7:G8" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B7 F7:F8 G7:G8">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" promptTitle="Age unstratified" prompt="Some values you can replace the ones to the left with if you want a manual calibration for the model without age stratification." sqref="H1" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B4:B16 C16 D16" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation showInputMessage="1" showErrorMessage="1" promptTitle="Age unstratified" prompt="Some values you can replace the ones to the left with if you want a manual calibration for the model without age stratification." sqref="H1"/>
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B4:B16 C16 D16">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
@@ -2742,7 +2741,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
@@ -2755,27 +2754,27 @@
       <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.88671875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" style="4" customWidth="1"/>
     <col min="3" max="3" width="11" style="4" customWidth="1"/>
     <col min="4" max="4" width="11" style="5" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" style="23" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" style="23" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" style="23" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="23" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" style="23" customWidth="1"/>
     <col min="8" max="12" width="7" style="23" customWidth="1"/>
-    <col min="13" max="14" width="7.44140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.44140625" style="23" customWidth="1"/>
-    <col min="16" max="16" width="7.88671875" style="23" customWidth="1"/>
+    <col min="13" max="14" width="7.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.42578125" style="23" customWidth="1"/>
+    <col min="16" max="16" width="7.85546875" style="23" customWidth="1"/>
     <col min="17" max="18" width="14" style="23" customWidth="1"/>
-    <col min="19" max="19" width="14.44140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="20" max="23" width="14.44140625" style="23" customWidth="1"/>
-    <col min="24" max="27" width="9.109375" style="23" customWidth="1"/>
-    <col min="28" max="16384" width="9.109375" style="23"/>
+    <col min="19" max="19" width="14.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="20" max="23" width="14.42578125" style="23" customWidth="1"/>
+    <col min="24" max="27" width="9.140625" style="23" customWidth="1"/>
+    <col min="28" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>64</v>
       </c>
@@ -2849,7 +2848,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>75</v>
       </c>
@@ -2865,7 +2864,7 @@
       <c r="S2" s="24"/>
       <c r="T2" s="24"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>77</v>
       </c>
@@ -2884,7 +2883,7 @@
       <c r="S3" s="24"/>
       <c r="T3" s="24"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>78</v>
       </c>
@@ -2904,7 +2903,7 @@
       <c r="T4" s="24"/>
       <c r="U4" s="24"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>79</v>
       </c>
@@ -2923,7 +2922,7 @@
       <c r="T5" s="24"/>
       <c r="U5" s="24"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>80</v>
       </c>
@@ -2940,7 +2939,7 @@
       <c r="T6" s="24"/>
       <c r="U6" s="24"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>81</v>
       </c>
@@ -2983,7 +2982,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>82</v>
       </c>
@@ -3002,7 +3001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>83</v>
       </c>
@@ -3024,7 +3023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>84</v>
       </c>
@@ -3040,7 +3039,7 @@
       </c>
       <c r="V10" s="24"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>85</v>
       </c>
@@ -3056,7 +3055,7 @@
       </c>
       <c r="V11" s="24"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>86</v>
       </c>
@@ -3088,7 +3087,7 @@
         <v>117.42738589211601</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>87</v>
       </c>
@@ -3111,7 +3110,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>88</v>
       </c>
@@ -3125,7 +3124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>89</v>
       </c>
@@ -3142,7 +3141,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>90</v>
       </c>
@@ -3164,7 +3163,7 @@
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
     </row>
-    <row r="18" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:23" x14ac:dyDescent="0.25">
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -3178,12 +3177,12 @@
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
     </row>
-    <row r="23" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:23" x14ac:dyDescent="0.25">
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:23" x14ac:dyDescent="0.25">
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
@@ -3195,61 +3194,61 @@
       <c r="V24" s="22"/>
       <c r="W24" s="22"/>
     </row>
-    <row r="25" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:23" x14ac:dyDescent="0.25">
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
       <c r="S25" s="24"/>
       <c r="T25" s="24"/>
     </row>
-    <row r="26" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:23" x14ac:dyDescent="0.25">
       <c r="S26" s="24"/>
       <c r="T26" s="24"/>
     </row>
-    <row r="27" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:23" x14ac:dyDescent="0.25">
       <c r="S27" s="24"/>
       <c r="T27" s="24"/>
       <c r="U27" s="24"/>
     </row>
-    <row r="28" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:23" x14ac:dyDescent="0.25">
       <c r="S28" s="24"/>
       <c r="T28" s="24"/>
       <c r="U28" s="24"/>
     </row>
-    <row r="29" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="5:23" x14ac:dyDescent="0.25">
       <c r="S29" s="24"/>
       <c r="T29" s="24"/>
       <c r="U29" s="24"/>
     </row>
-    <row r="31" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="5:23" x14ac:dyDescent="0.25">
       <c r="S31" s="24"/>
       <c r="T31" s="24"/>
       <c r="V31" s="24"/>
     </row>
-    <row r="32" spans="5:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:23" x14ac:dyDescent="0.25">
       <c r="S32" s="24"/>
       <c r="T32" s="24"/>
       <c r="U32" s="24"/>
       <c r="V32" s="24"/>
     </row>
-    <row r="33" spans="19:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="19:22" x14ac:dyDescent="0.25">
       <c r="S33" s="24"/>
       <c r="T33" s="24"/>
       <c r="V33" s="24"/>
     </row>
-    <row r="34" spans="19:22" x14ac:dyDescent="0.3">
+    <row r="34" spans="19:22" x14ac:dyDescent="0.25">
       <c r="S34" s="24"/>
       <c r="T34" s="24"/>
       <c r="V34" s="24"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="D7 E23:E25 F23:F25 G23:G25 H23:H25 I23:I25 J23:J25 K23:K25 L23:L25 M23:M25 N23:N25 O23:O25 P23:P25" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C1"/>
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="D7 E23:E25 F23:F25 G23:G25 H23:H25 I23:I25 J23:J25 K23:K25 L23:L25 M23:M25 N23:N25 O23:O25 P23:P25">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C1048576" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C1048576">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -3260,7 +3259,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
   </sheetPr>
@@ -3270,9 +3269,9 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -3286,7 +3285,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -3297,7 +3296,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>95</v>
       </c>

</xml_diff>

<commit_message>
Revise uncertainty parameters and values for short-course MDR-TB regimen
Plus another couple of very minor code revisions.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Documents\AuTuMN\autumn\xls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10350"/>
   </bookViews>
@@ -16,7 +11,7 @@
     <sheet name="time_variants" sheetId="2" r:id="rId2"/>
     <sheet name="dropdown_lists" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -2176,7 +2171,7 @@
   <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B14" sqref="B14:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2330,10 +2325,14 @@
         <v>14</v>
       </c>
       <c r="B14" s="11">
-        <v>1</v>
-      </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
+        <v>0.92</v>
+      </c>
+      <c r="C14" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="D14" s="11">
+        <v>1.25</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">

</xml_diff>

<commit_message>
Actually revise short-course outcome values again
Only implementing this intervention in Bulgaria, so remove from Bulgaria spreadsheet and move to default.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="95">
   <si>
     <t>parameter</t>
   </si>
@@ -61,12 +61,6 @@
   </si>
   <si>
     <t>int_timeperiod_shortcourse_mdr</t>
-  </si>
-  <si>
-    <t>program_prop_treatment_success_shortcoursemdr</t>
-  </si>
-  <si>
-    <t>Treatment success under shortcourse MDR-TB regimens</t>
   </si>
   <si>
     <t>mdr_introduce_time</t>
@@ -2168,10 +2162,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2338,123 +2332,118 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="11">
-        <v>0.89</v>
-      </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
+      <c r="B15" s="19">
+        <v>1964</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
       <c r="E15" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="19">
-        <v>1964</v>
-      </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="12" t="s">
-        <v>18</v>
+      <c r="B16" s="14">
+        <v>2015</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="14">
-        <v>2015</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="14">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="14">
-        <v>13</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="14">
-        <v>0.6</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="14">
         <v>0.03</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="14">
-        <v>0.03</v>
-      </c>
+      <c r="A22" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="C22" s="25">
+        <v>0.15</v>
+      </c>
+      <c r="D22" s="25">
+        <v>0.35</v>
+      </c>
+      <c r="E22" s="25"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="25">
+        <v>0.08</v>
+      </c>
+      <c r="C23" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="D23" s="25">
+        <v>0.12</v>
+      </c>
+      <c r="E23" s="25"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="C23" s="25">
-        <v>0.15</v>
-      </c>
-      <c r="D23" s="25">
-        <v>0.35</v>
-      </c>
-      <c r="E23" s="25"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
+      <c r="B24" s="14">
+        <v>92</v>
+      </c>
+      <c r="E24" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="25">
-        <v>0.08</v>
-      </c>
-      <c r="C24" s="25">
-        <v>0.05</v>
-      </c>
-      <c r="D24" s="25">
-        <v>0.12</v>
-      </c>
-      <c r="E24" s="25"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="14">
-        <v>92</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" s="14">
         <v>0</v>
@@ -2462,7 +2451,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27" s="14">
         <v>0</v>
@@ -2470,34 +2459,34 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" s="14">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" s="14">
-        <v>1.1000000000000001</v>
+        <v>857</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" s="14">
-        <v>857</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" s="14">
         <v>0</v>
@@ -2505,7 +2494,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32" s="14">
         <v>0</v>
@@ -2513,18 +2502,22 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" s="14">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="12">
+        <f>1.02+67.12</f>
+        <v>68.14</v>
+      </c>
+      <c r="E34" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="B34" s="14">
-        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2532,19 +2525,18 @@
         <v>38</v>
       </c>
       <c r="B35" s="12">
-        <f>1.02+67.12</f>
-        <v>68.14</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="12">
+        <v>8028</v>
+      </c>
+      <c r="E36" s="12" t="s">
         <v>40</v>
-      </c>
-      <c r="B36" s="12">
-        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2552,15 +2544,12 @@
         <v>41</v>
       </c>
       <c r="B37" s="12">
-        <v>8028</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" s="12">
         <v>1</v>
@@ -2568,43 +2557,46 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" s="12">
-        <v>1</v>
+        <v>43</v>
+      </c>
+      <c r="B39" s="21">
+        <f>6094-7861</f>
+        <v>-1767</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40" s="21">
-        <f>6094-7861</f>
-        <v>-1767</v>
+        <v>44</v>
+      </c>
+      <c r="B40" s="20">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41" s="20">
+        <v>45</v>
+      </c>
+      <c r="B41" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B42" s="12">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" s="12">
+        <v>751</v>
+      </c>
+      <c r="E43" s="12" t="s">
         <v>48</v>
-      </c>
-      <c r="B43" s="12">
-        <v>0.9</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2612,15 +2604,12 @@
         <v>49</v>
       </c>
       <c r="B44" s="12">
-        <v>751</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B45" s="12">
         <v>0</v>
@@ -2628,7 +2617,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B46" s="12">
         <v>0</v>
@@ -2636,84 +2625,76 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B47" s="12">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" s="12">
+        <v>862</v>
+      </c>
+      <c r="E48" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="12">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B49" s="12">
-        <v>862</v>
-      </c>
-      <c r="E49" s="12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="12" t="s">
-        <v>57</v>
       </c>
       <c r="B50" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B51" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52" s="12">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>59</v>
       </c>
-      <c r="B52" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="12" t="s">
+      <c r="B53">
+        <v>0.57773922585488524</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>60</v>
       </c>
-      <c r="B53" s="12">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="B54">
+        <v>0.72388695785815904</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>61</v>
       </c>
-      <c r="B54">
-        <v>0.57773922585488524</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>62</v>
-      </c>
       <c r="B55">
-        <v>0.72388695785815904</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>63</v>
-      </c>
-      <c r="B56">
         <v>2.7632552333346339</v>
       </c>
     </row>
@@ -2732,7 +2713,7 @@
       <formula2>1</formula2>
     </dataValidation>
     <dataValidation showInputMessage="1" showErrorMessage="1" promptTitle="Age unstratified" prompt="Some values you can replace the ones to the left with if you want a manual calibration for the model without age stratification." sqref="H1"/>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B4:B16 C16 D16">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="C15:D15 B4:B15">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
@@ -2781,13 +2762,13 @@
   <sheetData>
     <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>66</v>
       </c>
       <c r="D1" s="1">
         <v>1920</v>
@@ -2829,36 +2810,36 @@
         <v>2015</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P2" s="23">
         <v>0</v>
@@ -2871,10 +2852,10 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G3" s="23">
         <v>0</v>
@@ -2890,10 +2871,10 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G4" s="23">
         <v>0</v>
@@ -2910,10 +2891,10 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G5" s="23">
         <v>0</v>
@@ -2929,10 +2910,10 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G6" s="23">
         <v>0</v>
@@ -2946,10 +2927,10 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D7" s="17"/>
       <c r="I7" s="23">
@@ -2989,10 +2970,10 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P8" s="23">
         <v>100</v>
@@ -3008,10 +2989,10 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P9" s="23">
         <v>100</v>
@@ -3030,10 +3011,10 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P10" s="23">
         <v>0</v>
@@ -3046,10 +3027,10 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P11" s="23">
         <v>0</v>
@@ -3062,10 +3043,10 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D12" s="5">
         <v>1</v>
@@ -3094,10 +3075,10 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H13" s="23">
         <v>5.4</v>
@@ -3117,10 +3098,10 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G14" s="23">
         <v>1</v>
@@ -3131,10 +3112,10 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G15" s="23">
         <v>8</v>
@@ -3148,10 +3129,10 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5">
@@ -3278,35 +3259,35 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Simplify short-course entry again - only put in defaults
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="94">
   <si>
     <t>parameter</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>tb_timeperiod_ontreatment_mdr</t>
-  </si>
-  <si>
-    <t>int_timeperiod_shortcourse_mdr</t>
   </si>
   <si>
     <t>mdr_introduce_time</t>
@@ -2162,10 +2159,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2315,33 +2312,24 @@
       <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="11">
-        <f>11/12</f>
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="C14" s="11">
-        <f>9/12</f>
-        <v>0.75</v>
-      </c>
-      <c r="D14" s="11">
-        <f>15/12</f>
-        <v>1.25</v>
+      <c r="B14" s="19">
+        <v>1964</v>
+      </c>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="12" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="19">
-        <v>1964</v>
-      </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="12" t="s">
+      <c r="A15" s="12" t="s">
         <v>16</v>
+      </c>
+      <c r="B15" s="14">
+        <v>2015</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2349,7 +2337,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="14">
-        <v>2015</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2357,7 +2345,7 @@
         <v>18</v>
       </c>
       <c r="B17" s="14">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2365,7 +2353,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="14">
-        <v>13</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2373,7 +2361,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="14">
-        <v>0.6</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2385,52 +2373,52 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="14">
-        <v>0.03</v>
-      </c>
+      <c r="B21" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="C21" s="25">
+        <v>0.15</v>
+      </c>
+      <c r="D21" s="25">
+        <v>0.35</v>
+      </c>
+      <c r="E21" s="25"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="25">
-        <v>0.25</v>
+        <v>0.08</v>
       </c>
       <c r="C22" s="25">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="D22" s="25">
-        <v>0.35</v>
+        <v>0.12</v>
       </c>
       <c r="E22" s="25"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="25">
-        <v>0.08</v>
-      </c>
-      <c r="C23" s="25">
-        <v>0.05</v>
-      </c>
-      <c r="D23" s="25">
-        <v>0.12</v>
-      </c>
-      <c r="E23" s="25"/>
+      <c r="B23" s="14">
+        <v>92</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B24" s="14">
-        <v>92</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2454,7 +2442,7 @@
         <v>29</v>
       </c>
       <c r="B27" s="14">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2462,7 +2450,10 @@
         <v>30</v>
       </c>
       <c r="B28" s="14">
-        <v>1.1000000000000001</v>
+        <v>857</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2470,10 +2461,7 @@
         <v>31</v>
       </c>
       <c r="B29" s="14">
-        <v>857</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2497,27 +2485,27 @@
         <v>34</v>
       </c>
       <c r="B32" s="14">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="14">
-        <v>1.1000000000000001</v>
+      <c r="B33" s="12">
+        <f>1.02+67.12</f>
+        <v>68.14</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B34" s="12">
-        <f>1.02+67.12</f>
-        <v>68.14</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2525,18 +2513,18 @@
         <v>38</v>
       </c>
       <c r="B35" s="12">
-        <v>0</v>
+        <v>8028</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B36" s="12">
-        <v>8028</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2551,24 +2539,24 @@
       <c r="A38" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="12">
-        <v>1</v>
+      <c r="B38" s="21">
+        <f>6094-7861</f>
+        <v>-1767</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="21">
-        <f>6094-7861</f>
-        <v>-1767</v>
+      <c r="B39" s="20">
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="20">
+      <c r="B40" s="12">
         <v>0</v>
       </c>
     </row>
@@ -2577,7 +2565,7 @@
         <v>45</v>
       </c>
       <c r="B41" s="12">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2585,18 +2573,18 @@
         <v>46</v>
       </c>
       <c r="B42" s="12">
-        <v>0.9</v>
+        <v>751</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B43" s="12">
-        <v>751</v>
-      </c>
-      <c r="E43" s="12" t="s">
-        <v>48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2620,7 +2608,7 @@
         <v>51</v>
       </c>
       <c r="B46" s="12">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2628,18 +2616,18 @@
         <v>52</v>
       </c>
       <c r="B47" s="12">
-        <v>1.1000000000000001</v>
+        <v>862</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B48" s="12">
-        <v>862</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2663,15 +2651,15 @@
         <v>57</v>
       </c>
       <c r="B51" s="12">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="12" t="s">
+      <c r="A52" t="s">
         <v>58</v>
       </c>
-      <c r="B52" s="12">
-        <v>1.1000000000000001</v>
+      <c r="B52">
+        <v>0.57773922585488524</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2679,7 +2667,7 @@
         <v>59</v>
       </c>
       <c r="B53">
-        <v>0.57773922585488524</v>
+        <v>0.72388695785815904</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2687,14 +2675,6 @@
         <v>60</v>
       </c>
       <c r="B54">
-        <v>0.72388695785815904</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>61</v>
-      </c>
-      <c r="B55">
         <v>2.7632552333346339</v>
       </c>
     </row>
@@ -2713,7 +2693,7 @@
       <formula2>1</formula2>
     </dataValidation>
     <dataValidation showInputMessage="1" showErrorMessage="1" promptTitle="Age unstratified" prompt="Some values you can replace the ones to the left with if you want a manual calibration for the model without age stratification." sqref="H1"/>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="C15:D15 B4:B15">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="C14:D14 B4:B14">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
@@ -2762,13 +2742,13 @@
   <sheetData>
     <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>64</v>
       </c>
       <c r="D1" s="1">
         <v>1920</v>
@@ -2810,36 +2790,36 @@
         <v>2015</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="P2" s="23">
         <v>0</v>
@@ -2852,10 +2832,10 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G3" s="23">
         <v>0</v>
@@ -2871,10 +2851,10 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G4" s="23">
         <v>0</v>
@@ -2891,10 +2871,10 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G5" s="23">
         <v>0</v>
@@ -2910,10 +2890,10 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G6" s="23">
         <v>0</v>
@@ -2927,10 +2907,10 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" s="17"/>
       <c r="I7" s="23">
@@ -2970,10 +2950,10 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P8" s="23">
         <v>100</v>
@@ -2989,10 +2969,10 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P9" s="23">
         <v>100</v>
@@ -3011,10 +2991,10 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P10" s="23">
         <v>0</v>
@@ -3027,10 +3007,10 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P11" s="23">
         <v>0</v>
@@ -3043,10 +3023,10 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D12" s="5">
         <v>1</v>
@@ -3075,10 +3055,10 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H13" s="23">
         <v>5.4</v>
@@ -3098,10 +3078,10 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G14" s="23">
         <v>1</v>
@@ -3112,10 +3092,10 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G15" s="23">
         <v>8</v>
@@ -3129,10 +3109,10 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5">
@@ -3259,35 +3239,35 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" t="s">
         <v>90</v>
-      </c>
-      <c r="D2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" t="s">
         <v>93</v>
-      </c>
-      <c r="C4" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make the assignment a var rather than a local variable for outputting during debugging
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10350"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="23040" windowHeight="10290"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -2161,8 +2161,8 @@
   </sheetPr>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2573,7 +2573,8 @@
         <v>46</v>
       </c>
       <c r="B42" s="12">
-        <v>751</v>
+        <f>751-1643</f>
+        <v>-892</v>
       </c>
       <c r="E42" s="12" t="s">
         <v>47</v>
@@ -2616,7 +2617,8 @@
         <v>52</v>
       </c>
       <c r="B47" s="12">
-        <v>862</v>
+        <f>862-1746</f>
+        <v>-884</v>
       </c>
       <c r="E47" s="12" t="s">
         <v>53</v>
@@ -2717,7 +2719,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2983,9 +2985,6 @@
         <v>0</v>
       </c>
       <c r="V9" s="24">
-        <v>0</v>
-      </c>
-      <c r="X9" s="23">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Include intervention uncertainty parameters for DST
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="23040" windowHeight="10290"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="20730" windowHeight="10290" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -2161,7 +2161,7 @@
   </sheetPr>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -2715,11 +2715,11 @@
   </sheetPr>
   <dimension ref="A1:X34"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2949,6 +2949,9 @@
       <c r="R7" s="23">
         <v>95</v>
       </c>
+      <c r="X7" s="23">
+        <v>95</v>
+      </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
@@ -2963,9 +2966,6 @@
       <c r="S8" s="24"/>
       <c r="T8" s="24"/>
       <c r="V8" s="24">
-        <v>0</v>
-      </c>
-      <c r="X8" s="23">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update intervention uncertainty values for DST
Otherwise we get a negative average impact of the intervention.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtrauer\Desktop\AuTuMN\autumn\xls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="20730" windowHeight="10290" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="20730" windowHeight="10230" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
     <sheet name="time_variants" sheetId="2" r:id="rId2"/>
     <sheet name="dropdown_lists" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -308,7 +303,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -1917,7 +1912,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1952,7 +1947,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2718,10 +2713,10 @@
   <dimension ref="A1:X34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
+      <selection pane="bottomRight" activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2949,9 +2944,6 @@
         <v>86.189258312020456</v>
       </c>
       <c r="R7" s="23">
-        <v>95</v>
-      </c>
-      <c r="X7" s="23">
         <v>95</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MDR TB Non success death rate
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="94">
   <si>
     <t>parameter</t>
   </si>
@@ -2164,10 +2164,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A55" sqref="A55:XFD56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2321,7 +2321,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="19">
-        <v>1962</v>
+        <v>1964</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
@@ -2683,22 +2683,6 @@
       </c>
       <c r="B54">
         <v>2.794363613083874</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>2</v>
-      </c>
-      <c r="B55">
-        <v>2.3129967495631889</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>2</v>
-      </c>
-      <c r="B56">
-        <v>2.3129967495631889</v>
       </c>
     </row>
   </sheetData>
@@ -2734,10 +2718,10 @@
   <dimension ref="A1:X34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O6" sqref="O6"/>
+      <selection pane="bottomRight" activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2920,9 +2904,6 @@
       </c>
       <c r="K6" s="23">
         <v>99.99</v>
-      </c>
-      <c r="O6" s="23">
-        <v>78.150000000000006</v>
       </c>
       <c r="S6" s="24"/>
       <c r="T6" s="24"/>

</xml_diff>

<commit_message>
Romain: Provisional fix for ageing rates proportional to riskgroup prevalence. Further fix to follow by Sachin
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="20730" windowHeight="10230"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="15360" windowHeight="7635"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
     <sheet name="time_variants" sheetId="2" r:id="rId2"/>
     <sheet name="dropdown_lists" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -308,7 +308,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -400,7 +400,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -411,6 +411,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB9DAED"/>
         <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1156,7 +1162,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="662" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="3" xfId="662" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1196,6 +1202,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="241"/>
     <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="662" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="9" fillId="3" borderId="0" xfId="662" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="663">
     <cellStyle name="Comma 2" xfId="614"/>
@@ -2168,12 +2175,12 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.28515625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="54.5703125" style="12" customWidth="1"/>
     <col min="2" max="2" width="18" style="14" customWidth="1"/>
     <col min="3" max="5" width="9.140625" style="12" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" style="12" bestFit="1" customWidth="1"/>
@@ -2196,13 +2203,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="9">
-        <v>2.93</v>
+        <v>4.2</v>
       </c>
       <c r="C2" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -2335,7 +2342,7 @@
         <v>16</v>
       </c>
       <c r="B15" s="14">
-        <v>2015</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2350,7 +2357,7 @@
       <c r="A17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="27">
         <v>13</v>
       </c>
     </row>
@@ -2719,10 +2726,10 @@
   <dimension ref="A1:X34"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P15" sqref="P15"/>
+      <selection pane="bottomRight" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3059,20 +3066,11 @@
       <c r="B13" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="H13" s="23">
-        <v>5.4</v>
-      </c>
-      <c r="I13" s="23">
-        <v>5.6</v>
-      </c>
-      <c r="M13" s="23">
-        <v>6</v>
-      </c>
-      <c r="N13" s="23">
-        <v>7.63</v>
-      </c>
-      <c r="P13" s="23">
-        <v>8.4</v>
+      <c r="H13" s="26">
+        <v>4</v>
+      </c>
+      <c r="P13" s="26">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
@@ -3083,10 +3081,10 @@
         <v>73</v>
       </c>
       <c r="G14" s="26">
-        <v>1.3</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="P14" s="26">
-        <v>1.3</v>
+        <v>1.0000000000000001E-9</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
@@ -3097,10 +3095,10 @@
         <v>73</v>
       </c>
       <c r="G15" s="23">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="P15" s="23">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="W15" s="23">
         <v>5.0999999999999996</v>
@@ -3209,7 +3207,7 @@
   </sheetData>
   <dataValidations count="3">
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C1"/>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="D7 E23:E25 F23:F25 G23:G25 H23:H25 I23:I25 J23:J25 K23:K25 L23:L25 M23:M25 N23:N25 O23:O25 P23:P25">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="D7 E23:P25">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Romain: additional fix for set ageing flow
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -2174,8 +2174,8 @@
   </sheetPr>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2203,13 +2203,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="9">
-        <v>4.2</v>
+        <v>2.8</v>
       </c>
       <c r="C2" s="12">
         <v>2</v>
       </c>
       <c r="D2" s="12">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -2219,7 +2219,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="13">
-        <v>1.7265492869089989</v>
+        <v>2</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
@@ -2358,7 +2358,7 @@
         <v>18</v>
       </c>
       <c r="B17" s="27">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2726,10 +2726,10 @@
   <dimension ref="A1:X34"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2741,7 +2741,8 @@
     <col min="5" max="5" width="7.140625" style="23" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" style="23" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" style="23" customWidth="1"/>
-    <col min="8" max="12" width="7" style="23" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" style="23" customWidth="1"/>
+    <col min="9" max="12" width="7" style="23" customWidth="1"/>
     <col min="13" max="14" width="7.42578125" style="23" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7.42578125" style="23" customWidth="1"/>
     <col min="16" max="16" width="16.140625" style="23" customWidth="1"/>
@@ -3067,10 +3068,10 @@
         <v>73</v>
       </c>
       <c r="H13" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P13" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
@@ -3081,10 +3082,10 @@
         <v>73</v>
       </c>
       <c r="G14" s="26">
-        <v>1.0000000000000001E-9</v>
+        <v>0.1</v>
       </c>
       <c r="P14" s="26">
-        <v>1.0000000000000001E-9</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Romain: pushing calibrated parameters for Bulgaria after model revision for age-specific risk-groups
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -2174,8 +2174,8 @@
   </sheetPr>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2186,8 +2186,8 @@
     <col min="6" max="6" width="13.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="15" width="9.140625" style="12" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="12"/>
+    <col min="9" max="16" width="9.140625" style="12" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2203,7 +2203,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="9">
-        <v>2.8</v>
+        <v>2.6438731853772901</v>
       </c>
       <c r="C2" s="12">
         <v>2</v>
@@ -2229,7 +2229,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="13">
-        <v>1901.7272282274721</v>
+        <v>1898.79316844513</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -2329,7 +2329,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="19">
-        <v>1964</v>
+        <v>1965</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
@@ -2342,7 +2342,7 @@
         <v>16</v>
       </c>
       <c r="B15" s="14">
-        <v>1902</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2674,7 +2674,7 @@
         <v>58</v>
       </c>
       <c r="B52">
-        <v>0.58395303893975359</v>
+        <v>0.57503904271460604</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2682,7 +2682,7 @@
         <v>59</v>
       </c>
       <c r="B53">
-        <v>0.73514401257925854</v>
+        <v>0.71786452587670602</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2690,7 +2690,7 @@
         <v>60</v>
       </c>
       <c r="B54">
-        <v>2.794363613083874</v>
+        <v>2.93482296191877</v>
       </c>
     </row>
   </sheetData>
@@ -2749,8 +2749,8 @@
     <col min="17" max="18" width="14" style="23" customWidth="1"/>
     <col min="19" max="19" width="14.42578125" style="23" bestFit="1" customWidth="1"/>
     <col min="20" max="23" width="14.42578125" style="23" customWidth="1"/>
-    <col min="24" max="29" width="9.140625" style="23" customWidth="1"/>
-    <col min="30" max="16384" width="9.140625" style="23"/>
+    <col min="24" max="30" width="9.140625" style="23" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Romain: prison multiplier back to baseline value of 13.0
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -2174,8 +2174,8 @@
   </sheetPr>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2203,7 +2203,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="9">
-        <v>2.6438731853772901</v>
+        <v>3.3</v>
       </c>
       <c r="C2" s="12">
         <v>2</v>
@@ -2358,7 +2358,7 @@
         <v>18</v>
       </c>
       <c r="B17" s="27">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2726,10 +2726,10 @@
   <dimension ref="A1:X34"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomRight" activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Romain: new calibration Bulgaria
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -2175,7 +2175,7 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2203,13 +2203,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="9">
-        <v>3.3</v>
+        <v>2.90884124107445</v>
       </c>
       <c r="C2" s="12">
-        <v>2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D2" s="12">
-        <v>4</v>
+        <v>4.3</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -2229,7 +2229,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="13">
-        <v>1898.79316844513</v>
+        <v>1878.3129881772099</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -2259,7 +2259,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="11">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
@@ -2674,7 +2674,7 @@
         <v>58</v>
       </c>
       <c r="B52">
-        <v>0.57503904271460604</v>
+        <v>0.59435254157623596</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2682,7 +2682,7 @@
         <v>59</v>
       </c>
       <c r="B53">
-        <v>0.71786452587670602</v>
+        <v>0.74733094259578403</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2690,12 +2690,12 @@
         <v>60</v>
       </c>
       <c r="B54">
-        <v>2.93482296191877</v>
+        <v>2.90267793145552</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="5">
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="B3:B10 F9:F10 G9:G10">
+  <dataValidations count="6">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="G9:G10 F9:F10 B3:B6 B8:B10">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
@@ -2712,6 +2712,7 @@
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B7"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2729,7 +2730,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X8" sqref="X8"/>
+      <selection pane="bottomRight" activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2900,6 +2901,9 @@
       </c>
       <c r="T5" s="24"/>
       <c r="U5" s="24"/>
+      <c r="X5" s="23">
+        <v>100</v>
+      </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">

</xml_diff>

<commit_message>
Add combined scenario + related intervention uncertainty (Bulgaria)
</commit_message>
<xml_diff>
--- a/autumn/xls/data_bulgaria.xlsx
+++ b/autumn/xls/data_bulgaria.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20339"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swas0001\swas_AuTuMN\autumn\xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\swasnik_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD17288-4A0F-43FF-8711-57A76703FABA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="15360" windowHeight="7635"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="15360" windowHeight="7640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
     <sheet name="time_variants" sheetId="2" r:id="rId2"/>
     <sheet name="dropdown_lists" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -308,7 +309,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -1205,669 +1206,669 @@
     <xf numFmtId="2" fontId="9" fillId="3" borderId="0" xfId="662" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="663">
-    <cellStyle name="Comma 2" xfId="614"/>
-    <cellStyle name="Comma 2 2" xfId="626"/>
-    <cellStyle name="Input 2" xfId="378"/>
+    <cellStyle name="Comma 2" xfId="614" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Comma 2 2" xfId="626" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Input 2" xfId="378" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="545"/>
-    <cellStyle name="Normal 2" xfId="449"/>
-    <cellStyle name="Normal 2 2" xfId="439"/>
-    <cellStyle name="Normal 3" xfId="448"/>
-    <cellStyle name="Normal 3 2" xfId="500"/>
-    <cellStyle name="Normal 4" xfId="451"/>
-    <cellStyle name="Normal 4 2" xfId="81"/>
-    <cellStyle name="Normal 5" xfId="450"/>
-    <cellStyle name="Normal 5 2" xfId="242"/>
-    <cellStyle name="Normal 6" xfId="453"/>
-    <cellStyle name="Normal 6 10" xfId="41"/>
-    <cellStyle name="Normal 6 10 2" xfId="121"/>
-    <cellStyle name="Normal 6 10 2 2" xfId="168"/>
-    <cellStyle name="Normal 6 10 2 3" xfId="167"/>
-    <cellStyle name="Normal 6 10 3" xfId="118"/>
-    <cellStyle name="Normal 6 10 4" xfId="117"/>
-    <cellStyle name="Normal 6 11" xfId="40"/>
-    <cellStyle name="Normal 6 11 2" xfId="251"/>
-    <cellStyle name="Normal 6 11 2 2" xfId="421"/>
-    <cellStyle name="Normal 6 11 2 3" xfId="422"/>
-    <cellStyle name="Normal 6 11 3" xfId="252"/>
-    <cellStyle name="Normal 6 11 4" xfId="250"/>
-    <cellStyle name="Normal 6 12" xfId="43"/>
-    <cellStyle name="Normal 6 12 2" xfId="227"/>
-    <cellStyle name="Normal 6 12 2 2" xfId="181"/>
-    <cellStyle name="Normal 6 12 2 3" xfId="180"/>
-    <cellStyle name="Normal 6 12 3" xfId="226"/>
-    <cellStyle name="Normal 6 12 4" xfId="225"/>
-    <cellStyle name="Normal 6 13" xfId="42"/>
-    <cellStyle name="Normal 6 13 2" xfId="16"/>
-    <cellStyle name="Normal 6 13 2 2" xfId="503"/>
-    <cellStyle name="Normal 6 13 2 3" xfId="504"/>
-    <cellStyle name="Normal 6 13 3" xfId="17"/>
-    <cellStyle name="Normal 6 13 4" xfId="11"/>
-    <cellStyle name="Normal 6 14" xfId="45"/>
-    <cellStyle name="Normal 6 14 2" xfId="337"/>
-    <cellStyle name="Normal 6 14 2 2" xfId="76"/>
-    <cellStyle name="Normal 6 14 2 3" xfId="75"/>
-    <cellStyle name="Normal 6 14 3" xfId="336"/>
-    <cellStyle name="Normal 6 14 4" xfId="338"/>
-    <cellStyle name="Normal 6 15" xfId="44"/>
-    <cellStyle name="Normal 6 15 2" xfId="130"/>
-    <cellStyle name="Normal 6 15 3" xfId="131"/>
-    <cellStyle name="Normal 6 16" xfId="47"/>
-    <cellStyle name="Normal 6 17" xfId="46"/>
-    <cellStyle name="Normal 6 2" xfId="315"/>
-    <cellStyle name="Normal 6 2 10" xfId="233"/>
-    <cellStyle name="Normal 6 2 11" xfId="232"/>
-    <cellStyle name="Normal 6 2 2" xfId="578"/>
-    <cellStyle name="Normal 6 2 2 10" xfId="528"/>
-    <cellStyle name="Normal 6 2 2 2" xfId="465"/>
-    <cellStyle name="Normal 6 2 2 2 2" xfId="485"/>
-    <cellStyle name="Normal 6 2 2 2 2 2" xfId="512"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 2" xfId="7"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 2 2" xfId="329"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 2 3" xfId="328"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 3" xfId="6"/>
-    <cellStyle name="Normal 6 2 2 2 2 2 4" xfId="8"/>
-    <cellStyle name="Normal 6 2 2 2 2 3" xfId="511"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 2" xfId="218"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 2 2" xfId="67"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 2 3" xfId="68"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 3" xfId="219"/>
-    <cellStyle name="Normal 6 2 2 2 2 3 4" xfId="220"/>
-    <cellStyle name="Normal 6 2 2 2 2 4" xfId="309"/>
-    <cellStyle name="Normal 6 2 2 2 2 4 2" xfId="437"/>
-    <cellStyle name="Normal 6 2 2 2 2 4 3" xfId="436"/>
-    <cellStyle name="Normal 6 2 2 2 2 5" xfId="260"/>
-    <cellStyle name="Normal 6 2 2 2 2 6" xfId="508"/>
-    <cellStyle name="Normal 6 2 2 2 3" xfId="191"/>
-    <cellStyle name="Normal 6 2 2 2 3 2" xfId="56"/>
-    <cellStyle name="Normal 6 2 2 2 3 2 2" xfId="496"/>
-    <cellStyle name="Normal 6 2 2 2 3 2 3" xfId="497"/>
-    <cellStyle name="Normal 6 2 2 2 3 3" xfId="57"/>
-    <cellStyle name="Normal 6 2 2 2 3 4" xfId="54"/>
-    <cellStyle name="Normal 6 2 2 2 4" xfId="178"/>
-    <cellStyle name="Normal 6 2 2 2 4 2" xfId="385"/>
-    <cellStyle name="Normal 6 2 2 2 4 2 2" xfId="73"/>
-    <cellStyle name="Normal 6 2 2 2 4 2 3" xfId="71"/>
-    <cellStyle name="Normal 6 2 2 2 4 3" xfId="384"/>
-    <cellStyle name="Normal 6 2 2 2 4 4" xfId="389"/>
-    <cellStyle name="Normal 6 2 2 2 5" xfId="177"/>
-    <cellStyle name="Normal 6 2 2 2 5 2" xfId="592"/>
-    <cellStyle name="Normal 6 2 2 2 5 3" xfId="593"/>
-    <cellStyle name="Normal 6 2 2 2 6" xfId="483"/>
-    <cellStyle name="Normal 6 2 2 2 7" xfId="482"/>
-    <cellStyle name="Normal 6 2 2 3" xfId="464"/>
-    <cellStyle name="Normal 6 2 2 3 2" xfId="24"/>
-    <cellStyle name="Normal 6 2 2 3 2 2" xfId="230"/>
-    <cellStyle name="Normal 6 2 2 3 2 2 2" xfId="560"/>
-    <cellStyle name="Normal 6 2 2 3 2 2 3" xfId="561"/>
-    <cellStyle name="Normal 6 2 2 3 2 3" xfId="231"/>
-    <cellStyle name="Normal 6 2 2 3 2 4" xfId="228"/>
-    <cellStyle name="Normal 6 2 2 3 3" xfId="25"/>
-    <cellStyle name="Normal 6 2 2 3 3 2" xfId="31"/>
-    <cellStyle name="Normal 6 2 2 3 3 2 2" xfId="133"/>
-    <cellStyle name="Normal 6 2 2 3 3 2 3" xfId="132"/>
-    <cellStyle name="Normal 6 2 2 3 3 3" xfId="30"/>
-    <cellStyle name="Normal 6 2 2 3 3 4" xfId="27"/>
-    <cellStyle name="Normal 6 2 2 3 4" xfId="20"/>
-    <cellStyle name="Normal 6 2 2 3 4 2" xfId="193"/>
-    <cellStyle name="Normal 6 2 2 3 4 3" xfId="194"/>
-    <cellStyle name="Normal 6 2 2 3 5" xfId="21"/>
-    <cellStyle name="Normal 6 2 2 3 6" xfId="22"/>
-    <cellStyle name="Normal 6 2 2 4" xfId="467"/>
-    <cellStyle name="Normal 6 2 2 4 2" xfId="206"/>
-    <cellStyle name="Normal 6 2 2 4 2 2" xfId="143"/>
-    <cellStyle name="Normal 6 2 2 4 2 3" xfId="544"/>
-    <cellStyle name="Normal 6 2 2 4 3" xfId="205"/>
-    <cellStyle name="Normal 6 2 2 4 4" xfId="533"/>
-    <cellStyle name="Normal 6 2 2 5" xfId="466"/>
-    <cellStyle name="Normal 6 2 2 5 2" xfId="405"/>
-    <cellStyle name="Normal 6 2 2 5 2 2" xfId="248"/>
-    <cellStyle name="Normal 6 2 2 5 2 3" xfId="249"/>
-    <cellStyle name="Normal 6 2 2 5 3" xfId="406"/>
-    <cellStyle name="Normal 6 2 2 5 4" xfId="408"/>
-    <cellStyle name="Normal 6 2 2 6" xfId="469"/>
-    <cellStyle name="Normal 6 2 2 6 2" xfId="602"/>
-    <cellStyle name="Normal 6 2 2 6 2 2" xfId="590"/>
-    <cellStyle name="Normal 6 2 2 6 2 3" xfId="589"/>
-    <cellStyle name="Normal 6 2 2 6 3" xfId="601"/>
-    <cellStyle name="Normal 6 2 2 6 4" xfId="603"/>
-    <cellStyle name="Normal 6 2 2 7" xfId="468"/>
-    <cellStyle name="Normal 6 2 2 7 2" xfId="156"/>
-    <cellStyle name="Normal 6 2 2 7 2 2" xfId="262"/>
-    <cellStyle name="Normal 6 2 2 7 2 3" xfId="263"/>
-    <cellStyle name="Normal 6 2 2 7 3" xfId="157"/>
-    <cellStyle name="Normal 6 2 2 7 4" xfId="158"/>
-    <cellStyle name="Normal 6 2 2 8" xfId="101"/>
-    <cellStyle name="Normal 6 2 2 8 2" xfId="349"/>
-    <cellStyle name="Normal 6 2 2 8 3" xfId="348"/>
-    <cellStyle name="Normal 6 2 2 9" xfId="99"/>
-    <cellStyle name="Normal 6 2 3" xfId="577"/>
-    <cellStyle name="Normal 6 2 3 2" xfId="12"/>
-    <cellStyle name="Normal 6 2 3 2 2" xfId="294"/>
-    <cellStyle name="Normal 6 2 3 2 2 2" xfId="360"/>
-    <cellStyle name="Normal 6 2 3 2 2 2 2" xfId="526"/>
-    <cellStyle name="Normal 6 2 3 2 2 2 3" xfId="527"/>
-    <cellStyle name="Normal 6 2 3 2 2 3" xfId="361"/>
-    <cellStyle name="Normal 6 2 3 2 2 4" xfId="355"/>
-    <cellStyle name="Normal 6 2 3 2 3" xfId="295"/>
-    <cellStyle name="Normal 6 2 3 2 3 2" xfId="173"/>
-    <cellStyle name="Normal 6 2 3 2 3 2 2" xfId="443"/>
-    <cellStyle name="Normal 6 2 3 2 3 2 3" xfId="442"/>
-    <cellStyle name="Normal 6 2 3 2 3 3" xfId="172"/>
-    <cellStyle name="Normal 6 2 3 2 3 4" xfId="169"/>
-    <cellStyle name="Normal 6 2 3 2 4" xfId="289"/>
-    <cellStyle name="Normal 6 2 3 2 4 2" xfId="213"/>
-    <cellStyle name="Normal 6 2 3 2 4 3" xfId="214"/>
-    <cellStyle name="Normal 6 2 3 2 5" xfId="290"/>
-    <cellStyle name="Normal 6 2 3 2 6" xfId="291"/>
-    <cellStyle name="Normal 6 2 3 3" xfId="13"/>
-    <cellStyle name="Normal 6 2 3 3 2" xfId="84"/>
-    <cellStyle name="Normal 6 2 3 3 2 2" xfId="543"/>
-    <cellStyle name="Normal 6 2 3 3 2 3" xfId="542"/>
-    <cellStyle name="Normal 6 2 3 3 3" xfId="83"/>
-    <cellStyle name="Normal 6 2 3 3 4" xfId="82"/>
-    <cellStyle name="Normal 6 2 3 4" xfId="14"/>
-    <cellStyle name="Normal 6 2 3 4 2" xfId="216"/>
-    <cellStyle name="Normal 6 2 3 4 2 2" xfId="660"/>
-    <cellStyle name="Normal 6 2 3 4 2 3" xfId="661"/>
-    <cellStyle name="Normal 6 2 3 4 3" xfId="55"/>
-    <cellStyle name="Normal 6 2 3 4 4" xfId="223"/>
-    <cellStyle name="Normal 6 2 3 5" xfId="15"/>
-    <cellStyle name="Normal 6 2 3 5 2" xfId="506"/>
-    <cellStyle name="Normal 6 2 3 5 3" xfId="505"/>
-    <cellStyle name="Normal 6 2 3 6" xfId="69"/>
-    <cellStyle name="Normal 6 2 3 7" xfId="72"/>
-    <cellStyle name="Normal 6 2 4" xfId="331"/>
-    <cellStyle name="Normal 6 2 4 2" xfId="400"/>
-    <cellStyle name="Normal 6 2 4 2 2" xfId="256"/>
-    <cellStyle name="Normal 6 2 4 2 2 2" xfId="274"/>
-    <cellStyle name="Normal 6 2 4 2 2 3" xfId="270"/>
-    <cellStyle name="Normal 6 2 4 2 3" xfId="255"/>
-    <cellStyle name="Normal 6 2 4 2 4" xfId="257"/>
-    <cellStyle name="Normal 6 2 4 3" xfId="399"/>
-    <cellStyle name="Normal 6 2 4 3 2" xfId="458"/>
-    <cellStyle name="Normal 6 2 4 3 2 2" xfId="150"/>
-    <cellStyle name="Normal 6 2 4 3 2 3" xfId="151"/>
-    <cellStyle name="Normal 6 2 4 3 3" xfId="459"/>
-    <cellStyle name="Normal 6 2 4 3 4" xfId="463"/>
-    <cellStyle name="Normal 6 2 4 4" xfId="398"/>
-    <cellStyle name="Normal 6 2 4 4 2" xfId="522"/>
-    <cellStyle name="Normal 6 2 4 4 3" xfId="521"/>
-    <cellStyle name="Normal 6 2 4 5" xfId="397"/>
-    <cellStyle name="Normal 6 2 4 6" xfId="396"/>
-    <cellStyle name="Normal 6 2 5" xfId="330"/>
-    <cellStyle name="Normal 6 2 5 2" xfId="569"/>
-    <cellStyle name="Normal 6 2 5 2 2" xfId="376"/>
-    <cellStyle name="Normal 6 2 5 2 3" xfId="377"/>
-    <cellStyle name="Normal 6 2 5 3" xfId="570"/>
-    <cellStyle name="Normal 6 2 5 4" xfId="568"/>
-    <cellStyle name="Normal 6 2 6" xfId="333"/>
-    <cellStyle name="Normal 6 2 6 2" xfId="632"/>
-    <cellStyle name="Normal 6 2 6 2 2" xfId="175"/>
-    <cellStyle name="Normal 6 2 6 2 3" xfId="174"/>
-    <cellStyle name="Normal 6 2 6 3" xfId="631"/>
-    <cellStyle name="Normal 6 2 6 4" xfId="630"/>
-    <cellStyle name="Normal 6 2 7" xfId="332"/>
-    <cellStyle name="Normal 6 2 7 2" xfId="195"/>
-    <cellStyle name="Normal 6 2 7 2 2" xfId="635"/>
-    <cellStyle name="Normal 6 2 7 2 3" xfId="636"/>
-    <cellStyle name="Normal 6 2 7 3" xfId="196"/>
-    <cellStyle name="Normal 6 2 7 4" xfId="427"/>
-    <cellStyle name="Normal 6 2 8" xfId="335"/>
-    <cellStyle name="Normal 6 2 8 2" xfId="474"/>
-    <cellStyle name="Normal 6 2 8 2 2" xfId="524"/>
-    <cellStyle name="Normal 6 2 8 2 3" xfId="523"/>
-    <cellStyle name="Normal 6 2 8 3" xfId="473"/>
-    <cellStyle name="Normal 6 2 8 4" xfId="479"/>
-    <cellStyle name="Normal 6 2 9" xfId="334"/>
-    <cellStyle name="Normal 6 2 9 2" xfId="26"/>
-    <cellStyle name="Normal 6 2 9 3" xfId="98"/>
-    <cellStyle name="Normal 6 3" xfId="314"/>
-    <cellStyle name="Normal 6 3 10" xfId="183"/>
-    <cellStyle name="Normal 6 3 2" xfId="548"/>
-    <cellStyle name="Normal 6 3 2 2" xfId="207"/>
-    <cellStyle name="Normal 6 3 2 2 2" xfId="237"/>
-    <cellStyle name="Normal 6 3 2 2 2 2" xfId="50"/>
-    <cellStyle name="Normal 6 3 2 2 2 2 2" xfId="89"/>
-    <cellStyle name="Normal 6 3 2 2 2 2 3" xfId="90"/>
-    <cellStyle name="Normal 6 3 2 2 2 3" xfId="51"/>
-    <cellStyle name="Normal 6 3 2 2 2 4" xfId="48"/>
-    <cellStyle name="Normal 6 3 2 2 3" xfId="238"/>
-    <cellStyle name="Normal 6 3 2 2 3 2" xfId="499"/>
-    <cellStyle name="Normal 6 3 2 2 3 2 2" xfId="288"/>
-    <cellStyle name="Normal 6 3 2 2 3 2 3" xfId="287"/>
-    <cellStyle name="Normal 6 3 2 2 3 3" xfId="498"/>
-    <cellStyle name="Normal 6 3 2 2 3 4" xfId="495"/>
-    <cellStyle name="Normal 6 3 2 2 4" xfId="234"/>
-    <cellStyle name="Normal 6 3 2 2 4 2" xfId="612"/>
-    <cellStyle name="Normal 6 3 2 2 4 3" xfId="613"/>
-    <cellStyle name="Normal 6 3 2 2 5" xfId="235"/>
-    <cellStyle name="Normal 6 3 2 2 6" xfId="236"/>
-    <cellStyle name="Normal 6 3 2 3" xfId="208"/>
-    <cellStyle name="Normal 6 3 2 3 2" xfId="37"/>
-    <cellStyle name="Normal 6 3 2 3 2 2" xfId="394"/>
-    <cellStyle name="Normal 6 3 2 3 2 3" xfId="393"/>
-    <cellStyle name="Normal 6 3 2 3 3" xfId="36"/>
-    <cellStyle name="Normal 6 3 2 3 4" xfId="35"/>
-    <cellStyle name="Normal 6 3 2 4" xfId="209"/>
-    <cellStyle name="Normal 6 3 2 4 2" xfId="627"/>
-    <cellStyle name="Normal 6 3 2 4 2 2" xfId="486"/>
-    <cellStyle name="Normal 6 3 2 4 2 3" xfId="487"/>
-    <cellStyle name="Normal 6 3 2 4 3" xfId="628"/>
-    <cellStyle name="Normal 6 3 2 4 4" xfId="629"/>
-    <cellStyle name="Normal 6 3 2 5" xfId="210"/>
-    <cellStyle name="Normal 6 3 2 5 2" xfId="431"/>
-    <cellStyle name="Normal 6 3 2 5 3" xfId="430"/>
-    <cellStyle name="Normal 6 3 2 6" xfId="211"/>
-    <cellStyle name="Normal 6 3 2 7" xfId="212"/>
-    <cellStyle name="Normal 6 3 3" xfId="549"/>
-    <cellStyle name="Normal 6 3 3 2" xfId="645"/>
-    <cellStyle name="Normal 6 3 3 2 2" xfId="558"/>
-    <cellStyle name="Normal 6 3 3 2 2 2" xfId="190"/>
-    <cellStyle name="Normal 6 3 3 2 2 3" xfId="189"/>
-    <cellStyle name="Normal 6 3 3 2 3" xfId="557"/>
-    <cellStyle name="Normal 6 3 3 2 4" xfId="556"/>
-    <cellStyle name="Normal 6 3 3 3" xfId="644"/>
-    <cellStyle name="Normal 6 3 3 3 2" xfId="114"/>
-    <cellStyle name="Normal 6 3 3 3 2 2" xfId="653"/>
-    <cellStyle name="Normal 6 3 3 3 2 3" xfId="654"/>
-    <cellStyle name="Normal 6 3 3 3 3" xfId="115"/>
-    <cellStyle name="Normal 6 3 3 3 4" xfId="112"/>
-    <cellStyle name="Normal 6 3 3 4" xfId="647"/>
-    <cellStyle name="Normal 6 3 3 4 2" xfId="317"/>
-    <cellStyle name="Normal 6 3 3 4 3" xfId="316"/>
-    <cellStyle name="Normal 6 3 3 5" xfId="646"/>
-    <cellStyle name="Normal 6 3 3 6" xfId="648"/>
-    <cellStyle name="Normal 6 3 4" xfId="550"/>
-    <cellStyle name="Normal 6 3 4 2" xfId="160"/>
-    <cellStyle name="Normal 6 3 4 2 2" xfId="470"/>
-    <cellStyle name="Normal 6 3 4 2 3" xfId="471"/>
-    <cellStyle name="Normal 6 3 4 3" xfId="164"/>
-    <cellStyle name="Normal 6 3 4 4" xfId="155"/>
-    <cellStyle name="Normal 6 3 5" xfId="551"/>
-    <cellStyle name="Normal 6 3 5 2" xfId="493"/>
-    <cellStyle name="Normal 6 3 5 2 2" xfId="53"/>
-    <cellStyle name="Normal 6 3 5 2 3" xfId="52"/>
-    <cellStyle name="Normal 6 3 5 3" xfId="492"/>
-    <cellStyle name="Normal 6 3 5 4" xfId="491"/>
-    <cellStyle name="Normal 6 3 6" xfId="552"/>
-    <cellStyle name="Normal 6 3 6 2" xfId="323"/>
-    <cellStyle name="Normal 6 3 6 2 2" xfId="153"/>
-    <cellStyle name="Normal 6 3 6 2 3" xfId="154"/>
-    <cellStyle name="Normal 6 3 6 3" xfId="324"/>
-    <cellStyle name="Normal 6 3 6 4" xfId="322"/>
-    <cellStyle name="Normal 6 3 7" xfId="553"/>
-    <cellStyle name="Normal 6 3 7 2" xfId="111"/>
-    <cellStyle name="Normal 6 3 7 2 2" xfId="347"/>
-    <cellStyle name="Normal 6 3 7 2 3" xfId="346"/>
-    <cellStyle name="Normal 6 3 7 3" xfId="110"/>
-    <cellStyle name="Normal 6 3 7 4" xfId="109"/>
-    <cellStyle name="Normal 6 3 8" xfId="501"/>
-    <cellStyle name="Normal 6 3 8 2" xfId="305"/>
-    <cellStyle name="Normal 6 3 8 3" xfId="306"/>
-    <cellStyle name="Normal 6 3 9" xfId="502"/>
-    <cellStyle name="Normal 6 4" xfId="311"/>
-    <cellStyle name="Normal 6 4 10" xfId="100"/>
-    <cellStyle name="Normal 6 4 2" xfId="92"/>
-    <cellStyle name="Normal 6 4 2 2" xfId="140"/>
-    <cellStyle name="Normal 6 4 2 2 2" xfId="375"/>
-    <cellStyle name="Normal 6 4 2 2 2 2" xfId="267"/>
-    <cellStyle name="Normal 6 4 2 2 2 2 2" xfId="382"/>
-    <cellStyle name="Normal 6 4 2 2 2 2 3" xfId="381"/>
-    <cellStyle name="Normal 6 4 2 2 2 3" xfId="266"/>
-    <cellStyle name="Normal 6 4 2 2 2 4" xfId="268"/>
-    <cellStyle name="Normal 6 4 2 2 3" xfId="395"/>
-    <cellStyle name="Normal 6 4 2 2 3 2" xfId="480"/>
-    <cellStyle name="Normal 6 4 2 2 3 2 2" xfId="187"/>
-    <cellStyle name="Normal 6 4 2 2 3 2 3" xfId="188"/>
-    <cellStyle name="Normal 6 4 2 2 3 3" xfId="481"/>
-    <cellStyle name="Normal 6 4 2 2 3 4" xfId="484"/>
-    <cellStyle name="Normal 6 4 2 2 4" xfId="402"/>
-    <cellStyle name="Normal 6 4 2 2 4 2" xfId="429"/>
-    <cellStyle name="Normal 6 4 2 2 4 3" xfId="428"/>
-    <cellStyle name="Normal 6 4 2 2 5" xfId="401"/>
-    <cellStyle name="Normal 6 4 2 2 6" xfId="379"/>
-    <cellStyle name="Normal 6 4 2 3" xfId="139"/>
-    <cellStyle name="Normal 6 4 2 3 2" xfId="587"/>
-    <cellStyle name="Normal 6 4 2 3 2 2" xfId="655"/>
-    <cellStyle name="Normal 6 4 2 3 2 3" xfId="656"/>
-    <cellStyle name="Normal 6 4 2 3 3" xfId="588"/>
-    <cellStyle name="Normal 6 4 2 3 4" xfId="591"/>
-    <cellStyle name="Normal 6 4 2 4" xfId="138"/>
-    <cellStyle name="Normal 6 4 2 4 2" xfId="623"/>
-    <cellStyle name="Normal 6 4 2 4 2 2" xfId="605"/>
-    <cellStyle name="Normal 6 4 2 4 2 3" xfId="604"/>
-    <cellStyle name="Normal 6 4 2 4 3" xfId="622"/>
-    <cellStyle name="Normal 6 4 2 4 4" xfId="621"/>
-    <cellStyle name="Normal 6 4 2 5" xfId="137"/>
-    <cellStyle name="Normal 6 4 2 5 2" xfId="184"/>
-    <cellStyle name="Normal 6 4 2 5 3" xfId="185"/>
-    <cellStyle name="Normal 6 4 2 6" xfId="136"/>
-    <cellStyle name="Normal 6 4 2 7" xfId="135"/>
-    <cellStyle name="Normal 6 4 3" xfId="91"/>
-    <cellStyle name="Normal 6 4 3 2" xfId="342"/>
-    <cellStyle name="Normal 6 4 3 2 2" xfId="200"/>
-    <cellStyle name="Normal 6 4 3 2 2 2" xfId="127"/>
-    <cellStyle name="Normal 6 4 3 2 2 3" xfId="128"/>
-    <cellStyle name="Normal 6 4 3 2 3" xfId="201"/>
-    <cellStyle name="Normal 6 4 3 2 4" xfId="204"/>
-    <cellStyle name="Normal 6 4 3 3" xfId="343"/>
-    <cellStyle name="Normal 6 4 3 3 2" xfId="643"/>
-    <cellStyle name="Normal 6 4 3 3 2 2" xfId="298"/>
-    <cellStyle name="Normal 6 4 3 3 2 3" xfId="297"/>
-    <cellStyle name="Normal 6 4 3 3 3" xfId="642"/>
-    <cellStyle name="Normal 6 4 3 3 4" xfId="583"/>
-    <cellStyle name="Normal 6 4 3 4" xfId="340"/>
-    <cellStyle name="Normal 6 4 3 4 2" xfId="444"/>
-    <cellStyle name="Normal 6 4 3 4 3" xfId="445"/>
-    <cellStyle name="Normal 6 4 3 5" xfId="341"/>
-    <cellStyle name="Normal 6 4 3 6" xfId="339"/>
-    <cellStyle name="Normal 6 4 4" xfId="441"/>
-    <cellStyle name="Normal 6 4 4 2" xfId="292"/>
-    <cellStyle name="Normal 6 4 4 2 2" xfId="247"/>
-    <cellStyle name="Normal 6 4 4 2 3" xfId="246"/>
-    <cellStyle name="Normal 6 4 4 3" xfId="412"/>
-    <cellStyle name="Normal 6 4 4 4" xfId="293"/>
-    <cellStyle name="Normal 6 4 5" xfId="440"/>
-    <cellStyle name="Normal 6 4 5 2" xfId="460"/>
-    <cellStyle name="Normal 6 4 5 2 2" xfId="517"/>
-    <cellStyle name="Normal 6 4 5 2 3" xfId="520"/>
-    <cellStyle name="Normal 6 4 5 3" xfId="461"/>
-    <cellStyle name="Normal 6 4 5 4" xfId="462"/>
-    <cellStyle name="Normal 6 4 6" xfId="88"/>
-    <cellStyle name="Normal 6 4 6 2" xfId="5"/>
-    <cellStyle name="Normal 6 4 6 2 2" xfId="595"/>
-    <cellStyle name="Normal 6 4 6 2 3" xfId="594"/>
-    <cellStyle name="Normal 6 4 6 3" xfId="4"/>
-    <cellStyle name="Normal 6 4 6 4" xfId="10"/>
-    <cellStyle name="Normal 6 4 7" xfId="87"/>
-    <cellStyle name="Normal 6 4 7 2" xfId="221"/>
-    <cellStyle name="Normal 6 4 7 2 2" xfId="403"/>
-    <cellStyle name="Normal 6 4 7 2 3" xfId="404"/>
-    <cellStyle name="Normal 6 4 7 3" xfId="222"/>
-    <cellStyle name="Normal 6 4 7 4" xfId="224"/>
-    <cellStyle name="Normal 6 4 8" xfId="97"/>
-    <cellStyle name="Normal 6 4 8 2" xfId="95"/>
-    <cellStyle name="Normal 6 4 8 3" xfId="380"/>
-    <cellStyle name="Normal 6 4 9" xfId="96"/>
-    <cellStyle name="Normal 6 5" xfId="310"/>
-    <cellStyle name="Normal 6 5 2" xfId="285"/>
-    <cellStyle name="Normal 6 5 2 2" xfId="534"/>
-    <cellStyle name="Normal 6 5 2 2 2" xfId="182"/>
-    <cellStyle name="Normal 6 5 2 2 2 2" xfId="258"/>
-    <cellStyle name="Normal 6 5 2 2 2 2 2" xfId="546"/>
-    <cellStyle name="Normal 6 5 2 2 2 2 3" xfId="547"/>
-    <cellStyle name="Normal 6 5 2 2 2 3" xfId="259"/>
-    <cellStyle name="Normal 6 5 2 2 2 4" xfId="261"/>
-    <cellStyle name="Normal 6 5 2 2 3" xfId="417"/>
-    <cellStyle name="Normal 6 5 2 2 3 2" xfId="302"/>
-    <cellStyle name="Normal 6 5 2 2 3 2 2" xfId="107"/>
-    <cellStyle name="Normal 6 5 2 2 3 2 3" xfId="106"/>
-    <cellStyle name="Normal 6 5 2 2 3 3" xfId="301"/>
-    <cellStyle name="Normal 6 5 2 2 3 4" xfId="79"/>
-    <cellStyle name="Normal 6 5 2 2 4" xfId="253"/>
-    <cellStyle name="Normal 6 5 2 2 4 2" xfId="419"/>
-    <cellStyle name="Normal 6 5 2 2 4 3" xfId="420"/>
-    <cellStyle name="Normal 6 5 2 2 5" xfId="254"/>
-    <cellStyle name="Normal 6 5 2 2 6" xfId="192"/>
-    <cellStyle name="Normal 6 5 2 3" xfId="535"/>
-    <cellStyle name="Normal 6 5 2 3 2" xfId="649"/>
-    <cellStyle name="Normal 6 5 2 3 2 2" xfId="370"/>
-    <cellStyle name="Normal 6 5 2 3 2 3" xfId="369"/>
-    <cellStyle name="Normal 6 5 2 3 3" xfId="70"/>
-    <cellStyle name="Normal 6 5 2 3 4" xfId="276"/>
-    <cellStyle name="Normal 6 5 2 4" xfId="532"/>
-    <cellStyle name="Normal 6 5 2 4 2" xfId="518"/>
-    <cellStyle name="Normal 6 5 2 4 2 2" xfId="633"/>
-    <cellStyle name="Normal 6 5 2 4 2 3" xfId="634"/>
-    <cellStyle name="Normal 6 5 2 4 3" xfId="519"/>
-    <cellStyle name="Normal 6 5 2 4 4" xfId="514"/>
-    <cellStyle name="Normal 6 5 2 5" xfId="447"/>
-    <cellStyle name="Normal 6 5 2 5 2" xfId="304"/>
-    <cellStyle name="Normal 6 5 2 5 3" xfId="303"/>
-    <cellStyle name="Normal 6 5 2 6" xfId="530"/>
-    <cellStyle name="Normal 6 5 2 7" xfId="531"/>
-    <cellStyle name="Normal 6 5 3" xfId="286"/>
-    <cellStyle name="Normal 6 5 3 2" xfId="321"/>
-    <cellStyle name="Normal 6 5 3 2 2" xfId="134"/>
-    <cellStyle name="Normal 6 5 3 2 2 2" xfId="600"/>
-    <cellStyle name="Normal 6 5 3 2 2 3" xfId="599"/>
-    <cellStyle name="Normal 6 5 3 2 3" xfId="229"/>
-    <cellStyle name="Normal 6 5 3 2 4" xfId="472"/>
-    <cellStyle name="Normal 6 5 3 3" xfId="320"/>
-    <cellStyle name="Normal 6 5 3 3 2" xfId="32"/>
-    <cellStyle name="Normal 6 5 3 3 2 2" xfId="423"/>
-    <cellStyle name="Normal 6 5 3 3 2 3" xfId="424"/>
-    <cellStyle name="Normal 6 5 3 3 3" xfId="34"/>
-    <cellStyle name="Normal 6 5 3 3 4" xfId="9"/>
-    <cellStyle name="Normal 6 5 3 4" xfId="319"/>
-    <cellStyle name="Normal 6 5 3 4 2" xfId="94"/>
-    <cellStyle name="Normal 6 5 3 4 3" xfId="93"/>
-    <cellStyle name="Normal 6 5 3 5" xfId="318"/>
-    <cellStyle name="Normal 6 5 3 6" xfId="525"/>
-    <cellStyle name="Normal 6 5 4" xfId="283"/>
-    <cellStyle name="Normal 6 5 4 2" xfId="582"/>
-    <cellStyle name="Normal 6 5 4 2 2" xfId="478"/>
-    <cellStyle name="Normal 6 5 4 2 3" xfId="639"/>
-    <cellStyle name="Normal 6 5 4 3" xfId="197"/>
-    <cellStyle name="Normal 6 5 4 4" xfId="584"/>
-    <cellStyle name="Normal 6 5 5" xfId="284"/>
-    <cellStyle name="Normal 6 5 5 2" xfId="387"/>
-    <cellStyle name="Normal 6 5 5 2 2" xfId="119"/>
-    <cellStyle name="Normal 6 5 5 2 3" xfId="33"/>
-    <cellStyle name="Normal 6 5 5 3" xfId="386"/>
-    <cellStyle name="Normal 6 5 5 4" xfId="388"/>
-    <cellStyle name="Normal 6 5 6" xfId="281"/>
-    <cellStyle name="Normal 6 5 6 2" xfId="74"/>
-    <cellStyle name="Normal 6 5 6 3" xfId="356"/>
-    <cellStyle name="Normal 6 5 7" xfId="282"/>
-    <cellStyle name="Normal 6 5 8" xfId="280"/>
-    <cellStyle name="Normal 6 6" xfId="313"/>
-    <cellStyle name="Normal 6 6 2" xfId="326"/>
-    <cellStyle name="Normal 6 6 2 2" xfId="245"/>
-    <cellStyle name="Normal 6 6 2 2 2" xfId="64"/>
-    <cellStyle name="Normal 6 6 2 2 2 2" xfId="618"/>
-    <cellStyle name="Normal 6 6 2 2 2 2 2" xfId="39"/>
-    <cellStyle name="Normal 6 6 2 2 2 2 3" xfId="515"/>
-    <cellStyle name="Normal 6 6 2 2 2 3" xfId="617"/>
-    <cellStyle name="Normal 6 6 2 2 2 4" xfId="619"/>
-    <cellStyle name="Normal 6 6 2 2 3" xfId="113"/>
-    <cellStyle name="Normal 6 6 2 2 3 2" xfId="116"/>
-    <cellStyle name="Normal 6 6 2 2 3 2 2" xfId="456"/>
-    <cellStyle name="Normal 6 6 2 2 3 2 3" xfId="457"/>
-    <cellStyle name="Normal 6 6 2 2 3 3" xfId="296"/>
-    <cellStyle name="Normal 6 6 2 2 3 4" xfId="176"/>
-    <cellStyle name="Normal 6 6 2 2 4" xfId="80"/>
-    <cellStyle name="Normal 6 6 2 2 4 2" xfId="199"/>
-    <cellStyle name="Normal 6 6 2 2 4 3" xfId="198"/>
-    <cellStyle name="Normal 6 6 2 2 5" xfId="77"/>
-    <cellStyle name="Normal 6 6 2 2 6" xfId="129"/>
-    <cellStyle name="Normal 6 6 2 3" xfId="163"/>
-    <cellStyle name="Normal 6 6 2 3 2" xfId="662"/>
-    <cellStyle name="Normal 6 6 2 3 2 2" xfId="278"/>
-    <cellStyle name="Normal 6 6 2 3 2 3" xfId="279"/>
-    <cellStyle name="Normal 6 6 2 3 3" xfId="1"/>
-    <cellStyle name="Normal 6 6 2 3 4" xfId="2"/>
-    <cellStyle name="Normal 6 6 2 4" xfId="586"/>
-    <cellStyle name="Normal 6 6 2 4 2" xfId="581"/>
-    <cellStyle name="Normal 6 6 2 4 2 2" xfId="383"/>
-    <cellStyle name="Normal 6 6 2 4 2 3" xfId="516"/>
-    <cellStyle name="Normal 6 6 2 4 3" xfId="580"/>
-    <cellStyle name="Normal 6 6 2 4 4" xfId="579"/>
-    <cellStyle name="Normal 6 6 2 5" xfId="159"/>
-    <cellStyle name="Normal 6 6 2 5 2" xfId="141"/>
-    <cellStyle name="Normal 6 6 2 5 3" xfId="142"/>
-    <cellStyle name="Normal 6 6 2 6" xfId="162"/>
-    <cellStyle name="Normal 6 6 2 7" xfId="161"/>
-    <cellStyle name="Normal 6 6 3" xfId="325"/>
-    <cellStyle name="Normal 6 6 3 2" xfId="374"/>
-    <cellStyle name="Normal 6 6 3 2 2" xfId="275"/>
-    <cellStyle name="Normal 6 6 3 2 2 2" xfId="410"/>
-    <cellStyle name="Normal 6 6 3 2 2 3" xfId="411"/>
-    <cellStyle name="Normal 6 6 3 2 3" xfId="362"/>
-    <cellStyle name="Normal 6 6 3 2 4" xfId="277"/>
-    <cellStyle name="Normal 6 6 3 3" xfId="186"/>
-    <cellStyle name="Normal 6 6 3 3 2" xfId="105"/>
-    <cellStyle name="Normal 6 6 3 3 2 2" xfId="300"/>
-    <cellStyle name="Normal 6 6 3 3 2 3" xfId="299"/>
-    <cellStyle name="Normal 6 6 3 3 3" xfId="104"/>
-    <cellStyle name="Normal 6 6 3 3 4" xfId="574"/>
-    <cellStyle name="Normal 6 6 3 4" xfId="371"/>
-    <cellStyle name="Normal 6 6 3 4 2" xfId="391"/>
-    <cellStyle name="Normal 6 6 3 4 3" xfId="392"/>
-    <cellStyle name="Normal 6 6 3 5" xfId="372"/>
-    <cellStyle name="Normal 6 6 3 6" xfId="373"/>
-    <cellStyle name="Normal 6 6 4" xfId="108"/>
-    <cellStyle name="Normal 6 6 4 2" xfId="435"/>
-    <cellStyle name="Normal 6 6 4 2 2" xfId="433"/>
-    <cellStyle name="Normal 6 6 4 2 3" xfId="432"/>
-    <cellStyle name="Normal 6 6 4 3" xfId="434"/>
-    <cellStyle name="Normal 6 6 4 4" xfId="438"/>
-    <cellStyle name="Normal 6 6 5" xfId="585"/>
-    <cellStyle name="Normal 6 6 5 2" xfId="596"/>
-    <cellStyle name="Normal 6 6 5 2 2" xfId="554"/>
-    <cellStyle name="Normal 6 6 5 2 3" xfId="555"/>
-    <cellStyle name="Normal 6 6 5 3" xfId="597"/>
-    <cellStyle name="Normal 6 6 5 4" xfId="598"/>
-    <cellStyle name="Normal 6 6 6" xfId="616"/>
-    <cellStyle name="Normal 6 6 6 2" xfId="29"/>
-    <cellStyle name="Normal 6 6 6 3" xfId="28"/>
-    <cellStyle name="Normal 6 6 7" xfId="507"/>
-    <cellStyle name="Normal 6 6 8" xfId="513"/>
-    <cellStyle name="Normal 6 7" xfId="312"/>
-    <cellStyle name="Normal 6 7 2" xfId="65"/>
-    <cellStyle name="Normal 6 7 2 2" xfId="610"/>
-    <cellStyle name="Normal 6 7 2 2 2" xfId="122"/>
-    <cellStyle name="Normal 6 7 2 2 2 2" xfId="615"/>
-    <cellStyle name="Normal 6 7 2 2 2 2 2" xfId="243"/>
-    <cellStyle name="Normal 6 7 2 2 2 2 3" xfId="244"/>
-    <cellStyle name="Normal 6 7 2 2 2 3" xfId="120"/>
-    <cellStyle name="Normal 6 7 2 2 2 4" xfId="562"/>
-    <cellStyle name="Normal 6 7 2 2 3" xfId="123"/>
-    <cellStyle name="Normal 6 7 2 2 3 2" xfId="358"/>
-    <cellStyle name="Normal 6 7 2 2 3 2 2" xfId="390"/>
-    <cellStyle name="Normal 6 7 2 2 3 2 3" xfId="144"/>
-    <cellStyle name="Normal 6 7 2 2 3 3" xfId="357"/>
-    <cellStyle name="Normal 6 7 2 2 3 4" xfId="359"/>
-    <cellStyle name="Normal 6 7 2 2 4" xfId="124"/>
-    <cellStyle name="Normal 6 7 2 2 4 2" xfId="170"/>
-    <cellStyle name="Normal 6 7 2 2 4 3" xfId="171"/>
-    <cellStyle name="Normal 6 7 2 2 5" xfId="125"/>
-    <cellStyle name="Normal 6 7 2 2 6" xfId="126"/>
-    <cellStyle name="Normal 6 7 2 3" xfId="611"/>
-    <cellStyle name="Normal 6 7 2 3 2" xfId="572"/>
-    <cellStyle name="Normal 6 7 2 3 2 2" xfId="49"/>
-    <cellStyle name="Normal 6 7 2 3 2 3" xfId="327"/>
-    <cellStyle name="Normal 6 7 2 3 3" xfId="571"/>
-    <cellStyle name="Normal 6 7 2 3 4" xfId="573"/>
-    <cellStyle name="Normal 6 7 2 4" xfId="606"/>
-    <cellStyle name="Normal 6 7 2 4 2" xfId="272"/>
-    <cellStyle name="Normal 6 7 2 4 2 2" xfId="179"/>
-    <cellStyle name="Normal 6 7 2 4 2 3" xfId="536"/>
-    <cellStyle name="Normal 6 7 2 4 3" xfId="273"/>
-    <cellStyle name="Normal 6 7 2 4 4" xfId="271"/>
-    <cellStyle name="Normal 6 7 2 5" xfId="607"/>
-    <cellStyle name="Normal 6 7 2 5 2" xfId="86"/>
-    <cellStyle name="Normal 6 7 2 5 3" xfId="85"/>
-    <cellStyle name="Normal 6 7 2 6" xfId="608"/>
-    <cellStyle name="Normal 6 7 2 7" xfId="609"/>
-    <cellStyle name="Normal 6 7 3" xfId="66"/>
-    <cellStyle name="Normal 6 7 3 2" xfId="409"/>
-    <cellStyle name="Normal 6 7 3 2 2" xfId="476"/>
-    <cellStyle name="Normal 6 7 3 2 2 2" xfId="353"/>
-    <cellStyle name="Normal 6 7 3 2 2 3" xfId="352"/>
-    <cellStyle name="Normal 6 7 3 2 3" xfId="475"/>
-    <cellStyle name="Normal 6 7 3 2 4" xfId="477"/>
-    <cellStyle name="Normal 6 7 3 3" xfId="418"/>
-    <cellStyle name="Normal 6 7 3 3 2" xfId="650"/>
-    <cellStyle name="Normal 6 7 3 3 2 2" xfId="19"/>
-    <cellStyle name="Normal 6 7 3 3 2 3" xfId="23"/>
-    <cellStyle name="Normal 6 7 3 3 3" xfId="651"/>
-    <cellStyle name="Normal 6 7 3 3 4" xfId="652"/>
-    <cellStyle name="Normal 6 7 3 4" xfId="414"/>
-    <cellStyle name="Normal 6 7 3 4 2" xfId="563"/>
-    <cellStyle name="Normal 6 7 3 4 3" xfId="620"/>
-    <cellStyle name="Normal 6 7 3 5" xfId="413"/>
-    <cellStyle name="Normal 6 7 3 6" xfId="407"/>
-    <cellStyle name="Normal 6 7 4" xfId="60"/>
-    <cellStyle name="Normal 6 7 4 2" xfId="166"/>
-    <cellStyle name="Normal 6 7 4 2 2" xfId="509"/>
-    <cellStyle name="Normal 6 7 4 2 3" xfId="510"/>
-    <cellStyle name="Normal 6 7 4 3" xfId="490"/>
-    <cellStyle name="Normal 6 7 4 4" xfId="494"/>
-    <cellStyle name="Normal 6 7 5" xfId="61"/>
-    <cellStyle name="Normal 6 7 5 2" xfId="638"/>
-    <cellStyle name="Normal 6 7 5 2 2" xfId="152"/>
-    <cellStyle name="Normal 6 7 5 2 3" xfId="38"/>
-    <cellStyle name="Normal 6 7 5 3" xfId="637"/>
-    <cellStyle name="Normal 6 7 5 4" xfId="641"/>
-    <cellStyle name="Normal 6 7 6" xfId="62"/>
-    <cellStyle name="Normal 6 7 6 2" xfId="415"/>
-    <cellStyle name="Normal 6 7 6 3" xfId="416"/>
-    <cellStyle name="Normal 6 7 7" xfId="63"/>
-    <cellStyle name="Normal 6 7 8" xfId="59"/>
-    <cellStyle name="Normal 6 8" xfId="308"/>
-    <cellStyle name="Normal 6 8 2" xfId="364"/>
-    <cellStyle name="Normal 6 8 2 2" xfId="146"/>
-    <cellStyle name="Normal 6 8 2 2 2" xfId="3"/>
-    <cellStyle name="Normal 6 8 2 2 2 2" xfId="345"/>
-    <cellStyle name="Normal 6 8 2 2 2 3" xfId="344"/>
-    <cellStyle name="Normal 6 8 2 2 3" xfId="18"/>
-    <cellStyle name="Normal 6 8 2 2 4" xfId="575"/>
-    <cellStyle name="Normal 6 8 2 3" xfId="145"/>
-    <cellStyle name="Normal 6 8 2 3 2" xfId="240"/>
-    <cellStyle name="Normal 6 8 2 3 2 2" xfId="202"/>
-    <cellStyle name="Normal 6 8 2 3 2 3" xfId="203"/>
-    <cellStyle name="Normal 6 8 2 3 3" xfId="241"/>
-    <cellStyle name="Normal 6 8 2 3 4" xfId="239"/>
-    <cellStyle name="Normal 6 8 2 4" xfId="149"/>
-    <cellStyle name="Normal 6 8 2 4 2" xfId="625"/>
-    <cellStyle name="Normal 6 8 2 4 3" xfId="624"/>
-    <cellStyle name="Normal 6 8 2 5" xfId="148"/>
-    <cellStyle name="Normal 6 8 2 6" xfId="147"/>
-    <cellStyle name="Normal 6 8 3" xfId="363"/>
-    <cellStyle name="Normal 6 8 3 2" xfId="350"/>
-    <cellStyle name="Normal 6 8 3 2 2" xfId="488"/>
-    <cellStyle name="Normal 6 8 3 2 3" xfId="489"/>
-    <cellStyle name="Normal 6 8 3 3" xfId="351"/>
-    <cellStyle name="Normal 6 8 3 4" xfId="354"/>
-    <cellStyle name="Normal 6 8 4" xfId="368"/>
-    <cellStyle name="Normal 6 8 4 2" xfId="565"/>
-    <cellStyle name="Normal 6 8 4 2 2" xfId="165"/>
-    <cellStyle name="Normal 6 8 4 2 3" xfId="446"/>
-    <cellStyle name="Normal 6 8 4 3" xfId="564"/>
-    <cellStyle name="Normal 6 8 4 4" xfId="559"/>
-    <cellStyle name="Normal 6 8 5" xfId="367"/>
-    <cellStyle name="Normal 6 8 5 2" xfId="102"/>
-    <cellStyle name="Normal 6 8 5 3" xfId="103"/>
-    <cellStyle name="Normal 6 8 6" xfId="366"/>
-    <cellStyle name="Normal 6 8 7" xfId="365"/>
-    <cellStyle name="Normal 6 9" xfId="307"/>
-    <cellStyle name="Normal 6 9 2" xfId="537"/>
-    <cellStyle name="Normal 6 9 2 2" xfId="215"/>
-    <cellStyle name="Normal 6 9 2 2 2" xfId="264"/>
-    <cellStyle name="Normal 6 9 2 2 3" xfId="265"/>
-    <cellStyle name="Normal 6 9 2 3" xfId="566"/>
-    <cellStyle name="Normal 6 9 2 4" xfId="217"/>
-    <cellStyle name="Normal 6 9 3" xfId="538"/>
-    <cellStyle name="Normal 6 9 3 2" xfId="658"/>
-    <cellStyle name="Normal 6 9 3 2 2" xfId="426"/>
-    <cellStyle name="Normal 6 9 3 2 3" xfId="425"/>
-    <cellStyle name="Normal 6 9 3 3" xfId="657"/>
-    <cellStyle name="Normal 6 9 3 4" xfId="659"/>
-    <cellStyle name="Normal 6 9 4" xfId="540"/>
-    <cellStyle name="Normal 6 9 4 2" xfId="640"/>
-    <cellStyle name="Normal 6 9 4 3" xfId="567"/>
-    <cellStyle name="Normal 6 9 5" xfId="541"/>
-    <cellStyle name="Normal 6 9 6" xfId="539"/>
-    <cellStyle name="Normal 7" xfId="452"/>
-    <cellStyle name="Normal 7 2" xfId="529"/>
-    <cellStyle name="Normal 8" xfId="455"/>
-    <cellStyle name="Normal 8 2" xfId="576"/>
-    <cellStyle name="Normal 9" xfId="454"/>
-    <cellStyle name="Normal 9 2" xfId="58"/>
-    <cellStyle name="Percent 2" xfId="269"/>
-    <cellStyle name="Percent 2 2" xfId="78"/>
+    <cellStyle name="Normal 10" xfId="545" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2" xfId="449" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2 2" xfId="439" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 3" xfId="448" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 3 2" xfId="500" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 4" xfId="451" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 4 2" xfId="81" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal 5" xfId="450" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Normal 5 2" xfId="242" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normal 6" xfId="453" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 6 10" xfId="41" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normal 6 10 2" xfId="121" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal 6 10 2 2" xfId="168" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normal 6 10 2 3" xfId="167" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Normal 6 10 3" xfId="118" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Normal 6 10 4" xfId="117" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Normal 6 11" xfId="40" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Normal 6 11 2" xfId="251" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Normal 6 11 2 2" xfId="421" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Normal 6 11 2 3" xfId="422" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Normal 6 11 3" xfId="252" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Normal 6 11 4" xfId="250" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Normal 6 12" xfId="43" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Normal 6 12 2" xfId="227" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Normal 6 12 2 2" xfId="181" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Normal 6 12 2 3" xfId="180" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Normal 6 12 3" xfId="226" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Normal 6 12 4" xfId="225" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Normal 6 13" xfId="42" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Normal 6 13 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Normal 6 13 2 2" xfId="503" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Normal 6 13 2 3" xfId="504" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Normal 6 13 3" xfId="17" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Normal 6 13 4" xfId="11" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Normal 6 14" xfId="45" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Normal 6 14 2" xfId="337" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Normal 6 14 2 2" xfId="76" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Normal 6 14 2 3" xfId="75" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Normal 6 14 3" xfId="336" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Normal 6 14 4" xfId="338" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Normal 6 15" xfId="44" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Normal 6 15 2" xfId="130" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Normal 6 15 3" xfId="131" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Normal 6 16" xfId="47" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Normal 6 17" xfId="46" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Normal 6 2" xfId="315" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Normal 6 2 10" xfId="233" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Normal 6 2 11" xfId="232" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Normal 6 2 2" xfId="578" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Normal 6 2 2 10" xfId="528" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Normal 6 2 2 2" xfId="465" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2" xfId="485" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 2" xfId="512" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 2 2" xfId="329" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 2 3" xfId="328" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 3" xfId="6" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 2 4" xfId="8" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 3" xfId="511" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 2" xfId="218" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 2 2" xfId="67" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 2 3" xfId="68" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 3" xfId="219" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 3 4" xfId="220" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 4" xfId="309" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 4 2" xfId="437" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 4 3" xfId="436" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 5" xfId="260" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="Normal 6 2 2 2 2 6" xfId="508" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3" xfId="191" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3 2" xfId="56" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3 2 2" xfId="496" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3 2 3" xfId="497" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3 3" xfId="57" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="Normal 6 2 2 2 3 4" xfId="54" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Normal 6 2 2 2 4" xfId="178" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="Normal 6 2 2 2 4 2" xfId="385" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="Normal 6 2 2 2 4 2 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="Normal 6 2 2 2 4 2 3" xfId="71" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
+    <cellStyle name="Normal 6 2 2 2 4 3" xfId="384" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="Normal 6 2 2 2 4 4" xfId="389" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="Normal 6 2 2 2 5" xfId="177" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
+    <cellStyle name="Normal 6 2 2 2 5 2" xfId="592" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="Normal 6 2 2 2 5 3" xfId="593" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="Normal 6 2 2 2 6" xfId="483" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Normal 6 2 2 2 7" xfId="482" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="Normal 6 2 2 3" xfId="464" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="Normal 6 2 2 3 2" xfId="24" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="Normal 6 2 2 3 2 2" xfId="230" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
+    <cellStyle name="Normal 6 2 2 3 2 2 2" xfId="560" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
+    <cellStyle name="Normal 6 2 2 3 2 2 3" xfId="561" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
+    <cellStyle name="Normal 6 2 2 3 2 3" xfId="231" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
+    <cellStyle name="Normal 6 2 2 3 2 4" xfId="228" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
+    <cellStyle name="Normal 6 2 2 3 3" xfId="25" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
+    <cellStyle name="Normal 6 2 2 3 3 2" xfId="31" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
+    <cellStyle name="Normal 6 2 2 3 3 2 2" xfId="133" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
+    <cellStyle name="Normal 6 2 2 3 3 2 3" xfId="132" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
+    <cellStyle name="Normal 6 2 2 3 3 3" xfId="30" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
+    <cellStyle name="Normal 6 2 2 3 3 4" xfId="27" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
+    <cellStyle name="Normal 6 2 2 3 4" xfId="20" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
+    <cellStyle name="Normal 6 2 2 3 4 2" xfId="193" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
+    <cellStyle name="Normal 6 2 2 3 4 3" xfId="194" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
+    <cellStyle name="Normal 6 2 2 3 5" xfId="21" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
+    <cellStyle name="Normal 6 2 2 3 6" xfId="22" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
+    <cellStyle name="Normal 6 2 2 4" xfId="467" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
+    <cellStyle name="Normal 6 2 2 4 2" xfId="206" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
+    <cellStyle name="Normal 6 2 2 4 2 2" xfId="143" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
+    <cellStyle name="Normal 6 2 2 4 2 3" xfId="544" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
+    <cellStyle name="Normal 6 2 2 4 3" xfId="205" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
+    <cellStyle name="Normal 6 2 2 4 4" xfId="533" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
+    <cellStyle name="Normal 6 2 2 5" xfId="466" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
+    <cellStyle name="Normal 6 2 2 5 2" xfId="405" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
+    <cellStyle name="Normal 6 2 2 5 2 2" xfId="248" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
+    <cellStyle name="Normal 6 2 2 5 2 3" xfId="249" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
+    <cellStyle name="Normal 6 2 2 5 3" xfId="406" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
+    <cellStyle name="Normal 6 2 2 5 4" xfId="408" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
+    <cellStyle name="Normal 6 2 2 6" xfId="469" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="Normal 6 2 2 6 2" xfId="602" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
+    <cellStyle name="Normal 6 2 2 6 2 2" xfId="590" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
+    <cellStyle name="Normal 6 2 2 6 2 3" xfId="589" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
+    <cellStyle name="Normal 6 2 2 6 3" xfId="601" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
+    <cellStyle name="Normal 6 2 2 6 4" xfId="603" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
+    <cellStyle name="Normal 6 2 2 7" xfId="468" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
+    <cellStyle name="Normal 6 2 2 7 2" xfId="156" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
+    <cellStyle name="Normal 6 2 2 7 2 2" xfId="262" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
+    <cellStyle name="Normal 6 2 2 7 2 3" xfId="263" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
+    <cellStyle name="Normal 6 2 2 7 3" xfId="157" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
+    <cellStyle name="Normal 6 2 2 7 4" xfId="158" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
+    <cellStyle name="Normal 6 2 2 8" xfId="101" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
+    <cellStyle name="Normal 6 2 2 8 2" xfId="349" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
+    <cellStyle name="Normal 6 2 2 8 3" xfId="348" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
+    <cellStyle name="Normal 6 2 2 9" xfId="99" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
+    <cellStyle name="Normal 6 2 3" xfId="577" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
+    <cellStyle name="Normal 6 2 3 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
+    <cellStyle name="Normal 6 2 3 2 2" xfId="294" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
+    <cellStyle name="Normal 6 2 3 2 2 2" xfId="360" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
+    <cellStyle name="Normal 6 2 3 2 2 2 2" xfId="526" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
+    <cellStyle name="Normal 6 2 3 2 2 2 3" xfId="527" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
+    <cellStyle name="Normal 6 2 3 2 2 3" xfId="361" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
+    <cellStyle name="Normal 6 2 3 2 2 4" xfId="355" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
+    <cellStyle name="Normal 6 2 3 2 3" xfId="295" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
+    <cellStyle name="Normal 6 2 3 2 3 2" xfId="173" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
+    <cellStyle name="Normal 6 2 3 2 3 2 2" xfId="443" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
+    <cellStyle name="Normal 6 2 3 2 3 2 3" xfId="442" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
+    <cellStyle name="Normal 6 2 3 2 3 3" xfId="172" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
+    <cellStyle name="Normal 6 2 3 2 3 4" xfId="169" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
+    <cellStyle name="Normal 6 2 3 2 4" xfId="289" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
+    <cellStyle name="Normal 6 2 3 2 4 2" xfId="213" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
+    <cellStyle name="Normal 6 2 3 2 4 3" xfId="214" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
+    <cellStyle name="Normal 6 2 3 2 5" xfId="290" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
+    <cellStyle name="Normal 6 2 3 2 6" xfId="291" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
+    <cellStyle name="Normal 6 2 3 3" xfId="13" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
+    <cellStyle name="Normal 6 2 3 3 2" xfId="84" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
+    <cellStyle name="Normal 6 2 3 3 2 2" xfId="543" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
+    <cellStyle name="Normal 6 2 3 3 2 3" xfId="542" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
+    <cellStyle name="Normal 6 2 3 3 3" xfId="83" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
+    <cellStyle name="Normal 6 2 3 3 4" xfId="82" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
+    <cellStyle name="Normal 6 2 3 4" xfId="14" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
+    <cellStyle name="Normal 6 2 3 4 2" xfId="216" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
+    <cellStyle name="Normal 6 2 3 4 2 2" xfId="660" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
+    <cellStyle name="Normal 6 2 3 4 2 3" xfId="661" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
+    <cellStyle name="Normal 6 2 3 4 3" xfId="55" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
+    <cellStyle name="Normal 6 2 3 4 4" xfId="223" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
+    <cellStyle name="Normal 6 2 3 5" xfId="15" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
+    <cellStyle name="Normal 6 2 3 5 2" xfId="506" xr:uid="{00000000-0005-0000-0000-0000A8000000}"/>
+    <cellStyle name="Normal 6 2 3 5 3" xfId="505" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
+    <cellStyle name="Normal 6 2 3 6" xfId="69" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
+    <cellStyle name="Normal 6 2 3 7" xfId="72" xr:uid="{00000000-0005-0000-0000-0000AB000000}"/>
+    <cellStyle name="Normal 6 2 4" xfId="331" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
+    <cellStyle name="Normal 6 2 4 2" xfId="400" xr:uid="{00000000-0005-0000-0000-0000AD000000}"/>
+    <cellStyle name="Normal 6 2 4 2 2" xfId="256" xr:uid="{00000000-0005-0000-0000-0000AE000000}"/>
+    <cellStyle name="Normal 6 2 4 2 2 2" xfId="274" xr:uid="{00000000-0005-0000-0000-0000AF000000}"/>
+    <cellStyle name="Normal 6 2 4 2 2 3" xfId="270" xr:uid="{00000000-0005-0000-0000-0000B0000000}"/>
+    <cellStyle name="Normal 6 2 4 2 3" xfId="255" xr:uid="{00000000-0005-0000-0000-0000B1000000}"/>
+    <cellStyle name="Normal 6 2 4 2 4" xfId="257" xr:uid="{00000000-0005-0000-0000-0000B2000000}"/>
+    <cellStyle name="Normal 6 2 4 3" xfId="399" xr:uid="{00000000-0005-0000-0000-0000B3000000}"/>
+    <cellStyle name="Normal 6 2 4 3 2" xfId="458" xr:uid="{00000000-0005-0000-0000-0000B4000000}"/>
+    <cellStyle name="Normal 6 2 4 3 2 2" xfId="150" xr:uid="{00000000-0005-0000-0000-0000B5000000}"/>
+    <cellStyle name="Normal 6 2 4 3 2 3" xfId="151" xr:uid="{00000000-0005-0000-0000-0000B6000000}"/>
+    <cellStyle name="Normal 6 2 4 3 3" xfId="459" xr:uid="{00000000-0005-0000-0000-0000B7000000}"/>
+    <cellStyle name="Normal 6 2 4 3 4" xfId="463" xr:uid="{00000000-0005-0000-0000-0000B8000000}"/>
+    <cellStyle name="Normal 6 2 4 4" xfId="398" xr:uid="{00000000-0005-0000-0000-0000B9000000}"/>
+    <cellStyle name="Normal 6 2 4 4 2" xfId="522" xr:uid="{00000000-0005-0000-0000-0000BA000000}"/>
+    <cellStyle name="Normal 6 2 4 4 3" xfId="521" xr:uid="{00000000-0005-0000-0000-0000BB000000}"/>
+    <cellStyle name="Normal 6 2 4 5" xfId="397" xr:uid="{00000000-0005-0000-0000-0000BC000000}"/>
+    <cellStyle name="Normal 6 2 4 6" xfId="396" xr:uid="{00000000-0005-0000-0000-0000BD000000}"/>
+    <cellStyle name="Normal 6 2 5" xfId="330" xr:uid="{00000000-0005-0000-0000-0000BE000000}"/>
+    <cellStyle name="Normal 6 2 5 2" xfId="569" xr:uid="{00000000-0005-0000-0000-0000BF000000}"/>
+    <cellStyle name="Normal 6 2 5 2 2" xfId="376" xr:uid="{00000000-0005-0000-0000-0000C0000000}"/>
+    <cellStyle name="Normal 6 2 5 2 3" xfId="377" xr:uid="{00000000-0005-0000-0000-0000C1000000}"/>
+    <cellStyle name="Normal 6 2 5 3" xfId="570" xr:uid="{00000000-0005-0000-0000-0000C2000000}"/>
+    <cellStyle name="Normal 6 2 5 4" xfId="568" xr:uid="{00000000-0005-0000-0000-0000C3000000}"/>
+    <cellStyle name="Normal 6 2 6" xfId="333" xr:uid="{00000000-0005-0000-0000-0000C4000000}"/>
+    <cellStyle name="Normal 6 2 6 2" xfId="632" xr:uid="{00000000-0005-0000-0000-0000C5000000}"/>
+    <cellStyle name="Normal 6 2 6 2 2" xfId="175" xr:uid="{00000000-0005-0000-0000-0000C6000000}"/>
+    <cellStyle name="Normal 6 2 6 2 3" xfId="174" xr:uid="{00000000-0005-0000-0000-0000C7000000}"/>
+    <cellStyle name="Normal 6 2 6 3" xfId="631" xr:uid="{00000000-0005-0000-0000-0000C8000000}"/>
+    <cellStyle name="Normal 6 2 6 4" xfId="630" xr:uid="{00000000-0005-0000-0000-0000C9000000}"/>
+    <cellStyle name="Normal 6 2 7" xfId="332" xr:uid="{00000000-0005-0000-0000-0000CA000000}"/>
+    <cellStyle name="Normal 6 2 7 2" xfId="195" xr:uid="{00000000-0005-0000-0000-0000CB000000}"/>
+    <cellStyle name="Normal 6 2 7 2 2" xfId="635" xr:uid="{00000000-0005-0000-0000-0000CC000000}"/>
+    <cellStyle name="Normal 6 2 7 2 3" xfId="636" xr:uid="{00000000-0005-0000-0000-0000CD000000}"/>
+    <cellStyle name="Normal 6 2 7 3" xfId="196" xr:uid="{00000000-0005-0000-0000-0000CE000000}"/>
+    <cellStyle name="Normal 6 2 7 4" xfId="427" xr:uid="{00000000-0005-0000-0000-0000CF000000}"/>
+    <cellStyle name="Normal 6 2 8" xfId="335" xr:uid="{00000000-0005-0000-0000-0000D0000000}"/>
+    <cellStyle name="Normal 6 2 8 2" xfId="474" xr:uid="{00000000-0005-0000-0000-0000D1000000}"/>
+    <cellStyle name="Normal 6 2 8 2 2" xfId="524" xr:uid="{00000000-0005-0000-0000-0000D2000000}"/>
+    <cellStyle name="Normal 6 2 8 2 3" xfId="523" xr:uid="{00000000-0005-0000-0000-0000D3000000}"/>
+    <cellStyle name="Normal 6 2 8 3" xfId="473" xr:uid="{00000000-0005-0000-0000-0000D4000000}"/>
+    <cellStyle name="Normal 6 2 8 4" xfId="479" xr:uid="{00000000-0005-0000-0000-0000D5000000}"/>
+    <cellStyle name="Normal 6 2 9" xfId="334" xr:uid="{00000000-0005-0000-0000-0000D6000000}"/>
+    <cellStyle name="Normal 6 2 9 2" xfId="26" xr:uid="{00000000-0005-0000-0000-0000D7000000}"/>
+    <cellStyle name="Normal 6 2 9 3" xfId="98" xr:uid="{00000000-0005-0000-0000-0000D8000000}"/>
+    <cellStyle name="Normal 6 3" xfId="314" xr:uid="{00000000-0005-0000-0000-0000D9000000}"/>
+    <cellStyle name="Normal 6 3 10" xfId="183" xr:uid="{00000000-0005-0000-0000-0000DA000000}"/>
+    <cellStyle name="Normal 6 3 2" xfId="548" xr:uid="{00000000-0005-0000-0000-0000DB000000}"/>
+    <cellStyle name="Normal 6 3 2 2" xfId="207" xr:uid="{00000000-0005-0000-0000-0000DC000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2" xfId="237" xr:uid="{00000000-0005-0000-0000-0000DD000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2 2" xfId="50" xr:uid="{00000000-0005-0000-0000-0000DE000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2 2 2" xfId="89" xr:uid="{00000000-0005-0000-0000-0000DF000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2 2 3" xfId="90" xr:uid="{00000000-0005-0000-0000-0000E0000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2 3" xfId="51" xr:uid="{00000000-0005-0000-0000-0000E1000000}"/>
+    <cellStyle name="Normal 6 3 2 2 2 4" xfId="48" xr:uid="{00000000-0005-0000-0000-0000E2000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3" xfId="238" xr:uid="{00000000-0005-0000-0000-0000E3000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3 2" xfId="499" xr:uid="{00000000-0005-0000-0000-0000E4000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3 2 2" xfId="288" xr:uid="{00000000-0005-0000-0000-0000E5000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3 2 3" xfId="287" xr:uid="{00000000-0005-0000-0000-0000E6000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3 3" xfId="498" xr:uid="{00000000-0005-0000-0000-0000E7000000}"/>
+    <cellStyle name="Normal 6 3 2 2 3 4" xfId="495" xr:uid="{00000000-0005-0000-0000-0000E8000000}"/>
+    <cellStyle name="Normal 6 3 2 2 4" xfId="234" xr:uid="{00000000-0005-0000-0000-0000E9000000}"/>
+    <cellStyle name="Normal 6 3 2 2 4 2" xfId="612" xr:uid="{00000000-0005-0000-0000-0000EA000000}"/>
+    <cellStyle name="Normal 6 3 2 2 4 3" xfId="613" xr:uid="{00000000-0005-0000-0000-0000EB000000}"/>
+    <cellStyle name="Normal 6 3 2 2 5" xfId="235" xr:uid="{00000000-0005-0000-0000-0000EC000000}"/>
+    <cellStyle name="Normal 6 3 2 2 6" xfId="236" xr:uid="{00000000-0005-0000-0000-0000ED000000}"/>
+    <cellStyle name="Normal 6 3 2 3" xfId="208" xr:uid="{00000000-0005-0000-0000-0000EE000000}"/>
+    <cellStyle name="Normal 6 3 2 3 2" xfId="37" xr:uid="{00000000-0005-0000-0000-0000EF000000}"/>
+    <cellStyle name="Normal 6 3 2 3 2 2" xfId="394" xr:uid="{00000000-0005-0000-0000-0000F0000000}"/>
+    <cellStyle name="Normal 6 3 2 3 2 3" xfId="393" xr:uid="{00000000-0005-0000-0000-0000F1000000}"/>
+    <cellStyle name="Normal 6 3 2 3 3" xfId="36" xr:uid="{00000000-0005-0000-0000-0000F2000000}"/>
+    <cellStyle name="Normal 6 3 2 3 4" xfId="35" xr:uid="{00000000-0005-0000-0000-0000F3000000}"/>
+    <cellStyle name="Normal 6 3 2 4" xfId="209" xr:uid="{00000000-0005-0000-0000-0000F4000000}"/>
+    <cellStyle name="Normal 6 3 2 4 2" xfId="627" xr:uid="{00000000-0005-0000-0000-0000F5000000}"/>
+    <cellStyle name="Normal 6 3 2 4 2 2" xfId="486" xr:uid="{00000000-0005-0000-0000-0000F6000000}"/>
+    <cellStyle name="Normal 6 3 2 4 2 3" xfId="487" xr:uid="{00000000-0005-0000-0000-0000F7000000}"/>
+    <cellStyle name="Normal 6 3 2 4 3" xfId="628" xr:uid="{00000000-0005-0000-0000-0000F8000000}"/>
+    <cellStyle name="Normal 6 3 2 4 4" xfId="629" xr:uid="{00000000-0005-0000-0000-0000F9000000}"/>
+    <cellStyle name="Normal 6 3 2 5" xfId="210" xr:uid="{00000000-0005-0000-0000-0000FA000000}"/>
+    <cellStyle name="Normal 6 3 2 5 2" xfId="431" xr:uid="{00000000-0005-0000-0000-0000FB000000}"/>
+    <cellStyle name="Normal 6 3 2 5 3" xfId="430" xr:uid="{00000000-0005-0000-0000-0000FC000000}"/>
+    <cellStyle name="Normal 6 3 2 6" xfId="211" xr:uid="{00000000-0005-0000-0000-0000FD000000}"/>
+    <cellStyle name="Normal 6 3 2 7" xfId="212" xr:uid="{00000000-0005-0000-0000-0000FE000000}"/>
+    <cellStyle name="Normal 6 3 3" xfId="549" xr:uid="{00000000-0005-0000-0000-0000FF000000}"/>
+    <cellStyle name="Normal 6 3 3 2" xfId="645" xr:uid="{00000000-0005-0000-0000-000000010000}"/>
+    <cellStyle name="Normal 6 3 3 2 2" xfId="558" xr:uid="{00000000-0005-0000-0000-000001010000}"/>
+    <cellStyle name="Normal 6 3 3 2 2 2" xfId="190" xr:uid="{00000000-0005-0000-0000-000002010000}"/>
+    <cellStyle name="Normal 6 3 3 2 2 3" xfId="189" xr:uid="{00000000-0005-0000-0000-000003010000}"/>
+    <cellStyle name="Normal 6 3 3 2 3" xfId="557" xr:uid="{00000000-0005-0000-0000-000004010000}"/>
+    <cellStyle name="Normal 6 3 3 2 4" xfId="556" xr:uid="{00000000-0005-0000-0000-000005010000}"/>
+    <cellStyle name="Normal 6 3 3 3" xfId="644" xr:uid="{00000000-0005-0000-0000-000006010000}"/>
+    <cellStyle name="Normal 6 3 3 3 2" xfId="114" xr:uid="{00000000-0005-0000-0000-000007010000}"/>
+    <cellStyle name="Normal 6 3 3 3 2 2" xfId="653" xr:uid="{00000000-0005-0000-0000-000008010000}"/>
+    <cellStyle name="Normal 6 3 3 3 2 3" xfId="654" xr:uid="{00000000-0005-0000-0000-000009010000}"/>
+    <cellStyle name="Normal 6 3 3 3 3" xfId="115" xr:uid="{00000000-0005-0000-0000-00000A010000}"/>
+    <cellStyle name="Normal 6 3 3 3 4" xfId="112" xr:uid="{00000000-0005-0000-0000-00000B010000}"/>
+    <cellStyle name="Normal 6 3 3 4" xfId="647" xr:uid="{00000000-0005-0000-0000-00000C010000}"/>
+    <cellStyle name="Normal 6 3 3 4 2" xfId="317" xr:uid="{00000000-0005-0000-0000-00000D010000}"/>
+    <cellStyle name="Normal 6 3 3 4 3" xfId="316" xr:uid="{00000000-0005-0000-0000-00000E010000}"/>
+    <cellStyle name="Normal 6 3 3 5" xfId="646" xr:uid="{00000000-0005-0000-0000-00000F010000}"/>
+    <cellStyle name="Normal 6 3 3 6" xfId="648" xr:uid="{00000000-0005-0000-0000-000010010000}"/>
+    <cellStyle name="Normal 6 3 4" xfId="550" xr:uid="{00000000-0005-0000-0000-000011010000}"/>
+    <cellStyle name="Normal 6 3 4 2" xfId="160" xr:uid="{00000000-0005-0000-0000-000012010000}"/>
+    <cellStyle name="Normal 6 3 4 2 2" xfId="470" xr:uid="{00000000-0005-0000-0000-000013010000}"/>
+    <cellStyle name="Normal 6 3 4 2 3" xfId="471" xr:uid="{00000000-0005-0000-0000-000014010000}"/>
+    <cellStyle name="Normal 6 3 4 3" xfId="164" xr:uid="{00000000-0005-0000-0000-000015010000}"/>
+    <cellStyle name="Normal 6 3 4 4" xfId="155" xr:uid="{00000000-0005-0000-0000-000016010000}"/>
+    <cellStyle name="Normal 6 3 5" xfId="551" xr:uid="{00000000-0005-0000-0000-000017010000}"/>
+    <cellStyle name="Normal 6 3 5 2" xfId="493" xr:uid="{00000000-0005-0000-0000-000018010000}"/>
+    <cellStyle name="Normal 6 3 5 2 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000019010000}"/>
+    <cellStyle name="Normal 6 3 5 2 3" xfId="52" xr:uid="{00000000-0005-0000-0000-00001A010000}"/>
+    <cellStyle name="Normal 6 3 5 3" xfId="492" xr:uid="{00000000-0005-0000-0000-00001B010000}"/>
+    <cellStyle name="Normal 6 3 5 4" xfId="491" xr:uid="{00000000-0005-0000-0000-00001C010000}"/>
+    <cellStyle name="Normal 6 3 6" xfId="552" xr:uid="{00000000-0005-0000-0000-00001D010000}"/>
+    <cellStyle name="Normal 6 3 6 2" xfId="323" xr:uid="{00000000-0005-0000-0000-00001E010000}"/>
+    <cellStyle name="Normal 6 3 6 2 2" xfId="153" xr:uid="{00000000-0005-0000-0000-00001F010000}"/>
+    <cellStyle name="Normal 6 3 6 2 3" xfId="154" xr:uid="{00000000-0005-0000-0000-000020010000}"/>
+    <cellStyle name="Normal 6 3 6 3" xfId="324" xr:uid="{00000000-0005-0000-0000-000021010000}"/>
+    <cellStyle name="Normal 6 3 6 4" xfId="322" xr:uid="{00000000-0005-0000-0000-000022010000}"/>
+    <cellStyle name="Normal 6 3 7" xfId="553" xr:uid="{00000000-0005-0000-0000-000023010000}"/>
+    <cellStyle name="Normal 6 3 7 2" xfId="111" xr:uid="{00000000-0005-0000-0000-000024010000}"/>
+    <cellStyle name="Normal 6 3 7 2 2" xfId="347" xr:uid="{00000000-0005-0000-0000-000025010000}"/>
+    <cellStyle name="Normal 6 3 7 2 3" xfId="346" xr:uid="{00000000-0005-0000-0000-000026010000}"/>
+    <cellStyle name="Normal 6 3 7 3" xfId="110" xr:uid="{00000000-0005-0000-0000-000027010000}"/>
+    <cellStyle name="Normal 6 3 7 4" xfId="109" xr:uid="{00000000-0005-0000-0000-000028010000}"/>
+    <cellStyle name="Normal 6 3 8" xfId="501" xr:uid="{00000000-0005-0000-0000-000029010000}"/>
+    <cellStyle name="Normal 6 3 8 2" xfId="305" xr:uid="{00000000-0005-0000-0000-00002A010000}"/>
+    <cellStyle name="Normal 6 3 8 3" xfId="306" xr:uid="{00000000-0005-0000-0000-00002B010000}"/>
+    <cellStyle name="Normal 6 3 9" xfId="502" xr:uid="{00000000-0005-0000-0000-00002C010000}"/>
+    <cellStyle name="Normal 6 4" xfId="311" xr:uid="{00000000-0005-0000-0000-00002D010000}"/>
+    <cellStyle name="Normal 6 4 10" xfId="100" xr:uid="{00000000-0005-0000-0000-00002E010000}"/>
+    <cellStyle name="Normal 6 4 2" xfId="92" xr:uid="{00000000-0005-0000-0000-00002F010000}"/>
+    <cellStyle name="Normal 6 4 2 2" xfId="140" xr:uid="{00000000-0005-0000-0000-000030010000}"/>
+    <cellStyle name="Normal 6 4 2 2 2" xfId="375" xr:uid="{00000000-0005-0000-0000-000031010000}"/>
+    <cellStyle name="Normal 6 4 2 2 2 2" xfId="267" xr:uid="{00000000-0005-0000-0000-000032010000}"/>
+    <cellStyle name="Normal 6 4 2 2 2 2 2" xfId="382" xr:uid="{00000000-0005-0000-0000-000033010000}"/>
+    <cellStyle name="Normal 6 4 2 2 2 2 3" xfId="381" xr:uid="{00000000-0005-0000-0000-000034010000}"/>
+    <cellStyle name="Normal 6 4 2 2 2 3" xfId="266" xr:uid="{00000000-0005-0000-0000-000035010000}"/>
+    <cellStyle name="Normal 6 4 2 2 2 4" xfId="268" xr:uid="{00000000-0005-0000-0000-000036010000}"/>
+    <cellStyle name="Normal 6 4 2 2 3" xfId="395" xr:uid="{00000000-0005-0000-0000-000037010000}"/>
+    <cellStyle name="Normal 6 4 2 2 3 2" xfId="480" xr:uid="{00000000-0005-0000-0000-000038010000}"/>
+    <cellStyle name="Normal 6 4 2 2 3 2 2" xfId="187" xr:uid="{00000000-0005-0000-0000-000039010000}"/>
+    <cellStyle name="Normal 6 4 2 2 3 2 3" xfId="188" xr:uid="{00000000-0005-0000-0000-00003A010000}"/>
+    <cellStyle name="Normal 6 4 2 2 3 3" xfId="481" xr:uid="{00000000-0005-0000-0000-00003B010000}"/>
+    <cellStyle name="Normal 6 4 2 2 3 4" xfId="484" xr:uid="{00000000-0005-0000-0000-00003C010000}"/>
+    <cellStyle name="Normal 6 4 2 2 4" xfId="402" xr:uid="{00000000-0005-0000-0000-00003D010000}"/>
+    <cellStyle name="Normal 6 4 2 2 4 2" xfId="429" xr:uid="{00000000-0005-0000-0000-00003E010000}"/>
+    <cellStyle name="Normal 6 4 2 2 4 3" xfId="428" xr:uid="{00000000-0005-0000-0000-00003F010000}"/>
+    <cellStyle name="Normal 6 4 2 2 5" xfId="401" xr:uid="{00000000-0005-0000-0000-000040010000}"/>
+    <cellStyle name="Normal 6 4 2 2 6" xfId="379" xr:uid="{00000000-0005-0000-0000-000041010000}"/>
+    <cellStyle name="Normal 6 4 2 3" xfId="139" xr:uid="{00000000-0005-0000-0000-000042010000}"/>
+    <cellStyle name="Normal 6 4 2 3 2" xfId="587" xr:uid="{00000000-0005-0000-0000-000043010000}"/>
+    <cellStyle name="Normal 6 4 2 3 2 2" xfId="655" xr:uid="{00000000-0005-0000-0000-000044010000}"/>
+    <cellStyle name="Normal 6 4 2 3 2 3" xfId="656" xr:uid="{00000000-0005-0000-0000-000045010000}"/>
+    <cellStyle name="Normal 6 4 2 3 3" xfId="588" xr:uid="{00000000-0005-0000-0000-000046010000}"/>
+    <cellStyle name="Normal 6 4 2 3 4" xfId="591" xr:uid="{00000000-0005-0000-0000-000047010000}"/>
+    <cellStyle name="Normal 6 4 2 4" xfId="138" xr:uid="{00000000-0005-0000-0000-000048010000}"/>
+    <cellStyle name="Normal 6 4 2 4 2" xfId="623" xr:uid="{00000000-0005-0000-0000-000049010000}"/>
+    <cellStyle name="Normal 6 4 2 4 2 2" xfId="605" xr:uid="{00000000-0005-0000-0000-00004A010000}"/>
+    <cellStyle name="Normal 6 4 2 4 2 3" xfId="604" xr:uid="{00000000-0005-0000-0000-00004B010000}"/>
+    <cellStyle name="Normal 6 4 2 4 3" xfId="622" xr:uid="{00000000-0005-0000-0000-00004C010000}"/>
+    <cellStyle name="Normal 6 4 2 4 4" xfId="621" xr:uid="{00000000-0005-0000-0000-00004D010000}"/>
+    <cellStyle name="Normal 6 4 2 5" xfId="137" xr:uid="{00000000-0005-0000-0000-00004E010000}"/>
+    <cellStyle name="Normal 6 4 2 5 2" xfId="184" xr:uid="{00000000-0005-0000-0000-00004F010000}"/>
+    <cellStyle name="Normal 6 4 2 5 3" xfId="185" xr:uid="{00000000-0005-0000-0000-000050010000}"/>
+    <cellStyle name="Normal 6 4 2 6" xfId="136" xr:uid="{00000000-0005-0000-0000-000051010000}"/>
+    <cellStyle name="Normal 6 4 2 7" xfId="135" xr:uid="{00000000-0005-0000-0000-000052010000}"/>
+    <cellStyle name="Normal 6 4 3" xfId="91" xr:uid="{00000000-0005-0000-0000-000053010000}"/>
+    <cellStyle name="Normal 6 4 3 2" xfId="342" xr:uid="{00000000-0005-0000-0000-000054010000}"/>
+    <cellStyle name="Normal 6 4 3 2 2" xfId="200" xr:uid="{00000000-0005-0000-0000-000055010000}"/>
+    <cellStyle name="Normal 6 4 3 2 2 2" xfId="127" xr:uid="{00000000-0005-0000-0000-000056010000}"/>
+    <cellStyle name="Normal 6 4 3 2 2 3" xfId="128" xr:uid="{00000000-0005-0000-0000-000057010000}"/>
+    <cellStyle name="Normal 6 4 3 2 3" xfId="201" xr:uid="{00000000-0005-0000-0000-000058010000}"/>
+    <cellStyle name="Normal 6 4 3 2 4" xfId="204" xr:uid="{00000000-0005-0000-0000-000059010000}"/>
+    <cellStyle name="Normal 6 4 3 3" xfId="343" xr:uid="{00000000-0005-0000-0000-00005A010000}"/>
+    <cellStyle name="Normal 6 4 3 3 2" xfId="643" xr:uid="{00000000-0005-0000-0000-00005B010000}"/>
+    <cellStyle name="Normal 6 4 3 3 2 2" xfId="298" xr:uid="{00000000-0005-0000-0000-00005C010000}"/>
+    <cellStyle name="Normal 6 4 3 3 2 3" xfId="297" xr:uid="{00000000-0005-0000-0000-00005D010000}"/>
+    <cellStyle name="Normal 6 4 3 3 3" xfId="642" xr:uid="{00000000-0005-0000-0000-00005E010000}"/>
+    <cellStyle name="Normal 6 4 3 3 4" xfId="583" xr:uid="{00000000-0005-0000-0000-00005F010000}"/>
+    <cellStyle name="Normal 6 4 3 4" xfId="340" xr:uid="{00000000-0005-0000-0000-000060010000}"/>
+    <cellStyle name="Normal 6 4 3 4 2" xfId="444" xr:uid="{00000000-0005-0000-0000-000061010000}"/>
+    <cellStyle name="Normal 6 4 3 4 3" xfId="445" xr:uid="{00000000-0005-0000-0000-000062010000}"/>
+    <cellStyle name="Normal 6 4 3 5" xfId="341" xr:uid="{00000000-0005-0000-0000-000063010000}"/>
+    <cellStyle name="Normal 6 4 3 6" xfId="339" xr:uid="{00000000-0005-0000-0000-000064010000}"/>
+    <cellStyle name="Normal 6 4 4" xfId="441" xr:uid="{00000000-0005-0000-0000-000065010000}"/>
+    <cellStyle name="Normal 6 4 4 2" xfId="292" xr:uid="{00000000-0005-0000-0000-000066010000}"/>
+    <cellStyle name="Normal 6 4 4 2 2" xfId="247" xr:uid="{00000000-0005-0000-0000-000067010000}"/>
+    <cellStyle name="Normal 6 4 4 2 3" xfId="246" xr:uid="{00000000-0005-0000-0000-000068010000}"/>
+    <cellStyle name="Normal 6 4 4 3" xfId="412" xr:uid="{00000000-0005-0000-0000-000069010000}"/>
+    <cellStyle name="Normal 6 4 4 4" xfId="293" xr:uid="{00000000-0005-0000-0000-00006A010000}"/>
+    <cellStyle name="Normal 6 4 5" xfId="440" xr:uid="{00000000-0005-0000-0000-00006B010000}"/>
+    <cellStyle name="Normal 6 4 5 2" xfId="460" xr:uid="{00000000-0005-0000-0000-00006C010000}"/>
+    <cellStyle name="Normal 6 4 5 2 2" xfId="517" xr:uid="{00000000-0005-0000-0000-00006D010000}"/>
+    <cellStyle name="Normal 6 4 5 2 3" xfId="520" xr:uid="{00000000-0005-0000-0000-00006E010000}"/>
+    <cellStyle name="Normal 6 4 5 3" xfId="461" xr:uid="{00000000-0005-0000-0000-00006F010000}"/>
+    <cellStyle name="Normal 6 4 5 4" xfId="462" xr:uid="{00000000-0005-0000-0000-000070010000}"/>
+    <cellStyle name="Normal 6 4 6" xfId="88" xr:uid="{00000000-0005-0000-0000-000071010000}"/>
+    <cellStyle name="Normal 6 4 6 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000072010000}"/>
+    <cellStyle name="Normal 6 4 6 2 2" xfId="595" xr:uid="{00000000-0005-0000-0000-000073010000}"/>
+    <cellStyle name="Normal 6 4 6 2 3" xfId="594" xr:uid="{00000000-0005-0000-0000-000074010000}"/>
+    <cellStyle name="Normal 6 4 6 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000075010000}"/>
+    <cellStyle name="Normal 6 4 6 4" xfId="10" xr:uid="{00000000-0005-0000-0000-000076010000}"/>
+    <cellStyle name="Normal 6 4 7" xfId="87" xr:uid="{00000000-0005-0000-0000-000077010000}"/>
+    <cellStyle name="Normal 6 4 7 2" xfId="221" xr:uid="{00000000-0005-0000-0000-000078010000}"/>
+    <cellStyle name="Normal 6 4 7 2 2" xfId="403" xr:uid="{00000000-0005-0000-0000-000079010000}"/>
+    <cellStyle name="Normal 6 4 7 2 3" xfId="404" xr:uid="{00000000-0005-0000-0000-00007A010000}"/>
+    <cellStyle name="Normal 6 4 7 3" xfId="222" xr:uid="{00000000-0005-0000-0000-00007B010000}"/>
+    <cellStyle name="Normal 6 4 7 4" xfId="224" xr:uid="{00000000-0005-0000-0000-00007C010000}"/>
+    <cellStyle name="Normal 6 4 8" xfId="97" xr:uid="{00000000-0005-0000-0000-00007D010000}"/>
+    <cellStyle name="Normal 6 4 8 2" xfId="95" xr:uid="{00000000-0005-0000-0000-00007E010000}"/>
+    <cellStyle name="Normal 6 4 8 3" xfId="380" xr:uid="{00000000-0005-0000-0000-00007F010000}"/>
+    <cellStyle name="Normal 6 4 9" xfId="96" xr:uid="{00000000-0005-0000-0000-000080010000}"/>
+    <cellStyle name="Normal 6 5" xfId="310" xr:uid="{00000000-0005-0000-0000-000081010000}"/>
+    <cellStyle name="Normal 6 5 2" xfId="285" xr:uid="{00000000-0005-0000-0000-000082010000}"/>
+    <cellStyle name="Normal 6 5 2 2" xfId="534" xr:uid="{00000000-0005-0000-0000-000083010000}"/>
+    <cellStyle name="Normal 6 5 2 2 2" xfId="182" xr:uid="{00000000-0005-0000-0000-000084010000}"/>
+    <cellStyle name="Normal 6 5 2 2 2 2" xfId="258" xr:uid="{00000000-0005-0000-0000-000085010000}"/>
+    <cellStyle name="Normal 6 5 2 2 2 2 2" xfId="546" xr:uid="{00000000-0005-0000-0000-000086010000}"/>
+    <cellStyle name="Normal 6 5 2 2 2 2 3" xfId="547" xr:uid="{00000000-0005-0000-0000-000087010000}"/>
+    <cellStyle name="Normal 6 5 2 2 2 3" xfId="259" xr:uid="{00000000-0005-0000-0000-000088010000}"/>
+    <cellStyle name="Normal 6 5 2 2 2 4" xfId="261" xr:uid="{00000000-0005-0000-0000-000089010000}"/>
+    <cellStyle name="Normal 6 5 2 2 3" xfId="417" xr:uid="{00000000-0005-0000-0000-00008A010000}"/>
+    <cellStyle name="Normal 6 5 2 2 3 2" xfId="302" xr:uid="{00000000-0005-0000-0000-00008B010000}"/>
+    <cellStyle name="Normal 6 5 2 2 3 2 2" xfId="107" xr:uid="{00000000-0005-0000-0000-00008C010000}"/>
+    <cellStyle name="Normal 6 5 2 2 3 2 3" xfId="106" xr:uid="{00000000-0005-0000-0000-00008D010000}"/>
+    <cellStyle name="Normal 6 5 2 2 3 3" xfId="301" xr:uid="{00000000-0005-0000-0000-00008E010000}"/>
+    <cellStyle name="Normal 6 5 2 2 3 4" xfId="79" xr:uid="{00000000-0005-0000-0000-00008F010000}"/>
+    <cellStyle name="Normal 6 5 2 2 4" xfId="253" xr:uid="{00000000-0005-0000-0000-000090010000}"/>
+    <cellStyle name="Normal 6 5 2 2 4 2" xfId="419" xr:uid="{00000000-0005-0000-0000-000091010000}"/>
+    <cellStyle name="Normal 6 5 2 2 4 3" xfId="420" xr:uid="{00000000-0005-0000-0000-000092010000}"/>
+    <cellStyle name="Normal 6 5 2 2 5" xfId="254" xr:uid="{00000000-0005-0000-0000-000093010000}"/>
+    <cellStyle name="Normal 6 5 2 2 6" xfId="192" xr:uid="{00000000-0005-0000-0000-000094010000}"/>
+    <cellStyle name="Normal 6 5 2 3" xfId="535" xr:uid="{00000000-0005-0000-0000-000095010000}"/>
+    <cellStyle name="Normal 6 5 2 3 2" xfId="649" xr:uid="{00000000-0005-0000-0000-000096010000}"/>
+    <cellStyle name="Normal 6 5 2 3 2 2" xfId="370" xr:uid="{00000000-0005-0000-0000-000097010000}"/>
+    <cellStyle name="Normal 6 5 2 3 2 3" xfId="369" xr:uid="{00000000-0005-0000-0000-000098010000}"/>
+    <cellStyle name="Normal 6 5 2 3 3" xfId="70" xr:uid="{00000000-0005-0000-0000-000099010000}"/>
+    <cellStyle name="Normal 6 5 2 3 4" xfId="276" xr:uid="{00000000-0005-0000-0000-00009A010000}"/>
+    <cellStyle name="Normal 6 5 2 4" xfId="532" xr:uid="{00000000-0005-0000-0000-00009B010000}"/>
+    <cellStyle name="Normal 6 5 2 4 2" xfId="518" xr:uid="{00000000-0005-0000-0000-00009C010000}"/>
+    <cellStyle name="Normal 6 5 2 4 2 2" xfId="633" xr:uid="{00000000-0005-0000-0000-00009D010000}"/>
+    <cellStyle name="Normal 6 5 2 4 2 3" xfId="634" xr:uid="{00000000-0005-0000-0000-00009E010000}"/>
+    <cellStyle name="Normal 6 5 2 4 3" xfId="519" xr:uid="{00000000-0005-0000-0000-00009F010000}"/>
+    <cellStyle name="Normal 6 5 2 4 4" xfId="514" xr:uid="{00000000-0005-0000-0000-0000A0010000}"/>
+    <cellStyle name="Normal 6 5 2 5" xfId="447" xr:uid="{00000000-0005-0000-0000-0000A1010000}"/>
+    <cellStyle name="Normal 6 5 2 5 2" xfId="304" xr:uid="{00000000-0005-0000-0000-0000A2010000}"/>
+    <cellStyle name="Normal 6 5 2 5 3" xfId="303" xr:uid="{00000000-0005-0000-0000-0000A3010000}"/>
+    <cellStyle name="Normal 6 5 2 6" xfId="530" xr:uid="{00000000-0005-0000-0000-0000A4010000}"/>
+    <cellStyle name="Normal 6 5 2 7" xfId="531" xr:uid="{00000000-0005-0000-0000-0000A5010000}"/>
+    <cellStyle name="Normal 6 5 3" xfId="286" xr:uid="{00000000-0005-0000-0000-0000A6010000}"/>
+    <cellStyle name="Normal 6 5 3 2" xfId="321" xr:uid="{00000000-0005-0000-0000-0000A7010000}"/>
+    <cellStyle name="Normal 6 5 3 2 2" xfId="134" xr:uid="{00000000-0005-0000-0000-0000A8010000}"/>
+    <cellStyle name="Normal 6 5 3 2 2 2" xfId="600" xr:uid="{00000000-0005-0000-0000-0000A9010000}"/>
+    <cellStyle name="Normal 6 5 3 2 2 3" xfId="599" xr:uid="{00000000-0005-0000-0000-0000AA010000}"/>
+    <cellStyle name="Normal 6 5 3 2 3" xfId="229" xr:uid="{00000000-0005-0000-0000-0000AB010000}"/>
+    <cellStyle name="Normal 6 5 3 2 4" xfId="472" xr:uid="{00000000-0005-0000-0000-0000AC010000}"/>
+    <cellStyle name="Normal 6 5 3 3" xfId="320" xr:uid="{00000000-0005-0000-0000-0000AD010000}"/>
+    <cellStyle name="Normal 6 5 3 3 2" xfId="32" xr:uid="{00000000-0005-0000-0000-0000AE010000}"/>
+    <cellStyle name="Normal 6 5 3 3 2 2" xfId="423" xr:uid="{00000000-0005-0000-0000-0000AF010000}"/>
+    <cellStyle name="Normal 6 5 3 3 2 3" xfId="424" xr:uid="{00000000-0005-0000-0000-0000B0010000}"/>
+    <cellStyle name="Normal 6 5 3 3 3" xfId="34" xr:uid="{00000000-0005-0000-0000-0000B1010000}"/>
+    <cellStyle name="Normal 6 5 3 3 4" xfId="9" xr:uid="{00000000-0005-0000-0000-0000B2010000}"/>
+    <cellStyle name="Normal 6 5 3 4" xfId="319" xr:uid="{00000000-0005-0000-0000-0000B3010000}"/>
+    <cellStyle name="Normal 6 5 3 4 2" xfId="94" xr:uid="{00000000-0005-0000-0000-0000B4010000}"/>
+    <cellStyle name="Normal 6 5 3 4 3" xfId="93" xr:uid="{00000000-0005-0000-0000-0000B5010000}"/>
+    <cellStyle name="Normal 6 5 3 5" xfId="318" xr:uid="{00000000-0005-0000-0000-0000B6010000}"/>
+    <cellStyle name="Normal 6 5 3 6" xfId="525" xr:uid="{00000000-0005-0000-0000-0000B7010000}"/>
+    <cellStyle name="Normal 6 5 4" xfId="283" xr:uid="{00000000-0005-0000-0000-0000B8010000}"/>
+    <cellStyle name="Normal 6 5 4 2" xfId="582" xr:uid="{00000000-0005-0000-0000-0000B9010000}"/>
+    <cellStyle name="Normal 6 5 4 2 2" xfId="478" xr:uid="{00000000-0005-0000-0000-0000BA010000}"/>
+    <cellStyle name="Normal 6 5 4 2 3" xfId="639" xr:uid="{00000000-0005-0000-0000-0000BB010000}"/>
+    <cellStyle name="Normal 6 5 4 3" xfId="197" xr:uid="{00000000-0005-0000-0000-0000BC010000}"/>
+    <cellStyle name="Normal 6 5 4 4" xfId="584" xr:uid="{00000000-0005-0000-0000-0000BD010000}"/>
+    <cellStyle name="Normal 6 5 5" xfId="284" xr:uid="{00000000-0005-0000-0000-0000BE010000}"/>
+    <cellStyle name="Normal 6 5 5 2" xfId="387" xr:uid="{00000000-0005-0000-0000-0000BF010000}"/>
+    <cellStyle name="Normal 6 5 5 2 2" xfId="119" xr:uid="{00000000-0005-0000-0000-0000C0010000}"/>
+    <cellStyle name="Normal 6 5 5 2 3" xfId="33" xr:uid="{00000000-0005-0000-0000-0000C1010000}"/>
+    <cellStyle name="Normal 6 5 5 3" xfId="386" xr:uid="{00000000-0005-0000-0000-0000C2010000}"/>
+    <cellStyle name="Normal 6 5 5 4" xfId="388" xr:uid="{00000000-0005-0000-0000-0000C3010000}"/>
+    <cellStyle name="Normal 6 5 6" xfId="281" xr:uid="{00000000-0005-0000-0000-0000C4010000}"/>
+    <cellStyle name="Normal 6 5 6 2" xfId="74" xr:uid="{00000000-0005-0000-0000-0000C5010000}"/>
+    <cellStyle name="Normal 6 5 6 3" xfId="356" xr:uid="{00000000-0005-0000-0000-0000C6010000}"/>
+    <cellStyle name="Normal 6 5 7" xfId="282" xr:uid="{00000000-0005-0000-0000-0000C7010000}"/>
+    <cellStyle name="Normal 6 5 8" xfId="280" xr:uid="{00000000-0005-0000-0000-0000C8010000}"/>
+    <cellStyle name="Normal 6 6" xfId="313" xr:uid="{00000000-0005-0000-0000-0000C9010000}"/>
+    <cellStyle name="Normal 6 6 2" xfId="326" xr:uid="{00000000-0005-0000-0000-0000CA010000}"/>
+    <cellStyle name="Normal 6 6 2 2" xfId="245" xr:uid="{00000000-0005-0000-0000-0000CB010000}"/>
+    <cellStyle name="Normal 6 6 2 2 2" xfId="64" xr:uid="{00000000-0005-0000-0000-0000CC010000}"/>
+    <cellStyle name="Normal 6 6 2 2 2 2" xfId="618" xr:uid="{00000000-0005-0000-0000-0000CD010000}"/>
+    <cellStyle name="Normal 6 6 2 2 2 2 2" xfId="39" xr:uid="{00000000-0005-0000-0000-0000CE010000}"/>
+    <cellStyle name="Normal 6 6 2 2 2 2 3" xfId="515" xr:uid="{00000000-0005-0000-0000-0000CF010000}"/>
+    <cellStyle name="Normal 6 6 2 2 2 3" xfId="617" xr:uid="{00000000-0005-0000-0000-0000D0010000}"/>
+    <cellStyle name="Normal 6 6 2 2 2 4" xfId="619" xr:uid="{00000000-0005-0000-0000-0000D1010000}"/>
+    <cellStyle name="Normal 6 6 2 2 3" xfId="113" xr:uid="{00000000-0005-0000-0000-0000D2010000}"/>
+    <cellStyle name="Normal 6 6 2 2 3 2" xfId="116" xr:uid="{00000000-0005-0000-0000-0000D3010000}"/>
+    <cellStyle name="Normal 6 6 2 2 3 2 2" xfId="456" xr:uid="{00000000-0005-0000-0000-0000D4010000}"/>
+    <cellStyle name="Normal 6 6 2 2 3 2 3" xfId="457" xr:uid="{00000000-0005-0000-0000-0000D5010000}"/>
+    <cellStyle name="Normal 6 6 2 2 3 3" xfId="296" xr:uid="{00000000-0005-0000-0000-0000D6010000}"/>
+    <cellStyle name="Normal 6 6 2 2 3 4" xfId="176" xr:uid="{00000000-0005-0000-0000-0000D7010000}"/>
+    <cellStyle name="Normal 6 6 2 2 4" xfId="80" xr:uid="{00000000-0005-0000-0000-0000D8010000}"/>
+    <cellStyle name="Normal 6 6 2 2 4 2" xfId="199" xr:uid="{00000000-0005-0000-0000-0000D9010000}"/>
+    <cellStyle name="Normal 6 6 2 2 4 3" xfId="198" xr:uid="{00000000-0005-0000-0000-0000DA010000}"/>
+    <cellStyle name="Normal 6 6 2 2 5" xfId="77" xr:uid="{00000000-0005-0000-0000-0000DB010000}"/>
+    <cellStyle name="Normal 6 6 2 2 6" xfId="129" xr:uid="{00000000-0005-0000-0000-0000DC010000}"/>
+    <cellStyle name="Normal 6 6 2 3" xfId="163" xr:uid="{00000000-0005-0000-0000-0000DD010000}"/>
+    <cellStyle name="Normal 6 6 2 3 2" xfId="662" xr:uid="{00000000-0005-0000-0000-0000DE010000}"/>
+    <cellStyle name="Normal 6 6 2 3 2 2" xfId="278" xr:uid="{00000000-0005-0000-0000-0000DF010000}"/>
+    <cellStyle name="Normal 6 6 2 3 2 3" xfId="279" xr:uid="{00000000-0005-0000-0000-0000E0010000}"/>
+    <cellStyle name="Normal 6 6 2 3 3" xfId="1" xr:uid="{00000000-0005-0000-0000-0000E1010000}"/>
+    <cellStyle name="Normal 6 6 2 3 4" xfId="2" xr:uid="{00000000-0005-0000-0000-0000E2010000}"/>
+    <cellStyle name="Normal 6 6 2 4" xfId="586" xr:uid="{00000000-0005-0000-0000-0000E3010000}"/>
+    <cellStyle name="Normal 6 6 2 4 2" xfId="581" xr:uid="{00000000-0005-0000-0000-0000E4010000}"/>
+    <cellStyle name="Normal 6 6 2 4 2 2" xfId="383" xr:uid="{00000000-0005-0000-0000-0000E5010000}"/>
+    <cellStyle name="Normal 6 6 2 4 2 3" xfId="516" xr:uid="{00000000-0005-0000-0000-0000E6010000}"/>
+    <cellStyle name="Normal 6 6 2 4 3" xfId="580" xr:uid="{00000000-0005-0000-0000-0000E7010000}"/>
+    <cellStyle name="Normal 6 6 2 4 4" xfId="579" xr:uid="{00000000-0005-0000-0000-0000E8010000}"/>
+    <cellStyle name="Normal 6 6 2 5" xfId="159" xr:uid="{00000000-0005-0000-0000-0000E9010000}"/>
+    <cellStyle name="Normal 6 6 2 5 2" xfId="141" xr:uid="{00000000-0005-0000-0000-0000EA010000}"/>
+    <cellStyle name="Normal 6 6 2 5 3" xfId="142" xr:uid="{00000000-0005-0000-0000-0000EB010000}"/>
+    <cellStyle name="Normal 6 6 2 6" xfId="162" xr:uid="{00000000-0005-0000-0000-0000EC010000}"/>
+    <cellStyle name="Normal 6 6 2 7" xfId="161" xr:uid="{00000000-0005-0000-0000-0000ED010000}"/>
+    <cellStyle name="Normal 6 6 3" xfId="325" xr:uid="{00000000-0005-0000-0000-0000EE010000}"/>
+    <cellStyle name="Normal 6 6 3 2" xfId="374" xr:uid="{00000000-0005-0000-0000-0000EF010000}"/>
+    <cellStyle name="Normal 6 6 3 2 2" xfId="275" xr:uid="{00000000-0005-0000-0000-0000F0010000}"/>
+    <cellStyle name="Normal 6 6 3 2 2 2" xfId="410" xr:uid="{00000000-0005-0000-0000-0000F1010000}"/>
+    <cellStyle name="Normal 6 6 3 2 2 3" xfId="411" xr:uid="{00000000-0005-0000-0000-0000F2010000}"/>
+    <cellStyle name="Normal 6 6 3 2 3" xfId="362" xr:uid="{00000000-0005-0000-0000-0000F3010000}"/>
+    <cellStyle name="Normal 6 6 3 2 4" xfId="277" xr:uid="{00000000-0005-0000-0000-0000F4010000}"/>
+    <cellStyle name="Normal 6 6 3 3" xfId="186" xr:uid="{00000000-0005-0000-0000-0000F5010000}"/>
+    <cellStyle name="Normal 6 6 3 3 2" xfId="105" xr:uid="{00000000-0005-0000-0000-0000F6010000}"/>
+    <cellStyle name="Normal 6 6 3 3 2 2" xfId="300" xr:uid="{00000000-0005-0000-0000-0000F7010000}"/>
+    <cellStyle name="Normal 6 6 3 3 2 3" xfId="299" xr:uid="{00000000-0005-0000-0000-0000F8010000}"/>
+    <cellStyle name="Normal 6 6 3 3 3" xfId="104" xr:uid="{00000000-0005-0000-0000-0000F9010000}"/>
+    <cellStyle name="Normal 6 6 3 3 4" xfId="574" xr:uid="{00000000-0005-0000-0000-0000FA010000}"/>
+    <cellStyle name="Normal 6 6 3 4" xfId="371" xr:uid="{00000000-0005-0000-0000-0000FB010000}"/>
+    <cellStyle name="Normal 6 6 3 4 2" xfId="391" xr:uid="{00000000-0005-0000-0000-0000FC010000}"/>
+    <cellStyle name="Normal 6 6 3 4 3" xfId="392" xr:uid="{00000000-0005-0000-0000-0000FD010000}"/>
+    <cellStyle name="Normal 6 6 3 5" xfId="372" xr:uid="{00000000-0005-0000-0000-0000FE010000}"/>
+    <cellStyle name="Normal 6 6 3 6" xfId="373" xr:uid="{00000000-0005-0000-0000-0000FF010000}"/>
+    <cellStyle name="Normal 6 6 4" xfId="108" xr:uid="{00000000-0005-0000-0000-000000020000}"/>
+    <cellStyle name="Normal 6 6 4 2" xfId="435" xr:uid="{00000000-0005-0000-0000-000001020000}"/>
+    <cellStyle name="Normal 6 6 4 2 2" xfId="433" xr:uid="{00000000-0005-0000-0000-000002020000}"/>
+    <cellStyle name="Normal 6 6 4 2 3" xfId="432" xr:uid="{00000000-0005-0000-0000-000003020000}"/>
+    <cellStyle name="Normal 6 6 4 3" xfId="434" xr:uid="{00000000-0005-0000-0000-000004020000}"/>
+    <cellStyle name="Normal 6 6 4 4" xfId="438" xr:uid="{00000000-0005-0000-0000-000005020000}"/>
+    <cellStyle name="Normal 6 6 5" xfId="585" xr:uid="{00000000-0005-0000-0000-000006020000}"/>
+    <cellStyle name="Normal 6 6 5 2" xfId="596" xr:uid="{00000000-0005-0000-0000-000007020000}"/>
+    <cellStyle name="Normal 6 6 5 2 2" xfId="554" xr:uid="{00000000-0005-0000-0000-000008020000}"/>
+    <cellStyle name="Normal 6 6 5 2 3" xfId="555" xr:uid="{00000000-0005-0000-0000-000009020000}"/>
+    <cellStyle name="Normal 6 6 5 3" xfId="597" xr:uid="{00000000-0005-0000-0000-00000A020000}"/>
+    <cellStyle name="Normal 6 6 5 4" xfId="598" xr:uid="{00000000-0005-0000-0000-00000B020000}"/>
+    <cellStyle name="Normal 6 6 6" xfId="616" xr:uid="{00000000-0005-0000-0000-00000C020000}"/>
+    <cellStyle name="Normal 6 6 6 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00000D020000}"/>
+    <cellStyle name="Normal 6 6 6 3" xfId="28" xr:uid="{00000000-0005-0000-0000-00000E020000}"/>
+    <cellStyle name="Normal 6 6 7" xfId="507" xr:uid="{00000000-0005-0000-0000-00000F020000}"/>
+    <cellStyle name="Normal 6 6 8" xfId="513" xr:uid="{00000000-0005-0000-0000-000010020000}"/>
+    <cellStyle name="Normal 6 7" xfId="312" xr:uid="{00000000-0005-0000-0000-000011020000}"/>
+    <cellStyle name="Normal 6 7 2" xfId="65" xr:uid="{00000000-0005-0000-0000-000012020000}"/>
+    <cellStyle name="Normal 6 7 2 2" xfId="610" xr:uid="{00000000-0005-0000-0000-000013020000}"/>
+    <cellStyle name="Normal 6 7 2 2 2" xfId="122" xr:uid="{00000000-0005-0000-0000-000014020000}"/>
+    <cellStyle name="Normal 6 7 2 2 2 2" xfId="615" xr:uid="{00000000-0005-0000-0000-000015020000}"/>
+    <cellStyle name="Normal 6 7 2 2 2 2 2" xfId="243" xr:uid="{00000000-0005-0000-0000-000016020000}"/>
+    <cellStyle name="Normal 6 7 2 2 2 2 3" xfId="244" xr:uid="{00000000-0005-0000-0000-000017020000}"/>
+    <cellStyle name="Normal 6 7 2 2 2 3" xfId="120" xr:uid="{00000000-0005-0000-0000-000018020000}"/>
+    <cellStyle name="Normal 6 7 2 2 2 4" xfId="562" xr:uid="{00000000-0005-0000-0000-000019020000}"/>
+    <cellStyle name="Normal 6 7 2 2 3" xfId="123" xr:uid="{00000000-0005-0000-0000-00001A020000}"/>
+    <cellStyle name="Normal 6 7 2 2 3 2" xfId="358" xr:uid="{00000000-0005-0000-0000-00001B020000}"/>
+    <cellStyle name="Normal 6 7 2 2 3 2 2" xfId="390" xr:uid="{00000000-0005-0000-0000-00001C020000}"/>
+    <cellStyle name="Normal 6 7 2 2 3 2 3" xfId="144" xr:uid="{00000000-0005-0000-0000-00001D020000}"/>
+    <cellStyle name="Normal 6 7 2 2 3 3" xfId="357" xr:uid="{00000000-0005-0000-0000-00001E020000}"/>
+    <cellStyle name="Normal 6 7 2 2 3 4" xfId="359" xr:uid="{00000000-0005-0000-0000-00001F020000}"/>
+    <cellStyle name="Normal 6 7 2 2 4" xfId="124" xr:uid="{00000000-0005-0000-0000-000020020000}"/>
+    <cellStyle name="Normal 6 7 2 2 4 2" xfId="170" xr:uid="{00000000-0005-0000-0000-000021020000}"/>
+    <cellStyle name="Normal 6 7 2 2 4 3" xfId="171" xr:uid="{00000000-0005-0000-0000-000022020000}"/>
+    <cellStyle name="Normal 6 7 2 2 5" xfId="125" xr:uid="{00000000-0005-0000-0000-000023020000}"/>
+    <cellStyle name="Normal 6 7 2 2 6" xfId="126" xr:uid="{00000000-0005-0000-0000-000024020000}"/>
+    <cellStyle name="Normal 6 7 2 3" xfId="611" xr:uid="{00000000-0005-0000-0000-000025020000}"/>
+    <cellStyle name="Normal 6 7 2 3 2" xfId="572" xr:uid="{00000000-0005-0000-0000-000026020000}"/>
+    <cellStyle name="Normal 6 7 2 3 2 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000027020000}"/>
+    <cellStyle name="Normal 6 7 2 3 2 3" xfId="327" xr:uid="{00000000-0005-0000-0000-000028020000}"/>
+    <cellStyle name="Normal 6 7 2 3 3" xfId="571" xr:uid="{00000000-0005-0000-0000-000029020000}"/>
+    <cellStyle name="Normal 6 7 2 3 4" xfId="573" xr:uid="{00000000-0005-0000-0000-00002A020000}"/>
+    <cellStyle name="Normal 6 7 2 4" xfId="606" xr:uid="{00000000-0005-0000-0000-00002B020000}"/>
+    <cellStyle name="Normal 6 7 2 4 2" xfId="272" xr:uid="{00000000-0005-0000-0000-00002C020000}"/>
+    <cellStyle name="Normal 6 7 2 4 2 2" xfId="179" xr:uid="{00000000-0005-0000-0000-00002D020000}"/>
+    <cellStyle name="Normal 6 7 2 4 2 3" xfId="536" xr:uid="{00000000-0005-0000-0000-00002E020000}"/>
+    <cellStyle name="Normal 6 7 2 4 3" xfId="273" xr:uid="{00000000-0005-0000-0000-00002F020000}"/>
+    <cellStyle name="Normal 6 7 2 4 4" xfId="271" xr:uid="{00000000-0005-0000-0000-000030020000}"/>
+    <cellStyle name="Normal 6 7 2 5" xfId="607" xr:uid="{00000000-0005-0000-0000-000031020000}"/>
+    <cellStyle name="Normal 6 7 2 5 2" xfId="86" xr:uid="{00000000-0005-0000-0000-000032020000}"/>
+    <cellStyle name="Normal 6 7 2 5 3" xfId="85" xr:uid="{00000000-0005-0000-0000-000033020000}"/>
+    <cellStyle name="Normal 6 7 2 6" xfId="608" xr:uid="{00000000-0005-0000-0000-000034020000}"/>
+    <cellStyle name="Normal 6 7 2 7" xfId="609" xr:uid="{00000000-0005-0000-0000-000035020000}"/>
+    <cellStyle name="Normal 6 7 3" xfId="66" xr:uid="{00000000-0005-0000-0000-000036020000}"/>
+    <cellStyle name="Normal 6 7 3 2" xfId="409" xr:uid="{00000000-0005-0000-0000-000037020000}"/>
+    <cellStyle name="Normal 6 7 3 2 2" xfId="476" xr:uid="{00000000-0005-0000-0000-000038020000}"/>
+    <cellStyle name="Normal 6 7 3 2 2 2" xfId="353" xr:uid="{00000000-0005-0000-0000-000039020000}"/>
+    <cellStyle name="Normal 6 7 3 2 2 3" xfId="352" xr:uid="{00000000-0005-0000-0000-00003A020000}"/>
+    <cellStyle name="Normal 6 7 3 2 3" xfId="475" xr:uid="{00000000-0005-0000-0000-00003B020000}"/>
+    <cellStyle name="Normal 6 7 3 2 4" xfId="477" xr:uid="{00000000-0005-0000-0000-00003C020000}"/>
+    <cellStyle name="Normal 6 7 3 3" xfId="418" xr:uid="{00000000-0005-0000-0000-00003D020000}"/>
+    <cellStyle name="Normal 6 7 3 3 2" xfId="650" xr:uid="{00000000-0005-0000-0000-00003E020000}"/>
+    <cellStyle name="Normal 6 7 3 3 2 2" xfId="19" xr:uid="{00000000-0005-0000-0000-00003F020000}"/>
+    <cellStyle name="Normal 6 7 3 3 2 3" xfId="23" xr:uid="{00000000-0005-0000-0000-000040020000}"/>
+    <cellStyle name="Normal 6 7 3 3 3" xfId="651" xr:uid="{00000000-0005-0000-0000-000041020000}"/>
+    <cellStyle name="Normal 6 7 3 3 4" xfId="652" xr:uid="{00000000-0005-0000-0000-000042020000}"/>
+    <cellStyle name="Normal 6 7 3 4" xfId="414" xr:uid="{00000000-0005-0000-0000-000043020000}"/>
+    <cellStyle name="Normal 6 7 3 4 2" xfId="563" xr:uid="{00000000-0005-0000-0000-000044020000}"/>
+    <cellStyle name="Normal 6 7 3 4 3" xfId="620" xr:uid="{00000000-0005-0000-0000-000045020000}"/>
+    <cellStyle name="Normal 6 7 3 5" xfId="413" xr:uid="{00000000-0005-0000-0000-000046020000}"/>
+    <cellStyle name="Normal 6 7 3 6" xfId="407" xr:uid="{00000000-0005-0000-0000-000047020000}"/>
+    <cellStyle name="Normal 6 7 4" xfId="60" xr:uid="{00000000-0005-0000-0000-000048020000}"/>
+    <cellStyle name="Normal 6 7 4 2" xfId="166" xr:uid="{00000000-0005-0000-0000-000049020000}"/>
+    <cellStyle name="Normal 6 7 4 2 2" xfId="509" xr:uid="{00000000-0005-0000-0000-00004A020000}"/>
+    <cellStyle name="Normal 6 7 4 2 3" xfId="510" xr:uid="{00000000-0005-0000-0000-00004B020000}"/>
+    <cellStyle name="Normal 6 7 4 3" xfId="490" xr:uid="{00000000-0005-0000-0000-00004C020000}"/>
+    <cellStyle name="Normal 6 7 4 4" xfId="494" xr:uid="{00000000-0005-0000-0000-00004D020000}"/>
+    <cellStyle name="Normal 6 7 5" xfId="61" xr:uid="{00000000-0005-0000-0000-00004E020000}"/>
+    <cellStyle name="Normal 6 7 5 2" xfId="638" xr:uid="{00000000-0005-0000-0000-00004F020000}"/>
+    <cellStyle name="Normal 6 7 5 2 2" xfId="152" xr:uid="{00000000-0005-0000-0000-000050020000}"/>
+    <cellStyle name="Normal 6 7 5 2 3" xfId="38" xr:uid="{00000000-0005-0000-0000-000051020000}"/>
+    <cellStyle name="Normal 6 7 5 3" xfId="637" xr:uid="{00000000-0005-0000-0000-000052020000}"/>
+    <cellStyle name="Normal 6 7 5 4" xfId="641" xr:uid="{00000000-0005-0000-0000-000053020000}"/>
+    <cellStyle name="Normal 6 7 6" xfId="62" xr:uid="{00000000-0005-0000-0000-000054020000}"/>
+    <cellStyle name="Normal 6 7 6 2" xfId="415" xr:uid="{00000000-0005-0000-0000-000055020000}"/>
+    <cellStyle name="Normal 6 7 6 3" xfId="416" xr:uid="{00000000-0005-0000-0000-000056020000}"/>
+    <cellStyle name="Normal 6 7 7" xfId="63" xr:uid="{00000000-0005-0000-0000-000057020000}"/>
+    <cellStyle name="Normal 6 7 8" xfId="59" xr:uid="{00000000-0005-0000-0000-000058020000}"/>
+    <cellStyle name="Normal 6 8" xfId="308" xr:uid="{00000000-0005-0000-0000-000059020000}"/>
+    <cellStyle name="Normal 6 8 2" xfId="364" xr:uid="{00000000-0005-0000-0000-00005A020000}"/>
+    <cellStyle name="Normal 6 8 2 2" xfId="146" xr:uid="{00000000-0005-0000-0000-00005B020000}"/>
+    <cellStyle name="Normal 6 8 2 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-00005C020000}"/>
+    <cellStyle name="Normal 6 8 2 2 2 2" xfId="345" xr:uid="{00000000-0005-0000-0000-00005D020000}"/>
+    <cellStyle name="Normal 6 8 2 2 2 3" xfId="344" xr:uid="{00000000-0005-0000-0000-00005E020000}"/>
+    <cellStyle name="Normal 6 8 2 2 3" xfId="18" xr:uid="{00000000-0005-0000-0000-00005F020000}"/>
+    <cellStyle name="Normal 6 8 2 2 4" xfId="575" xr:uid="{00000000-0005-0000-0000-000060020000}"/>
+    <cellStyle name="Normal 6 8 2 3" xfId="145" xr:uid="{00000000-0005-0000-0000-000061020000}"/>
+    <cellStyle name="Normal 6 8 2 3 2" xfId="240" xr:uid="{00000000-0005-0000-0000-000062020000}"/>
+    <cellStyle name="Normal 6 8 2 3 2 2" xfId="202" xr:uid="{00000000-0005-0000-0000-000063020000}"/>
+    <cellStyle name="Normal 6 8 2 3 2 3" xfId="203" xr:uid="{00000000-0005-0000-0000-000064020000}"/>
+    <cellStyle name="Normal 6 8 2 3 3" xfId="241" xr:uid="{00000000-0005-0000-0000-000065020000}"/>
+    <cellStyle name="Normal 6 8 2 3 4" xfId="239" xr:uid="{00000000-0005-0000-0000-000066020000}"/>
+    <cellStyle name="Normal 6 8 2 4" xfId="149" xr:uid="{00000000-0005-0000-0000-000067020000}"/>
+    <cellStyle name="Normal 6 8 2 4 2" xfId="625" xr:uid="{00000000-0005-0000-0000-000068020000}"/>
+    <cellStyle name="Normal 6 8 2 4 3" xfId="624" xr:uid="{00000000-0005-0000-0000-000069020000}"/>
+    <cellStyle name="Normal 6 8 2 5" xfId="148" xr:uid="{00000000-0005-0000-0000-00006A020000}"/>
+    <cellStyle name="Normal 6 8 2 6" xfId="147" xr:uid="{00000000-0005-0000-0000-00006B020000}"/>
+    <cellStyle name="Normal 6 8 3" xfId="363" xr:uid="{00000000-0005-0000-0000-00006C020000}"/>
+    <cellStyle name="Normal 6 8 3 2" xfId="350" xr:uid="{00000000-0005-0000-0000-00006D020000}"/>
+    <cellStyle name="Normal 6 8 3 2 2" xfId="488" xr:uid="{00000000-0005-0000-0000-00006E020000}"/>
+    <cellStyle name="Normal 6 8 3 2 3" xfId="489" xr:uid="{00000000-0005-0000-0000-00006F020000}"/>
+    <cellStyle name="Normal 6 8 3 3" xfId="351" xr:uid="{00000000-0005-0000-0000-000070020000}"/>
+    <cellStyle name="Normal 6 8 3 4" xfId="354" xr:uid="{00000000-0005-0000-0000-000071020000}"/>
+    <cellStyle name="Normal 6 8 4" xfId="368" xr:uid="{00000000-0005-0000-0000-000072020000}"/>
+    <cellStyle name="Normal 6 8 4 2" xfId="565" xr:uid="{00000000-0005-0000-0000-000073020000}"/>
+    <cellStyle name="Normal 6 8 4 2 2" xfId="165" xr:uid="{00000000-0005-0000-0000-000074020000}"/>
+    <cellStyle name="Normal 6 8 4 2 3" xfId="446" xr:uid="{00000000-0005-0000-0000-000075020000}"/>
+    <cellStyle name="Normal 6 8 4 3" xfId="564" xr:uid="{00000000-0005-0000-0000-000076020000}"/>
+    <cellStyle name="Normal 6 8 4 4" xfId="559" xr:uid="{00000000-0005-0000-0000-000077020000}"/>
+    <cellStyle name="Normal 6 8 5" xfId="367" xr:uid="{00000000-0005-0000-0000-000078020000}"/>
+    <cellStyle name="Normal 6 8 5 2" xfId="102" xr:uid="{00000000-0005-0000-0000-000079020000}"/>
+    <cellStyle name="Normal 6 8 5 3" xfId="103" xr:uid="{00000000-0005-0000-0000-00007A020000}"/>
+    <cellStyle name="Normal 6 8 6" xfId="366" xr:uid="{00000000-0005-0000-0000-00007B020000}"/>
+    <cellStyle name="Normal 6 8 7" xfId="365" xr:uid="{00000000-0005-0000-0000-00007C020000}"/>
+    <cellStyle name="Normal 6 9" xfId="307" xr:uid="{00000000-0005-0000-0000-00007D020000}"/>
+    <cellStyle name="Normal 6 9 2" xfId="537" xr:uid="{00000000-0005-0000-0000-00007E020000}"/>
+    <cellStyle name="Normal 6 9 2 2" xfId="215" xr:uid="{00000000-0005-0000-0000-00007F020000}"/>
+    <cellStyle name="Normal 6 9 2 2 2" xfId="264" xr:uid="{00000000-0005-0000-0000-000080020000}"/>
+    <cellStyle name="Normal 6 9 2 2 3" xfId="265" xr:uid="{00000000-0005-0000-0000-000081020000}"/>
+    <cellStyle name="Normal 6 9 2 3" xfId="566" xr:uid="{00000000-0005-0000-0000-000082020000}"/>
+    <cellStyle name="Normal 6 9 2 4" xfId="217" xr:uid="{00000000-0005-0000-0000-000083020000}"/>
+    <cellStyle name="Normal 6 9 3" xfId="538" xr:uid="{00000000-0005-0000-0000-000084020000}"/>
+    <cellStyle name="Normal 6 9 3 2" xfId="658" xr:uid="{00000000-0005-0000-0000-000085020000}"/>
+    <cellStyle name="Normal 6 9 3 2 2" xfId="426" xr:uid="{00000000-0005-0000-0000-000086020000}"/>
+    <cellStyle name="Normal 6 9 3 2 3" xfId="425" xr:uid="{00000000-0005-0000-0000-000087020000}"/>
+    <cellStyle name="Normal 6 9 3 3" xfId="657" xr:uid="{00000000-0005-0000-0000-000088020000}"/>
+    <cellStyle name="Normal 6 9 3 4" xfId="659" xr:uid="{00000000-0005-0000-0000-000089020000}"/>
+    <cellStyle name="Normal 6 9 4" xfId="540" xr:uid="{00000000-0005-0000-0000-00008A020000}"/>
+    <cellStyle name="Normal 6 9 4 2" xfId="640" xr:uid="{00000000-0005-0000-0000-00008B020000}"/>
+    <cellStyle name="Normal 6 9 4 3" xfId="567" xr:uid="{00000000-0005-0000-0000-00008C020000}"/>
+    <cellStyle name="Normal 6 9 5" xfId="541" xr:uid="{00000000-0005-0000-0000-00008D020000}"/>
+    <cellStyle name="Normal 6 9 6" xfId="539" xr:uid="{00000000-0005-0000-0000-00008E020000}"/>
+    <cellStyle name="Normal 7" xfId="452" xr:uid="{00000000-0005-0000-0000-00008F020000}"/>
+    <cellStyle name="Normal 7 2" xfId="529" xr:uid="{00000000-0005-0000-0000-000090020000}"/>
+    <cellStyle name="Normal 8" xfId="455" xr:uid="{00000000-0005-0000-0000-000091020000}"/>
+    <cellStyle name="Normal 8 2" xfId="576" xr:uid="{00000000-0005-0000-0000-000092020000}"/>
+    <cellStyle name="Normal 9" xfId="454" xr:uid="{00000000-0005-0000-0000-000093020000}"/>
+    <cellStyle name="Normal 9 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000094020000}"/>
+    <cellStyle name="Percent 2" xfId="269" xr:uid="{00000000-0005-0000-0000-000095020000}"/>
+    <cellStyle name="Percent 2 2" xfId="78" xr:uid="{00000000-0005-0000-0000-000096020000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1958,6 +1959,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1993,6 +2011,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2168,29 +2203,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="54.5703125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="54.54296875" style="12" customWidth="1"/>
     <col min="2" max="2" width="18" style="14" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="16" width="9.140625" style="12" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="12"/>
+    <col min="3" max="5" width="9.1796875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7265625" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="16" width="9.1796875" style="12" customWidth="1"/>
+    <col min="17" max="16384" width="9.1796875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2198,7 +2233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -2214,7 +2249,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>3</v>
       </c>
@@ -2224,7 +2259,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>4</v>
       </c>
@@ -2234,7 +2269,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
@@ -2244,7 +2279,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>6</v>
       </c>
@@ -2254,7 +2289,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>7</v>
       </c>
@@ -2264,7 +2299,7 @@
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>8</v>
       </c>
@@ -2277,17 +2312,17 @@
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="18">
-        <v>6474559.8259087466</v>
-      </c>
-      <c r="F9" s="13"/>
+        <v>6000000</v>
+      </c>
+      <c r="F9" s="18"/>
       <c r="G9" s="13"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>10</v>
       </c>
@@ -2297,7 +2332,7 @@
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
         <v>11</v>
       </c>
@@ -2305,7 +2340,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>12</v>
       </c>
@@ -2313,7 +2348,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>13</v>
       </c>
@@ -2324,7 +2359,7 @@
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>14</v>
       </c>
@@ -2337,7 +2372,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>16</v>
       </c>
@@ -2345,7 +2380,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
         <v>17</v>
       </c>
@@ -2353,7 +2388,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
         <v>18</v>
       </c>
@@ -2361,7 +2396,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>19</v>
       </c>
@@ -2369,7 +2404,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>20</v>
       </c>
@@ -2377,7 +2412,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>21</v>
       </c>
@@ -2385,7 +2420,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="25" t="s">
         <v>22</v>
       </c>
@@ -2400,7 +2435,7 @@
       </c>
       <c r="E21" s="25"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="25" t="s">
         <v>23</v>
       </c>
@@ -2415,7 +2450,7 @@
       </c>
       <c r="E22" s="25"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
         <v>24</v>
       </c>
@@ -2426,7 +2461,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
         <v>26</v>
       </c>
@@ -2434,7 +2469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
         <v>27</v>
       </c>
@@ -2442,7 +2477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
         <v>28</v>
       </c>
@@ -2450,7 +2485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
         <v>29</v>
       </c>
@@ -2458,7 +2493,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
         <v>30</v>
       </c>
@@ -2469,7 +2504,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>31</v>
       </c>
@@ -2477,7 +2512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="12" t="s">
         <v>32</v>
       </c>
@@ -2485,7 +2520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
         <v>33</v>
       </c>
@@ -2493,7 +2528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
         <v>34</v>
       </c>
@@ -2501,7 +2536,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="12" t="s">
         <v>35</v>
       </c>
@@ -2513,7 +2548,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="12" t="s">
         <v>37</v>
       </c>
@@ -2521,7 +2556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="12" t="s">
         <v>38</v>
       </c>
@@ -2532,7 +2567,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="12" t="s">
         <v>40</v>
       </c>
@@ -2540,7 +2575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
         <v>41</v>
       </c>
@@ -2548,7 +2583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
         <v>42</v>
       </c>
@@ -2557,7 +2592,7 @@
         <v>-1767</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
         <v>43</v>
       </c>
@@ -2565,7 +2600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="12" t="s">
         <v>44</v>
       </c>
@@ -2573,7 +2608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
         <v>45</v>
       </c>
@@ -2581,19 +2616,18 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="12" t="s">
         <v>46</v>
       </c>
       <c r="B42" s="12">
-        <f>751-1643</f>
-        <v>-892</v>
+        <v>1643</v>
       </c>
       <c r="E42" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="12" t="s">
         <v>48</v>
       </c>
@@ -2601,7 +2635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="12" t="s">
         <v>49</v>
       </c>
@@ -2609,7 +2643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="12" t="s">
         <v>50</v>
       </c>
@@ -2617,7 +2651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="12" t="s">
         <v>51</v>
       </c>
@@ -2625,19 +2659,18 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="12" t="s">
         <v>52</v>
       </c>
       <c r="B47" s="12">
-        <f>862-1746</f>
-        <v>-884</v>
+        <v>1746</v>
       </c>
       <c r="E47" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="12" t="s">
         <v>54</v>
       </c>
@@ -2645,7 +2678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="12" t="s">
         <v>55</v>
       </c>
@@ -2653,7 +2686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="12" t="s">
         <v>56</v>
       </c>
@@ -2661,7 +2694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="12" t="s">
         <v>57</v>
       </c>
@@ -2669,7 +2702,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -2677,7 +2710,7 @@
         <v>0.59435254157623596</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -2685,7 +2718,7 @@
         <v>0.74733094259578403</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -2695,24 +2728,24 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="G9:G10 F9:F10 B3:B6 B8:B10">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="F9:G10 B3:B6 B8 B10" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B2 F2:F6 G2:G6">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B2 F2:G6" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B7 F7:F8 G7:G8">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B7 F7:G8" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" promptTitle="Age unstratified" prompt="Some values you can replace the ones to the left with if you want a manual calibration for the model without age stratification." sqref="H1"/>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B4:B14 C14 D14">
+    <dataValidation showInputMessage="1" showErrorMessage="1" promptTitle="Age unstratified" prompt="Some values you can replace the ones to the left with if you want a manual calibration for the model without age stratification." sqref="H1" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="F9 C14:D14 B4:B8 B10:B14" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B7"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B7 B9 B9" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2720,41 +2753,41 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:X34"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X10" sqref="X10"/>
+      <selection pane="bottomRight" activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" style="4" customWidth="1"/>
     <col min="3" max="3" width="11" style="4" customWidth="1"/>
     <col min="4" max="4" width="11" style="5" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" style="23" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" style="23" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" style="23" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" style="23" customWidth="1"/>
+    <col min="5" max="5" width="7.1796875" style="23" customWidth="1"/>
+    <col min="6" max="6" width="7.453125" style="23" customWidth="1"/>
+    <col min="7" max="7" width="17.54296875" style="23" customWidth="1"/>
+    <col min="8" max="8" width="11.26953125" style="23" customWidth="1"/>
     <col min="9" max="12" width="7" style="23" customWidth="1"/>
-    <col min="13" max="14" width="7.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.42578125" style="23" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" style="23" customWidth="1"/>
+    <col min="13" max="14" width="7.453125" style="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.453125" style="23" customWidth="1"/>
+    <col min="16" max="16" width="16.1796875" style="23" customWidth="1"/>
     <col min="17" max="18" width="14" style="23" customWidth="1"/>
-    <col min="19" max="19" width="14.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="20" max="23" width="14.42578125" style="23" customWidth="1"/>
-    <col min="24" max="30" width="9.140625" style="23" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="23"/>
+    <col min="19" max="19" width="14.453125" style="23" bestFit="1" customWidth="1"/>
+    <col min="20" max="23" width="14.453125" style="23" customWidth="1"/>
+    <col min="24" max="30" width="9.1796875" style="23" customWidth="1"/>
+    <col min="31" max="16384" width="9.1796875" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>61</v>
       </c>
@@ -2828,7 +2861,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
         <v>72</v>
       </c>
@@ -2843,8 +2876,14 @@
       </c>
       <c r="S2" s="24"/>
       <c r="T2" s="24"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W2" s="23">
+        <v>50</v>
+      </c>
+      <c r="X2" s="23">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
         <v>74</v>
       </c>
@@ -2863,7 +2902,7 @@
       <c r="S3" s="24"/>
       <c r="T3" s="24"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
         <v>75</v>
       </c>
@@ -2883,7 +2922,7 @@
       <c r="T4" s="24"/>
       <c r="U4" s="24"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
         <v>76</v>
       </c>
@@ -2901,11 +2940,14 @@
       </c>
       <c r="T5" s="24"/>
       <c r="U5" s="24"/>
+      <c r="W5" s="23">
+        <v>100</v>
+      </c>
       <c r="X5" s="23">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
         <v>77</v>
       </c>
@@ -2922,7 +2964,7 @@
       <c r="T6" s="24"/>
       <c r="U6" s="24"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
         <v>78</v>
       </c>
@@ -2964,8 +3006,14 @@
       <c r="R7" s="23">
         <v>95</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W7" s="23">
+        <v>95</v>
+      </c>
+      <c r="X7" s="23">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
         <v>79</v>
       </c>
@@ -2981,7 +3029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" s="16" t="s">
         <v>80</v>
       </c>
@@ -3000,7 +3048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" s="16" t="s">
         <v>81</v>
       </c>
@@ -3015,8 +3063,14 @@
         <v>100</v>
       </c>
       <c r="V10" s="24"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W10" s="23">
+        <v>100</v>
+      </c>
+      <c r="X10" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="s">
         <v>82</v>
       </c>
@@ -3031,8 +3085,14 @@
         <v>100</v>
       </c>
       <c r="V11" s="24"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W11" s="23">
+        <v>100</v>
+      </c>
+      <c r="X11" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A12" s="16" t="s">
         <v>83</v>
       </c>
@@ -3064,7 +3124,7 @@
         <v>117.42738589211601</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
         <v>84</v>
       </c>
@@ -3078,7 +3138,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
         <v>85</v>
       </c>
@@ -3092,7 +3152,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
         <v>86</v>
       </c>
@@ -3105,11 +3165,8 @@
       <c r="P15" s="23">
         <v>8.5</v>
       </c>
-      <c r="W15" s="23">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
         <v>87</v>
       </c>
@@ -3131,7 +3188,7 @@
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
     </row>
-    <row r="18" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:23" x14ac:dyDescent="0.35">
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -3145,12 +3202,12 @@
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
     </row>
-    <row r="23" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:23" x14ac:dyDescent="0.35">
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:23" x14ac:dyDescent="0.35">
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
@@ -3162,61 +3219,61 @@
       <c r="V24" s="22"/>
       <c r="W24" s="22"/>
     </row>
-    <row r="25" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:23" x14ac:dyDescent="0.35">
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
       <c r="S25" s="24"/>
       <c r="T25" s="24"/>
     </row>
-    <row r="26" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:23" x14ac:dyDescent="0.35">
       <c r="S26" s="24"/>
       <c r="T26" s="24"/>
     </row>
-    <row r="27" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:23" x14ac:dyDescent="0.35">
       <c r="S27" s="24"/>
       <c r="T27" s="24"/>
       <c r="U27" s="24"/>
     </row>
-    <row r="28" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:23" x14ac:dyDescent="0.35">
       <c r="S28" s="24"/>
       <c r="T28" s="24"/>
       <c r="U28" s="24"/>
     </row>
-    <row r="29" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:23" x14ac:dyDescent="0.35">
       <c r="S29" s="24"/>
       <c r="T29" s="24"/>
       <c r="U29" s="24"/>
     </row>
-    <row r="31" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:23" x14ac:dyDescent="0.35">
       <c r="S31" s="24"/>
       <c r="T31" s="24"/>
       <c r="V31" s="24"/>
     </row>
-    <row r="32" spans="5:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:23" x14ac:dyDescent="0.35">
       <c r="S32" s="24"/>
       <c r="T32" s="24"/>
       <c r="U32" s="24"/>
       <c r="V32" s="24"/>
     </row>
-    <row r="33" spans="19:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="19:22" x14ac:dyDescent="0.35">
       <c r="S33" s="24"/>
       <c r="T33" s="24"/>
       <c r="V33" s="24"/>
     </row>
-    <row r="34" spans="19:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="19:22" x14ac:dyDescent="0.35">
       <c r="S34" s="24"/>
       <c r="T34" s="24"/>
       <c r="V34" s="24"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C1"/>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="D7 E23:P25">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="D7 E23:P25" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C1048576">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C1048576" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -3227,7 +3284,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
   </sheetPr>
@@ -3237,9 +3294,9 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -3253,7 +3310,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -3264,7 +3321,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>92</v>
       </c>

</xml_diff>